<commit_message>
Results from July 14, 2020 05:13:49 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/work/WashingtonDC/data.xlsx
+++ b/workflow/python/work/WashingtonDC/data.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="180">
   <si>
     <t>Testing</t>
   </si>
@@ -527,13 +527,7 @@
     <t>13; (10)</t>
   </si>
   <si>
-    <t>66; (23)</t>
-  </si>
-  <si>
     <t>4; (3)</t>
-  </si>
-  <si>
-    <t>98; (51)</t>
   </si>
   <si>
     <t>57; (4)</t>
@@ -554,26 +548,32 @@
     <t>21; (17)</t>
   </si>
   <si>
-    <t>65; (40)</t>
+    <t>113; (52)</t>
   </si>
   <si>
-    <t>38; (33)</t>
+    <t>67; (23)</t>
   </si>
   <si>
-    <t>676; (385)</t>
+    <t>66; (40)</t>
   </si>
   <si>
-    <t>302; (162)</t>
+    <t>40; (36)</t>
   </si>
   <si>
-    <t>978; (547)</t>
+    <t>693; (386)</t>
   </si>
   <si>
-    <t>As of June 28, 2020</t>
+    <t>304; (165)</t>
+  </si>
+  <si>
+    <t>997; (551)</t>
+  </si>
+  <si>
+    <t>As of July 10, 2020</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of July 7, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of July 13, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -1323,11 +1323,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DV119"/>
+  <dimension ref="A1:EA119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="DN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DW1" sqref="DW1"/>
+      <pane xSplit="2" topLeftCell="DV1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="EC1" sqref="EC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1343,9 +1343,10 @@
     <col min="98" max="102" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="104" max="118" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="128" max="131" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:126">
+    <row r="1" spans="1:131">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1707,19 +1708,34 @@
         <v>44016</v>
       </c>
       <c r="DS1" s="52">
-        <v>43987</v>
+        <v>44017</v>
       </c>
       <c r="DT1" s="52">
         <v>44018</v>
       </c>
       <c r="DU1" s="52">
-        <v>43989</v>
+        <v>44019</v>
       </c>
       <c r="DV1" s="52">
         <v>44020</v>
       </c>
+      <c r="DW1" s="52">
+        <v>44021</v>
+      </c>
+      <c r="DX1" s="52">
+        <v>44022</v>
+      </c>
+      <c r="DY1" s="52">
+        <v>44023</v>
+      </c>
+      <c r="DZ1" s="52">
+        <v>44024</v>
+      </c>
+      <c r="EA1" s="52">
+        <v>44025</v>
+      </c>
     </row>
-    <row r="2" spans="1:126">
+    <row r="2" spans="1:131">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1743,7 +1759,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:126">
+    <row r="3" spans="1:131">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2101,8 +2117,23 @@
       <c r="DV3">
         <v>115923</v>
       </c>
+      <c r="DW3">
+        <v>120884</v>
+      </c>
+      <c r="DX3">
+        <v>124050</v>
+      </c>
+      <c r="DY3">
+        <v>126883</v>
+      </c>
+      <c r="DZ3">
+        <v>130220</v>
+      </c>
+      <c r="EA3">
+        <v>133916</v>
+      </c>
     </row>
-    <row r="4" spans="1:126">
+    <row r="4" spans="1:131">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2255,8 +2286,23 @@
       <c r="DV4">
         <v>88060</v>
       </c>
+      <c r="DW4">
+        <v>91143</v>
+      </c>
+      <c r="DX4">
+        <v>93312</v>
+      </c>
+      <c r="DY4">
+        <v>94567</v>
+      </c>
+      <c r="DZ4">
+        <v>96163</v>
+      </c>
+      <c r="EA4">
+        <v>97908</v>
+      </c>
     </row>
-    <row r="5" spans="1:126">
+    <row r="5" spans="1:131">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2635,8 +2681,23 @@
       <c r="DV5">
         <v>10679</v>
       </c>
+      <c r="DW5">
+        <v>10743</v>
+      </c>
+      <c r="DX5">
+        <v>10801</v>
+      </c>
+      <c r="DY5">
+        <v>10847</v>
+      </c>
+      <c r="DZ5">
+        <v>10906</v>
+      </c>
+      <c r="EA5">
+        <v>10946</v>
+      </c>
     </row>
-    <row r="6" spans="1:126">
+    <row r="6" spans="1:131">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2997,8 +3058,23 @@
       <c r="DV6">
         <v>568</v>
       </c>
+      <c r="DW6">
+        <v>568</v>
+      </c>
+      <c r="DX6">
+        <v>568</v>
+      </c>
+      <c r="DY6">
+        <v>568</v>
+      </c>
+      <c r="DZ6">
+        <v>568</v>
+      </c>
+      <c r="EA6">
+        <v>568</v>
+      </c>
     </row>
-    <row r="7" spans="1:126">
+    <row r="7" spans="1:131">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3329,11 +3405,26 @@
       <c r="DV7">
         <v>1662</v>
       </c>
+      <c r="DW7">
+        <v>1703</v>
+      </c>
+      <c r="DX7">
+        <v>1717</v>
+      </c>
+      <c r="DY7">
+        <v>1737</v>
+      </c>
+      <c r="DZ7">
+        <v>1756</v>
+      </c>
+      <c r="EA7">
+        <v>1774</v>
+      </c>
     </row>
-    <row r="8" spans="1:126">
+    <row r="8" spans="1:131">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:126">
+    <row r="9" spans="1:131">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3556,8 +3647,23 @@
       <c r="DV9">
         <v>345</v>
       </c>
+      <c r="DW9">
+        <v>345</v>
+      </c>
+      <c r="DX9">
+        <v>345</v>
+      </c>
+      <c r="DY9">
+        <v>345</v>
+      </c>
+      <c r="DZ9">
+        <v>345</v>
+      </c>
+      <c r="EA9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:126">
+    <row r="10" spans="1:131">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -3882,8 +3988,23 @@
       <c r="DV10">
         <v>68</v>
       </c>
+      <c r="DW10">
+        <v>74</v>
+      </c>
+      <c r="DX10">
+        <v>73</v>
+      </c>
+      <c r="DY10">
+        <v>83</v>
+      </c>
+      <c r="DZ10">
+        <v>84</v>
+      </c>
+      <c r="EA10">
+        <v>82</v>
+      </c>
     </row>
-    <row r="11" spans="1:126">
+    <row r="11" spans="1:131">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4208,8 +4329,23 @@
       <c r="DV11">
         <v>440</v>
       </c>
+      <c r="DW11">
+        <v>440</v>
+      </c>
+      <c r="DX11">
+        <v>440</v>
+      </c>
+      <c r="DY11">
+        <v>440</v>
+      </c>
+      <c r="DZ11">
+        <v>440</v>
+      </c>
+      <c r="EA11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:126">
+    <row r="12" spans="1:131">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4534,8 +4670,23 @@
       <c r="DV12">
         <v>207</v>
       </c>
+      <c r="DW12">
+        <v>208</v>
+      </c>
+      <c r="DX12">
+        <v>204</v>
+      </c>
+      <c r="DY12">
+        <v>205</v>
+      </c>
+      <c r="DZ12">
+        <v>201</v>
+      </c>
+      <c r="EA12">
+        <v>204</v>
+      </c>
     </row>
-    <row r="13" spans="1:126">
+    <row r="13" spans="1:131">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -4860,8 +5011,23 @@
       <c r="DV13">
         <v>233</v>
       </c>
+      <c r="DW13">
+        <v>232</v>
+      </c>
+      <c r="DX13">
+        <v>236</v>
+      </c>
+      <c r="DY13">
+        <v>235</v>
+      </c>
+      <c r="DZ13">
+        <v>239</v>
+      </c>
+      <c r="EA13">
+        <v>236</v>
+      </c>
     </row>
-    <row r="14" spans="1:126">
+    <row r="14" spans="1:131">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -5048,8 +5214,23 @@
       <c r="DV14">
         <v>92</v>
       </c>
+      <c r="DW14">
+        <v>96</v>
+      </c>
+      <c r="DX14">
+        <v>92</v>
+      </c>
+      <c r="DY14">
+        <v>95</v>
+      </c>
+      <c r="DZ14">
+        <v>93</v>
+      </c>
+      <c r="EA14">
+        <v>91</v>
+      </c>
     </row>
-    <row r="15" spans="1:126">
+    <row r="15" spans="1:131">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -5206,8 +5387,23 @@
       <c r="DV15">
         <v>26</v>
       </c>
+      <c r="DW15">
+        <v>26</v>
+      </c>
+      <c r="DX15">
+        <v>29</v>
+      </c>
+      <c r="DY15">
+        <v>30</v>
+      </c>
+      <c r="DZ15">
+        <v>25</v>
+      </c>
+      <c r="EA15">
+        <v>21</v>
+      </c>
     </row>
-    <row r="16" spans="1:126">
+    <row r="16" spans="1:131">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -5394,8 +5590,23 @@
       <c r="DV16">
         <v>1963</v>
       </c>
+      <c r="DW16">
+        <v>1978</v>
+      </c>
+      <c r="DX16">
+        <v>1981</v>
+      </c>
+      <c r="DY16">
+        <v>1918</v>
+      </c>
+      <c r="DZ16">
+        <v>1874</v>
+      </c>
+      <c r="EA16">
+        <v>1866</v>
+      </c>
     </row>
-    <row r="17" spans="1:126">
+    <row r="17" spans="1:131">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -5582,13 +5793,28 @@
       <c r="DV17" s="23">
         <v>0.79</v>
       </c>
+      <c r="DW17" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="DX17" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="DY17" s="23">
+        <v>0.77</v>
+      </c>
+      <c r="DZ17" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="EA17" s="23">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="19" spans="1:126">
+    <row r="19" spans="1:131">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:126">
+    <row r="20" spans="1:131">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -5596,7 +5822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:126">
+    <row r="21" spans="1:131">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -5921,8 +6147,23 @@
       <c r="DV21">
         <v>120</v>
       </c>
+      <c r="DW21">
+        <v>120</v>
+      </c>
+      <c r="DX21">
+        <v>120</v>
+      </c>
+      <c r="DY21">
+        <v>120</v>
+      </c>
+      <c r="DZ21">
+        <v>120</v>
+      </c>
+      <c r="EA21">
+        <v>120</v>
+      </c>
     </row>
-    <row r="22" spans="1:126">
+    <row r="22" spans="1:131">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -6193,8 +6434,23 @@
       <c r="DV22">
         <v>7</v>
       </c>
+      <c r="DW22">
+        <v>7</v>
+      </c>
+      <c r="DX22">
+        <v>6</v>
+      </c>
+      <c r="DY22">
+        <v>6</v>
+      </c>
+      <c r="DZ22">
+        <v>6</v>
+      </c>
+      <c r="EA22">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="1:126">
+    <row r="23" spans="1:131">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -6465,8 +6721,23 @@
       <c r="DV23">
         <v>113</v>
       </c>
+      <c r="DW23">
+        <v>113</v>
+      </c>
+      <c r="DX23">
+        <v>114</v>
+      </c>
+      <c r="DY23">
+        <v>114</v>
+      </c>
+      <c r="DZ23">
+        <v>114</v>
+      </c>
+      <c r="EA23">
+        <v>114</v>
+      </c>
     </row>
-    <row r="24" spans="1:126">
+    <row r="24" spans="1:131">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -6782,8 +7053,23 @@
       <c r="DV24">
         <v>89</v>
       </c>
+      <c r="DW24">
+        <v>91</v>
+      </c>
+      <c r="DX24">
+        <v>85</v>
+      </c>
+      <c r="DY24">
+        <v>86</v>
+      </c>
+      <c r="DZ24">
+        <v>86</v>
+      </c>
+      <c r="EA24">
+        <v>82</v>
+      </c>
     </row>
-    <row r="25" spans="1:126">
+    <row r="25" spans="1:131">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -7099,8 +7385,23 @@
       <c r="DV25">
         <v>96</v>
       </c>
+      <c r="DW25">
+        <v>98</v>
+      </c>
+      <c r="DX25">
+        <v>91</v>
+      </c>
+      <c r="DY25">
+        <v>92</v>
+      </c>
+      <c r="DZ25">
+        <v>92</v>
+      </c>
+      <c r="EA25">
+        <v>88</v>
+      </c>
     </row>
-    <row r="26" spans="1:126">
+    <row r="26" spans="1:131">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -7416,13 +7717,28 @@
       <c r="DV26">
         <v>1684</v>
       </c>
+      <c r="DW26">
+        <v>1694</v>
+      </c>
+      <c r="DX26">
+        <v>1698</v>
+      </c>
+      <c r="DY26">
+        <v>1700</v>
+      </c>
+      <c r="DZ26">
+        <v>1700</v>
+      </c>
+      <c r="EA26">
+        <v>1704</v>
+      </c>
     </row>
-    <row r="28" spans="1:126">
+    <row r="28" spans="1:131">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:126">
+    <row r="29" spans="1:131">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -7747,8 +8063,23 @@
       <c r="DV29">
         <v>158</v>
       </c>
+      <c r="DW29">
+        <v>159</v>
+      </c>
+      <c r="DX29">
+        <v>160</v>
+      </c>
+      <c r="DY29">
+        <v>161</v>
+      </c>
+      <c r="DZ29">
+        <v>161</v>
+      </c>
+      <c r="EA29">
+        <v>165</v>
+      </c>
     </row>
-    <row r="30" spans="1:126">
+    <row r="30" spans="1:131">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -8019,8 +8350,23 @@
       <c r="DV30">
         <v>23</v>
       </c>
+      <c r="DW30">
+        <v>22</v>
+      </c>
+      <c r="DX30">
+        <v>23</v>
+      </c>
+      <c r="DY30">
+        <v>24</v>
+      </c>
+      <c r="DZ30">
+        <v>24</v>
+      </c>
+      <c r="EA30">
+        <v>28</v>
+      </c>
     </row>
-    <row r="31" spans="1:126">
+    <row r="31" spans="1:131">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -8291,8 +8637,23 @@
       <c r="DV31">
         <v>134</v>
       </c>
+      <c r="DW31">
+        <v>136</v>
+      </c>
+      <c r="DX31">
+        <v>136</v>
+      </c>
+      <c r="DY31">
+        <v>136</v>
+      </c>
+      <c r="DZ31">
+        <v>136</v>
+      </c>
+      <c r="EA31">
+        <v>136</v>
+      </c>
     </row>
-    <row r="32" spans="1:126">
+    <row r="32" spans="1:131">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -8608,8 +8969,23 @@
       <c r="DV32">
         <v>76</v>
       </c>
+      <c r="DW32">
+        <v>72</v>
+      </c>
+      <c r="DX32">
+        <v>72</v>
+      </c>
+      <c r="DY32">
+        <v>73</v>
+      </c>
+      <c r="DZ32">
+        <v>73</v>
+      </c>
+      <c r="EA32">
+        <v>93</v>
+      </c>
     </row>
-    <row r="33" spans="1:126">
+    <row r="33" spans="1:131">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -8925,8 +9301,23 @@
       <c r="DV33">
         <v>99</v>
       </c>
+      <c r="DW33">
+        <v>94</v>
+      </c>
+      <c r="DX33">
+        <v>94</v>
+      </c>
+      <c r="DY33">
+        <v>97</v>
+      </c>
+      <c r="DZ33">
+        <v>97</v>
+      </c>
+      <c r="EA33">
+        <v>121</v>
+      </c>
     </row>
-    <row r="34" spans="1:126">
+    <row r="34" spans="1:131">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -9242,8 +9633,23 @@
       <c r="DV34">
         <v>1380</v>
       </c>
+      <c r="DW34">
+        <v>1397</v>
+      </c>
+      <c r="DX34">
+        <v>1397</v>
+      </c>
+      <c r="DY34">
+        <v>1402</v>
+      </c>
+      <c r="DZ34">
+        <v>1402</v>
+      </c>
+      <c r="EA34">
+        <v>1405</v>
+      </c>
     </row>
-    <row r="35" spans="1:126">
+    <row r="35" spans="1:131">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -9340,13 +9746,28 @@
       <c r="DV35">
         <v>1</v>
       </c>
+      <c r="DW35">
+        <v>1</v>
+      </c>
+      <c r="DX35">
+        <v>1</v>
+      </c>
+      <c r="DY35">
+        <v>1</v>
+      </c>
+      <c r="DZ35">
+        <v>1</v>
+      </c>
+      <c r="EA35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:126">
+    <row r="37" spans="1:131">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:126">
+    <row r="38" spans="1:131">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -9659,8 +10080,23 @@
       <c r="DV38">
         <v>87</v>
       </c>
+      <c r="DW38">
+        <v>87</v>
+      </c>
+      <c r="DX38">
+        <v>87</v>
+      </c>
+      <c r="DY38">
+        <v>87</v>
+      </c>
+      <c r="DZ38">
+        <v>87</v>
+      </c>
+      <c r="EA38">
+        <v>87</v>
+      </c>
     </row>
-    <row r="39" spans="1:126">
+    <row r="39" spans="1:131">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -9925,8 +10361,23 @@
       <c r="DV39">
         <v>3</v>
       </c>
+      <c r="DW39">
+        <v>3</v>
+      </c>
+      <c r="DX39">
+        <v>3</v>
+      </c>
+      <c r="DY39">
+        <v>3</v>
+      </c>
+      <c r="DZ39">
+        <v>3</v>
+      </c>
+      <c r="EA39">
+        <v>3</v>
+      </c>
     </row>
-    <row r="40" spans="1:126">
+    <row r="40" spans="1:131">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -10191,8 +10642,23 @@
       <c r="DV40">
         <v>83</v>
       </c>
+      <c r="DW40">
+        <v>83</v>
+      </c>
+      <c r="DX40">
+        <v>83</v>
+      </c>
+      <c r="DY40">
+        <v>83</v>
+      </c>
+      <c r="DZ40">
+        <v>83</v>
+      </c>
+      <c r="EA40">
+        <v>83</v>
+      </c>
     </row>
-    <row r="41" spans="1:126">
+    <row r="41" spans="1:131">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -10502,8 +10968,23 @@
       <c r="DV41">
         <v>0</v>
       </c>
+      <c r="DW41">
+        <v>0</v>
+      </c>
+      <c r="DX41">
+        <v>0</v>
+      </c>
+      <c r="DY41">
+        <v>0</v>
+      </c>
+      <c r="DZ41">
+        <v>0</v>
+      </c>
+      <c r="EA41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:126">
+    <row r="42" spans="1:131">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -10810,8 +11291,23 @@
       <c r="DV42">
         <v>3</v>
       </c>
+      <c r="DW42">
+        <v>3</v>
+      </c>
+      <c r="DX42">
+        <v>3</v>
+      </c>
+      <c r="DY42">
+        <v>3</v>
+      </c>
+      <c r="DZ42">
+        <v>3</v>
+      </c>
+      <c r="EA42">
+        <v>3</v>
+      </c>
     </row>
-    <row r="43" spans="1:126">
+    <row r="43" spans="1:131">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -11124,8 +11620,23 @@
       <c r="DV43">
         <v>294</v>
       </c>
+      <c r="DW43">
+        <v>294</v>
+      </c>
+      <c r="DX43">
+        <v>294</v>
+      </c>
+      <c r="DY43">
+        <v>294</v>
+      </c>
+      <c r="DZ43">
+        <v>294</v>
+      </c>
+      <c r="EA43">
+        <v>294</v>
+      </c>
     </row>
-    <row r="44" spans="1:126">
+    <row r="44" spans="1:131">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -11372,16 +11883,31 @@
       <c r="DV44">
         <v>1</v>
       </c>
+      <c r="DW44">
+        <v>1</v>
+      </c>
+      <c r="DX44">
+        <v>1</v>
+      </c>
+      <c r="DY44">
+        <v>1</v>
+      </c>
+      <c r="DZ44">
+        <v>1</v>
+      </c>
+      <c r="EA44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:126">
+    <row r="45" spans="1:131">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:126">
+    <row r="46" spans="1:131">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:126">
+    <row r="47" spans="1:131">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -11700,8 +12226,23 @@
       <c r="DV47">
         <v>207</v>
       </c>
+      <c r="DW47">
+        <v>207</v>
+      </c>
+      <c r="DX47">
+        <v>207</v>
+      </c>
+      <c r="DY47">
+        <v>207</v>
+      </c>
+      <c r="DZ47">
+        <v>207</v>
+      </c>
+      <c r="EA47">
+        <v>207</v>
+      </c>
     </row>
-    <row r="48" spans="1:126">
+    <row r="48" spans="1:131">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -11972,8 +12513,23 @@
       <c r="DV48">
         <v>0</v>
       </c>
+      <c r="DW48">
+        <v>0</v>
+      </c>
+      <c r="DX48">
+        <v>0</v>
+      </c>
+      <c r="DY48">
+        <v>0</v>
+      </c>
+      <c r="DZ48">
+        <v>0</v>
+      </c>
+      <c r="EA48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:126">
+    <row r="49" spans="1:131">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -12244,8 +12800,23 @@
       <c r="DV49">
         <v>200</v>
       </c>
+      <c r="DW49">
+        <v>200</v>
+      </c>
+      <c r="DX49">
+        <v>200</v>
+      </c>
+      <c r="DY49">
+        <v>200</v>
+      </c>
+      <c r="DZ49">
+        <v>200</v>
+      </c>
+      <c r="EA49">
+        <v>200</v>
+      </c>
     </row>
-    <row r="50" spans="1:126">
+    <row r="50" spans="1:131">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -12561,8 +13132,23 @@
       <c r="DV50">
         <v>52</v>
       </c>
+      <c r="DW50">
+        <v>46</v>
+      </c>
+      <c r="DX50">
+        <v>48</v>
+      </c>
+      <c r="DY50">
+        <v>50</v>
+      </c>
+      <c r="DZ50">
+        <v>51</v>
+      </c>
+      <c r="EA50">
+        <v>51</v>
+      </c>
     </row>
-    <row r="51" spans="1:126">
+    <row r="51" spans="1:131">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -12833,8 +13419,23 @@
       <c r="DV51">
         <v>52</v>
       </c>
+      <c r="DW51">
+        <v>46</v>
+      </c>
+      <c r="DX51">
+        <v>48</v>
+      </c>
+      <c r="DY51">
+        <v>50</v>
+      </c>
+      <c r="DZ51">
+        <v>51</v>
+      </c>
+      <c r="EA51">
+        <v>51</v>
+      </c>
     </row>
-    <row r="52" spans="1:126">
+    <row r="52" spans="1:131">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -13102,8 +13703,23 @@
       <c r="DV52">
         <v>1015</v>
       </c>
+      <c r="DW52">
+        <v>1218</v>
+      </c>
+      <c r="DX52">
+        <v>1215</v>
+      </c>
+      <c r="DY52">
+        <v>1213</v>
+      </c>
+      <c r="DZ52">
+        <v>1215</v>
+      </c>
+      <c r="EA52">
+        <v>1215</v>
+      </c>
     </row>
-    <row r="53" spans="1:126">
+    <row r="53" spans="1:131">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -13365,16 +13981,31 @@
       <c r="DV53">
         <v>1</v>
       </c>
+      <c r="DW53">
+        <v>1</v>
+      </c>
+      <c r="DX53">
+        <v>1</v>
+      </c>
+      <c r="DY53">
+        <v>1</v>
+      </c>
+      <c r="DZ53">
+        <v>1</v>
+      </c>
+      <c r="EA53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:126">
+    <row r="54" spans="1:131">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:126">
+    <row r="55" spans="1:131">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:126">
+    <row r="56" spans="1:131">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -13678,8 +14309,23 @@
       <c r="DV56">
         <v>35</v>
       </c>
+      <c r="DW56">
+        <v>35</v>
+      </c>
+      <c r="DX56">
+        <v>35</v>
+      </c>
+      <c r="DY56">
+        <v>35</v>
+      </c>
+      <c r="DZ56">
+        <v>35</v>
+      </c>
+      <c r="EA56">
+        <v>35</v>
+      </c>
     </row>
-    <row r="57" spans="1:126">
+    <row r="57" spans="1:131">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -13947,8 +14593,23 @@
       <c r="DV57">
         <v>2</v>
       </c>
+      <c r="DW57">
+        <v>2</v>
+      </c>
+      <c r="DX57">
+        <v>2</v>
+      </c>
+      <c r="DY57">
+        <v>2</v>
+      </c>
+      <c r="DZ57">
+        <v>2</v>
+      </c>
+      <c r="EA57">
+        <v>2</v>
+      </c>
     </row>
-    <row r="58" spans="1:126">
+    <row r="58" spans="1:131">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -14216,8 +14877,23 @@
       <c r="DV58">
         <v>32</v>
       </c>
+      <c r="DW58">
+        <v>32</v>
+      </c>
+      <c r="DX58">
+        <v>32</v>
+      </c>
+      <c r="DY58">
+        <v>32</v>
+      </c>
+      <c r="DZ58">
+        <v>32</v>
+      </c>
+      <c r="EA58">
+        <v>32</v>
+      </c>
     </row>
-    <row r="59" spans="1:126">
+    <row r="59" spans="1:131">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -14521,8 +15197,23 @@
       <c r="DV59">
         <v>2</v>
       </c>
+      <c r="DW59">
+        <v>2</v>
+      </c>
+      <c r="DX59">
+        <v>2</v>
+      </c>
+      <c r="DY59">
+        <v>2</v>
+      </c>
+      <c r="DZ59">
+        <v>2</v>
+      </c>
+      <c r="EA59">
+        <v>2</v>
+      </c>
     </row>
-    <row r="60" spans="1:126">
+    <row r="60" spans="1:131">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -14826,8 +15517,23 @@
       <c r="DV60">
         <v>4</v>
       </c>
+      <c r="DW60">
+        <v>4</v>
+      </c>
+      <c r="DX60">
+        <v>4</v>
+      </c>
+      <c r="DY60">
+        <v>4</v>
+      </c>
+      <c r="DZ60">
+        <v>4</v>
+      </c>
+      <c r="EA60">
+        <v>4</v>
+      </c>
     </row>
-    <row r="61" spans="1:126">
+    <row r="61" spans="1:131">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -15131,8 +15837,23 @@
       <c r="DV61">
         <v>175</v>
       </c>
+      <c r="DW61">
+        <v>175</v>
+      </c>
+      <c r="DX61">
+        <v>175</v>
+      </c>
+      <c r="DY61">
+        <v>175</v>
+      </c>
+      <c r="DZ61">
+        <v>175</v>
+      </c>
+      <c r="EA61">
+        <v>175</v>
+      </c>
     </row>
-    <row r="62" spans="1:126">
+    <row r="62" spans="1:131">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -15394,8 +16115,23 @@
       <c r="DV62">
         <v>1</v>
       </c>
+      <c r="DW62">
+        <v>1</v>
+      </c>
+      <c r="DX62">
+        <v>1</v>
+      </c>
+      <c r="DY62">
+        <v>1</v>
+      </c>
+      <c r="DZ62">
+        <v>1</v>
+      </c>
+      <c r="EA62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:126">
+    <row r="64" spans="1:131">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -15699,8 +16435,23 @@
       <c r="DV64">
         <v>13</v>
       </c>
+      <c r="DW64">
+        <v>13</v>
+      </c>
+      <c r="DX64">
+        <v>13</v>
+      </c>
+      <c r="DY64">
+        <v>13</v>
+      </c>
+      <c r="DZ64">
+        <v>13</v>
+      </c>
+      <c r="EA64">
+        <v>13</v>
+      </c>
     </row>
-    <row r="65" spans="1:126">
+    <row r="65" spans="1:131">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -15968,8 +16719,23 @@
       <c r="DV65">
         <v>0</v>
       </c>
+      <c r="DW65">
+        <v>0</v>
+      </c>
+      <c r="DX65">
+        <v>0</v>
+      </c>
+      <c r="DY65">
+        <v>0</v>
+      </c>
+      <c r="DZ65">
+        <v>0</v>
+      </c>
+      <c r="EA65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:126">
+    <row r="66" spans="1:131">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -16237,8 +17003,23 @@
       <c r="DV66">
         <v>13</v>
       </c>
+      <c r="DW66">
+        <v>13</v>
+      </c>
+      <c r="DX66">
+        <v>13</v>
+      </c>
+      <c r="DY66">
+        <v>13</v>
+      </c>
+      <c r="DZ66">
+        <v>13</v>
+      </c>
+      <c r="EA66">
+        <v>13</v>
+      </c>
     </row>
-    <row r="67" spans="1:126">
+    <row r="67" spans="1:131">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -16542,8 +17323,23 @@
       <c r="DV67">
         <v>69</v>
       </c>
+      <c r="DW67">
+        <v>71</v>
+      </c>
+      <c r="DX67">
+        <v>71</v>
+      </c>
+      <c r="DY67">
+        <v>71</v>
+      </c>
+      <c r="DZ67">
+        <v>71</v>
+      </c>
+      <c r="EA67">
+        <v>68</v>
+      </c>
     </row>
-    <row r="68" spans="1:126">
+    <row r="68" spans="1:131">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -16848,8 +17644,23 @@
       <c r="DV68">
         <v>69</v>
       </c>
+      <c r="DW68">
+        <v>71</v>
+      </c>
+      <c r="DX68">
+        <v>71</v>
+      </c>
+      <c r="DY68">
+        <v>71</v>
+      </c>
+      <c r="DZ68">
+        <v>71</v>
+      </c>
+      <c r="EA68">
+        <v>68</v>
+      </c>
     </row>
-    <row r="69" spans="1:126">
+    <row r="69" spans="1:131">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -17153,8 +17964,23 @@
       <c r="DV69">
         <v>0</v>
       </c>
+      <c r="DW69">
+        <v>0</v>
+      </c>
+      <c r="DX69">
+        <v>0</v>
+      </c>
+      <c r="DY69">
+        <v>0</v>
+      </c>
+      <c r="DZ69">
+        <v>0</v>
+      </c>
+      <c r="EA69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:126">
+    <row r="70" spans="1:131">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -17422,11 +18248,26 @@
       <c r="DV70">
         <v>0</v>
       </c>
+      <c r="DW70">
+        <v>0</v>
+      </c>
+      <c r="DX70">
+        <v>0</v>
+      </c>
+      <c r="DY70">
+        <v>0</v>
+      </c>
+      <c r="DZ70">
+        <v>0</v>
+      </c>
+      <c r="EA70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:126">
+    <row r="71" spans="1:131">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:126">
+    <row r="72" spans="1:131">
       <c r="A72" s="2" t="s">
         <v>119</v>
       </c>
@@ -17580,8 +18421,23 @@
       <c r="DV72">
         <v>10</v>
       </c>
+      <c r="DW72">
+        <v>10</v>
+      </c>
+      <c r="DX72">
+        <v>10</v>
+      </c>
+      <c r="DY72">
+        <v>10</v>
+      </c>
+      <c r="DZ72">
+        <v>10</v>
+      </c>
+      <c r="EA72">
+        <v>10</v>
+      </c>
     </row>
-    <row r="73" spans="1:126">
+    <row r="73" spans="1:131">
       <c r="A73" s="2" t="s">
         <v>119</v>
       </c>
@@ -17735,8 +18591,23 @@
       <c r="DV73">
         <v>1</v>
       </c>
+      <c r="DW73">
+        <v>1</v>
+      </c>
+      <c r="DX73">
+        <v>1</v>
+      </c>
+      <c r="DY73">
+        <v>1</v>
+      </c>
+      <c r="DZ73">
+        <v>1</v>
+      </c>
+      <c r="EA73">
+        <v>1</v>
+      </c>
     </row>
-    <row r="74" spans="1:126">
+    <row r="74" spans="1:131">
       <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
@@ -17890,8 +18761,23 @@
       <c r="DV74">
         <v>9</v>
       </c>
+      <c r="DW74">
+        <v>9</v>
+      </c>
+      <c r="DX74">
+        <v>9</v>
+      </c>
+      <c r="DY74">
+        <v>9</v>
+      </c>
+      <c r="DZ74">
+        <v>9</v>
+      </c>
+      <c r="EA74">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:126">
+    <row r="75" spans="1:131">
       <c r="A75" s="2" t="s">
         <v>119</v>
       </c>
@@ -18045,8 +18931,23 @@
       <c r="DV75">
         <v>2</v>
       </c>
+      <c r="DW75">
+        <v>1</v>
+      </c>
+      <c r="DX75">
+        <v>1</v>
+      </c>
+      <c r="DY75">
+        <v>1</v>
+      </c>
+      <c r="DZ75">
+        <v>2</v>
+      </c>
+      <c r="EA75">
+        <v>2</v>
+      </c>
     </row>
-    <row r="76" spans="1:126">
+    <row r="76" spans="1:131">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -18200,8 +19101,23 @@
       <c r="DV76">
         <v>3</v>
       </c>
+      <c r="DW76">
+        <v>2</v>
+      </c>
+      <c r="DX76">
+        <v>2</v>
+      </c>
+      <c r="DY76">
+        <v>2</v>
+      </c>
+      <c r="DZ76">
+        <v>3</v>
+      </c>
+      <c r="EA76">
+        <v>3</v>
+      </c>
     </row>
-    <row r="77" spans="1:126">
+    <row r="77" spans="1:131">
       <c r="A77" s="2" t="s">
         <v>119</v>
       </c>
@@ -18355,13 +19271,28 @@
       <c r="DV77">
         <v>47</v>
       </c>
+      <c r="DW77">
+        <v>48</v>
+      </c>
+      <c r="DX77">
+        <v>48</v>
+      </c>
+      <c r="DY77">
+        <v>48</v>
+      </c>
+      <c r="DZ77">
+        <v>48</v>
+      </c>
+      <c r="EA77">
+        <v>48</v>
+      </c>
     </row>
-    <row r="79" spans="1:126">
+    <row r="79" spans="1:131">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:126">
+    <row r="80" spans="1:131">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -18668,8 +19599,23 @@
       <c r="DV80">
         <v>318</v>
       </c>
+      <c r="DW80">
+        <v>318</v>
+      </c>
+      <c r="DX80">
+        <v>319</v>
+      </c>
+      <c r="DY80">
+        <v>319</v>
+      </c>
+      <c r="DZ80">
+        <v>319</v>
+      </c>
+      <c r="EA80">
+        <v>325</v>
+      </c>
     </row>
-    <row r="81" spans="1:126">
+    <row r="81" spans="1:131">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -18976,8 +19922,23 @@
       <c r="DV81">
         <v>50</v>
       </c>
+      <c r="DW81">
+        <v>53</v>
+      </c>
+      <c r="DX81">
+        <v>49</v>
+      </c>
+      <c r="DY81">
+        <v>51</v>
+      </c>
+      <c r="DZ81">
+        <v>57</v>
+      </c>
+      <c r="EA81">
+        <v>70</v>
+      </c>
     </row>
-    <row r="82" spans="1:126">
+    <row r="82" spans="1:131">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -19284,8 +20245,23 @@
       <c r="DV82">
         <v>43</v>
       </c>
+      <c r="DW82">
+        <v>44</v>
+      </c>
+      <c r="DX82">
+        <v>47</v>
+      </c>
+      <c r="DY82">
+        <v>47</v>
+      </c>
+      <c r="DZ82">
+        <v>50</v>
+      </c>
+      <c r="EA82">
+        <v>67</v>
+      </c>
     </row>
-    <row r="83" spans="1:126">
+    <row r="83" spans="1:131">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -19550,8 +20526,23 @@
       <c r="DV83">
         <v>20</v>
       </c>
+      <c r="DW83">
+        <v>20</v>
+      </c>
+      <c r="DX83">
+        <v>20</v>
+      </c>
+      <c r="DY83">
+        <v>20</v>
+      </c>
+      <c r="DZ83">
+        <v>20</v>
+      </c>
+      <c r="EA83">
+        <v>20</v>
+      </c>
     </row>
-    <row r="85" spans="1:126">
+    <row r="85" spans="1:131">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -19858,8 +20849,23 @@
       <c r="DV85">
         <v>123</v>
       </c>
+      <c r="DW85">
+        <v>123</v>
+      </c>
+      <c r="DX85">
+        <v>123</v>
+      </c>
+      <c r="DY85">
+        <v>124</v>
+      </c>
+      <c r="DZ85">
+        <v>124</v>
+      </c>
+      <c r="EA85">
+        <v>124</v>
+      </c>
     </row>
-    <row r="86" spans="1:126">
+    <row r="86" spans="1:131">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -20166,8 +21172,23 @@
       <c r="DV86">
         <v>1</v>
       </c>
+      <c r="DW86">
+        <v>5</v>
+      </c>
+      <c r="DX86">
+        <v>5</v>
+      </c>
+      <c r="DY86">
+        <v>5</v>
+      </c>
+      <c r="DZ86">
+        <v>5</v>
+      </c>
+      <c r="EA86">
+        <v>5</v>
+      </c>
     </row>
-    <row r="87" spans="1:126">
+    <row r="87" spans="1:131">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -20474,8 +21495,23 @@
       <c r="DV87">
         <v>22</v>
       </c>
+      <c r="DW87">
+        <v>21</v>
+      </c>
+      <c r="DX87">
+        <v>21</v>
+      </c>
+      <c r="DY87">
+        <v>21</v>
+      </c>
+      <c r="DZ87">
+        <v>21</v>
+      </c>
+      <c r="EA87">
+        <v>21</v>
+      </c>
     </row>
-    <row r="88" spans="1:126">
+    <row r="88" spans="1:131">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -20782,8 +21818,23 @@
       <c r="DV88">
         <v>252</v>
       </c>
+      <c r="DW88">
+        <v>256</v>
+      </c>
+      <c r="DX88">
+        <v>256</v>
+      </c>
+      <c r="DY88">
+        <v>256</v>
+      </c>
+      <c r="DZ88">
+        <v>256</v>
+      </c>
+      <c r="EA88">
+        <v>256</v>
+      </c>
     </row>
-    <row r="89" spans="1:126">
+    <row r="89" spans="1:131">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -20964,8 +22015,23 @@
       <c r="DV89">
         <v>1</v>
       </c>
+      <c r="DW89">
+        <v>1</v>
+      </c>
+      <c r="DX89">
+        <v>1</v>
+      </c>
+      <c r="DY89">
+        <v>1</v>
+      </c>
+      <c r="DZ89">
+        <v>1</v>
+      </c>
+      <c r="EA89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:126">
+    <row r="91" spans="1:131">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -21272,8 +22338,23 @@
       <c r="DV91">
         <v>81</v>
       </c>
+      <c r="DW91">
+        <v>82</v>
+      </c>
+      <c r="DX91">
+        <v>82</v>
+      </c>
+      <c r="DY91">
+        <v>82</v>
+      </c>
+      <c r="DZ91">
+        <v>82</v>
+      </c>
+      <c r="EA91">
+        <v>82</v>
+      </c>
     </row>
-    <row r="92" spans="1:126">
+    <row r="92" spans="1:131">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -21580,8 +22661,23 @@
       <c r="DV92">
         <v>0</v>
       </c>
+      <c r="DW92">
+        <v>1</v>
+      </c>
+      <c r="DX92">
+        <v>1</v>
+      </c>
+      <c r="DY92">
+        <v>1</v>
+      </c>
+      <c r="DZ92">
+        <v>1</v>
+      </c>
+      <c r="EA92">
+        <v>1</v>
+      </c>
     </row>
-    <row r="93" spans="1:126">
+    <row r="93" spans="1:131">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -21876,8 +22972,23 @@
       <c r="DV93">
         <v>191</v>
       </c>
+      <c r="DW93">
+        <v>191</v>
+      </c>
+      <c r="DX93">
+        <v>191</v>
+      </c>
+      <c r="DY93">
+        <v>191</v>
+      </c>
+      <c r="DZ93">
+        <v>191</v>
+      </c>
+      <c r="EA93">
+        <v>192</v>
+      </c>
     </row>
-    <row r="94" spans="1:126">
+    <row r="94" spans="1:131">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -22184,8 +23295,23 @@
       <c r="DV94">
         <v>62</v>
       </c>
+      <c r="DW94">
+        <v>62</v>
+      </c>
+      <c r="DX94">
+        <v>62</v>
+      </c>
+      <c r="DY94">
+        <v>62</v>
+      </c>
+      <c r="DZ94">
+        <v>62</v>
+      </c>
+      <c r="EA94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:126">
+    <row r="95" spans="1:131">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -22450,11 +23576,26 @@
       <c r="DV95">
         <v>14</v>
       </c>
+      <c r="DW95">
+        <v>14</v>
+      </c>
+      <c r="DX95">
+        <v>14</v>
+      </c>
+      <c r="DY95">
+        <v>14</v>
+      </c>
+      <c r="DZ95">
+        <v>14</v>
+      </c>
+      <c r="EA95">
+        <v>14</v>
+      </c>
     </row>
-    <row r="96" spans="1:126">
+    <row r="96" spans="1:131">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:126">
+    <row r="97" spans="1:131">
       <c r="A97" s="2" t="s">
         <v>130</v>
       </c>
@@ -22578,8 +23719,23 @@
       <c r="DV97">
         <v>12</v>
       </c>
+      <c r="DW97">
+        <v>12</v>
+      </c>
+      <c r="DX97">
+        <v>12</v>
+      </c>
+      <c r="DY97">
+        <v>12</v>
+      </c>
+      <c r="DZ97">
+        <v>12</v>
+      </c>
+      <c r="EA97">
+        <v>12</v>
+      </c>
     </row>
-    <row r="98" spans="1:126">
+    <row r="98" spans="1:131">
       <c r="A98" s="2" t="s">
         <v>130</v>
       </c>
@@ -22703,8 +23859,23 @@
       <c r="DV98">
         <v>9</v>
       </c>
+      <c r="DW98">
+        <v>9</v>
+      </c>
+      <c r="DX98">
+        <v>9</v>
+      </c>
+      <c r="DY98">
+        <v>9</v>
+      </c>
+      <c r="DZ98">
+        <v>9</v>
+      </c>
+      <c r="EA98">
+        <v>9</v>
+      </c>
     </row>
-    <row r="99" spans="1:126">
+    <row r="99" spans="1:131">
       <c r="A99" s="2" t="s">
         <v>130</v>
       </c>
@@ -22828,8 +23999,23 @@
       <c r="DV99">
         <v>52</v>
       </c>
+      <c r="DW99">
+        <v>52</v>
+      </c>
+      <c r="DX99">
+        <v>52</v>
+      </c>
+      <c r="DY99">
+        <v>52</v>
+      </c>
+      <c r="DZ99">
+        <v>52</v>
+      </c>
+      <c r="EA99">
+        <v>52</v>
+      </c>
     </row>
-    <row r="100" spans="1:126">
+    <row r="100" spans="1:131">
       <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
@@ -22953,8 +24139,23 @@
       <c r="DV100">
         <v>1</v>
       </c>
+      <c r="DW100">
+        <v>1</v>
+      </c>
+      <c r="DX100">
+        <v>1</v>
+      </c>
+      <c r="DY100">
+        <v>1</v>
+      </c>
+      <c r="DZ100">
+        <v>1</v>
+      </c>
+      <c r="EA100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:126">
+    <row r="102" spans="1:131">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -23180,8 +24381,23 @@
       <c r="DV102">
         <v>209</v>
       </c>
+      <c r="DW102">
+        <v>209</v>
+      </c>
+      <c r="DX102">
+        <v>209</v>
+      </c>
+      <c r="DY102">
+        <v>210</v>
+      </c>
+      <c r="DZ102">
+        <v>210</v>
+      </c>
+      <c r="EA102">
+        <v>211</v>
+      </c>
     </row>
-    <row r="103" spans="1:126">
+    <row r="103" spans="1:131">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -23407,8 +24623,23 @@
       <c r="DV103">
         <v>110</v>
       </c>
+      <c r="DW103">
+        <v>117</v>
+      </c>
+      <c r="DX103">
+        <v>124</v>
+      </c>
+      <c r="DY103">
+        <v>124</v>
+      </c>
+      <c r="DZ103">
+        <v>131</v>
+      </c>
+      <c r="EA103">
+        <v>133</v>
+      </c>
     </row>
-    <row r="104" spans="1:126">
+    <row r="104" spans="1:131">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -23632,6 +24863,21 @@
         <v>28</v>
       </c>
       <c r="DV104">
+        <v>28</v>
+      </c>
+      <c r="DW104">
+        <v>28</v>
+      </c>
+      <c r="DX104">
+        <v>28</v>
+      </c>
+      <c r="DY104">
+        <v>28</v>
+      </c>
+      <c r="DZ104">
+        <v>28</v>
+      </c>
+      <c r="EA104">
         <v>28</v>
       </c>
     </row>
@@ -23648,11 +24894,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:CW11"/>
+  <dimension ref="A2:DB11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CX2" sqref="CX2"/>
+      <pane xSplit="1" topLeftCell="CO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CT3" sqref="CT3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23662,7 +24908,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:101" s="2" customFormat="1">
+    <row r="2" spans="1:106" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -23955,19 +25201,34 @@
         <v>44016</v>
       </c>
       <c r="CT2" s="9">
-        <v>43987</v>
+        <v>44017</v>
       </c>
       <c r="CU2" s="9">
         <v>44018</v>
       </c>
       <c r="CV2" s="9">
-        <v>43989</v>
+        <v>44019</v>
       </c>
       <c r="CW2" s="9">
         <v>44020</v>
       </c>
+      <c r="CX2" s="9">
+        <v>44021</v>
+      </c>
+      <c r="CY2" s="9">
+        <v>44022</v>
+      </c>
+      <c r="CZ2" s="9">
+        <v>44023</v>
+      </c>
+      <c r="DA2" s="9">
+        <v>44024</v>
+      </c>
+      <c r="DB2" s="9">
+        <v>44025</v>
+      </c>
     </row>
-    <row r="3" spans="1:101">
+    <row r="3" spans="1:106">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -24271,8 +25532,23 @@
       <c r="CW3">
         <v>1522</v>
       </c>
+      <c r="CX3">
+        <v>1526</v>
+      </c>
+      <c r="CY3">
+        <v>1536</v>
+      </c>
+      <c r="CZ3">
+        <v>1541</v>
+      </c>
+      <c r="DA3">
+        <v>1549</v>
+      </c>
+      <c r="DB3">
+        <v>1556</v>
+      </c>
     </row>
-    <row r="4" spans="1:101">
+    <row r="4" spans="1:106">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -24576,8 +25852,23 @@
       <c r="CW4">
         <v>625</v>
       </c>
+      <c r="CX4">
+        <v>633</v>
+      </c>
+      <c r="CY4">
+        <v>638</v>
+      </c>
+      <c r="CZ4">
+        <v>641</v>
+      </c>
+      <c r="DA4">
+        <v>645</v>
+      </c>
+      <c r="DB4">
+        <v>649</v>
+      </c>
     </row>
-    <row r="5" spans="1:101">
+    <row r="5" spans="1:106">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -24881,8 +26172,23 @@
       <c r="CW5">
         <v>501</v>
       </c>
+      <c r="CX5">
+        <v>507</v>
+      </c>
+      <c r="CY5">
+        <v>510</v>
+      </c>
+      <c r="CZ5">
+        <v>511</v>
+      </c>
+      <c r="DA5">
+        <v>513</v>
+      </c>
+      <c r="DB5">
+        <v>514</v>
+      </c>
     </row>
-    <row r="6" spans="1:101">
+    <row r="6" spans="1:106">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -25186,8 +26492,23 @@
       <c r="CW6">
         <v>2209</v>
       </c>
+      <c r="CX6">
+        <v>2216</v>
+      </c>
+      <c r="CY6">
+        <v>2225</v>
+      </c>
+      <c r="CZ6">
+        <v>2232</v>
+      </c>
+      <c r="DA6">
+        <v>2239</v>
+      </c>
+      <c r="DB6">
+        <v>2244</v>
+      </c>
     </row>
-    <row r="7" spans="1:101">
+    <row r="7" spans="1:106">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -25491,8 +26812,23 @@
       <c r="CW7">
         <v>1590</v>
       </c>
+      <c r="CX7">
+        <v>1595</v>
+      </c>
+      <c r="CY7">
+        <v>1601</v>
+      </c>
+      <c r="CZ7">
+        <v>1608</v>
+      </c>
+      <c r="DA7">
+        <v>1617</v>
+      </c>
+      <c r="DB7">
+        <v>1624</v>
+      </c>
     </row>
-    <row r="8" spans="1:101">
+    <row r="8" spans="1:106">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -25796,8 +27132,23 @@
       <c r="CW8">
         <v>961</v>
       </c>
+      <c r="CX8">
+        <v>973</v>
+      </c>
+      <c r="CY8">
+        <v>980</v>
+      </c>
+      <c r="CZ8">
+        <v>988</v>
+      </c>
+      <c r="DA8">
+        <v>992</v>
+      </c>
+      <c r="DB8">
+        <v>998</v>
+      </c>
     </row>
-    <row r="9" spans="1:101">
+    <row r="9" spans="1:106">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -26101,8 +27452,23 @@
       <c r="CW9">
         <v>1531</v>
       </c>
+      <c r="CX9">
+        <v>1538</v>
+      </c>
+      <c r="CY9">
+        <v>1547</v>
+      </c>
+      <c r="CZ9">
+        <v>1551</v>
+      </c>
+      <c r="DA9">
+        <v>1563</v>
+      </c>
+      <c r="DB9">
+        <v>1572</v>
+      </c>
     </row>
-    <row r="10" spans="1:101">
+    <row r="10" spans="1:106">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -26406,8 +27772,23 @@
       <c r="CW10">
         <v>1565</v>
       </c>
+      <c r="CX10">
+        <v>1576</v>
+      </c>
+      <c r="CY10">
+        <v>1586</v>
+      </c>
+      <c r="CZ10">
+        <v>1597</v>
+      </c>
+      <c r="DA10">
+        <v>1604</v>
+      </c>
+      <c r="DB10">
+        <v>1610</v>
+      </c>
     </row>
-    <row r="11" spans="1:101">
+    <row r="11" spans="1:106">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -26710,6 +28091,21 @@
       </c>
       <c r="CW11">
         <v>175</v>
+      </c>
+      <c r="CX11">
+        <v>179</v>
+      </c>
+      <c r="CY11">
+        <v>178</v>
+      </c>
+      <c r="CZ11">
+        <v>178</v>
+      </c>
+      <c r="DA11">
+        <v>184</v>
+      </c>
+      <c r="DB11">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -26720,11 +28116,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:CR17"/>
+  <dimension ref="A2:CW17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CS2" sqref="CS2"/>
+      <selection pane="topRight" activeCell="CQ3" sqref="CQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26734,7 +28130,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:96" s="2" customFormat="1">
+    <row r="2" spans="1:101" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -27010,19 +28406,34 @@
         <v>44016</v>
       </c>
       <c r="CO2" s="9">
-        <v>43987</v>
+        <v>44017</v>
       </c>
       <c r="CP2" s="9">
         <v>44018</v>
       </c>
       <c r="CQ2" s="9">
-        <v>43989</v>
+        <v>44019</v>
       </c>
       <c r="CR2" s="9">
         <v>44020</v>
       </c>
+      <c r="CS2" s="9">
+        <v>44021</v>
+      </c>
+      <c r="CT2" s="9">
+        <v>44022</v>
+      </c>
+      <c r="CU2" s="9">
+        <v>44023</v>
+      </c>
+      <c r="CV2" s="9">
+        <v>44024</v>
+      </c>
+      <c r="CW2" s="9">
+        <v>44025</v>
+      </c>
     </row>
-    <row r="3" spans="1:96" s="2" customFormat="1">
+    <row r="3" spans="1:101" s="2" customFormat="1">
       <c r="A3" s="41" t="s">
         <v>36</v>
       </c>
@@ -27031,7 +28442,7 @@
       <c r="D3" s="9"/>
       <c r="CP3" s="4"/>
     </row>
-    <row r="4" spans="1:96">
+    <row r="4" spans="1:101">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -27320,8 +28731,23 @@
       <c r="CR4">
         <v>10679</v>
       </c>
+      <c r="CS4">
+        <v>10743</v>
+      </c>
+      <c r="CT4">
+        <v>10801</v>
+      </c>
+      <c r="CU4">
+        <v>10847</v>
+      </c>
+      <c r="CV4">
+        <v>10906</v>
+      </c>
+      <c r="CW4">
+        <v>10946</v>
+      </c>
     </row>
-    <row r="5" spans="1:96">
+    <row r="5" spans="1:101">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -27610,8 +29036,23 @@
       <c r="CR5">
         <v>183</v>
       </c>
+      <c r="CS5">
+        <v>142</v>
+      </c>
+      <c r="CT5">
+        <v>149</v>
+      </c>
+      <c r="CU5">
+        <v>178</v>
+      </c>
+      <c r="CV5">
+        <v>152</v>
+      </c>
+      <c r="CW5">
+        <v>183</v>
+      </c>
     </row>
-    <row r="6" spans="1:96">
+    <row r="6" spans="1:101">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -27900,8 +29341,23 @@
       <c r="CR6">
         <v>2175</v>
       </c>
+      <c r="CS6">
+        <v>2209</v>
+      </c>
+      <c r="CT6">
+        <v>2217</v>
+      </c>
+      <c r="CU6">
+        <v>2218</v>
+      </c>
+      <c r="CV6">
+        <v>2230</v>
+      </c>
+      <c r="CW6">
+        <v>2234</v>
+      </c>
     </row>
-    <row r="7" spans="1:96">
+    <row r="7" spans="1:101">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -28190,8 +29646,23 @@
       <c r="CR7">
         <v>5266</v>
       </c>
+      <c r="CS7">
+        <v>5315</v>
+      </c>
+      <c r="CT7">
+        <v>2779</v>
+      </c>
+      <c r="CU7">
+        <v>5354</v>
+      </c>
+      <c r="CV7">
+        <v>5390</v>
+      </c>
+      <c r="CW7">
+        <v>5395</v>
+      </c>
     </row>
-    <row r="8" spans="1:96">
+    <row r="8" spans="1:101">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -28480,8 +29951,23 @@
       <c r="CR8">
         <v>168</v>
       </c>
+      <c r="CS8">
+        <v>168</v>
+      </c>
+      <c r="CT8">
+        <v>168</v>
+      </c>
+      <c r="CU8">
+        <v>169</v>
+      </c>
+      <c r="CV8">
+        <v>170</v>
+      </c>
+      <c r="CW8">
+        <v>170</v>
+      </c>
     </row>
-    <row r="9" spans="1:96" ht="30">
+    <row r="9" spans="1:101" ht="30">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -28770,8 +30256,23 @@
       <c r="CR9">
         <v>26</v>
       </c>
+      <c r="CS9">
+        <v>26</v>
+      </c>
+      <c r="CT9">
+        <v>27</v>
+      </c>
+      <c r="CU9">
+        <v>27</v>
+      </c>
+      <c r="CV9">
+        <v>27</v>
+      </c>
+      <c r="CW9">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:96" ht="30">
+    <row r="10" spans="1:101" ht="30">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -29056,8 +30557,23 @@
       <c r="CR10">
         <v>29</v>
       </c>
+      <c r="CS10">
+        <v>29</v>
+      </c>
+      <c r="CT10">
+        <v>29</v>
+      </c>
+      <c r="CU10">
+        <v>29</v>
+      </c>
+      <c r="CV10">
+        <v>29</v>
+      </c>
+      <c r="CW10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="11" spans="1:96">
+    <row r="11" spans="1:101">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -29346,8 +30862,23 @@
       <c r="CR11">
         <v>2739</v>
       </c>
+      <c r="CS11">
+        <v>2762</v>
+      </c>
+      <c r="CT11">
+        <v>2779</v>
+      </c>
+      <c r="CU11">
+        <v>2781</v>
+      </c>
+      <c r="CV11">
+        <v>2818</v>
+      </c>
+      <c r="CW11">
+        <v>2818</v>
+      </c>
     </row>
-    <row r="12" spans="1:96" ht="30">
+    <row r="12" spans="1:101" ht="30">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -29636,8 +31167,23 @@
       <c r="CR12">
         <v>93</v>
       </c>
+      <c r="CS12">
+        <v>92</v>
+      </c>
+      <c r="CT12">
+        <v>91</v>
+      </c>
+      <c r="CU12">
+        <v>91</v>
+      </c>
+      <c r="CV12">
+        <v>90</v>
+      </c>
+      <c r="CW12">
+        <v>90</v>
+      </c>
     </row>
-    <row r="13" spans="1:96">
+    <row r="13" spans="1:101">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -29648,7 +31194,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:96">
+    <row r="14" spans="1:101">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -29937,8 +31483,23 @@
       <c r="CR14">
         <v>1315</v>
       </c>
+      <c r="CS14">
+        <v>1270</v>
+      </c>
+      <c r="CT14">
+        <v>1291</v>
+      </c>
+      <c r="CU14">
+        <v>1328</v>
+      </c>
+      <c r="CV14">
+        <v>1318</v>
+      </c>
+      <c r="CW14">
+        <v>1349</v>
+      </c>
     </row>
-    <row r="15" spans="1:96">
+    <row r="15" spans="1:101">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -30227,8 +31788,23 @@
       <c r="CR15">
         <v>3008</v>
       </c>
+      <c r="CS15">
+        <v>3032</v>
+      </c>
+      <c r="CT15">
+        <v>3036</v>
+      </c>
+      <c r="CU15">
+        <v>3037</v>
+      </c>
+      <c r="CV15">
+        <v>3056</v>
+      </c>
+      <c r="CW15">
+        <v>3058</v>
+      </c>
     </row>
-    <row r="16" spans="1:96">
+    <row r="16" spans="1:101">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -30517,8 +32093,23 @@
       <c r="CR16">
         <v>6337</v>
       </c>
+      <c r="CS16">
+        <v>6423</v>
+      </c>
+      <c r="CT16">
+        <v>6456</v>
+      </c>
+      <c r="CU16">
+        <v>6464</v>
+      </c>
+      <c r="CV16">
+        <v>6514</v>
+      </c>
+      <c r="CW16">
+        <v>6521</v>
+      </c>
     </row>
-    <row r="17" spans="1:96" ht="30">
+    <row r="17" spans="1:101" ht="30">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -30806,6 +32397,21 @@
       </c>
       <c r="CR17">
         <v>19</v>
+      </c>
+      <c r="CS17">
+        <v>18</v>
+      </c>
+      <c r="CT17">
+        <v>18</v>
+      </c>
+      <c r="CU17">
+        <v>18</v>
+      </c>
+      <c r="CV17">
+        <v>18</v>
+      </c>
+      <c r="CW17">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -30816,11 +32422,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CR9"/>
+  <dimension ref="A1:CX9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CS1" sqref="CS1"/>
+      <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CO2" sqref="CO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30829,7 +32435,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" s="2" customFormat="1">
+    <row r="1" spans="1:102" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -31104,7 +32710,7 @@
         <v>44016</v>
       </c>
       <c r="CO1" s="9">
-        <v>43987</v>
+        <v>44017</v>
       </c>
       <c r="CP1" s="9">
         <v>44018</v>
@@ -31115,14 +32721,32 @@
       <c r="CR1" s="9">
         <v>44020</v>
       </c>
+      <c r="CS1" s="9">
+        <v>44021</v>
+      </c>
+      <c r="CT1" s="9">
+        <v>44022</v>
+      </c>
+      <c r="CU1" s="9">
+        <v>44023</v>
+      </c>
+      <c r="CV1" s="9">
+        <v>44024</v>
+      </c>
+      <c r="CW1" s="9">
+        <v>44025</v>
+      </c>
+      <c r="CX1" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="2" spans="1:96">
+    <row r="2" spans="1:102">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:96">
+    <row r="3" spans="1:102">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -31412,8 +33036,23 @@
       <c r="CR3">
         <v>568</v>
       </c>
+      <c r="CS3">
+        <v>568</v>
+      </c>
+      <c r="CT3">
+        <v>568</v>
+      </c>
+      <c r="CU3">
+        <v>568</v>
+      </c>
+      <c r="CV3">
+        <v>568</v>
+      </c>
+      <c r="CW3">
+        <v>568</v>
+      </c>
     </row>
-    <row r="4" spans="1:96">
+    <row r="4" spans="1:102">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -31702,8 +33341,23 @@
       <c r="CR4">
         <v>8</v>
       </c>
+      <c r="CS4">
+        <v>8</v>
+      </c>
+      <c r="CT4">
+        <v>8</v>
+      </c>
+      <c r="CU4">
+        <v>8</v>
+      </c>
+      <c r="CV4">
+        <v>8</v>
+      </c>
+      <c r="CW4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:96" ht="30">
+    <row r="5" spans="1:102" ht="30">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -31992,8 +33646,23 @@
       <c r="CR5">
         <v>421</v>
       </c>
+      <c r="CS5">
+        <v>421</v>
+      </c>
+      <c r="CT5">
+        <v>421</v>
+      </c>
+      <c r="CU5">
+        <v>421</v>
+      </c>
+      <c r="CV5">
+        <v>421</v>
+      </c>
+      <c r="CW5">
+        <v>421</v>
+      </c>
     </row>
-    <row r="6" spans="1:96">
+    <row r="6" spans="1:102">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -32282,8 +33951,23 @@
       <c r="CR6">
         <v>74</v>
       </c>
+      <c r="CS6">
+        <v>74</v>
+      </c>
+      <c r="CT6">
+        <v>74</v>
+      </c>
+      <c r="CU6">
+        <v>74</v>
+      </c>
+      <c r="CV6">
+        <v>74</v>
+      </c>
+      <c r="CW6">
+        <v>74</v>
+      </c>
     </row>
-    <row r="7" spans="1:96" ht="30">
+    <row r="7" spans="1:102" ht="30">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -32572,8 +34256,23 @@
       <c r="CR7">
         <v>60</v>
       </c>
+      <c r="CS7">
+        <v>60</v>
+      </c>
+      <c r="CT7">
+        <v>60</v>
+      </c>
+      <c r="CU7">
+        <v>60</v>
+      </c>
+      <c r="CV7">
+        <v>60</v>
+      </c>
+      <c r="CW7">
+        <v>60</v>
+      </c>
     </row>
-    <row r="8" spans="1:96">
+    <row r="8" spans="1:102">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -32862,8 +34561,23 @@
       <c r="CR8">
         <v>5</v>
       </c>
+      <c r="CS8">
+        <v>5</v>
+      </c>
+      <c r="CT8">
+        <v>5</v>
+      </c>
+      <c r="CU8">
+        <v>5</v>
+      </c>
+      <c r="CV8">
+        <v>5</v>
+      </c>
+      <c r="CW8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:96">
+    <row r="9" spans="1:102">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -32905,11 +34619,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ5"/>
+  <dimension ref="A1:CP5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CK1" sqref="CK1"/>
+    <sheetView zoomScale="95" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CI2" sqref="CI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32917,7 +34631,7 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" s="2" customFormat="1">
+    <row r="1" spans="1:94" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -33168,24 +34882,42 @@
         <v>44016</v>
       </c>
       <c r="CG1" s="9">
-        <v>43987</v>
+        <v>44017</v>
       </c>
       <c r="CH1" s="9">
         <v>44018</v>
       </c>
       <c r="CI1" s="9">
-        <v>43989</v>
+        <v>44019</v>
       </c>
       <c r="CJ1" s="9">
         <v>44020</v>
       </c>
+      <c r="CK1" s="9">
+        <v>44021</v>
+      </c>
+      <c r="CL1" s="9">
+        <v>44022</v>
+      </c>
+      <c r="CM1" s="9">
+        <v>44023</v>
+      </c>
+      <c r="CN1" s="9">
+        <v>44024</v>
+      </c>
+      <c r="CO1" s="9">
+        <v>44025</v>
+      </c>
+      <c r="CP1" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="2" spans="1:88">
+    <row r="2" spans="1:94">
       <c r="A2" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:88">
+    <row r="3" spans="1:94">
       <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
@@ -33450,8 +35182,23 @@
       <c r="CJ3">
         <v>568</v>
       </c>
+      <c r="CK3">
+        <v>568</v>
+      </c>
+      <c r="CL3">
+        <v>568</v>
+      </c>
+      <c r="CM3">
+        <v>568</v>
+      </c>
+      <c r="CN3">
+        <v>568</v>
+      </c>
+      <c r="CO3">
+        <v>568</v>
+      </c>
     </row>
-    <row r="4" spans="1:88">
+    <row r="4" spans="1:94">
       <c r="A4" s="42" t="s">
         <v>159</v>
       </c>
@@ -33716,8 +35463,23 @@
       <c r="CJ4">
         <v>243</v>
       </c>
+      <c r="CK4">
+        <v>243</v>
+      </c>
+      <c r="CL4">
+        <v>243</v>
+      </c>
+      <c r="CM4">
+        <v>243</v>
+      </c>
+      <c r="CN4">
+        <v>243</v>
+      </c>
+      <c r="CO4">
+        <v>243</v>
+      </c>
     </row>
-    <row r="5" spans="1:88">
+    <row r="5" spans="1:94">
       <c r="A5" s="42" t="s">
         <v>158</v>
       </c>
@@ -33980,6 +35742,21 @@
         <v>322</v>
       </c>
       <c r="CJ5">
+        <v>325</v>
+      </c>
+      <c r="CK5">
+        <v>325</v>
+      </c>
+      <c r="CL5">
+        <v>325</v>
+      </c>
+      <c r="CM5">
+        <v>325</v>
+      </c>
+      <c r="CN5">
+        <v>325</v>
+      </c>
+      <c r="CO5">
         <v>325</v>
       </c>
     </row>
@@ -33991,11 +35768,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ11"/>
+  <dimension ref="A1:CP11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CK1" sqref="CK1"/>
+      <selection pane="topRight" activeCell="CI2" sqref="CI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34003,7 +35780,7 @@
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" s="2" customFormat="1">
+    <row r="1" spans="1:94" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -34254,24 +36031,42 @@
         <v>44016</v>
       </c>
       <c r="CG1" s="9">
-        <v>43987</v>
+        <v>44017</v>
       </c>
       <c r="CH1" s="9">
         <v>44018</v>
       </c>
       <c r="CI1" s="9">
-        <v>43989</v>
+        <v>44019</v>
       </c>
       <c r="CJ1" s="9">
         <v>44020</v>
       </c>
+      <c r="CK1" s="9">
+        <v>44021</v>
+      </c>
+      <c r="CL1" s="9">
+        <v>44022</v>
+      </c>
+      <c r="CM1" s="9">
+        <v>44023</v>
+      </c>
+      <c r="CN1" s="9">
+        <v>44024</v>
+      </c>
+      <c r="CO1" s="9">
+        <v>44025</v>
+      </c>
+      <c r="CP1" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="2" spans="1:88">
+    <row r="2" spans="1:94">
       <c r="A2" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:88">
+    <row r="3" spans="1:94">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -34536,8 +36331,23 @@
       <c r="CJ3">
         <v>568</v>
       </c>
+      <c r="CK3">
+        <v>568</v>
+      </c>
+      <c r="CL3">
+        <v>568</v>
+      </c>
+      <c r="CM3">
+        <v>568</v>
+      </c>
+      <c r="CN3">
+        <v>568</v>
+      </c>
+      <c r="CO3">
+        <v>568</v>
+      </c>
     </row>
-    <row r="4" spans="1:88">
+    <row r="4" spans="1:94">
       <c r="A4" s="5" t="s">
         <v>149</v>
       </c>
@@ -34802,8 +36612,23 @@
       <c r="CJ4">
         <v>0</v>
       </c>
+      <c r="CK4">
+        <v>0</v>
+      </c>
+      <c r="CL4">
+        <v>0</v>
+      </c>
+      <c r="CM4">
+        <v>0</v>
+      </c>
+      <c r="CN4">
+        <v>0</v>
+      </c>
+      <c r="CO4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:88">
+    <row r="5" spans="1:94">
       <c r="A5" s="5" t="s">
         <v>150</v>
       </c>
@@ -35068,8 +36893,23 @@
       <c r="CJ5">
         <v>3</v>
       </c>
+      <c r="CK5">
+        <v>3</v>
+      </c>
+      <c r="CL5">
+        <v>3</v>
+      </c>
+      <c r="CM5">
+        <v>3</v>
+      </c>
+      <c r="CN5">
+        <v>3</v>
+      </c>
+      <c r="CO5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:88">
+    <row r="6" spans="1:94">
       <c r="A6" s="5" t="s">
         <v>151</v>
       </c>
@@ -35334,8 +37174,23 @@
       <c r="CJ6">
         <v>7</v>
       </c>
+      <c r="CK6">
+        <v>7</v>
+      </c>
+      <c r="CL6">
+        <v>7</v>
+      </c>
+      <c r="CM6">
+        <v>7</v>
+      </c>
+      <c r="CN6">
+        <v>7</v>
+      </c>
+      <c r="CO6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="7" spans="1:88">
+    <row r="7" spans="1:94">
       <c r="A7" s="5" t="s">
         <v>152</v>
       </c>
@@ -35600,8 +37455,23 @@
       <c r="CJ7">
         <v>19</v>
       </c>
+      <c r="CK7">
+        <v>19</v>
+      </c>
+      <c r="CL7">
+        <v>19</v>
+      </c>
+      <c r="CM7">
+        <v>19</v>
+      </c>
+      <c r="CN7">
+        <v>19</v>
+      </c>
+      <c r="CO7">
+        <v>19</v>
+      </c>
     </row>
-    <row r="8" spans="1:88">
+    <row r="8" spans="1:94">
       <c r="A8" s="5" t="s">
         <v>153</v>
       </c>
@@ -35866,8 +37736,23 @@
       <c r="CJ8">
         <v>66</v>
       </c>
+      <c r="CK8">
+        <v>66</v>
+      </c>
+      <c r="CL8">
+        <v>66</v>
+      </c>
+      <c r="CM8">
+        <v>66</v>
+      </c>
+      <c r="CN8">
+        <v>66</v>
+      </c>
+      <c r="CO8">
+        <v>66</v>
+      </c>
     </row>
-    <row r="9" spans="1:88">
+    <row r="9" spans="1:94">
       <c r="A9" s="5" t="s">
         <v>154</v>
       </c>
@@ -36132,8 +38017,23 @@
       <c r="CJ9">
         <v>134</v>
       </c>
+      <c r="CK9">
+        <v>134</v>
+      </c>
+      <c r="CL9">
+        <v>134</v>
+      </c>
+      <c r="CM9">
+        <v>134</v>
+      </c>
+      <c r="CN9">
+        <v>134</v>
+      </c>
+      <c r="CO9">
+        <v>134</v>
+      </c>
     </row>
-    <row r="10" spans="1:88">
+    <row r="10" spans="1:94">
       <c r="A10" s="6" t="s">
         <v>155</v>
       </c>
@@ -36398,8 +38298,23 @@
       <c r="CJ10">
         <v>144</v>
       </c>
+      <c r="CK10">
+        <v>144</v>
+      </c>
+      <c r="CL10">
+        <v>144</v>
+      </c>
+      <c r="CM10">
+        <v>144</v>
+      </c>
+      <c r="CN10">
+        <v>144</v>
+      </c>
+      <c r="CO10">
+        <v>144</v>
+      </c>
     </row>
-    <row r="11" spans="1:88">
+    <row r="11" spans="1:94">
       <c r="A11" s="6" t="s">
         <v>156</v>
       </c>
@@ -36662,6 +38577,21 @@
         <v>195</v>
       </c>
       <c r="CJ11">
+        <v>195</v>
+      </c>
+      <c r="CK11">
+        <v>195</v>
+      </c>
+      <c r="CL11">
+        <v>195</v>
+      </c>
+      <c r="CM11">
+        <v>195</v>
+      </c>
+      <c r="CN11">
+        <v>195</v>
+      </c>
+      <c r="CO11">
         <v>195</v>
       </c>
     </row>
@@ -36673,11 +38603,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:CD13"/>
+  <dimension ref="A2:CJ13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="BS1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CE2" sqref="CE2"/>
+      <selection pane="topRight" activeCell="CC3" sqref="CC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36686,7 +38616,7 @@
     <col min="57" max="57" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:82" s="2" customFormat="1">
+    <row r="2" spans="1:88" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -36922,19 +38852,37 @@
         <v>44016</v>
       </c>
       <c r="CA2" s="9">
-        <v>43987</v>
+        <v>44017</v>
       </c>
       <c r="CB2" s="9">
         <v>44018</v>
       </c>
       <c r="CC2" s="9">
-        <v>43989</v>
+        <v>44019</v>
       </c>
       <c r="CD2" s="9">
         <v>44020</v>
       </c>
+      <c r="CE2" s="9">
+        <v>44021</v>
+      </c>
+      <c r="CF2" s="9">
+        <v>44022</v>
+      </c>
+      <c r="CG2" s="9">
+        <v>44023</v>
+      </c>
+      <c r="CH2" s="9">
+        <v>44024</v>
+      </c>
+      <c r="CI2" s="9">
+        <v>44025</v>
+      </c>
+      <c r="CJ2" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="3" spans="1:82">
+    <row r="3" spans="1:88">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -37181,8 +39129,23 @@
       <c r="CD3">
         <v>568</v>
       </c>
+      <c r="CE3">
+        <v>568</v>
+      </c>
+      <c r="CF3">
+        <v>568</v>
+      </c>
+      <c r="CG3">
+        <v>568</v>
+      </c>
+      <c r="CH3">
+        <v>568</v>
+      </c>
+      <c r="CI3">
+        <v>568</v>
+      </c>
     </row>
-    <row r="4" spans="1:82">
+    <row r="4" spans="1:88">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -37429,8 +39392,23 @@
       <c r="CD4">
         <v>62</v>
       </c>
+      <c r="CE4">
+        <v>62</v>
+      </c>
+      <c r="CF4">
+        <v>62</v>
+      </c>
+      <c r="CG4">
+        <v>62</v>
+      </c>
+      <c r="CH4">
+        <v>62</v>
+      </c>
+      <c r="CI4">
+        <v>62</v>
+      </c>
     </row>
-    <row r="5" spans="1:82">
+    <row r="5" spans="1:88">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -37677,8 +39655,23 @@
       <c r="CD5">
         <v>31</v>
       </c>
+      <c r="CE5">
+        <v>31</v>
+      </c>
+      <c r="CF5">
+        <v>31</v>
+      </c>
+      <c r="CG5">
+        <v>31</v>
+      </c>
+      <c r="CH5">
+        <v>31</v>
+      </c>
+      <c r="CI5">
+        <v>31</v>
+      </c>
     </row>
-    <row r="6" spans="1:82">
+    <row r="6" spans="1:88">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -37925,8 +39918,23 @@
       <c r="CD6">
         <v>33</v>
       </c>
+      <c r="CE6">
+        <v>33</v>
+      </c>
+      <c r="CF6">
+        <v>33</v>
+      </c>
+      <c r="CG6">
+        <v>33</v>
+      </c>
+      <c r="CH6">
+        <v>33</v>
+      </c>
+      <c r="CI6">
+        <v>33</v>
+      </c>
     </row>
-    <row r="7" spans="1:82">
+    <row r="7" spans="1:88">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -38173,8 +40181,23 @@
       <c r="CD7">
         <v>81</v>
       </c>
+      <c r="CE7">
+        <v>81</v>
+      </c>
+      <c r="CF7">
+        <v>81</v>
+      </c>
+      <c r="CG7">
+        <v>81</v>
+      </c>
+      <c r="CH7">
+        <v>81</v>
+      </c>
+      <c r="CI7">
+        <v>81</v>
+      </c>
     </row>
-    <row r="8" spans="1:82">
+    <row r="8" spans="1:88">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -38421,8 +40444,23 @@
       <c r="CD8">
         <v>91</v>
       </c>
+      <c r="CE8">
+        <v>91</v>
+      </c>
+      <c r="CF8">
+        <v>91</v>
+      </c>
+      <c r="CG8">
+        <v>91</v>
+      </c>
+      <c r="CH8">
+        <v>91</v>
+      </c>
+      <c r="CI8">
+        <v>91</v>
+      </c>
     </row>
-    <row r="9" spans="1:82">
+    <row r="9" spans="1:88">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -38669,8 +40707,23 @@
       <c r="CD9">
         <v>49</v>
       </c>
+      <c r="CE9">
+        <v>49</v>
+      </c>
+      <c r="CF9">
+        <v>49</v>
+      </c>
+      <c r="CG9">
+        <v>49</v>
+      </c>
+      <c r="CH9">
+        <v>49</v>
+      </c>
+      <c r="CI9">
+        <v>49</v>
+      </c>
     </row>
-    <row r="10" spans="1:82">
+    <row r="10" spans="1:88">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -38917,8 +40970,23 @@
       <c r="CD10">
         <v>85</v>
       </c>
+      <c r="CE10">
+        <v>85</v>
+      </c>
+      <c r="CF10">
+        <v>85</v>
+      </c>
+      <c r="CG10">
+        <v>85</v>
+      </c>
+      <c r="CH10">
+        <v>85</v>
+      </c>
+      <c r="CI10">
+        <v>85</v>
+      </c>
     </row>
-    <row r="11" spans="1:82">
+    <row r="11" spans="1:88">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -39165,8 +41233,23 @@
       <c r="CD11">
         <v>116</v>
       </c>
+      <c r="CE11">
+        <v>116</v>
+      </c>
+      <c r="CF11">
+        <v>116</v>
+      </c>
+      <c r="CG11">
+        <v>116</v>
+      </c>
+      <c r="CH11">
+        <v>116</v>
+      </c>
+      <c r="CI11">
+        <v>116</v>
+      </c>
     </row>
-    <row r="12" spans="1:82" ht="30">
+    <row r="12" spans="1:88" ht="30">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -39413,8 +41496,23 @@
       <c r="CD12">
         <v>20</v>
       </c>
+      <c r="CE12">
+        <v>20</v>
+      </c>
+      <c r="CF12">
+        <v>20</v>
+      </c>
+      <c r="CG12">
+        <v>20</v>
+      </c>
+      <c r="CH12">
+        <v>20</v>
+      </c>
+      <c r="CI12">
+        <v>20</v>
+      </c>
     </row>
-    <row r="13" spans="1:82">
+    <row r="13" spans="1:88">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -39659,6 +41757,21 @@
         <v>0</v>
       </c>
       <c r="CD13">
+        <v>0</v>
+      </c>
+      <c r="CE13">
+        <v>0</v>
+      </c>
+      <c r="CF13">
+        <v>0</v>
+      </c>
+      <c r="CG13">
+        <v>0</v>
+      </c>
+      <c r="CH13">
+        <v>0</v>
+      </c>
+      <c r="CI13">
         <v>0</v>
       </c>
     </row>
@@ -39670,10 +41783,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ23"/>
+  <dimension ref="A1:BF23"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="BA5" sqref="BA5"/>
+    <sheetView topLeftCell="AN1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="AY5" sqref="AY5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39682,7 +41795,7 @@
     <col min="42" max="45" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:58">
       <c r="C1" s="53" t="s">
         <v>179</v>
       </c>
@@ -39699,7 +41812,7 @@
       <c r="N1" s="53"/>
       <c r="O1" s="53"/>
     </row>
-    <row r="2" spans="1:52">
+    <row r="2" spans="1:58">
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
       <c r="E2" s="53"/>
@@ -39714,7 +41827,7 @@
       <c r="N2" s="53"/>
       <c r="O2" s="53"/>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:58">
       <c r="C3" s="53"/>
       <c r="D3" s="53"/>
       <c r="E3" s="53"/>
@@ -39729,7 +41842,7 @@
       <c r="N3" s="53"/>
       <c r="O3" s="53"/>
     </row>
-    <row r="4" spans="1:52">
+    <row r="4" spans="1:58">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -39744,7 +41857,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:58">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -39884,7 +41997,7 @@
         <v>44016</v>
       </c>
       <c r="AW5" s="9">
-        <v>43987</v>
+        <v>44017</v>
       </c>
       <c r="AX5" s="9">
         <v>44018</v>
@@ -39895,8 +42008,26 @@
       <c r="AZ5" s="9">
         <v>44020</v>
       </c>
+      <c r="BA5" s="9">
+        <v>44021</v>
+      </c>
+      <c r="BB5" s="9">
+        <v>44022</v>
+      </c>
+      <c r="BC5" s="9">
+        <v>44023</v>
+      </c>
+      <c r="BD5" s="9">
+        <v>44024</v>
+      </c>
+      <c r="BE5" s="9">
+        <v>44025</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="6" spans="1:52">
+    <row r="6" spans="1:58">
       <c r="A6" s="2" t="s">
         <v>120</v>
       </c>
@@ -40050,8 +42181,23 @@
       <c r="AZ6">
         <v>153</v>
       </c>
+      <c r="BA6">
+        <v>153</v>
+      </c>
+      <c r="BB6">
+        <v>153</v>
+      </c>
+      <c r="BC6">
+        <v>153</v>
+      </c>
+      <c r="BD6">
+        <v>153</v>
+      </c>
+      <c r="BE6">
+        <v>153</v>
+      </c>
     </row>
-    <row r="7" spans="1:52">
+    <row r="7" spans="1:58">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -40205,8 +42351,23 @@
       <c r="AZ7">
         <v>36</v>
       </c>
+      <c r="BA7">
+        <v>36</v>
+      </c>
+      <c r="BB7">
+        <v>36</v>
+      </c>
+      <c r="BC7">
+        <v>36</v>
+      </c>
+      <c r="BD7">
+        <v>36</v>
+      </c>
+      <c r="BE7">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" spans="1:52">
+    <row r="8" spans="1:58">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
@@ -40214,7 +42375,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:52">
+    <row r="9" spans="1:58">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -40368,8 +42529,23 @@
       <c r="AZ9">
         <v>1</v>
       </c>
+      <c r="BA9">
+        <v>1</v>
+      </c>
+      <c r="BB9">
+        <v>1</v>
+      </c>
+      <c r="BC9">
+        <v>1</v>
+      </c>
+      <c r="BD9">
+        <v>1</v>
+      </c>
+      <c r="BE9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:58">
       <c r="A10" s="31" t="s">
         <v>121</v>
       </c>
@@ -40523,8 +42699,23 @@
       <c r="AZ10">
         <v>23</v>
       </c>
+      <c r="BA10">
+        <v>23</v>
+      </c>
+      <c r="BB10">
+        <v>23</v>
+      </c>
+      <c r="BC10">
+        <v>23</v>
+      </c>
+      <c r="BD10">
+        <v>23</v>
+      </c>
+      <c r="BE10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:52">
+    <row r="11" spans="1:58">
       <c r="A11" s="31" t="s">
         <v>122</v>
       </c>
@@ -40678,8 +42869,23 @@
       <c r="AZ11">
         <v>9</v>
       </c>
+      <c r="BA11">
+        <v>9</v>
+      </c>
+      <c r="BB11">
+        <v>9</v>
+      </c>
+      <c r="BC11">
+        <v>9</v>
+      </c>
+      <c r="BD11">
+        <v>9</v>
+      </c>
+      <c r="BE11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:52">
+    <row r="12" spans="1:58">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -40833,13 +43039,28 @@
       <c r="AZ12">
         <v>3</v>
       </c>
+      <c r="BA12">
+        <v>3</v>
+      </c>
+      <c r="BB12">
+        <v>3</v>
+      </c>
+      <c r="BC12">
+        <v>3</v>
+      </c>
+      <c r="BD12">
+        <v>3</v>
+      </c>
+      <c r="BE12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:52">
+    <row r="13" spans="1:58">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:52">
+    <row r="14" spans="1:58">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -40993,8 +43214,23 @@
       <c r="AZ14">
         <v>1</v>
       </c>
+      <c r="BA14">
+        <v>1</v>
+      </c>
+      <c r="BB14">
+        <v>1</v>
+      </c>
+      <c r="BC14">
+        <v>1</v>
+      </c>
+      <c r="BD14">
+        <v>1</v>
+      </c>
+      <c r="BE14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:52">
+    <row r="15" spans="1:58">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -41148,8 +43384,23 @@
       <c r="AZ15">
         <v>0</v>
       </c>
+      <c r="BA15">
+        <v>0</v>
+      </c>
+      <c r="BB15">
+        <v>0</v>
+      </c>
+      <c r="BC15">
+        <v>0</v>
+      </c>
+      <c r="BD15">
+        <v>0</v>
+      </c>
+      <c r="BE15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:52">
+    <row r="16" spans="1:58">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -41303,8 +43554,23 @@
       <c r="AZ16">
         <v>3</v>
       </c>
+      <c r="BA16">
+        <v>3</v>
+      </c>
+      <c r="BB16">
+        <v>3</v>
+      </c>
+      <c r="BC16">
+        <v>3</v>
+      </c>
+      <c r="BD16">
+        <v>3</v>
+      </c>
+      <c r="BE16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:52">
+    <row r="17" spans="1:57">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -41458,8 +43724,23 @@
       <c r="AZ17">
         <v>12</v>
       </c>
+      <c r="BA17">
+        <v>12</v>
+      </c>
+      <c r="BB17">
+        <v>12</v>
+      </c>
+      <c r="BC17">
+        <v>12</v>
+      </c>
+      <c r="BD17">
+        <v>12</v>
+      </c>
+      <c r="BE17">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:52">
+    <row r="18" spans="1:57">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -41613,8 +43894,23 @@
       <c r="AZ18">
         <v>3</v>
       </c>
+      <c r="BA18">
+        <v>3</v>
+      </c>
+      <c r="BB18">
+        <v>3</v>
+      </c>
+      <c r="BC18">
+        <v>3</v>
+      </c>
+      <c r="BD18">
+        <v>3</v>
+      </c>
+      <c r="BE18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:52">
+    <row r="19" spans="1:57">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -41768,8 +44064,23 @@
       <c r="AZ19">
         <v>2</v>
       </c>
+      <c r="BA19">
+        <v>2</v>
+      </c>
+      <c r="BB19">
+        <v>2</v>
+      </c>
+      <c r="BC19">
+        <v>2</v>
+      </c>
+      <c r="BD19">
+        <v>2</v>
+      </c>
+      <c r="BE19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:52">
+    <row r="20" spans="1:57">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -41923,8 +44234,23 @@
       <c r="AZ20">
         <v>2</v>
       </c>
+      <c r="BA20">
+        <v>2</v>
+      </c>
+      <c r="BB20">
+        <v>2</v>
+      </c>
+      <c r="BC20">
+        <v>2</v>
+      </c>
+      <c r="BD20">
+        <v>2</v>
+      </c>
+      <c r="BE20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:52">
+    <row r="21" spans="1:57">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -42078,8 +44404,23 @@
       <c r="AZ21">
         <v>6</v>
       </c>
+      <c r="BA21">
+        <v>6</v>
+      </c>
+      <c r="BB21">
+        <v>6</v>
+      </c>
+      <c r="BC21">
+        <v>6</v>
+      </c>
+      <c r="BD21">
+        <v>6</v>
+      </c>
+      <c r="BE21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:52" ht="45">
+    <row r="22" spans="1:57" ht="45">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -42233,8 +44574,23 @@
       <c r="AZ22">
         <v>4</v>
       </c>
+      <c r="BA22">
+        <v>4</v>
+      </c>
+      <c r="BB22">
+        <v>4</v>
+      </c>
+      <c r="BC22">
+        <v>4</v>
+      </c>
+      <c r="BD22">
+        <v>4</v>
+      </c>
+      <c r="BE22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:52" ht="30">
+    <row r="23" spans="1:57" ht="30">
       <c r="A23" s="39" t="s">
         <v>123</v>
       </c>
@@ -42386,6 +44742,21 @@
         <v>3</v>
       </c>
       <c r="AZ23">
+        <v>3</v>
+      </c>
+      <c r="BA23">
+        <v>3</v>
+      </c>
+      <c r="BB23">
+        <v>3</v>
+      </c>
+      <c r="BC23">
+        <v>3</v>
+      </c>
+      <c r="BD23">
+        <v>3</v>
+      </c>
+      <c r="BE23">
         <v>3</v>
       </c>
     </row>
@@ -42548,7 +44919,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F9" s="28">
         <v>0</v>
@@ -42568,7 +44939,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="28">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E10" s="28" t="s">
         <v>141</v>
@@ -42585,22 +44956,22 @@
         <v>97</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C11" s="28">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" s="28">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F11" s="28">
         <v>0</v>
       </c>
       <c r="G11" s="28">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.45" customHeight="1">
@@ -42614,7 +44985,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E12" s="28" t="s">
         <v>161</v>
@@ -42623,7 +44994,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="28">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.45" customHeight="1">
@@ -42677,13 +45048,13 @@
         <v>100</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C15" s="28">
         <v>13</v>
       </c>
       <c r="D15" s="28">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E15" s="28" t="s">
         <v>135</v>
@@ -42706,7 +45077,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="28">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="28" t="s">
         <v>162</v>
@@ -42715,7 +45086,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="28">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.45" customHeight="1">
@@ -42746,7 +45117,7 @@
         <v>102</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C18" s="28">
         <v>9</v>
@@ -42772,19 +45143,19 @@
         <v>173</v>
       </c>
       <c r="C19" s="28">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19" s="28">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F19" s="28">
         <v>0</v>
       </c>
       <c r="G19" s="28">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="14.45" customHeight="1">
@@ -42792,13 +45163,13 @@
         <v>104</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C20" s="28">
         <v>14</v>
       </c>
       <c r="D20" s="28">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E20" s="28" t="s">
         <v>95</v>
@@ -42821,7 +45192,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21" s="28" t="s">
         <v>145</v>
@@ -42844,7 +45215,7 @@
         <v>26</v>
       </c>
       <c r="D22" s="28">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E22" s="28" t="s">
         <v>174</v>
@@ -42853,7 +45224,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="28">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.6" customHeight="1">
@@ -42884,16 +45255,16 @@
         <v>109</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C24" s="28">
         <v>7</v>
       </c>
       <c r="D24" s="28">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F24" s="28">
         <v>0</v>
@@ -42933,10 +45304,10 @@
         <v>175</v>
       </c>
       <c r="C26" s="28">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D26" s="28">
-        <v>349</v>
+        <v>458</v>
       </c>
       <c r="E26" s="28" t="s">
         <v>176</v>
@@ -42945,7 +45316,7 @@
         <v>7</v>
       </c>
       <c r="G26" s="28">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="H26" s="47"/>
     </row>
@@ -42985,21 +45356,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -43202,32 +45558,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -43244,4 +45590,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Results from July 15, 2020 04:07:13 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/work/WashingtonDC/data.xlsx
+++ b/workflow/python/work/WashingtonDC/data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="148" documentId="8_{DEC2A8EE-2CC1-4116-B97C-51343F77D983}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4CB225F1-8493-4887-BC94-9DEC8C5F87D2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7110" tabRatio="807"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7116" tabRatio="807" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
     <sheet name="Community Cases Tested By OCME" sheetId="7" r:id="rId8"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="180">
   <si>
     <t>Testing</t>
   </si>
@@ -573,7 +579,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of July 13, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of July 14, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -584,7 +590,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>153 cases</t>
+      <t>158 cases</t>
     </r>
     <r>
       <rPr>
@@ -594,14 +600,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> for COVID-19 testing,  and 36 (23.5%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
+      <t xml:space="preserve"> for COVID-19 testing,  and 36 (22.7%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -980,7 +986,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1315,38 +1321,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EA119"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:EB119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="DV1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="EC1" sqref="EC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="88" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="98" max="102" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="104" max="118" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="128" max="131" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="88" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="98" max="102" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="104" max="118" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="128" max="132" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:131">
+    <row r="1" spans="1:132">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1734,8 +1740,11 @@
       <c r="EA1" s="52">
         <v>44025</v>
       </c>
+      <c r="EB1" s="52">
+        <v>44026</v>
+      </c>
     </row>
-    <row r="2" spans="1:131">
+    <row r="2" spans="1:132">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1759,7 +1768,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:131">
+    <row r="3" spans="1:132">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2132,8 +2141,11 @@
       <c r="EA3">
         <v>133916</v>
       </c>
+      <c r="EB3">
+        <v>137944</v>
+      </c>
     </row>
-    <row r="4" spans="1:131">
+    <row r="4" spans="1:132">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2301,8 +2313,11 @@
       <c r="EA4">
         <v>97908</v>
       </c>
+      <c r="EB4">
+        <v>100691</v>
+      </c>
     </row>
-    <row r="5" spans="1:131">
+    <row r="5" spans="1:132">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2696,8 +2711,11 @@
       <c r="EA5">
         <v>10946</v>
       </c>
+      <c r="EB5">
+        <v>11026</v>
+      </c>
     </row>
-    <row r="6" spans="1:131">
+    <row r="6" spans="1:132">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3073,8 +3091,11 @@
       <c r="EA6">
         <v>568</v>
       </c>
+      <c r="EB6">
+        <v>571</v>
+      </c>
     </row>
-    <row r="7" spans="1:131">
+    <row r="7" spans="1:132">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3420,11 +3441,14 @@
       <c r="EA7">
         <v>1774</v>
       </c>
+      <c r="EB7">
+        <v>1809</v>
+      </c>
     </row>
-    <row r="8" spans="1:131">
+    <row r="8" spans="1:132">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:131">
+    <row r="9" spans="1:132">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3662,8 +3686,11 @@
       <c r="EA9">
         <v>345</v>
       </c>
+      <c r="EB9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:131">
+    <row r="10" spans="1:132">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -4003,8 +4030,11 @@
       <c r="EA10">
         <v>82</v>
       </c>
+      <c r="EB10">
+        <v>62</v>
+      </c>
     </row>
-    <row r="11" spans="1:131">
+    <row r="11" spans="1:132">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4344,8 +4374,11 @@
       <c r="EA11">
         <v>440</v>
       </c>
+      <c r="EB11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:131">
+    <row r="12" spans="1:132">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4685,8 +4718,11 @@
       <c r="EA12">
         <v>204</v>
       </c>
+      <c r="EB12">
+        <v>201</v>
+      </c>
     </row>
-    <row r="13" spans="1:131">
+    <row r="13" spans="1:132">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -5026,8 +5062,11 @@
       <c r="EA13">
         <v>236</v>
       </c>
+      <c r="EB13">
+        <v>239</v>
+      </c>
     </row>
-    <row r="14" spans="1:131">
+    <row r="14" spans="1:132">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -5229,8 +5268,11 @@
       <c r="EA14">
         <v>91</v>
       </c>
+      <c r="EB14">
+        <v>95</v>
+      </c>
     </row>
-    <row r="15" spans="1:131">
+    <row r="15" spans="1:132">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -5402,8 +5444,11 @@
       <c r="EA15">
         <v>21</v>
       </c>
+      <c r="EB15">
+        <v>24</v>
+      </c>
     </row>
-    <row r="16" spans="1:131">
+    <row r="16" spans="1:132">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -5605,8 +5650,11 @@
       <c r="EA16">
         <v>1866</v>
       </c>
+      <c r="EB16">
+        <v>1958</v>
+      </c>
     </row>
-    <row r="17" spans="1:131">
+    <row r="17" spans="1:132">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -5808,13 +5856,16 @@
       <c r="EA17" s="23">
         <v>0.75</v>
       </c>
+      <c r="EB17" s="23">
+        <v>0.79</v>
+      </c>
     </row>
-    <row r="19" spans="1:131">
+    <row r="19" spans="1:132">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:131">
+    <row r="20" spans="1:132">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -5822,7 +5873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:131">
+    <row r="21" spans="1:132">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -6162,8 +6213,11 @@
       <c r="EA21">
         <v>120</v>
       </c>
+      <c r="EB21">
+        <v>120</v>
+      </c>
     </row>
-    <row r="22" spans="1:131">
+    <row r="22" spans="1:132">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -6449,8 +6503,11 @@
       <c r="EA22">
         <v>6</v>
       </c>
+      <c r="EB22">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="1:131">
+    <row r="23" spans="1:132">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -6736,8 +6793,11 @@
       <c r="EA23">
         <v>114</v>
       </c>
+      <c r="EB23">
+        <v>114</v>
+      </c>
     </row>
-    <row r="24" spans="1:131">
+    <row r="24" spans="1:132">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -7068,8 +7128,11 @@
       <c r="EA24">
         <v>82</v>
       </c>
+      <c r="EB24">
+        <v>82</v>
+      </c>
     </row>
-    <row r="25" spans="1:131">
+    <row r="25" spans="1:132">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -7400,8 +7463,11 @@
       <c r="EA25">
         <v>88</v>
       </c>
+      <c r="EB25">
+        <v>88</v>
+      </c>
     </row>
-    <row r="26" spans="1:131">
+    <row r="26" spans="1:132">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -7732,13 +7798,16 @@
       <c r="EA26">
         <v>1704</v>
       </c>
+      <c r="EB26">
+        <v>1704</v>
+      </c>
     </row>
-    <row r="28" spans="1:131">
+    <row r="28" spans="1:132">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:131">
+    <row r="29" spans="1:132">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -8078,8 +8147,11 @@
       <c r="EA29">
         <v>165</v>
       </c>
+      <c r="EB29">
+        <v>169</v>
+      </c>
     </row>
-    <row r="30" spans="1:131">
+    <row r="30" spans="1:132">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -8365,8 +8437,11 @@
       <c r="EA30">
         <v>28</v>
       </c>
+      <c r="EB30">
+        <v>32</v>
+      </c>
     </row>
-    <row r="31" spans="1:131">
+    <row r="31" spans="1:132">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -8652,8 +8727,11 @@
       <c r="EA31">
         <v>136</v>
       </c>
+      <c r="EB31">
+        <v>136</v>
+      </c>
     </row>
-    <row r="32" spans="1:131">
+    <row r="32" spans="1:132">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -8984,8 +9062,11 @@
       <c r="EA32">
         <v>93</v>
       </c>
+      <c r="EB32">
+        <v>90</v>
+      </c>
     </row>
-    <row r="33" spans="1:131">
+    <row r="33" spans="1:132">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -9316,8 +9397,11 @@
       <c r="EA33">
         <v>121</v>
       </c>
+      <c r="EB33">
+        <v>122</v>
+      </c>
     </row>
-    <row r="34" spans="1:131">
+    <row r="34" spans="1:132">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -9648,8 +9732,11 @@
       <c r="EA34">
         <v>1405</v>
       </c>
+      <c r="EB34">
+        <v>1411</v>
+      </c>
     </row>
-    <row r="35" spans="1:131">
+    <row r="35" spans="1:132">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -9761,13 +9848,16 @@
       <c r="EA35">
         <v>1</v>
       </c>
+      <c r="EB35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:131">
+    <row r="37" spans="1:132">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:131">
+    <row r="38" spans="1:132">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -10095,8 +10185,11 @@
       <c r="EA38">
         <v>87</v>
       </c>
+      <c r="EB38">
+        <v>88</v>
+      </c>
     </row>
-    <row r="39" spans="1:131">
+    <row r="39" spans="1:132">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -10376,8 +10469,11 @@
       <c r="EA39">
         <v>3</v>
       </c>
+      <c r="EB39">
+        <v>2</v>
+      </c>
     </row>
-    <row r="40" spans="1:131">
+    <row r="40" spans="1:132">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -10657,8 +10753,11 @@
       <c r="EA40">
         <v>83</v>
       </c>
+      <c r="EB40">
+        <v>85</v>
+      </c>
     </row>
-    <row r="41" spans="1:131">
+    <row r="41" spans="1:132">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -10983,8 +11082,11 @@
       <c r="EA41">
         <v>0</v>
       </c>
+      <c r="EB41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:131">
+    <row r="42" spans="1:132">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -11306,8 +11408,11 @@
       <c r="EA42">
         <v>3</v>
       </c>
+      <c r="EB42">
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" spans="1:131">
+    <row r="43" spans="1:132">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -11635,8 +11740,11 @@
       <c r="EA43">
         <v>294</v>
       </c>
+      <c r="EB43">
+        <v>296</v>
+      </c>
     </row>
-    <row r="44" spans="1:131">
+    <row r="44" spans="1:132">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -11898,16 +12006,19 @@
       <c r="EA44">
         <v>1</v>
       </c>
+      <c r="EB44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:131">
+    <row r="45" spans="1:132">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:131">
+    <row r="46" spans="1:132">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:131">
+    <row r="47" spans="1:132">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -12241,8 +12352,11 @@
       <c r="EA47">
         <v>207</v>
       </c>
+      <c r="EB47">
+        <v>207</v>
+      </c>
     </row>
-    <row r="48" spans="1:131">
+    <row r="48" spans="1:132">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -12528,8 +12642,11 @@
       <c r="EA48">
         <v>0</v>
       </c>
+      <c r="EB48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:131">
+    <row r="49" spans="1:132">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -12815,8 +12932,11 @@
       <c r="EA49">
         <v>200</v>
       </c>
+      <c r="EB49">
+        <v>200</v>
+      </c>
     </row>
-    <row r="50" spans="1:131">
+    <row r="50" spans="1:132">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -13147,8 +13267,11 @@
       <c r="EA50">
         <v>51</v>
       </c>
+      <c r="EB50">
+        <v>55</v>
+      </c>
     </row>
-    <row r="51" spans="1:131">
+    <row r="51" spans="1:132">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -13434,8 +13557,11 @@
       <c r="EA51">
         <v>51</v>
       </c>
+      <c r="EB51">
+        <v>55</v>
+      </c>
     </row>
-    <row r="52" spans="1:131">
+    <row r="52" spans="1:132">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -13718,8 +13844,11 @@
       <c r="EA52">
         <v>1215</v>
       </c>
+      <c r="EB52">
+        <v>1211</v>
+      </c>
     </row>
-    <row r="53" spans="1:131">
+    <row r="53" spans="1:132">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -13996,16 +14125,19 @@
       <c r="EA53">
         <v>1</v>
       </c>
+      <c r="EB53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:131">
+    <row r="54" spans="1:132">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:131">
+    <row r="55" spans="1:132">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:131">
+    <row r="56" spans="1:132">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -14324,8 +14456,11 @@
       <c r="EA56">
         <v>35</v>
       </c>
+      <c r="EB56">
+        <v>35</v>
+      </c>
     </row>
-    <row r="57" spans="1:131">
+    <row r="57" spans="1:132">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -14608,8 +14743,11 @@
       <c r="EA57">
         <v>2</v>
       </c>
+      <c r="EB57">
+        <v>2</v>
+      </c>
     </row>
-    <row r="58" spans="1:131">
+    <row r="58" spans="1:132">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -14892,8 +15030,11 @@
       <c r="EA58">
         <v>32</v>
       </c>
+      <c r="EB58">
+        <v>32</v>
+      </c>
     </row>
-    <row r="59" spans="1:131">
+    <row r="59" spans="1:132">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -15212,8 +15353,11 @@
       <c r="EA59">
         <v>2</v>
       </c>
+      <c r="EB59">
+        <v>2</v>
+      </c>
     </row>
-    <row r="60" spans="1:131">
+    <row r="60" spans="1:132">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -15532,8 +15676,11 @@
       <c r="EA60">
         <v>4</v>
       </c>
+      <c r="EB60">
+        <v>4</v>
+      </c>
     </row>
-    <row r="61" spans="1:131">
+    <row r="61" spans="1:132">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -15852,8 +15999,11 @@
       <c r="EA61">
         <v>175</v>
       </c>
+      <c r="EB61">
+        <v>175</v>
+      </c>
     </row>
-    <row r="62" spans="1:131">
+    <row r="62" spans="1:132">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -16130,8 +16280,11 @@
       <c r="EA62">
         <v>1</v>
       </c>
+      <c r="EB62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:131">
+    <row r="64" spans="1:132">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -16450,8 +16603,11 @@
       <c r="EA64">
         <v>13</v>
       </c>
+      <c r="EB64">
+        <v>13</v>
+      </c>
     </row>
-    <row r="65" spans="1:131">
+    <row r="65" spans="1:132">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -16734,8 +16890,11 @@
       <c r="EA65">
         <v>0</v>
       </c>
+      <c r="EB65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:131">
+    <row r="66" spans="1:132">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -17018,8 +17177,11 @@
       <c r="EA66">
         <v>13</v>
       </c>
+      <c r="EB66">
+        <v>13</v>
+      </c>
     </row>
-    <row r="67" spans="1:131">
+    <row r="67" spans="1:132">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -17338,8 +17500,11 @@
       <c r="EA67">
         <v>68</v>
       </c>
+      <c r="EB67">
+        <v>68</v>
+      </c>
     </row>
-    <row r="68" spans="1:131">
+    <row r="68" spans="1:132">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -17659,8 +17824,11 @@
       <c r="EA68">
         <v>68</v>
       </c>
+      <c r="EB68">
+        <v>68</v>
+      </c>
     </row>
-    <row r="69" spans="1:131">
+    <row r="69" spans="1:132">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -17979,8 +18147,11 @@
       <c r="EA69">
         <v>0</v>
       </c>
+      <c r="EB69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:131">
+    <row r="70" spans="1:132">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -18263,11 +18434,14 @@
       <c r="EA70">
         <v>0</v>
       </c>
+      <c r="EB70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:131">
+    <row r="71" spans="1:132">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:131">
+    <row r="72" spans="1:132">
       <c r="A72" s="2" t="s">
         <v>119</v>
       </c>
@@ -18436,8 +18610,11 @@
       <c r="EA72">
         <v>10</v>
       </c>
+      <c r="EB72">
+        <v>11</v>
+      </c>
     </row>
-    <row r="73" spans="1:131">
+    <row r="73" spans="1:132">
       <c r="A73" s="2" t="s">
         <v>119</v>
       </c>
@@ -18606,8 +18783,11 @@
       <c r="EA73">
         <v>1</v>
       </c>
+      <c r="EB73">
+        <v>2</v>
+      </c>
     </row>
-    <row r="74" spans="1:131">
+    <row r="74" spans="1:132">
       <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
@@ -18776,8 +18956,11 @@
       <c r="EA74">
         <v>9</v>
       </c>
+      <c r="EB74">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:131">
+    <row r="75" spans="1:132">
       <c r="A75" s="2" t="s">
         <v>119</v>
       </c>
@@ -18946,8 +19129,11 @@
       <c r="EA75">
         <v>2</v>
       </c>
+      <c r="EB75">
+        <v>2</v>
+      </c>
     </row>
-    <row r="76" spans="1:131">
+    <row r="76" spans="1:132">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -19116,8 +19302,11 @@
       <c r="EA76">
         <v>3</v>
       </c>
+      <c r="EB76">
+        <v>4</v>
+      </c>
     </row>
-    <row r="77" spans="1:131">
+    <row r="77" spans="1:132">
       <c r="A77" s="2" t="s">
         <v>119</v>
       </c>
@@ -19286,13 +19475,16 @@
       <c r="EA77">
         <v>48</v>
       </c>
+      <c r="EB77">
+        <v>52</v>
+      </c>
     </row>
-    <row r="79" spans="1:131">
+    <row r="79" spans="1:132">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:131">
+    <row r="80" spans="1:132">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -19614,8 +19806,11 @@
       <c r="EA80">
         <v>325</v>
       </c>
+      <c r="EB80">
+        <v>325</v>
+      </c>
     </row>
-    <row r="81" spans="1:131">
+    <row r="81" spans="1:132">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -19937,8 +20132,11 @@
       <c r="EA81">
         <v>70</v>
       </c>
+      <c r="EB81">
+        <v>70</v>
+      </c>
     </row>
-    <row r="82" spans="1:131">
+    <row r="82" spans="1:132">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -20260,8 +20458,11 @@
       <c r="EA82">
         <v>67</v>
       </c>
+      <c r="EB82">
+        <v>67</v>
+      </c>
     </row>
-    <row r="83" spans="1:131">
+    <row r="83" spans="1:132">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -20541,8 +20742,11 @@
       <c r="EA83">
         <v>20</v>
       </c>
+      <c r="EB83">
+        <v>20</v>
+      </c>
     </row>
-    <row r="85" spans="1:131">
+    <row r="85" spans="1:132">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -20864,8 +21068,11 @@
       <c r="EA85">
         <v>124</v>
       </c>
+      <c r="EB85">
+        <v>125</v>
+      </c>
     </row>
-    <row r="86" spans="1:131">
+    <row r="86" spans="1:132">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -21187,8 +21394,11 @@
       <c r="EA86">
         <v>5</v>
       </c>
+      <c r="EB86">
+        <v>6</v>
+      </c>
     </row>
-    <row r="87" spans="1:131">
+    <row r="87" spans="1:132">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -21510,8 +21720,11 @@
       <c r="EA87">
         <v>21</v>
       </c>
+      <c r="EB87">
+        <v>21</v>
+      </c>
     </row>
-    <row r="88" spans="1:131">
+    <row r="88" spans="1:132">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -21833,8 +22046,11 @@
       <c r="EA88">
         <v>256</v>
       </c>
+      <c r="EB88">
+        <v>256</v>
+      </c>
     </row>
-    <row r="89" spans="1:131">
+    <row r="89" spans="1:132">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -22030,8 +22246,11 @@
       <c r="EA89">
         <v>1</v>
       </c>
+      <c r="EB89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:131">
+    <row r="91" spans="1:132">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -22353,8 +22572,11 @@
       <c r="EA91">
         <v>82</v>
       </c>
+      <c r="EB91">
+        <v>82</v>
+      </c>
     </row>
-    <row r="92" spans="1:131">
+    <row r="92" spans="1:132">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -22676,8 +22898,11 @@
       <c r="EA92">
         <v>1</v>
       </c>
+      <c r="EB92">
+        <v>1</v>
+      </c>
     </row>
-    <row r="93" spans="1:131">
+    <row r="93" spans="1:132">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -22987,8 +23212,11 @@
       <c r="EA93">
         <v>192</v>
       </c>
+      <c r="EB93">
+        <v>192</v>
+      </c>
     </row>
-    <row r="94" spans="1:131">
+    <row r="94" spans="1:132">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -23310,8 +23538,11 @@
       <c r="EA94">
         <v>62</v>
       </c>
+      <c r="EB94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:131">
+    <row r="95" spans="1:132">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -23591,11 +23822,14 @@
       <c r="EA95">
         <v>14</v>
       </c>
+      <c r="EB95">
+        <v>14</v>
+      </c>
     </row>
-    <row r="96" spans="1:131">
+    <row r="96" spans="1:132">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:131">
+    <row r="97" spans="1:132">
       <c r="A97" s="2" t="s">
         <v>130</v>
       </c>
@@ -23734,8 +23968,11 @@
       <c r="EA97">
         <v>12</v>
       </c>
+      <c r="EB97">
+        <v>12</v>
+      </c>
     </row>
-    <row r="98" spans="1:131">
+    <row r="98" spans="1:132">
       <c r="A98" s="2" t="s">
         <v>130</v>
       </c>
@@ -23874,8 +24111,11 @@
       <c r="EA98">
         <v>9</v>
       </c>
+      <c r="EB98">
+        <v>9</v>
+      </c>
     </row>
-    <row r="99" spans="1:131">
+    <row r="99" spans="1:132">
       <c r="A99" s="2" t="s">
         <v>130</v>
       </c>
@@ -24014,8 +24254,11 @@
       <c r="EA99">
         <v>52</v>
       </c>
+      <c r="EB99">
+        <v>52</v>
+      </c>
     </row>
-    <row r="100" spans="1:131">
+    <row r="100" spans="1:132">
       <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
@@ -24154,8 +24397,11 @@
       <c r="EA100">
         <v>1</v>
       </c>
+      <c r="EB100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:131">
+    <row r="102" spans="1:132">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -24396,8 +24642,11 @@
       <c r="EA102">
         <v>211</v>
       </c>
+      <c r="EB102">
+        <v>211</v>
+      </c>
     </row>
-    <row r="103" spans="1:131">
+    <row r="103" spans="1:132">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -24638,8 +24887,11 @@
       <c r="EA103">
         <v>133</v>
       </c>
+      <c r="EB103">
+        <v>140</v>
+      </c>
     </row>
-    <row r="104" spans="1:131">
+    <row r="104" spans="1:132">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -24878,6 +25130,9 @@
         <v>28</v>
       </c>
       <c r="EA104">
+        <v>28</v>
+      </c>
+      <c r="EB104">
         <v>28</v>
       </c>
     </row>
@@ -24893,22 +25148,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:DB11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:DC11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CT3" sqref="CT3"/>
+      <selection pane="topRight" activeCell="DD2" sqref="DD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:106" s="2" customFormat="1">
+    <row r="2" spans="1:107" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -25227,8 +25482,11 @@
       <c r="DB2" s="9">
         <v>44025</v>
       </c>
+      <c r="DC2" s="9">
+        <v>44026</v>
+      </c>
     </row>
-    <row r="3" spans="1:106">
+    <row r="3" spans="1:107">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -25547,8 +25805,11 @@
       <c r="DB3">
         <v>1556</v>
       </c>
+      <c r="DC3">
+        <v>1565</v>
+      </c>
     </row>
-    <row r="4" spans="1:106">
+    <row r="4" spans="1:107">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -25867,8 +26128,11 @@
       <c r="DB4">
         <v>649</v>
       </c>
+      <c r="DC4">
+        <v>662</v>
+      </c>
     </row>
-    <row r="5" spans="1:106">
+    <row r="5" spans="1:107">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -26187,8 +26451,11 @@
       <c r="DB5">
         <v>514</v>
       </c>
+      <c r="DC5">
+        <v>518</v>
+      </c>
     </row>
-    <row r="6" spans="1:106">
+    <row r="6" spans="1:107">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -26507,8 +26774,11 @@
       <c r="DB6">
         <v>2244</v>
       </c>
+      <c r="DC6">
+        <v>2252</v>
+      </c>
     </row>
-    <row r="7" spans="1:106">
+    <row r="7" spans="1:107">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -26827,8 +27097,11 @@
       <c r="DB7">
         <v>1624</v>
       </c>
+      <c r="DC7">
+        <v>1637</v>
+      </c>
     </row>
-    <row r="8" spans="1:106">
+    <row r="8" spans="1:107">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -27147,8 +27420,11 @@
       <c r="DB8">
         <v>998</v>
       </c>
+      <c r="DC8">
+        <v>1010</v>
+      </c>
     </row>
-    <row r="9" spans="1:106">
+    <row r="9" spans="1:107">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -27467,8 +27743,11 @@
       <c r="DB9">
         <v>1572</v>
       </c>
+      <c r="DC9">
+        <v>1584</v>
+      </c>
     </row>
-    <row r="10" spans="1:106">
+    <row r="10" spans="1:107">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -27787,8 +28066,11 @@
       <c r="DB10">
         <v>1610</v>
       </c>
+      <c r="DC10">
+        <v>1618</v>
+      </c>
     </row>
-    <row r="11" spans="1:106">
+    <row r="11" spans="1:107">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -28106,6 +28388,9 @@
       </c>
       <c r="DB11">
         <v>179</v>
+      </c>
+      <c r="DC11">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -28115,22 +28400,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:CW17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:CX17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CQ3" sqref="CQ3"/>
+      <selection pane="topRight" activeCell="CY2" sqref="CY2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" customWidth="1"/>
+    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:101" s="2" customFormat="1">
+    <row r="2" spans="1:102" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -28432,8 +28717,11 @@
       <c r="CW2" s="9">
         <v>44025</v>
       </c>
+      <c r="CX2" s="9">
+        <v>44026</v>
+      </c>
     </row>
-    <row r="3" spans="1:101" s="2" customFormat="1">
+    <row r="3" spans="1:102" s="2" customFormat="1">
       <c r="A3" s="41" t="s">
         <v>36</v>
       </c>
@@ -28442,7 +28730,7 @@
       <c r="D3" s="9"/>
       <c r="CP3" s="4"/>
     </row>
-    <row r="4" spans="1:101">
+    <row r="4" spans="1:102">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -28746,8 +29034,11 @@
       <c r="CW4">
         <v>10946</v>
       </c>
+      <c r="CX4">
+        <v>11206</v>
+      </c>
     </row>
-    <row r="5" spans="1:101">
+    <row r="5" spans="1:102">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -29051,8 +29342,11 @@
       <c r="CW5">
         <v>183</v>
       </c>
+      <c r="CX5">
+        <v>186</v>
+      </c>
     </row>
-    <row r="6" spans="1:101">
+    <row r="6" spans="1:102">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -29356,8 +29650,11 @@
       <c r="CW6">
         <v>2234</v>
       </c>
+      <c r="CX6">
+        <v>2253</v>
+      </c>
     </row>
-    <row r="7" spans="1:101">
+    <row r="7" spans="1:102">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -29661,8 +29958,11 @@
       <c r="CW7">
         <v>5395</v>
       </c>
+      <c r="CX7">
+        <v>5431</v>
+      </c>
     </row>
-    <row r="8" spans="1:101">
+    <row r="8" spans="1:102">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -29966,8 +30266,11 @@
       <c r="CW8">
         <v>170</v>
       </c>
+      <c r="CX8">
+        <v>170</v>
+      </c>
     </row>
-    <row r="9" spans="1:101" ht="30">
+    <row r="9" spans="1:102" ht="28.8">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -30271,8 +30574,11 @@
       <c r="CW9">
         <v>27</v>
       </c>
+      <c r="CX9">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:101" ht="30">
+    <row r="10" spans="1:102" ht="28.8">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -30572,8 +30878,11 @@
       <c r="CW10">
         <v>29</v>
       </c>
+      <c r="CX10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="11" spans="1:101">
+    <row r="11" spans="1:102">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -30877,8 +31186,11 @@
       <c r="CW11">
         <v>2818</v>
       </c>
+      <c r="CX11">
+        <v>2840</v>
+      </c>
     </row>
-    <row r="12" spans="1:101" ht="30">
+    <row r="12" spans="1:102">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -31182,8 +31494,11 @@
       <c r="CW12">
         <v>90</v>
       </c>
+      <c r="CX12">
+        <v>90</v>
+      </c>
     </row>
-    <row r="13" spans="1:101">
+    <row r="13" spans="1:102">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -31194,7 +31509,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:101">
+    <row r="14" spans="1:102">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -31498,8 +31813,11 @@
       <c r="CW14">
         <v>1349</v>
       </c>
+      <c r="CX14">
+        <v>1364</v>
+      </c>
     </row>
-    <row r="15" spans="1:101">
+    <row r="15" spans="1:102">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -31803,8 +32121,11 @@
       <c r="CW15">
         <v>3058</v>
       </c>
+      <c r="CX15">
+        <v>3069</v>
+      </c>
     </row>
-    <row r="16" spans="1:101">
+    <row r="16" spans="1:102">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -32108,8 +32429,11 @@
       <c r="CW16">
         <v>6521</v>
       </c>
+      <c r="CX16">
+        <v>6575</v>
+      </c>
     </row>
-    <row r="17" spans="1:101" ht="30">
+    <row r="17" spans="1:102">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -32411,6 +32735,9 @@
         <v>18</v>
       </c>
       <c r="CW17">
+        <v>18</v>
+      </c>
+      <c r="CX17">
         <v>18</v>
       </c>
     </row>
@@ -32421,18 +32748,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:CX9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CO2" sqref="CO2"/>
+      <selection pane="topRight" activeCell="CY1" sqref="CY1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:102" s="2" customFormat="1">
@@ -32736,8 +33063,8 @@
       <c r="CW1" s="9">
         <v>44025</v>
       </c>
-      <c r="CX1" s="2" t="s">
-        <v>129</v>
+      <c r="CX1" s="9">
+        <v>44026</v>
       </c>
     </row>
     <row r="2" spans="1:102">
@@ -33051,6 +33378,9 @@
       <c r="CW3">
         <v>568</v>
       </c>
+      <c r="CX3">
+        <v>571</v>
+      </c>
     </row>
     <row r="4" spans="1:102">
       <c r="A4" s="13" t="s">
@@ -33356,8 +33686,11 @@
       <c r="CW4">
         <v>8</v>
       </c>
+      <c r="CX4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:102" ht="30">
+    <row r="5" spans="1:102" ht="28.8">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -33660,6 +33993,9 @@
       </c>
       <c r="CW5">
         <v>421</v>
+      </c>
+      <c r="CX5">
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:102">
@@ -33966,8 +34302,11 @@
       <c r="CW6">
         <v>74</v>
       </c>
+      <c r="CX6">
+        <v>74</v>
+      </c>
     </row>
-    <row r="7" spans="1:102" ht="30">
+    <row r="7" spans="1:102">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -34269,6 +34608,9 @@
         <v>60</v>
       </c>
       <c r="CW7">
+        <v>60</v>
+      </c>
+      <c r="CX7">
         <v>60</v>
       </c>
     </row>
@@ -34574,6 +34916,9 @@
         <v>5</v>
       </c>
       <c r="CW8">
+        <v>5</v>
+      </c>
+      <c r="CX8">
         <v>5</v>
       </c>
     </row>
@@ -34618,17 +34963,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CP5"/>
   <sheetViews>
     <sheetView zoomScale="95" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CI2" sqref="CI2"/>
+      <selection pane="topRight" activeCell="CQ1" sqref="CQ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:94" s="2" customFormat="1">
@@ -34908,8 +35253,8 @@
       <c r="CO1" s="9">
         <v>44025</v>
       </c>
-      <c r="CP1" s="2" t="s">
-        <v>129</v>
+      <c r="CP1" s="9">
+        <v>44026</v>
       </c>
     </row>
     <row r="2" spans="1:94">
@@ -35197,6 +35542,9 @@
       <c r="CO3">
         <v>568</v>
       </c>
+      <c r="CP3">
+        <v>571</v>
+      </c>
     </row>
     <row r="4" spans="1:94">
       <c r="A4" s="42" t="s">
@@ -35478,6 +35826,9 @@
       <c r="CO4">
         <v>243</v>
       </c>
+      <c r="CP4">
+        <v>244</v>
+      </c>
     </row>
     <row r="5" spans="1:94">
       <c r="A5" s="42" t="s">
@@ -35758,6 +36109,9 @@
       </c>
       <c r="CO5">
         <v>325</v>
+      </c>
+      <c r="CP5">
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -35767,17 +36121,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:CP11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CI2" sqref="CI2"/>
+      <selection pane="topRight" activeCell="CQ1" sqref="CQ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:94" s="2" customFormat="1">
@@ -36057,8 +36411,8 @@
       <c r="CO1" s="9">
         <v>44025</v>
       </c>
-      <c r="CP1" s="2" t="s">
-        <v>129</v>
+      <c r="CP1" s="9">
+        <v>44026</v>
       </c>
     </row>
     <row r="2" spans="1:94">
@@ -36346,6 +36700,9 @@
       <c r="CO3">
         <v>568</v>
       </c>
+      <c r="CP3">
+        <v>571</v>
+      </c>
     </row>
     <row r="4" spans="1:94">
       <c r="A4" s="5" t="s">
@@ -36627,6 +36984,9 @@
       <c r="CO4">
         <v>0</v>
       </c>
+      <c r="CP4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:94">
       <c r="A5" s="5" t="s">
@@ -36908,6 +37268,9 @@
       <c r="CO5">
         <v>3</v>
       </c>
+      <c r="CP5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:94">
       <c r="A6" s="5" t="s">
@@ -37189,6 +37552,9 @@
       <c r="CO6">
         <v>7</v>
       </c>
+      <c r="CP6">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:94">
       <c r="A7" s="5" t="s">
@@ -37470,6 +37836,9 @@
       <c r="CO7">
         <v>19</v>
       </c>
+      <c r="CP7">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:94">
       <c r="A8" s="5" t="s">
@@ -37751,6 +38120,9 @@
       <c r="CO8">
         <v>66</v>
       </c>
+      <c r="CP8">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:94">
       <c r="A9" s="5" t="s">
@@ -38032,6 +38404,9 @@
       <c r="CO9">
         <v>134</v>
       </c>
+      <c r="CP9">
+        <v>135</v>
+      </c>
     </row>
     <row r="10" spans="1:94">
       <c r="A10" s="6" t="s">
@@ -38313,6 +38688,9 @@
       <c r="CO10">
         <v>144</v>
       </c>
+      <c r="CP10">
+        <v>146</v>
+      </c>
     </row>
     <row r="11" spans="1:94">
       <c r="A11" s="6" t="s">
@@ -38592,6 +38970,9 @@
         <v>195</v>
       </c>
       <c r="CO11">
+        <v>195</v>
+      </c>
+      <c r="CP11">
         <v>195</v>
       </c>
     </row>
@@ -38602,18 +38983,18 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:CJ13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="BS1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CC3" sqref="CC3"/>
+      <selection pane="topRight" activeCell="CK2" sqref="CK2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="57" max="57" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="57" max="57" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:88" s="2" customFormat="1">
@@ -38878,8 +39259,8 @@
       <c r="CI2" s="9">
         <v>44025</v>
       </c>
-      <c r="CJ2" s="2" t="s">
-        <v>129</v>
+      <c r="CJ2" s="9">
+        <v>44026</v>
       </c>
     </row>
     <row r="3" spans="1:88">
@@ -39144,6 +39525,9 @@
       <c r="CI3">
         <v>568</v>
       </c>
+      <c r="CJ3">
+        <v>571</v>
+      </c>
     </row>
     <row r="4" spans="1:88">
       <c r="A4" s="7">
@@ -39405,6 +39789,9 @@
         <v>62</v>
       </c>
       <c r="CI4">
+        <v>62</v>
+      </c>
+      <c r="CJ4">
         <v>62</v>
       </c>
     </row>
@@ -39670,6 +40057,9 @@
       <c r="CI5">
         <v>31</v>
       </c>
+      <c r="CJ5">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:88">
       <c r="A6" s="7">
@@ -39933,6 +40323,9 @@
       <c r="CI6">
         <v>33</v>
       </c>
+      <c r="CJ6">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:88">
       <c r="A7" s="7">
@@ -40196,6 +40589,9 @@
       <c r="CI7">
         <v>81</v>
       </c>
+      <c r="CJ7">
+        <v>83</v>
+      </c>
     </row>
     <row r="8" spans="1:88">
       <c r="A8" s="7">
@@ -40459,6 +40855,9 @@
       <c r="CI8">
         <v>91</v>
       </c>
+      <c r="CJ8">
+        <v>92</v>
+      </c>
     </row>
     <row r="9" spans="1:88">
       <c r="A9" s="7">
@@ -40722,6 +41121,9 @@
       <c r="CI9">
         <v>49</v>
       </c>
+      <c r="CJ9">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:88">
       <c r="A10" s="7">
@@ -40985,6 +41387,9 @@
       <c r="CI10">
         <v>85</v>
       </c>
+      <c r="CJ10">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:88">
       <c r="A11" s="7">
@@ -41248,8 +41653,11 @@
       <c r="CI11">
         <v>116</v>
       </c>
+      <c r="CJ11">
+        <v>116</v>
+      </c>
     </row>
-    <row r="12" spans="1:88" ht="30">
+    <row r="12" spans="1:88" ht="28.8">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -41509,6 +41917,9 @@
         <v>20</v>
       </c>
       <c r="CI12">
+        <v>20</v>
+      </c>
+      <c r="CJ12">
         <v>20</v>
       </c>
     </row>
@@ -41772,6 +42183,9 @@
         <v>0</v>
       </c>
       <c r="CI13">
+        <v>0</v>
+      </c>
+      <c r="CJ13">
         <v>0</v>
       </c>
     </row>
@@ -41782,17 +42196,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BF23"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="AY5" sqref="AY5"/>
+    <sheetView tabSelected="1" topLeftCell="AV10" zoomScale="96" workbookViewId="0">
+      <selection activeCell="BF9" sqref="BF9:BF12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="42" max="45" width="8.85546875" customWidth="1"/>
+    <col min="42" max="45" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58">
@@ -42023,8 +42437,8 @@
       <c r="BE5" s="9">
         <v>44025</v>
       </c>
-      <c r="BF5" t="s">
-        <v>129</v>
+      <c r="BF5" s="9">
+        <v>44026</v>
       </c>
     </row>
     <row r="6" spans="1:58">
@@ -42196,6 +42610,9 @@
       <c r="BE6">
         <v>153</v>
       </c>
+      <c r="BF6">
+        <v>158</v>
+      </c>
     </row>
     <row r="7" spans="1:58">
       <c r="A7" s="2" t="s">
@@ -42366,6 +42783,9 @@
       <c r="BE7">
         <v>36</v>
       </c>
+      <c r="BF7">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:58">
       <c r="A8" s="35" t="s">
@@ -42544,6 +42964,9 @@
       <c r="BE9">
         <v>1</v>
       </c>
+      <c r="BF9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:58">
       <c r="A10" s="31" t="s">
@@ -42714,6 +43137,9 @@
       <c r="BE10">
         <v>23</v>
       </c>
+      <c r="BF10">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:58">
       <c r="A11" s="31" t="s">
@@ -42884,6 +43310,9 @@
       <c r="BE11">
         <v>9</v>
       </c>
+      <c r="BF11">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:58">
       <c r="A12" s="31" t="s">
@@ -43054,6 +43483,9 @@
       <c r="BE12">
         <v>3</v>
       </c>
+      <c r="BF12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:58">
       <c r="A13" s="36" t="s">
@@ -43229,6 +43661,9 @@
       <c r="BE14">
         <v>1</v>
       </c>
+      <c r="BF14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:58">
       <c r="A15" s="31">
@@ -43399,6 +43834,9 @@
       <c r="BE15">
         <v>0</v>
       </c>
+      <c r="BF15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:58">
       <c r="A16" s="31">
@@ -43569,8 +44007,11 @@
       <c r="BE16">
         <v>3</v>
       </c>
+      <c r="BF16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:57">
+    <row r="17" spans="1:58">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -43739,8 +44180,11 @@
       <c r="BE17">
         <v>12</v>
       </c>
+      <c r="BF17">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:57">
+    <row r="18" spans="1:58">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -43909,8 +44353,11 @@
       <c r="BE18">
         <v>3</v>
       </c>
+      <c r="BF18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:57">
+    <row r="19" spans="1:58">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -44079,8 +44526,11 @@
       <c r="BE19">
         <v>2</v>
       </c>
+      <c r="BF19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:57">
+    <row r="20" spans="1:58">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -44249,8 +44699,11 @@
       <c r="BE20">
         <v>2</v>
       </c>
+      <c r="BF20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:57">
+    <row r="21" spans="1:58">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -44419,8 +44872,11 @@
       <c r="BE21">
         <v>6</v>
       </c>
+      <c r="BF21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:57" ht="45">
+    <row r="22" spans="1:58" ht="28.8">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -44590,7 +45046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:57" ht="30">
+    <row r="23" spans="1:58" ht="28.8">
       <c r="A23" s="39" t="s">
         <v>123</v>
       </c>
@@ -44769,21 +45225,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -44836,7 +45292,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A4" s="56"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -44849,7 +45305,7 @@
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A5" s="56"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
@@ -44860,7 +45316,7 @@
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A6" s="56"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
@@ -44871,7 +45327,7 @@
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1">
+    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1">
       <c r="A7" s="56"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
@@ -44882,7 +45338,7 @@
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" ht="14.45" customHeight="1">
+    <row r="8" spans="1:7" ht="14.4" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>94</v>
       </c>
@@ -44905,7 +45361,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.45" customHeight="1">
+    <row r="9" spans="1:7" ht="14.4" customHeight="1">
       <c r="A9" s="30" t="s">
         <v>147</v>
       </c>
@@ -44928,7 +45384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.45" customHeight="1">
+    <row r="10" spans="1:7" ht="14.4" customHeight="1">
       <c r="A10" s="27" t="s">
         <v>96</v>
       </c>
@@ -44951,7 +45407,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.45" customHeight="1">
+    <row r="11" spans="1:7" ht="14.4" customHeight="1">
       <c r="A11" s="27" t="s">
         <v>97</v>
       </c>
@@ -44974,7 +45430,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.45" customHeight="1">
+    <row r="12" spans="1:7" ht="14.4" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>98</v>
       </c>
@@ -44997,7 +45453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.45" customHeight="1">
+    <row r="13" spans="1:7" ht="14.4" customHeight="1">
       <c r="A13" s="27" t="s">
         <v>126</v>
       </c>
@@ -45020,7 +45476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.45" customHeight="1">
+    <row r="14" spans="1:7" ht="14.4" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>99</v>
       </c>
@@ -45043,7 +45499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.45" customHeight="1">
+    <row r="15" spans="1:7" ht="14.4" customHeight="1">
       <c r="A15" s="27" t="s">
         <v>100</v>
       </c>
@@ -45089,7 +45545,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.45" customHeight="1">
+    <row r="17" spans="1:8" ht="14.4" customHeight="1">
       <c r="A17" s="27" t="s">
         <v>101</v>
       </c>
@@ -45112,7 +45568,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.45" customHeight="1">
+    <row r="18" spans="1:8" ht="14.4" customHeight="1">
       <c r="A18" s="27" t="s">
         <v>102</v>
       </c>
@@ -45135,7 +45591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.45" customHeight="1">
+    <row r="19" spans="1:8" ht="14.4" customHeight="1">
       <c r="A19" s="27" t="s">
         <v>103</v>
       </c>
@@ -45158,7 +45614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.45" customHeight="1">
+    <row r="20" spans="1:8" ht="14.4" customHeight="1">
       <c r="A20" s="27" t="s">
         <v>104</v>
       </c>
@@ -45181,7 +45637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.45" customHeight="1">
+    <row r="21" spans="1:8" ht="14.4" customHeight="1">
       <c r="A21" s="27" t="s">
         <v>105</v>
       </c>
@@ -45204,7 +45660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.45" customHeight="1">
+    <row r="22" spans="1:8" ht="14.4" customHeight="1">
       <c r="A22" s="27" t="s">
         <v>107</v>
       </c>
@@ -45296,7 +45752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.45" customHeight="1">
+    <row r="26" spans="1:8" ht="17.399999999999999" customHeight="1">
       <c r="A26" s="46" t="s">
         <v>49</v>
       </c>
@@ -45320,7 +45776,7 @@
       </c>
       <c r="H26" s="47"/>
     </row>
-    <row r="27" spans="1:8" ht="17.45" customHeight="1">
+    <row r="27" spans="1:8" ht="17.399999999999999" customHeight="1">
       <c r="A27" s="24" t="s">
         <v>110</v>
       </c>
@@ -45334,7 +45790,7 @@
       <c r="G27" s="50"/>
       <c r="H27" s="49"/>
     </row>
-    <row r="28" spans="1:8" ht="17.45" customHeight="1">
+    <row r="28" spans="1:8" ht="17.399999999999999" customHeight="1">
       <c r="B28" s="27"/>
       <c r="C28" s="44"/>
       <c r="D28" s="44"/>
@@ -45342,7 +45798,7 @@
       <c r="F28" s="44"/>
       <c r="G28" s="44"/>
     </row>
-    <row r="29" spans="1:8" ht="17.45" customHeight="1"/>
+    <row r="29" spans="1:8" ht="17.399999999999999" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
@@ -45356,6 +45812,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -45558,15 +46023,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -45574,6 +46030,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -45592,27 +46056,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Results from July 16, 2020 04:23:11 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/work/WashingtonDC/data.xlsx
+++ b/workflow/python/work/WashingtonDC/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{DEC2A8EE-2CC1-4116-B97C-51343F77D983}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4CB225F1-8493-4887-BC94-9DEC8C5F87D2}"/>
+  <xr:revisionPtr revIDLastSave="279" documentId="8_{DEC2A8EE-2CC1-4116-B97C-51343F77D983}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{EF2C1E1D-AFE6-4D79-B2CB-FEEE8CDF7177}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7116" tabRatio="807" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7116" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Community Cases Tested By OCME" sheetId="7" r:id="rId8"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="180">
   <si>
     <t>Testing</t>
   </si>
@@ -579,7 +579,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of July 14, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of July 15, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -1329,11 +1329,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EB119"/>
+  <dimension ref="A1:EC119"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="DV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EC1" sqref="EC1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="DZ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="ED1" sqref="ED1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1349,10 +1349,10 @@
     <col min="98" max="102" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="104" max="118" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="128" max="132" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="128" max="133" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:132">
+    <row r="1" spans="1:133">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1743,8 +1743,11 @@
       <c r="EB1" s="52">
         <v>44026</v>
       </c>
+      <c r="EC1" s="52">
+        <v>44027</v>
+      </c>
     </row>
-    <row r="2" spans="1:132">
+    <row r="2" spans="1:133">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1768,7 +1771,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:132">
+    <row r="3" spans="1:133">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2144,8 +2147,11 @@
       <c r="EB3">
         <v>137944</v>
       </c>
+      <c r="EC3">
+        <v>140242</v>
+      </c>
     </row>
-    <row r="4" spans="1:132">
+    <row r="4" spans="1:133">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2316,8 +2322,11 @@
       <c r="EB4">
         <v>100691</v>
       </c>
+      <c r="EC4">
+        <v>102058</v>
+      </c>
     </row>
-    <row r="5" spans="1:132">
+    <row r="5" spans="1:133">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2714,8 +2723,11 @@
       <c r="EB5">
         <v>11026</v>
       </c>
+      <c r="EC5">
+        <v>11076</v>
+      </c>
     </row>
-    <row r="6" spans="1:132">
+    <row r="6" spans="1:133">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3094,8 +3106,11 @@
       <c r="EB6">
         <v>571</v>
       </c>
+      <c r="EC6">
+        <v>574</v>
+      </c>
     </row>
-    <row r="7" spans="1:132">
+    <row r="7" spans="1:133">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3444,11 +3459,14 @@
       <c r="EB7">
         <v>1809</v>
       </c>
+      <c r="EC7">
+        <v>1843</v>
+      </c>
     </row>
-    <row r="8" spans="1:132">
+    <row r="8" spans="1:133">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:132">
+    <row r="9" spans="1:133">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3689,8 +3707,11 @@
       <c r="EB9">
         <v>345</v>
       </c>
+      <c r="EC9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:132">
+    <row r="10" spans="1:133">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -4033,8 +4054,11 @@
       <c r="EB10">
         <v>62</v>
       </c>
+      <c r="EC10">
+        <v>68</v>
+      </c>
     </row>
-    <row r="11" spans="1:132">
+    <row r="11" spans="1:133">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4377,8 +4401,11 @@
       <c r="EB11">
         <v>440</v>
       </c>
+      <c r="EC11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:132">
+    <row r="12" spans="1:133">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4721,8 +4748,11 @@
       <c r="EB12">
         <v>201</v>
       </c>
+      <c r="EC12">
+        <v>191</v>
+      </c>
     </row>
-    <row r="13" spans="1:132">
+    <row r="13" spans="1:133">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -5065,8 +5095,11 @@
       <c r="EB13">
         <v>239</v>
       </c>
+      <c r="EC13">
+        <v>249</v>
+      </c>
     </row>
-    <row r="14" spans="1:132">
+    <row r="14" spans="1:133">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -5271,8 +5304,11 @@
       <c r="EB14">
         <v>95</v>
       </c>
+      <c r="EC14">
+        <v>86</v>
+      </c>
     </row>
-    <row r="15" spans="1:132">
+    <row r="15" spans="1:133">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -5447,8 +5483,11 @@
       <c r="EB15">
         <v>24</v>
       </c>
+      <c r="EC15">
+        <v>24</v>
+      </c>
     </row>
-    <row r="16" spans="1:132">
+    <row r="16" spans="1:133">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -5653,8 +5692,11 @@
       <c r="EB16">
         <v>1958</v>
       </c>
+      <c r="EC16">
+        <v>2009</v>
+      </c>
     </row>
-    <row r="17" spans="1:132">
+    <row r="17" spans="1:133">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -5859,13 +5901,16 @@
       <c r="EB17" s="23">
         <v>0.79</v>
       </c>
+      <c r="EC17" s="23">
+        <v>0.81</v>
+      </c>
     </row>
-    <row r="19" spans="1:132">
+    <row r="19" spans="1:133">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:132">
+    <row r="20" spans="1:133">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -5873,7 +5918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:132">
+    <row r="21" spans="1:133">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -6216,8 +6261,11 @@
       <c r="EB21">
         <v>120</v>
       </c>
+      <c r="EC21">
+        <v>120</v>
+      </c>
     </row>
-    <row r="22" spans="1:132">
+    <row r="22" spans="1:133">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -6506,8 +6554,11 @@
       <c r="EB22">
         <v>6</v>
       </c>
+      <c r="EC22">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="1:132">
+    <row r="23" spans="1:133">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -6796,8 +6847,11 @@
       <c r="EB23">
         <v>114</v>
       </c>
+      <c r="EC23">
+        <v>115</v>
+      </c>
     </row>
-    <row r="24" spans="1:132">
+    <row r="24" spans="1:133">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -7131,8 +7185,11 @@
       <c r="EB24">
         <v>82</v>
       </c>
+      <c r="EC24">
+        <v>88</v>
+      </c>
     </row>
-    <row r="25" spans="1:132">
+    <row r="25" spans="1:133">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -7466,8 +7523,11 @@
       <c r="EB25">
         <v>88</v>
       </c>
+      <c r="EC25">
+        <v>93</v>
+      </c>
     </row>
-    <row r="26" spans="1:132">
+    <row r="26" spans="1:133">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -7801,13 +7861,16 @@
       <c r="EB26">
         <v>1704</v>
       </c>
+      <c r="EC26">
+        <v>1708</v>
+      </c>
     </row>
-    <row r="28" spans="1:132">
+    <row r="28" spans="1:133">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:132">
+    <row r="29" spans="1:133">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -8150,8 +8213,11 @@
       <c r="EB29">
         <v>169</v>
       </c>
+      <c r="EC29">
+        <v>172</v>
+      </c>
     </row>
-    <row r="30" spans="1:132">
+    <row r="30" spans="1:133">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -8440,8 +8506,11 @@
       <c r="EB30">
         <v>32</v>
       </c>
+      <c r="EC30">
+        <v>34</v>
+      </c>
     </row>
-    <row r="31" spans="1:132">
+    <row r="31" spans="1:133">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -8730,8 +8799,11 @@
       <c r="EB31">
         <v>136</v>
       </c>
+      <c r="EC31">
+        <v>137</v>
+      </c>
     </row>
-    <row r="32" spans="1:132">
+    <row r="32" spans="1:133">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -9065,8 +9137,11 @@
       <c r="EB32">
         <v>90</v>
       </c>
+      <c r="EC32">
+        <v>110</v>
+      </c>
     </row>
-    <row r="33" spans="1:132">
+    <row r="33" spans="1:133">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -9400,8 +9475,11 @@
       <c r="EB33">
         <v>122</v>
       </c>
+      <c r="EC33">
+        <v>144</v>
+      </c>
     </row>
-    <row r="34" spans="1:132">
+    <row r="34" spans="1:133">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -9735,8 +9813,11 @@
       <c r="EB34">
         <v>1411</v>
       </c>
+      <c r="EC34">
+        <v>1408</v>
+      </c>
     </row>
-    <row r="35" spans="1:132">
+    <row r="35" spans="1:133">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -9851,13 +9932,16 @@
       <c r="EB35">
         <v>1</v>
       </c>
+      <c r="EC35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:132">
+    <row r="37" spans="1:133">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:132">
+    <row r="38" spans="1:133">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -10188,8 +10272,11 @@
       <c r="EB38">
         <v>88</v>
       </c>
+      <c r="EC38">
+        <v>88</v>
+      </c>
     </row>
-    <row r="39" spans="1:132">
+    <row r="39" spans="1:133">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -10472,8 +10559,11 @@
       <c r="EB39">
         <v>2</v>
       </c>
+      <c r="EC39">
+        <v>2</v>
+      </c>
     </row>
-    <row r="40" spans="1:132">
+    <row r="40" spans="1:133">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -10756,8 +10846,11 @@
       <c r="EB40">
         <v>85</v>
       </c>
+      <c r="EC40">
+        <v>85</v>
+      </c>
     </row>
-    <row r="41" spans="1:132">
+    <row r="41" spans="1:133">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -11085,8 +11178,11 @@
       <c r="EB41">
         <v>0</v>
       </c>
+      <c r="EC41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:132">
+    <row r="42" spans="1:133">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -11411,8 +11507,11 @@
       <c r="EB42">
         <v>2</v>
       </c>
+      <c r="EC42">
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" spans="1:132">
+    <row r="43" spans="1:133">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -11743,8 +11842,11 @@
       <c r="EB43">
         <v>296</v>
       </c>
+      <c r="EC43">
+        <v>296</v>
+      </c>
     </row>
-    <row r="44" spans="1:132">
+    <row r="44" spans="1:133">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -12009,16 +12111,19 @@
       <c r="EB44">
         <v>1</v>
       </c>
+      <c r="EC44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:132">
+    <row r="45" spans="1:133">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:132">
+    <row r="46" spans="1:133">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:132">
+    <row r="47" spans="1:133">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -12355,8 +12460,11 @@
       <c r="EB47">
         <v>207</v>
       </c>
+      <c r="EC47">
+        <v>207</v>
+      </c>
     </row>
-    <row r="48" spans="1:132">
+    <row r="48" spans="1:133">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -12645,8 +12753,11 @@
       <c r="EB48">
         <v>0</v>
       </c>
+      <c r="EC48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:132">
+    <row r="49" spans="1:133">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -12935,8 +13046,11 @@
       <c r="EB49">
         <v>200</v>
       </c>
+      <c r="EC49">
+        <v>200</v>
+      </c>
     </row>
-    <row r="50" spans="1:132">
+    <row r="50" spans="1:133">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -13270,8 +13384,11 @@
       <c r="EB50">
         <v>55</v>
       </c>
+      <c r="EC50">
+        <v>63</v>
+      </c>
     </row>
-    <row r="51" spans="1:132">
+    <row r="51" spans="1:133">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -13560,8 +13677,11 @@
       <c r="EB51">
         <v>55</v>
       </c>
+      <c r="EC51">
+        <v>63</v>
+      </c>
     </row>
-    <row r="52" spans="1:132">
+    <row r="52" spans="1:133">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -13847,8 +13967,11 @@
       <c r="EB52">
         <v>1211</v>
       </c>
+      <c r="EC52">
+        <v>1211</v>
+      </c>
     </row>
-    <row r="53" spans="1:132">
+    <row r="53" spans="1:133">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -14128,16 +14251,19 @@
       <c r="EB53">
         <v>1</v>
       </c>
+      <c r="EC53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:132">
+    <row r="54" spans="1:133">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:132">
+    <row r="55" spans="1:133">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:132">
+    <row r="56" spans="1:133">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -14459,8 +14585,11 @@
       <c r="EB56">
         <v>35</v>
       </c>
+      <c r="EC56">
+        <v>35</v>
+      </c>
     </row>
-    <row r="57" spans="1:132">
+    <row r="57" spans="1:133">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -14746,8 +14875,11 @@
       <c r="EB57">
         <v>2</v>
       </c>
+      <c r="EC57">
+        <v>2</v>
+      </c>
     </row>
-    <row r="58" spans="1:132">
+    <row r="58" spans="1:133">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -15033,8 +15165,11 @@
       <c r="EB58">
         <v>32</v>
       </c>
+      <c r="EC58">
+        <v>32</v>
+      </c>
     </row>
-    <row r="59" spans="1:132">
+    <row r="59" spans="1:133">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -15356,8 +15491,11 @@
       <c r="EB59">
         <v>2</v>
       </c>
+      <c r="EC59">
+        <v>2</v>
+      </c>
     </row>
-    <row r="60" spans="1:132">
+    <row r="60" spans="1:133">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -15679,8 +15817,11 @@
       <c r="EB60">
         <v>4</v>
       </c>
+      <c r="EC60">
+        <v>4</v>
+      </c>
     </row>
-    <row r="61" spans="1:132">
+    <row r="61" spans="1:133">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -16002,8 +16143,11 @@
       <c r="EB61">
         <v>175</v>
       </c>
+      <c r="EC61">
+        <v>175</v>
+      </c>
     </row>
-    <row r="62" spans="1:132">
+    <row r="62" spans="1:133">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -16283,8 +16427,11 @@
       <c r="EB62">
         <v>1</v>
       </c>
+      <c r="EC62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:132">
+    <row r="64" spans="1:133">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -16606,8 +16753,11 @@
       <c r="EB64">
         <v>13</v>
       </c>
+      <c r="EC64">
+        <v>13</v>
+      </c>
     </row>
-    <row r="65" spans="1:132">
+    <row r="65" spans="1:133">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -16893,8 +17043,11 @@
       <c r="EB65">
         <v>0</v>
       </c>
+      <c r="EC65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:132">
+    <row r="66" spans="1:133">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -17180,8 +17333,11 @@
       <c r="EB66">
         <v>13</v>
       </c>
+      <c r="EC66">
+        <v>13</v>
+      </c>
     </row>
-    <row r="67" spans="1:132">
+    <row r="67" spans="1:133">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -17503,8 +17659,11 @@
       <c r="EB67">
         <v>68</v>
       </c>
+      <c r="EC67">
+        <v>71</v>
+      </c>
     </row>
-    <row r="68" spans="1:132">
+    <row r="68" spans="1:133">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -17827,8 +17986,11 @@
       <c r="EB68">
         <v>68</v>
       </c>
+      <c r="EC68">
+        <v>71</v>
+      </c>
     </row>
-    <row r="69" spans="1:132">
+    <row r="69" spans="1:133">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -18150,8 +18312,11 @@
       <c r="EB69">
         <v>0</v>
       </c>
+      <c r="EC69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:132">
+    <row r="70" spans="1:133">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -18437,11 +18602,14 @@
       <c r="EB70">
         <v>0</v>
       </c>
+      <c r="EC70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:132">
+    <row r="71" spans="1:133">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:132">
+    <row r="72" spans="1:133">
       <c r="A72" s="2" t="s">
         <v>119</v>
       </c>
@@ -18613,8 +18781,11 @@
       <c r="EB72">
         <v>11</v>
       </c>
+      <c r="EC72">
+        <v>11</v>
+      </c>
     </row>
-    <row r="73" spans="1:132">
+    <row r="73" spans="1:133">
       <c r="A73" s="2" t="s">
         <v>119</v>
       </c>
@@ -18786,8 +18957,11 @@
       <c r="EB73">
         <v>2</v>
       </c>
+      <c r="EC73">
+        <v>2</v>
+      </c>
     </row>
-    <row r="74" spans="1:132">
+    <row r="74" spans="1:133">
       <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
@@ -18959,8 +19133,11 @@
       <c r="EB74">
         <v>9</v>
       </c>
+      <c r="EC74">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:132">
+    <row r="75" spans="1:133">
       <c r="A75" s="2" t="s">
         <v>119</v>
       </c>
@@ -19132,8 +19309,11 @@
       <c r="EB75">
         <v>2</v>
       </c>
+      <c r="EC75">
+        <v>2</v>
+      </c>
     </row>
-    <row r="76" spans="1:132">
+    <row r="76" spans="1:133">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -19305,8 +19485,11 @@
       <c r="EB76">
         <v>4</v>
       </c>
+      <c r="EC76">
+        <v>4</v>
+      </c>
     </row>
-    <row r="77" spans="1:132">
+    <row r="77" spans="1:133">
       <c r="A77" s="2" t="s">
         <v>119</v>
       </c>
@@ -19478,13 +19661,16 @@
       <c r="EB77">
         <v>52</v>
       </c>
+      <c r="EC77">
+        <v>48</v>
+      </c>
     </row>
-    <row r="79" spans="1:132">
+    <row r="79" spans="1:133">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:132">
+    <row r="80" spans="1:133">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -19809,8 +19995,11 @@
       <c r="EB80">
         <v>325</v>
       </c>
+      <c r="EC80">
+        <v>325</v>
+      </c>
     </row>
-    <row r="81" spans="1:132">
+    <row r="81" spans="1:133">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -20135,8 +20324,11 @@
       <c r="EB81">
         <v>70</v>
       </c>
+      <c r="EC81">
+        <v>68</v>
+      </c>
     </row>
-    <row r="82" spans="1:132">
+    <row r="82" spans="1:133">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -20461,8 +20653,11 @@
       <c r="EB82">
         <v>67</v>
       </c>
+      <c r="EC82">
+        <v>66</v>
+      </c>
     </row>
-    <row r="83" spans="1:132">
+    <row r="83" spans="1:133">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -20745,8 +20940,11 @@
       <c r="EB83">
         <v>20</v>
       </c>
+      <c r="EC83">
+        <v>20</v>
+      </c>
     </row>
-    <row r="85" spans="1:132">
+    <row r="85" spans="1:133">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -21071,8 +21269,11 @@
       <c r="EB85">
         <v>125</v>
       </c>
+      <c r="EC85">
+        <v>125</v>
+      </c>
     </row>
-    <row r="86" spans="1:132">
+    <row r="86" spans="1:133">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -21397,8 +21598,11 @@
       <c r="EB86">
         <v>6</v>
       </c>
+      <c r="EC86">
+        <v>6</v>
+      </c>
     </row>
-    <row r="87" spans="1:132">
+    <row r="87" spans="1:133">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -21723,8 +21927,11 @@
       <c r="EB87">
         <v>21</v>
       </c>
+      <c r="EC87">
+        <v>20</v>
+      </c>
     </row>
-    <row r="88" spans="1:132">
+    <row r="88" spans="1:133">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -22049,8 +22256,11 @@
       <c r="EB88">
         <v>256</v>
       </c>
+      <c r="EC88">
+        <v>258</v>
+      </c>
     </row>
-    <row r="89" spans="1:132">
+    <row r="89" spans="1:133">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -22249,8 +22459,11 @@
       <c r="EB89">
         <v>1</v>
       </c>
+      <c r="EC89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:132">
+    <row r="91" spans="1:133">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -22575,8 +22788,11 @@
       <c r="EB91">
         <v>82</v>
       </c>
+      <c r="EC91">
+        <v>82</v>
+      </c>
     </row>
-    <row r="92" spans="1:132">
+    <row r="92" spans="1:133">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -22901,8 +23117,11 @@
       <c r="EB92">
         <v>1</v>
       </c>
+      <c r="EC92">
+        <v>1</v>
+      </c>
     </row>
-    <row r="93" spans="1:132">
+    <row r="93" spans="1:133">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -23215,8 +23434,11 @@
       <c r="EB93">
         <v>192</v>
       </c>
+      <c r="EC93">
+        <v>193</v>
+      </c>
     </row>
-    <row r="94" spans="1:132">
+    <row r="94" spans="1:133">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -23541,8 +23763,11 @@
       <c r="EB94">
         <v>62</v>
       </c>
+      <c r="EC94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:132">
+    <row r="95" spans="1:133">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -23825,11 +24050,14 @@
       <c r="EB95">
         <v>14</v>
       </c>
+      <c r="EC95">
+        <v>14</v>
+      </c>
     </row>
-    <row r="96" spans="1:132">
+    <row r="96" spans="1:133">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:132">
+    <row r="97" spans="1:133">
       <c r="A97" s="2" t="s">
         <v>130</v>
       </c>
@@ -23971,8 +24199,11 @@
       <c r="EB97">
         <v>12</v>
       </c>
+      <c r="EC97">
+        <v>14</v>
+      </c>
     </row>
-    <row r="98" spans="1:132">
+    <row r="98" spans="1:133">
       <c r="A98" s="2" t="s">
         <v>130</v>
       </c>
@@ -24114,8 +24345,11 @@
       <c r="EB98">
         <v>9</v>
       </c>
+      <c r="EC98">
+        <v>11</v>
+      </c>
     </row>
-    <row r="99" spans="1:132">
+    <row r="99" spans="1:133">
       <c r="A99" s="2" t="s">
         <v>130</v>
       </c>
@@ -24257,8 +24491,11 @@
       <c r="EB99">
         <v>52</v>
       </c>
+      <c r="EC99">
+        <v>55</v>
+      </c>
     </row>
-    <row r="100" spans="1:132">
+    <row r="100" spans="1:133">
       <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
@@ -24400,8 +24637,11 @@
       <c r="EB100">
         <v>1</v>
       </c>
+      <c r="EC100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:132">
+    <row r="102" spans="1:133">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -24645,8 +24885,11 @@
       <c r="EB102">
         <v>211</v>
       </c>
+      <c r="EC102">
+        <v>211</v>
+      </c>
     </row>
-    <row r="103" spans="1:132">
+    <row r="103" spans="1:133">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -24890,8 +25133,11 @@
       <c r="EB103">
         <v>140</v>
       </c>
+      <c r="EC103">
+        <v>140</v>
+      </c>
     </row>
-    <row r="104" spans="1:132">
+    <row r="104" spans="1:133">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -25133,6 +25379,9 @@
         <v>28</v>
       </c>
       <c r="EB104">
+        <v>28</v>
+      </c>
+      <c r="EC104">
         <v>28</v>
       </c>
     </row>
@@ -25149,11 +25398,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:DC11"/>
+  <dimension ref="A2:DD11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DD2" sqref="DD2"/>
+      <selection pane="topRight" activeCell="DE2" sqref="DE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -25163,7 +25412,7 @@
     <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:107" s="2" customFormat="1">
+    <row r="2" spans="1:108" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -25485,8 +25734,11 @@
       <c r="DC2" s="9">
         <v>44026</v>
       </c>
+      <c r="DD2" s="9">
+        <v>44027</v>
+      </c>
     </row>
-    <row r="3" spans="1:107">
+    <row r="3" spans="1:108">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -25808,8 +26060,11 @@
       <c r="DC3">
         <v>1565</v>
       </c>
+      <c r="DD3">
+        <v>1572</v>
+      </c>
     </row>
-    <row r="4" spans="1:107">
+    <row r="4" spans="1:108">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -26131,8 +26386,11 @@
       <c r="DC4">
         <v>662</v>
       </c>
+      <c r="DD4">
+        <v>669</v>
+      </c>
     </row>
-    <row r="5" spans="1:107">
+    <row r="5" spans="1:108">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -26454,8 +26712,11 @@
       <c r="DC5">
         <v>518</v>
       </c>
+      <c r="DD5">
+        <v>519</v>
+      </c>
     </row>
-    <row r="6" spans="1:107">
+    <row r="6" spans="1:108">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -26777,8 +27038,11 @@
       <c r="DC6">
         <v>2252</v>
       </c>
+      <c r="DD6">
+        <v>2258</v>
+      </c>
     </row>
-    <row r="7" spans="1:107">
+    <row r="7" spans="1:108">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -27100,8 +27364,11 @@
       <c r="DC7">
         <v>1637</v>
       </c>
+      <c r="DD7">
+        <v>1646</v>
+      </c>
     </row>
-    <row r="8" spans="1:107">
+    <row r="8" spans="1:108">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -27423,8 +27690,11 @@
       <c r="DC8">
         <v>1010</v>
       </c>
+      <c r="DD8">
+        <v>1017</v>
+      </c>
     </row>
-    <row r="9" spans="1:107">
+    <row r="9" spans="1:108">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -27746,8 +28016,11 @@
       <c r="DC9">
         <v>1584</v>
       </c>
+      <c r="DD9">
+        <v>1592</v>
+      </c>
     </row>
-    <row r="10" spans="1:107">
+    <row r="10" spans="1:108">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -28069,8 +28342,11 @@
       <c r="DC10">
         <v>1618</v>
       </c>
+      <c r="DD10">
+        <v>1624</v>
+      </c>
     </row>
-    <row r="11" spans="1:107">
+    <row r="11" spans="1:108">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -28391,6 +28667,9 @@
       </c>
       <c r="DC11">
         <v>180</v>
+      </c>
+      <c r="DD11">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -28401,11 +28680,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:CX17"/>
+  <dimension ref="A2:CY17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CY2" sqref="CY2"/>
+      <selection pane="topRight" activeCell="CZ2" sqref="CZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -28415,7 +28694,7 @@
     <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:102" s="2" customFormat="1">
+    <row r="2" spans="1:103" s="2" customFormat="1">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -28720,8 +28999,11 @@
       <c r="CX2" s="9">
         <v>44026</v>
       </c>
+      <c r="CY2" s="9">
+        <v>44027</v>
+      </c>
     </row>
-    <row r="3" spans="1:102" s="2" customFormat="1">
+    <row r="3" spans="1:103" s="2" customFormat="1">
       <c r="A3" s="41" t="s">
         <v>36</v>
       </c>
@@ -28730,7 +29012,7 @@
       <c r="D3" s="9"/>
       <c r="CP3" s="4"/>
     </row>
-    <row r="4" spans="1:102">
+    <row r="4" spans="1:103">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -29037,8 +29319,11 @@
       <c r="CX4">
         <v>11206</v>
       </c>
+      <c r="CY4">
+        <v>11706</v>
+      </c>
     </row>
-    <row r="5" spans="1:102">
+    <row r="5" spans="1:103">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -29345,8 +29630,11 @@
       <c r="CX5">
         <v>186</v>
       </c>
+      <c r="CY5">
+        <v>207</v>
+      </c>
     </row>
-    <row r="6" spans="1:102">
+    <row r="6" spans="1:103">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -29653,8 +29941,11 @@
       <c r="CX6">
         <v>2253</v>
       </c>
+      <c r="CY6">
+        <v>2263</v>
+      </c>
     </row>
-    <row r="7" spans="1:102">
+    <row r="7" spans="1:103">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -29961,8 +30252,11 @@
       <c r="CX7">
         <v>5431</v>
       </c>
+      <c r="CY7">
+        <v>5448</v>
+      </c>
     </row>
-    <row r="8" spans="1:102">
+    <row r="8" spans="1:103">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -30269,8 +30563,11 @@
       <c r="CX8">
         <v>170</v>
       </c>
+      <c r="CY8">
+        <v>171</v>
+      </c>
     </row>
-    <row r="9" spans="1:102" ht="28.8">
+    <row r="9" spans="1:103" ht="28.8">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -30577,8 +30874,11 @@
       <c r="CX9">
         <v>27</v>
       </c>
+      <c r="CY9">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:102" ht="28.8">
+    <row r="10" spans="1:103" ht="28.8">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -30881,8 +31181,11 @@
       <c r="CX10">
         <v>29</v>
       </c>
+      <c r="CY10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="11" spans="1:102">
+    <row r="11" spans="1:103">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -31189,8 +31492,11 @@
       <c r="CX11">
         <v>2840</v>
       </c>
+      <c r="CY11">
+        <v>2841</v>
+      </c>
     </row>
-    <row r="12" spans="1:102">
+    <row r="12" spans="1:103">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -31497,8 +31803,11 @@
       <c r="CX12">
         <v>90</v>
       </c>
+      <c r="CY12">
+        <v>90</v>
+      </c>
     </row>
-    <row r="13" spans="1:102">
+    <row r="13" spans="1:103">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -31509,7 +31818,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:102">
+    <row r="14" spans="1:103">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -31816,8 +32125,11 @@
       <c r="CX14">
         <v>1364</v>
       </c>
+      <c r="CY14">
+        <v>1391</v>
+      </c>
     </row>
-    <row r="15" spans="1:102">
+    <row r="15" spans="1:103">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -32124,8 +32436,11 @@
       <c r="CX15">
         <v>3069</v>
       </c>
+      <c r="CY15">
+        <v>3072</v>
+      </c>
     </row>
-    <row r="16" spans="1:102">
+    <row r="16" spans="1:103">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -32432,8 +32747,11 @@
       <c r="CX16">
         <v>6575</v>
       </c>
+      <c r="CY16">
+        <v>6594</v>
+      </c>
     </row>
-    <row r="17" spans="1:102">
+    <row r="17" spans="1:103">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -32739,6 +33057,9 @@
       </c>
       <c r="CX17">
         <v>18</v>
+      </c>
+      <c r="CY17">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -32749,11 +33070,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:CX9"/>
+  <dimension ref="A1:CY9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CY1" sqref="CY1"/>
+      <selection pane="topRight" activeCell="CZ1" sqref="CZ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -32762,7 +33083,7 @@
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" s="2" customFormat="1">
+    <row r="1" spans="1:103" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -33066,14 +33387,17 @@
       <c r="CX1" s="9">
         <v>44026</v>
       </c>
+      <c r="CY1" s="9">
+        <v>44027</v>
+      </c>
     </row>
-    <row r="2" spans="1:102">
+    <row r="2" spans="1:103">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:102">
+    <row r="3" spans="1:103">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -33381,8 +33705,11 @@
       <c r="CX3">
         <v>571</v>
       </c>
+      <c r="CY3">
+        <v>574</v>
+      </c>
     </row>
-    <row r="4" spans="1:102">
+    <row r="4" spans="1:103">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -33689,8 +34016,11 @@
       <c r="CX4">
         <v>8</v>
       </c>
+      <c r="CY4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:102" ht="28.8">
+    <row r="5" spans="1:103" ht="28.8">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -33997,8 +34327,11 @@
       <c r="CX5">
         <v>424</v>
       </c>
+      <c r="CY5">
+        <v>425</v>
+      </c>
     </row>
-    <row r="6" spans="1:102">
+    <row r="6" spans="1:103">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -34305,8 +34638,11 @@
       <c r="CX6">
         <v>74</v>
       </c>
+      <c r="CY6">
+        <v>75</v>
+      </c>
     </row>
-    <row r="7" spans="1:102">
+    <row r="7" spans="1:103">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -34613,8 +34949,11 @@
       <c r="CX7">
         <v>60</v>
       </c>
+      <c r="CY7">
+        <v>61</v>
+      </c>
     </row>
-    <row r="8" spans="1:102">
+    <row r="8" spans="1:103">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -34921,8 +35260,11 @@
       <c r="CX8">
         <v>5</v>
       </c>
+      <c r="CY8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:102">
+    <row r="9" spans="1:103">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -34964,11 +35306,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:CP5"/>
+  <dimension ref="A1:CQ5"/>
   <sheetViews>
     <sheetView zoomScale="95" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CQ1" sqref="CQ1"/>
+      <selection pane="topRight" activeCell="CR1" sqref="CR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -34976,7 +35318,7 @@
     <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" s="2" customFormat="1">
+    <row r="1" spans="1:95" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -35256,13 +35598,16 @@
       <c r="CP1" s="9">
         <v>44026</v>
       </c>
+      <c r="CQ1" s="9">
+        <v>44027</v>
+      </c>
     </row>
-    <row r="2" spans="1:94">
+    <row r="2" spans="1:95">
       <c r="A2" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:94">
+    <row r="3" spans="1:95">
       <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
@@ -35545,8 +35890,11 @@
       <c r="CP3">
         <v>571</v>
       </c>
+      <c r="CQ3">
+        <v>574</v>
+      </c>
     </row>
-    <row r="4" spans="1:94">
+    <row r="4" spans="1:95">
       <c r="A4" s="42" t="s">
         <v>159</v>
       </c>
@@ -35829,8 +36177,11 @@
       <c r="CP4">
         <v>244</v>
       </c>
+      <c r="CQ4">
+        <v>244</v>
+      </c>
     </row>
-    <row r="5" spans="1:94">
+    <row r="5" spans="1:95">
       <c r="A5" s="42" t="s">
         <v>158</v>
       </c>
@@ -36112,6 +36463,9 @@
       </c>
       <c r="CP5">
         <v>327</v>
+      </c>
+      <c r="CQ5">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -36122,11 +36476,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:CP11"/>
+  <dimension ref="A1:CQ11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CQ1" sqref="CQ1"/>
+      <selection pane="topRight" activeCell="CR1" sqref="CR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36134,7 +36488,7 @@
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" s="2" customFormat="1">
+    <row r="1" spans="1:95" s="2" customFormat="1">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -36414,13 +36768,16 @@
       <c r="CP1" s="9">
         <v>44026</v>
       </c>
+      <c r="CQ1" s="9">
+        <v>44027</v>
+      </c>
     </row>
-    <row r="2" spans="1:94">
+    <row r="2" spans="1:95">
       <c r="A2" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:94">
+    <row r="3" spans="1:95">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -36703,8 +37060,11 @@
       <c r="CP3">
         <v>571</v>
       </c>
+      <c r="CQ3">
+        <v>574</v>
+      </c>
     </row>
-    <row r="4" spans="1:94">
+    <row r="4" spans="1:95">
       <c r="A4" s="5" t="s">
         <v>149</v>
       </c>
@@ -36987,8 +37347,11 @@
       <c r="CP4">
         <v>0</v>
       </c>
+      <c r="CQ4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:94">
+    <row r="5" spans="1:95">
       <c r="A5" s="5" t="s">
         <v>150</v>
       </c>
@@ -37271,8 +37634,11 @@
       <c r="CP5">
         <v>3</v>
       </c>
+      <c r="CQ5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:94">
+    <row r="6" spans="1:95">
       <c r="A6" s="5" t="s">
         <v>151</v>
       </c>
@@ -37555,8 +37921,11 @@
       <c r="CP6">
         <v>7</v>
       </c>
+      <c r="CQ6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:94">
+    <row r="7" spans="1:95">
       <c r="A7" s="5" t="s">
         <v>152</v>
       </c>
@@ -37839,8 +38208,11 @@
       <c r="CP7">
         <v>19</v>
       </c>
+      <c r="CQ7">
+        <v>19</v>
+      </c>
     </row>
-    <row r="8" spans="1:94">
+    <row r="8" spans="1:95">
       <c r="A8" s="5" t="s">
         <v>153</v>
       </c>
@@ -38123,8 +38495,11 @@
       <c r="CP8">
         <v>66</v>
       </c>
+      <c r="CQ8">
+        <v>66</v>
+      </c>
     </row>
-    <row r="9" spans="1:94">
+    <row r="9" spans="1:95">
       <c r="A9" s="5" t="s">
         <v>154</v>
       </c>
@@ -38407,8 +38782,11 @@
       <c r="CP9">
         <v>135</v>
       </c>
+      <c r="CQ9">
+        <v>136</v>
+      </c>
     </row>
-    <row r="10" spans="1:94">
+    <row r="10" spans="1:95">
       <c r="A10" s="6" t="s">
         <v>155</v>
       </c>
@@ -38691,8 +39069,11 @@
       <c r="CP10">
         <v>146</v>
       </c>
+      <c r="CQ10">
+        <v>146</v>
+      </c>
     </row>
-    <row r="11" spans="1:94">
+    <row r="11" spans="1:95">
       <c r="A11" s="6" t="s">
         <v>156</v>
       </c>
@@ -38974,6 +39355,9 @@
       </c>
       <c r="CP11">
         <v>195</v>
+      </c>
+      <c r="CQ11">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -38984,11 +39368,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A2:CJ13"/>
+  <dimension ref="A2:CK13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="BS1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CK2" sqref="CK2"/>
+      <selection pane="topRight" activeCell="CL2" sqref="CL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -38997,7 +39381,7 @@
     <col min="57" max="57" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:88" s="2" customFormat="1">
+    <row r="2" spans="1:89" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -39262,8 +39646,11 @@
       <c r="CJ2" s="9">
         <v>44026</v>
       </c>
+      <c r="CK2" s="9">
+        <v>44027</v>
+      </c>
     </row>
-    <row r="3" spans="1:88">
+    <row r="3" spans="1:89">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -39528,8 +39915,11 @@
       <c r="CJ3">
         <v>571</v>
       </c>
+      <c r="CK3">
+        <v>574</v>
+      </c>
     </row>
-    <row r="4" spans="1:88">
+    <row r="4" spans="1:89">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -39794,8 +40184,11 @@
       <c r="CJ4">
         <v>62</v>
       </c>
+      <c r="CK4">
+        <v>63</v>
+      </c>
     </row>
-    <row r="5" spans="1:88">
+    <row r="5" spans="1:89">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -40060,8 +40453,11 @@
       <c r="CJ5">
         <v>31</v>
       </c>
+      <c r="CK5">
+        <v>31</v>
+      </c>
     </row>
-    <row r="6" spans="1:88">
+    <row r="6" spans="1:89">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -40326,8 +40722,11 @@
       <c r="CJ6">
         <v>33</v>
       </c>
+      <c r="CK6">
+        <v>33</v>
+      </c>
     </row>
-    <row r="7" spans="1:88">
+    <row r="7" spans="1:89">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -40592,8 +40991,11 @@
       <c r="CJ7">
         <v>83</v>
       </c>
+      <c r="CK7">
+        <v>84</v>
+      </c>
     </row>
-    <row r="8" spans="1:88">
+    <row r="8" spans="1:89">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -40858,8 +41260,11 @@
       <c r="CJ8">
         <v>92</v>
       </c>
+      <c r="CK8">
+        <v>92</v>
+      </c>
     </row>
-    <row r="9" spans="1:88">
+    <row r="9" spans="1:89">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -41124,8 +41529,11 @@
       <c r="CJ9">
         <v>49</v>
       </c>
+      <c r="CK9">
+        <v>49</v>
+      </c>
     </row>
-    <row r="10" spans="1:88">
+    <row r="10" spans="1:89">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -41390,8 +41798,11 @@
       <c r="CJ10">
         <v>85</v>
       </c>
+      <c r="CK10">
+        <v>85</v>
+      </c>
     </row>
-    <row r="11" spans="1:88">
+    <row r="11" spans="1:89">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -41656,8 +42067,11 @@
       <c r="CJ11">
         <v>116</v>
       </c>
+      <c r="CK11">
+        <v>116</v>
+      </c>
     </row>
-    <row r="12" spans="1:88" ht="28.8">
+    <row r="12" spans="1:89" ht="28.8">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -41922,8 +42336,11 @@
       <c r="CJ12">
         <v>20</v>
       </c>
+      <c r="CK12">
+        <v>20</v>
+      </c>
     </row>
-    <row r="13" spans="1:88">
+    <row r="13" spans="1:89">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -42187,6 +42604,9 @@
       </c>
       <c r="CJ13">
         <v>0</v>
+      </c>
+      <c r="CK13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -42197,10 +42617,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:BF23"/>
+  <dimension ref="A1:BH23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV10" zoomScale="96" workbookViewId="0">
-      <selection activeCell="BF9" sqref="BF9:BF12"/>
+    <sheetView topLeftCell="AC1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="BH5" sqref="BH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -42209,7 +42629,7 @@
     <col min="42" max="45" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58">
+    <row r="1" spans="1:60">
       <c r="C1" s="53" t="s">
         <v>179</v>
       </c>
@@ -42226,7 +42646,7 @@
       <c r="N1" s="53"/>
       <c r="O1" s="53"/>
     </row>
-    <row r="2" spans="1:58">
+    <row r="2" spans="1:60">
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
       <c r="E2" s="53"/>
@@ -42241,7 +42661,7 @@
       <c r="N2" s="53"/>
       <c r="O2" s="53"/>
     </row>
-    <row r="3" spans="1:58">
+    <row r="3" spans="1:60">
       <c r="C3" s="53"/>
       <c r="D3" s="53"/>
       <c r="E3" s="53"/>
@@ -42256,7 +42676,7 @@
       <c r="N3" s="53"/>
       <c r="O3" s="53"/>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:60">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -42271,7 +42691,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:58">
+    <row r="5" spans="1:60">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -42440,8 +42860,14 @@
       <c r="BF5" s="9">
         <v>44026</v>
       </c>
+      <c r="BG5" s="9">
+        <v>44027</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="6" spans="1:58">
+    <row r="6" spans="1:60">
       <c r="A6" s="2" t="s">
         <v>120</v>
       </c>
@@ -42613,8 +43039,11 @@
       <c r="BF6">
         <v>158</v>
       </c>
+      <c r="BG6">
+        <v>158</v>
+      </c>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:60">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -42786,8 +43215,11 @@
       <c r="BF7">
         <v>36</v>
       </c>
+      <c r="BG7">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" spans="1:58">
+    <row r="8" spans="1:60">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
@@ -42795,7 +43227,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:58">
+    <row r="9" spans="1:60">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -42967,8 +43399,11 @@
       <c r="BF9">
         <v>1</v>
       </c>
+      <c r="BG9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:58">
+    <row r="10" spans="1:60">
       <c r="A10" s="31" t="s">
         <v>121</v>
       </c>
@@ -43140,8 +43575,11 @@
       <c r="BF10">
         <v>23</v>
       </c>
+      <c r="BG10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:58">
+    <row r="11" spans="1:60">
       <c r="A11" s="31" t="s">
         <v>122</v>
       </c>
@@ -43313,8 +43751,11 @@
       <c r="BF11">
         <v>9</v>
       </c>
+      <c r="BG11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:58">
+    <row r="12" spans="1:60">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -43486,13 +43927,16 @@
       <c r="BF12">
         <v>3</v>
       </c>
+      <c r="BG12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:58">
+    <row r="13" spans="1:60">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:58">
+    <row r="14" spans="1:60">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -43664,8 +44108,11 @@
       <c r="BF14">
         <v>1</v>
       </c>
+      <c r="BG14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:58">
+    <row r="15" spans="1:60">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -43837,8 +44284,11 @@
       <c r="BF15">
         <v>0</v>
       </c>
+      <c r="BG15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:58">
+    <row r="16" spans="1:60">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -44010,8 +44460,11 @@
       <c r="BF16">
         <v>3</v>
       </c>
+      <c r="BG16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:58">
+    <row r="17" spans="1:59">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -44183,8 +44636,11 @@
       <c r="BF17">
         <v>12</v>
       </c>
+      <c r="BG17">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:58">
+    <row r="18" spans="1:59">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -44356,8 +44812,11 @@
       <c r="BF18">
         <v>3</v>
       </c>
+      <c r="BG18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:58">
+    <row r="19" spans="1:59">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -44529,8 +44988,11 @@
       <c r="BF19">
         <v>2</v>
       </c>
+      <c r="BG19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:58">
+    <row r="20" spans="1:59">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -44702,8 +45164,11 @@
       <c r="BF20">
         <v>2</v>
       </c>
+      <c r="BG20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:58">
+    <row r="21" spans="1:59">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -44875,8 +45340,11 @@
       <c r="BF21">
         <v>6</v>
       </c>
+      <c r="BG21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:58" ht="28.8">
+    <row r="22" spans="1:59" ht="28.8">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -45045,8 +45513,14 @@
       <c r="BE22">
         <v>4</v>
       </c>
+      <c r="BF22">
+        <v>4</v>
+      </c>
+      <c r="BG22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:58" ht="28.8">
+    <row r="23" spans="1:59" ht="28.8">
       <c r="A23" s="39" t="s">
         <v>123</v>
       </c>
@@ -45213,6 +45687,12 @@
         <v>3</v>
       </c>
       <c r="BE23">
+        <v>3</v>
+      </c>
+      <c r="BF23">
+        <v>3</v>
+      </c>
+      <c r="BG23">
         <v>3</v>
       </c>
     </row>
@@ -45812,12 +46292,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46024,15 +46501,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -46057,18 +46546,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Results from July 17, 2020 06:33:36 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/work/WashingtonDC/data.xlsx
+++ b/workflow/python/work/WashingtonDC/data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="279" documentId="8_{DEC2A8EE-2CC1-4116-B97C-51343F77D983}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{EF2C1E1D-AFE6-4D79-B2CB-FEEE8CDF7177}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7116" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7110" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -23,7 +17,7 @@
     <sheet name="Community Cases Tested By OCME" sheetId="7" r:id="rId8"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="181">
   <si>
     <t>Testing</t>
   </si>
@@ -449,31 +443,13 @@
     <t>32; (20)</t>
   </si>
   <si>
-    <t>26; (17)</t>
-  </si>
-  <si>
     <t>10; (9)</t>
-  </si>
-  <si>
-    <t>23; (13)</t>
   </si>
   <si>
     <t>12; (9)</t>
   </si>
   <si>
-    <t>80; (77)</t>
-  </si>
-  <si>
     <t>19; (2)</t>
-  </si>
-  <si>
-    <t>149; (50)</t>
-  </si>
-  <si>
-    <t>22; (13)</t>
-  </si>
-  <si>
-    <t>5; (4)</t>
   </si>
   <si>
     <t>5; (1)</t>
@@ -521,12 +497,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>10; (7)</t>
-  </si>
-  <si>
-    <t>7; (2)</t>
-  </si>
-  <si>
     <t>16; (11)</t>
   </si>
   <si>
@@ -539,47 +509,17 @@
     <t>57; (4)</t>
   </si>
   <si>
-    <t>41; (37)</t>
-  </si>
-  <si>
     <t>24; (18)</t>
-  </si>
-  <si>
-    <t>40; (25)</t>
-  </si>
-  <si>
-    <t>17; (15)</t>
   </si>
   <si>
     <t>21; (17)</t>
   </si>
   <si>
-    <t>113; (52)</t>
-  </si>
-  <si>
-    <t>67; (23)</t>
-  </si>
-  <si>
-    <t>66; (40)</t>
-  </si>
-  <si>
     <t>40; (36)</t>
   </si>
   <si>
-    <t>693; (386)</t>
-  </si>
-  <si>
-    <t>304; (165)</t>
-  </si>
-  <si>
-    <t>997; (551)</t>
-  </si>
-  <si>
-    <t>As of July 10, 2020</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">As of July 15, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of July 16, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -603,12 +543,69 @@
       <t xml:space="preserve"> for COVID-19 testing,  and 36 (22.7%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
     </r>
   </si>
+  <si>
+    <t>As of July 16, 2020</t>
+  </si>
+  <si>
+    <t>10; (2)</t>
+  </si>
+  <si>
+    <t>24; (1)</t>
+  </si>
+  <si>
+    <t>113; (61)</t>
+  </si>
+  <si>
+    <t>8; (5)</t>
+  </si>
+  <si>
+    <t>3; (1)</t>
+  </si>
+  <si>
+    <t>67; (44)</t>
+  </si>
+  <si>
+    <t>22; (9)</t>
+  </si>
+  <si>
+    <t>26; (9)</t>
+  </si>
+  <si>
+    <t>42; (5)</t>
+  </si>
+  <si>
+    <t>66; (25)</t>
+  </si>
+  <si>
+    <t>41; (10)</t>
+  </si>
+  <si>
+    <t>150; (29)</t>
+  </si>
+  <si>
+    <t>23; (9)</t>
+  </si>
+  <si>
+    <t>17; (1)</t>
+  </si>
+  <si>
+    <t>80; (2)</t>
+  </si>
+  <si>
+    <t>697; (214)</t>
+  </si>
+  <si>
+    <t>305; (166)</t>
+  </si>
+  <si>
+    <t>1002; (380)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -672,13 +669,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF112277"/>
-      <name val="Albany AMT"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -709,14 +713,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -756,46 +754,9 @@
       <left style="thin">
         <color theme="2" tint="-9.9978637043366805E-2"/>
       </left>
-      <right style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </left>
       <right/>
       <top style="thin">
         <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -804,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -910,9 +871,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -923,17 +881,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -986,7 +941,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1321,38 +1276,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EC119"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ED119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="DZ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="ED1" sqref="ED1"/>
+      <selection pane="topRight" activeCell="EF4" sqref="EF4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" customWidth="1"/>
-    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="80" max="88" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="98" max="102" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="104" max="118" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="128" max="133" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="88" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="98" max="102" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="104" max="118" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="128" max="134" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:133">
+    <row r="1" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1707,47 +1662,50 @@
       <c r="DP1" s="1">
         <v>44014</v>
       </c>
-      <c r="DQ1" s="52">
+      <c r="DQ1" s="48">
         <v>44015</v>
       </c>
-      <c r="DR1" s="52">
+      <c r="DR1" s="48">
         <v>44016</v>
       </c>
-      <c r="DS1" s="52">
+      <c r="DS1" s="48">
         <v>44017</v>
       </c>
-      <c r="DT1" s="52">
+      <c r="DT1" s="48">
         <v>44018</v>
       </c>
-      <c r="DU1" s="52">
+      <c r="DU1" s="48">
         <v>44019</v>
       </c>
-      <c r="DV1" s="52">
+      <c r="DV1" s="48">
         <v>44020</v>
       </c>
-      <c r="DW1" s="52">
+      <c r="DW1" s="48">
         <v>44021</v>
       </c>
-      <c r="DX1" s="52">
+      <c r="DX1" s="48">
         <v>44022</v>
       </c>
-      <c r="DY1" s="52">
+      <c r="DY1" s="48">
         <v>44023</v>
       </c>
-      <c r="DZ1" s="52">
+      <c r="DZ1" s="48">
         <v>44024</v>
       </c>
-      <c r="EA1" s="52">
+      <c r="EA1" s="48">
         <v>44025</v>
       </c>
-      <c r="EB1" s="52">
+      <c r="EB1" s="48">
         <v>44026</v>
       </c>
-      <c r="EC1" s="52">
+      <c r="EC1" s="48">
         <v>44027</v>
       </c>
+      <c r="ED1" s="48">
+        <v>44028</v>
+      </c>
     </row>
-    <row r="2" spans="1:133">
+    <row r="2" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1771,7 +1729,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:133">
+    <row r="3" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2150,8 +2108,11 @@
       <c r="EC3">
         <v>140242</v>
       </c>
+      <c r="ED3">
+        <v>141607</v>
+      </c>
     </row>
-    <row r="4" spans="1:133">
+    <row r="4" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2325,8 +2286,11 @@
       <c r="EC4">
         <v>102058</v>
       </c>
+      <c r="ED4">
+        <v>103849</v>
+      </c>
     </row>
-    <row r="5" spans="1:133">
+    <row r="5" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2726,8 +2690,11 @@
       <c r="EC5">
         <v>11076</v>
       </c>
+      <c r="ED5">
+        <v>11115</v>
+      </c>
     </row>
-    <row r="6" spans="1:133">
+    <row r="6" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3109,8 +3076,11 @@
       <c r="EC6">
         <v>574</v>
       </c>
+      <c r="ED6">
+        <v>577</v>
+      </c>
     </row>
-    <row r="7" spans="1:133">
+    <row r="7" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3462,11 +3432,14 @@
       <c r="EC7">
         <v>1843</v>
       </c>
+      <c r="ED7">
+        <v>1863</v>
+      </c>
     </row>
-    <row r="8" spans="1:133">
+    <row r="8" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:133">
+    <row r="9" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3710,8 +3683,11 @@
       <c r="EC9">
         <v>345</v>
       </c>
+      <c r="ED9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:133">
+    <row r="10" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -4057,8 +4033,11 @@
       <c r="EC10">
         <v>68</v>
       </c>
+      <c r="ED10">
+        <v>96</v>
+      </c>
     </row>
-    <row r="11" spans="1:133">
+    <row r="11" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4404,8 +4383,11 @@
       <c r="EC11">
         <v>440</v>
       </c>
+      <c r="ED11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:133">
+    <row r="12" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4751,8 +4733,11 @@
       <c r="EC12">
         <v>191</v>
       </c>
+      <c r="ED12">
+        <v>199</v>
+      </c>
     </row>
-    <row r="13" spans="1:133">
+    <row r="13" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -5098,8 +5083,11 @@
       <c r="EC13">
         <v>249</v>
       </c>
+      <c r="ED13">
+        <v>241</v>
+      </c>
     </row>
-    <row r="14" spans="1:133">
+    <row r="14" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -5307,8 +5295,11 @@
       <c r="EC14">
         <v>86</v>
       </c>
+      <c r="ED14">
+        <v>87</v>
+      </c>
     </row>
-    <row r="15" spans="1:133">
+    <row r="15" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -5486,8 +5477,11 @@
       <c r="EC15">
         <v>24</v>
       </c>
+      <c r="ED15">
+        <v>17</v>
+      </c>
     </row>
-    <row r="16" spans="1:133">
+    <row r="16" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -5695,8 +5689,11 @@
       <c r="EC16">
         <v>2009</v>
       </c>
+      <c r="ED16">
+        <v>1999</v>
+      </c>
     </row>
-    <row r="17" spans="1:133">
+    <row r="17" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -5904,13 +5901,16 @@
       <c r="EC17" s="23">
         <v>0.81</v>
       </c>
+      <c r="ED17" s="23">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="19" spans="1:133">
+    <row r="19" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:133">
+    <row r="20" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:133">
+    <row r="21" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -6264,8 +6264,11 @@
       <c r="EC21">
         <v>120</v>
       </c>
+      <c r="ED21">
+        <v>120</v>
+      </c>
     </row>
-    <row r="22" spans="1:133">
+    <row r="22" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -6557,8 +6560,11 @@
       <c r="EC22">
         <v>5</v>
       </c>
+      <c r="ED22">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="1:133">
+    <row r="23" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -6850,8 +6856,11 @@
       <c r="EC23">
         <v>115</v>
       </c>
+      <c r="ED23">
+        <v>115</v>
+      </c>
     </row>
-    <row r="24" spans="1:133">
+    <row r="24" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -7188,8 +7197,11 @@
       <c r="EC24">
         <v>88</v>
       </c>
+      <c r="ED24">
+        <v>6</v>
+      </c>
     </row>
-    <row r="25" spans="1:133">
+    <row r="25" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -7526,8 +7538,11 @@
       <c r="EC25">
         <v>93</v>
       </c>
+      <c r="ED25">
+        <v>69</v>
+      </c>
     </row>
-    <row r="26" spans="1:133">
+    <row r="26" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -7864,13 +7879,16 @@
       <c r="EC26">
         <v>1708</v>
       </c>
+      <c r="ED26">
+        <v>1712</v>
+      </c>
     </row>
-    <row r="28" spans="1:133">
+    <row r="28" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:133">
+    <row r="29" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -8216,8 +8234,11 @@
       <c r="EC29">
         <v>172</v>
       </c>
+      <c r="ED29">
+        <v>176</v>
+      </c>
     </row>
-    <row r="30" spans="1:133">
+    <row r="30" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -8509,8 +8530,11 @@
       <c r="EC30">
         <v>34</v>
       </c>
+      <c r="ED30">
+        <v>39</v>
+      </c>
     </row>
-    <row r="31" spans="1:133">
+    <row r="31" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -8802,8 +8826,11 @@
       <c r="EC31">
         <v>137</v>
       </c>
+      <c r="ED31">
+        <v>137</v>
+      </c>
     </row>
-    <row r="32" spans="1:133">
+    <row r="32" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -9140,8 +9167,11 @@
       <c r="EC32">
         <v>110</v>
       </c>
+      <c r="ED32">
+        <v>125</v>
+      </c>
     </row>
-    <row r="33" spans="1:133">
+    <row r="33" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -9478,8 +9508,11 @@
       <c r="EC33">
         <v>144</v>
       </c>
+      <c r="ED33">
+        <v>164</v>
+      </c>
     </row>
-    <row r="34" spans="1:133">
+    <row r="34" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -9816,8 +9849,11 @@
       <c r="EC34">
         <v>1408</v>
       </c>
+      <c r="ED34">
+        <v>1401</v>
+      </c>
     </row>
-    <row r="35" spans="1:133">
+    <row r="35" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -9935,13 +9971,16 @@
       <c r="EC35">
         <v>1</v>
       </c>
+      <c r="ED35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:133">
+    <row r="37" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:133">
+    <row r="38" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -10275,8 +10314,11 @@
       <c r="EC38">
         <v>88</v>
       </c>
+      <c r="ED38">
+        <v>88</v>
+      </c>
     </row>
-    <row r="39" spans="1:133">
+    <row r="39" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -10562,8 +10604,11 @@
       <c r="EC39">
         <v>2</v>
       </c>
+      <c r="ED39">
+        <v>2</v>
+      </c>
     </row>
-    <row r="40" spans="1:133">
+    <row r="40" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -10849,8 +10894,11 @@
       <c r="EC40">
         <v>85</v>
       </c>
+      <c r="ED40">
+        <v>85</v>
+      </c>
     </row>
-    <row r="41" spans="1:133">
+    <row r="41" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -11181,8 +11229,11 @@
       <c r="EC41">
         <v>0</v>
       </c>
+      <c r="ED41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:133">
+    <row r="42" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -11510,8 +11561,11 @@
       <c r="EC42">
         <v>2</v>
       </c>
+      <c r="ED42">
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" spans="1:133">
+    <row r="43" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -11845,8 +11899,11 @@
       <c r="EC43">
         <v>296</v>
       </c>
+      <c r="ED43">
+        <v>296</v>
+      </c>
     </row>
-    <row r="44" spans="1:133">
+    <row r="44" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -12114,16 +12171,19 @@
       <c r="EC44">
         <v>1</v>
       </c>
+      <c r="ED44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:133">
+    <row r="45" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:133">
+    <row r="46" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:133">
+    <row r="47" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -12463,8 +12523,11 @@
       <c r="EC47">
         <v>207</v>
       </c>
+      <c r="ED47">
+        <v>207</v>
+      </c>
     </row>
-    <row r="48" spans="1:133">
+    <row r="48" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -12756,8 +12819,11 @@
       <c r="EC48">
         <v>0</v>
       </c>
+      <c r="ED48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:133">
+    <row r="49" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -13049,8 +13115,11 @@
       <c r="EC49">
         <v>200</v>
       </c>
+      <c r="ED49">
+        <v>200</v>
+      </c>
     </row>
-    <row r="50" spans="1:133">
+    <row r="50" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -13387,8 +13456,11 @@
       <c r="EC50">
         <v>63</v>
       </c>
+      <c r="ED50">
+        <v>66</v>
+      </c>
     </row>
-    <row r="51" spans="1:133">
+    <row r="51" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -13680,8 +13752,11 @@
       <c r="EC51">
         <v>63</v>
       </c>
+      <c r="ED51">
+        <v>66</v>
+      </c>
     </row>
-    <row r="52" spans="1:133">
+    <row r="52" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -13970,8 +14045,11 @@
       <c r="EC52">
         <v>1211</v>
       </c>
+      <c r="ED52">
+        <v>1209</v>
+      </c>
     </row>
-    <row r="53" spans="1:133">
+    <row r="53" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -14254,16 +14332,19 @@
       <c r="EC53">
         <v>1</v>
       </c>
+      <c r="ED53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:133">
+    <row r="54" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:133">
+    <row r="55" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:133">
+    <row r="56" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -14588,8 +14669,11 @@
       <c r="EC56">
         <v>35</v>
       </c>
+      <c r="ED56">
+        <v>35</v>
+      </c>
     </row>
-    <row r="57" spans="1:133">
+    <row r="57" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -14878,8 +14962,11 @@
       <c r="EC57">
         <v>2</v>
       </c>
+      <c r="ED57">
+        <v>2</v>
+      </c>
     </row>
-    <row r="58" spans="1:133">
+    <row r="58" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -15168,8 +15255,11 @@
       <c r="EC58">
         <v>32</v>
       </c>
+      <c r="ED58">
+        <v>32</v>
+      </c>
     </row>
-    <row r="59" spans="1:133">
+    <row r="59" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -15494,8 +15584,11 @@
       <c r="EC59">
         <v>2</v>
       </c>
+      <c r="ED59">
+        <v>2</v>
+      </c>
     </row>
-    <row r="60" spans="1:133">
+    <row r="60" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -15820,8 +15913,11 @@
       <c r="EC60">
         <v>4</v>
       </c>
+      <c r="ED60">
+        <v>5</v>
+      </c>
     </row>
-    <row r="61" spans="1:133">
+    <row r="61" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -16146,8 +16242,11 @@
       <c r="EC61">
         <v>175</v>
       </c>
+      <c r="ED61">
+        <v>176</v>
+      </c>
     </row>
-    <row r="62" spans="1:133">
+    <row r="62" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -16430,8 +16529,11 @@
       <c r="EC62">
         <v>1</v>
       </c>
+      <c r="ED62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:133">
+    <row r="64" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -16756,8 +16858,11 @@
       <c r="EC64">
         <v>13</v>
       </c>
+      <c r="ED64">
+        <v>13</v>
+      </c>
     </row>
-    <row r="65" spans="1:133">
+    <row r="65" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -17046,8 +17151,11 @@
       <c r="EC65">
         <v>0</v>
       </c>
+      <c r="ED65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:133">
+    <row r="66" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -17336,8 +17444,11 @@
       <c r="EC66">
         <v>13</v>
       </c>
+      <c r="ED66">
+        <v>13</v>
+      </c>
     </row>
-    <row r="67" spans="1:133">
+    <row r="67" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -17662,8 +17773,11 @@
       <c r="EC67">
         <v>71</v>
       </c>
+      <c r="ED67">
+        <v>67</v>
+      </c>
     </row>
-    <row r="68" spans="1:133">
+    <row r="68" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -17989,8 +18103,11 @@
       <c r="EC68">
         <v>71</v>
       </c>
+      <c r="ED68">
+        <v>67</v>
+      </c>
     </row>
-    <row r="69" spans="1:133">
+    <row r="69" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -18315,8 +18432,11 @@
       <c r="EC69">
         <v>0</v>
       </c>
+      <c r="ED69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:133">
+    <row r="70" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -18605,11 +18725,14 @@
       <c r="EC70">
         <v>0</v>
       </c>
+      <c r="ED70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:133">
+    <row r="71" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:133">
+    <row r="72" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>119</v>
       </c>
@@ -18784,8 +18907,11 @@
       <c r="EC72">
         <v>11</v>
       </c>
+      <c r="ED72">
+        <v>11</v>
+      </c>
     </row>
-    <row r="73" spans="1:133">
+    <row r="73" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>119</v>
       </c>
@@ -18960,8 +19086,11 @@
       <c r="EC73">
         <v>2</v>
       </c>
+      <c r="ED73">
+        <v>2</v>
+      </c>
     </row>
-    <row r="74" spans="1:133">
+    <row r="74" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
@@ -19136,8 +19265,11 @@
       <c r="EC74">
         <v>9</v>
       </c>
+      <c r="ED74">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:133">
+    <row r="75" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>119</v>
       </c>
@@ -19312,8 +19444,11 @@
       <c r="EC75">
         <v>2</v>
       </c>
+      <c r="ED75">
+        <v>2</v>
+      </c>
     </row>
-    <row r="76" spans="1:133">
+    <row r="76" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -19488,8 +19623,11 @@
       <c r="EC76">
         <v>4</v>
       </c>
+      <c r="ED76">
+        <v>4</v>
+      </c>
     </row>
-    <row r="77" spans="1:133">
+    <row r="77" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>119</v>
       </c>
@@ -19664,13 +19802,16 @@
       <c r="EC77">
         <v>48</v>
       </c>
+      <c r="ED77">
+        <v>48</v>
+      </c>
     </row>
-    <row r="79" spans="1:133">
+    <row r="79" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:133">
+    <row r="80" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -19998,8 +20139,11 @@
       <c r="EC80">
         <v>325</v>
       </c>
+      <c r="ED80">
+        <v>328</v>
+      </c>
     </row>
-    <row r="81" spans="1:133">
+    <row r="81" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -20327,8 +20471,11 @@
       <c r="EC81">
         <v>68</v>
       </c>
+      <c r="ED81">
+        <v>67</v>
+      </c>
     </row>
-    <row r="82" spans="1:133">
+    <row r="82" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -20656,8 +20803,11 @@
       <c r="EC82">
         <v>66</v>
       </c>
+      <c r="ED82">
+        <v>63</v>
+      </c>
     </row>
-    <row r="83" spans="1:133">
+    <row r="83" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -20943,8 +21093,11 @@
       <c r="EC83">
         <v>20</v>
       </c>
+      <c r="ED83">
+        <v>21</v>
+      </c>
     </row>
-    <row r="85" spans="1:133">
+    <row r="85" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -21272,8 +21425,11 @@
       <c r="EC85">
         <v>125</v>
       </c>
+      <c r="ED85">
+        <v>125</v>
+      </c>
     </row>
-    <row r="86" spans="1:133">
+    <row r="86" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -21601,8 +21757,11 @@
       <c r="EC86">
         <v>6</v>
       </c>
+      <c r="ED86">
+        <v>6</v>
+      </c>
     </row>
-    <row r="87" spans="1:133">
+    <row r="87" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -21930,8 +22089,11 @@
       <c r="EC87">
         <v>20</v>
       </c>
+      <c r="ED87">
+        <v>16</v>
+      </c>
     </row>
-    <row r="88" spans="1:133">
+    <row r="88" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -22259,8 +22421,11 @@
       <c r="EC88">
         <v>258</v>
       </c>
+      <c r="ED88">
+        <v>262</v>
+      </c>
     </row>
-    <row r="89" spans="1:133">
+    <row r="89" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -22462,8 +22627,11 @@
       <c r="EC89">
         <v>1</v>
       </c>
+      <c r="ED89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:133">
+    <row r="91" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -22791,8 +22959,11 @@
       <c r="EC91">
         <v>82</v>
       </c>
+      <c r="ED91">
+        <v>82</v>
+      </c>
     </row>
-    <row r="92" spans="1:133">
+    <row r="92" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -23120,8 +23291,11 @@
       <c r="EC92">
         <v>1</v>
       </c>
+      <c r="ED92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:133">
+    <row r="93" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -23437,8 +23611,11 @@
       <c r="EC93">
         <v>193</v>
       </c>
+      <c r="ED93">
+        <v>193</v>
+      </c>
     </row>
-    <row r="94" spans="1:133">
+    <row r="94" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -23766,8 +23943,11 @@
       <c r="EC94">
         <v>62</v>
       </c>
+      <c r="ED94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:133">
+    <row r="95" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -24053,11 +24233,14 @@
       <c r="EC95">
         <v>14</v>
       </c>
+      <c r="ED95">
+        <v>14</v>
+      </c>
     </row>
-    <row r="96" spans="1:133">
+    <row r="96" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:133">
+    <row r="97" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>130</v>
       </c>
@@ -24202,8 +24385,11 @@
       <c r="EC97">
         <v>14</v>
       </c>
+      <c r="ED97">
+        <v>14</v>
+      </c>
     </row>
-    <row r="98" spans="1:133">
+    <row r="98" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>130</v>
       </c>
@@ -24348,8 +24534,11 @@
       <c r="EC98">
         <v>11</v>
       </c>
+      <c r="ED98">
+        <v>11</v>
+      </c>
     </row>
-    <row r="99" spans="1:133">
+    <row r="99" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>130</v>
       </c>
@@ -24494,8 +24683,11 @@
       <c r="EC99">
         <v>55</v>
       </c>
+      <c r="ED99">
+        <v>55</v>
+      </c>
     </row>
-    <row r="100" spans="1:133">
+    <row r="100" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
@@ -24640,8 +24832,11 @@
       <c r="EC100">
         <v>1</v>
       </c>
+      <c r="ED100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:133">
+    <row r="102" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -24888,8 +25083,11 @@
       <c r="EC102">
         <v>211</v>
       </c>
+      <c r="ED102">
+        <v>212</v>
+      </c>
     </row>
-    <row r="103" spans="1:133">
+    <row r="103" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -25136,8 +25334,11 @@
       <c r="EC103">
         <v>140</v>
       </c>
+      <c r="ED103">
+        <v>140</v>
+      </c>
     </row>
-    <row r="104" spans="1:133">
+    <row r="104" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -25384,8 +25585,11 @@
       <c r="EC104">
         <v>28</v>
       </c>
+      <c r="ED104">
+        <v>28</v>
+      </c>
     </row>
-    <row r="119" spans="52:52">
+    <row r="119" spans="52:52" x14ac:dyDescent="0.25">
       <c r="AZ119">
         <v>9</v>
       </c>
@@ -25397,22 +25601,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:DD11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:DE11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DE2" sqref="DE2"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="DC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DE2" sqref="DE2:DE11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:108" s="2" customFormat="1">
+    <row r="2" spans="1:109" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -25737,8 +25941,11 @@
       <c r="DD2" s="9">
         <v>44027</v>
       </c>
+      <c r="DE2" s="9">
+        <v>44028</v>
+      </c>
     </row>
-    <row r="3" spans="1:108">
+    <row r="3" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -26063,8 +26270,11 @@
       <c r="DD3">
         <v>1572</v>
       </c>
+      <c r="DE3">
+        <v>1578</v>
+      </c>
     </row>
-    <row r="4" spans="1:108">
+    <row r="4" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -26389,8 +26599,11 @@
       <c r="DD4">
         <v>669</v>
       </c>
+      <c r="DE4">
+        <v>677</v>
+      </c>
     </row>
-    <row r="5" spans="1:108">
+    <row r="5" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -26715,8 +26928,11 @@
       <c r="DD5">
         <v>519</v>
       </c>
+      <c r="DE5">
+        <v>521</v>
+      </c>
     </row>
-    <row r="6" spans="1:108">
+    <row r="6" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -27041,8 +27257,11 @@
       <c r="DD6">
         <v>2258</v>
       </c>
+      <c r="DE6">
+        <v>2262</v>
+      </c>
     </row>
-    <row r="7" spans="1:108">
+    <row r="7" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -27367,8 +27586,11 @@
       <c r="DD7">
         <v>1646</v>
       </c>
+      <c r="DE7">
+        <v>1654</v>
+      </c>
     </row>
-    <row r="8" spans="1:108">
+    <row r="8" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -27693,8 +27915,11 @@
       <c r="DD8">
         <v>1017</v>
       </c>
+      <c r="DE8">
+        <v>1021</v>
+      </c>
     </row>
-    <row r="9" spans="1:108">
+    <row r="9" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -28019,8 +28244,11 @@
       <c r="DD9">
         <v>1592</v>
       </c>
+      <c r="DE9">
+        <v>1596</v>
+      </c>
     </row>
-    <row r="10" spans="1:108">
+    <row r="10" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -28345,8 +28573,11 @@
       <c r="DD10">
         <v>1624</v>
       </c>
+      <c r="DE10">
+        <v>1627</v>
+      </c>
     </row>
-    <row r="11" spans="1:108">
+    <row r="11" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -28669,6 +28900,9 @@
         <v>180</v>
       </c>
       <c r="DD11">
+        <v>179</v>
+      </c>
+      <c r="DE11">
         <v>179</v>
       </c>
     </row>
@@ -28679,22 +28913,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:CY17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:CZ17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CZ2" sqref="CZ2"/>
+      <pane xSplit="1" topLeftCell="CU1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CZ14" sqref="CZ14:CZ17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" customWidth="1"/>
-    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:103" s="2" customFormat="1">
+    <row r="2" spans="1:104" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -29002,8 +29236,11 @@
       <c r="CY2" s="9">
         <v>44027</v>
       </c>
+      <c r="CZ2" s="9">
+        <v>44028</v>
+      </c>
     </row>
-    <row r="3" spans="1:103" s="2" customFormat="1">
+    <row r="3" spans="1:104" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>36</v>
       </c>
@@ -29012,7 +29249,7 @@
       <c r="D3" s="9"/>
       <c r="CP3" s="4"/>
     </row>
-    <row r="4" spans="1:103">
+    <row r="4" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -29322,8 +29559,11 @@
       <c r="CY4">
         <v>11706</v>
       </c>
+      <c r="CZ4">
+        <v>11115</v>
+      </c>
     </row>
-    <row r="5" spans="1:103">
+    <row r="5" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -29633,8 +29873,11 @@
       <c r="CY5">
         <v>207</v>
       </c>
+      <c r="CZ5">
+        <v>144</v>
+      </c>
     </row>
-    <row r="6" spans="1:103">
+    <row r="6" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -29944,8 +30187,11 @@
       <c r="CY6">
         <v>2263</v>
       </c>
+      <c r="CZ6">
+        <v>2290</v>
+      </c>
     </row>
-    <row r="7" spans="1:103">
+    <row r="7" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -30255,8 +30501,11 @@
       <c r="CY7">
         <v>5448</v>
       </c>
+      <c r="CZ7">
+        <v>5496</v>
+      </c>
     </row>
-    <row r="8" spans="1:103">
+    <row r="8" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -30566,8 +30815,11 @@
       <c r="CY8">
         <v>171</v>
       </c>
+      <c r="CZ8">
+        <v>171</v>
+      </c>
     </row>
-    <row r="9" spans="1:103" ht="28.8">
+    <row r="9" spans="1:104" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -30877,8 +31129,11 @@
       <c r="CY9">
         <v>27</v>
       </c>
+      <c r="CZ9">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:103" ht="28.8">
+    <row r="10" spans="1:104" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -31184,8 +31439,11 @@
       <c r="CY10">
         <v>29</v>
       </c>
+      <c r="CZ10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="11" spans="1:103">
+    <row r="11" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -31495,8 +31753,11 @@
       <c r="CY11">
         <v>2841</v>
       </c>
+      <c r="CZ11">
+        <v>2867</v>
+      </c>
     </row>
-    <row r="12" spans="1:103">
+    <row r="12" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -31806,8 +32067,11 @@
       <c r="CY12">
         <v>90</v>
       </c>
+      <c r="CZ12">
+        <v>90</v>
+      </c>
     </row>
-    <row r="13" spans="1:103">
+    <row r="13" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -31818,7 +32082,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:103">
+    <row r="14" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -32128,8 +32392,11 @@
       <c r="CY14">
         <v>1391</v>
       </c>
+      <c r="CZ14">
+        <v>1355</v>
+      </c>
     </row>
-    <row r="15" spans="1:103">
+    <row r="15" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -32439,8 +32706,11 @@
       <c r="CY15">
         <v>3072</v>
       </c>
+      <c r="CZ15">
+        <v>3082</v>
+      </c>
     </row>
-    <row r="16" spans="1:103">
+    <row r="16" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -32750,8 +33020,11 @@
       <c r="CY16">
         <v>6594</v>
       </c>
+      <c r="CZ16">
+        <v>6569</v>
+      </c>
     </row>
-    <row r="17" spans="1:103">
+    <row r="17" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -33059,6 +33332,9 @@
         <v>18</v>
       </c>
       <c r="CY17">
+        <v>19</v>
+      </c>
+      <c r="CZ17">
         <v>19</v>
       </c>
     </row>
@@ -33069,21 +33345,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:CY9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CZ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CZ1" sqref="CZ1"/>
+      <pane xSplit="1" topLeftCell="CV1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CZ4" sqref="CZ4:CZ8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" s="2" customFormat="1">
+    <row r="1" spans="1:104" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -33390,14 +33666,17 @@
       <c r="CY1" s="9">
         <v>44027</v>
       </c>
+      <c r="CZ1" s="9">
+        <v>44028</v>
+      </c>
     </row>
-    <row r="2" spans="1:103">
+    <row r="2" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:103">
+    <row r="3" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -33708,8 +33987,11 @@
       <c r="CY3">
         <v>574</v>
       </c>
+      <c r="CZ3">
+        <v>577</v>
+      </c>
     </row>
-    <row r="4" spans="1:103">
+    <row r="4" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -34019,8 +34301,11 @@
       <c r="CY4">
         <v>8</v>
       </c>
+      <c r="CZ4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:103" ht="28.8">
+    <row r="5" spans="1:104" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -34330,8 +34615,11 @@
       <c r="CY5">
         <v>425</v>
       </c>
+      <c r="CZ5">
+        <v>426</v>
+      </c>
     </row>
-    <row r="6" spans="1:103">
+    <row r="6" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -34641,8 +34929,11 @@
       <c r="CY6">
         <v>75</v>
       </c>
+      <c r="CZ6">
+        <v>75</v>
+      </c>
     </row>
-    <row r="7" spans="1:103">
+    <row r="7" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -34952,8 +35243,11 @@
       <c r="CY7">
         <v>61</v>
       </c>
+      <c r="CZ7">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:103">
+    <row r="8" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -35263,8 +35557,11 @@
       <c r="CY8">
         <v>5</v>
       </c>
+      <c r="CZ8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:103">
+    <row r="9" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -35305,20 +35602,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:CQ5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CR5"/>
   <sheetViews>
     <sheetView zoomScale="95" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CR1" sqref="CR1"/>
+      <pane xSplit="1" topLeftCell="CN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CR3" sqref="CR3:CR5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" s="2" customFormat="1">
+    <row r="1" spans="1:96" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -35601,13 +35898,16 @@
       <c r="CQ1" s="9">
         <v>44027</v>
       </c>
+      <c r="CR1" s="9">
+        <v>44028</v>
+      </c>
     </row>
-    <row r="2" spans="1:95">
+    <row r="2" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:95">
+    <row r="3" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
@@ -35893,10 +36193,13 @@
       <c r="CQ3">
         <v>574</v>
       </c>
+      <c r="CR3">
+        <v>577</v>
+      </c>
     </row>
-    <row r="4" spans="1:95">
+    <row r="4" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B4">
         <v>26</v>
@@ -36180,10 +36483,13 @@
       <c r="CQ4">
         <v>244</v>
       </c>
+      <c r="CR4">
+        <v>245</v>
+      </c>
     </row>
-    <row r="5" spans="1:95">
+    <row r="5" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -36466,6 +36772,9 @@
       </c>
       <c r="CQ5">
         <v>330</v>
+      </c>
+      <c r="CR5">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -36475,20 +36784,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:CQ11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CR11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CR1" sqref="CR1"/>
+      <pane xSplit="1" topLeftCell="CN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CR3" sqref="CR3:CR11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" s="2" customFormat="1">
+    <row r="1" spans="1:96" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -36771,13 +37080,16 @@
       <c r="CQ1" s="9">
         <v>44027</v>
       </c>
+      <c r="CR1" s="9">
+        <v>44028</v>
+      </c>
     </row>
-    <row r="2" spans="1:95">
+    <row r="2" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:95">
+    <row r="3" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -37063,10 +37375,13 @@
       <c r="CQ3">
         <v>574</v>
       </c>
+      <c r="CR3">
+        <v>577</v>
+      </c>
     </row>
-    <row r="4" spans="1:95">
+    <row r="4" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -37350,10 +37665,13 @@
       <c r="CQ4">
         <v>0</v>
       </c>
+      <c r="CR4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:95">
+    <row r="5" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -37637,10 +37955,13 @@
       <c r="CQ5">
         <v>3</v>
       </c>
+      <c r="CR5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:95">
+    <row r="6" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -37924,10 +38245,13 @@
       <c r="CQ6">
         <v>8</v>
       </c>
+      <c r="CR6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:95">
+    <row r="7" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -38211,10 +38535,13 @@
       <c r="CQ7">
         <v>19</v>
       </c>
+      <c r="CR7">
+        <v>19</v>
+      </c>
     </row>
-    <row r="8" spans="1:95">
+    <row r="8" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -38498,10 +38825,13 @@
       <c r="CQ8">
         <v>66</v>
       </c>
+      <c r="CR8">
+        <v>66</v>
+      </c>
     </row>
-    <row r="9" spans="1:95">
+    <row r="9" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B9">
         <v>19</v>
@@ -38785,10 +39115,13 @@
       <c r="CQ9">
         <v>136</v>
       </c>
+      <c r="CR9">
+        <v>136</v>
+      </c>
     </row>
-    <row r="10" spans="1:95">
+    <row r="10" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B10">
         <v>15</v>
@@ -39072,10 +39405,13 @@
       <c r="CQ10">
         <v>146</v>
       </c>
+      <c r="CR10">
+        <v>147</v>
+      </c>
     </row>
-    <row r="11" spans="1:95">
+    <row r="11" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B11">
         <v>15</v>
@@ -39358,6 +39694,9 @@
       </c>
       <c r="CQ11">
         <v>196</v>
+      </c>
+      <c r="CR11">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -39367,21 +39706,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A2:CK13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:CL13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BS1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CL2" sqref="CL2"/>
+      <pane xSplit="1" topLeftCell="CB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CM12" sqref="CM12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="57" max="57" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="57" max="57" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:89" s="2" customFormat="1">
+    <row r="2" spans="1:90" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -39649,8 +39988,11 @@
       <c r="CK2" s="9">
         <v>44027</v>
       </c>
+      <c r="CL2" s="9">
+        <v>44028</v>
+      </c>
     </row>
-    <row r="3" spans="1:89">
+    <row r="3" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -39918,8 +40260,11 @@
       <c r="CK3">
         <v>574</v>
       </c>
+      <c r="CL3">
+        <v>577</v>
+      </c>
     </row>
-    <row r="4" spans="1:89">
+    <row r="4" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -40187,8 +40532,11 @@
       <c r="CK4">
         <v>63</v>
       </c>
+      <c r="CL4">
+        <v>62</v>
+      </c>
     </row>
-    <row r="5" spans="1:89">
+    <row r="5" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -40456,8 +40804,11 @@
       <c r="CK5">
         <v>31</v>
       </c>
+      <c r="CL5">
+        <v>33</v>
+      </c>
     </row>
-    <row r="6" spans="1:89">
+    <row r="6" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -40725,8 +41076,11 @@
       <c r="CK6">
         <v>33</v>
       </c>
+      <c r="CL6">
+        <v>33</v>
+      </c>
     </row>
-    <row r="7" spans="1:89">
+    <row r="7" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -40994,8 +41348,11 @@
       <c r="CK7">
         <v>84</v>
       </c>
+      <c r="CL7">
+        <v>84</v>
+      </c>
     </row>
-    <row r="8" spans="1:89">
+    <row r="8" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -41263,8 +41620,11 @@
       <c r="CK8">
         <v>92</v>
       </c>
+      <c r="CL8">
+        <v>92</v>
+      </c>
     </row>
-    <row r="9" spans="1:89">
+    <row r="9" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -41532,8 +41892,11 @@
       <c r="CK9">
         <v>49</v>
       </c>
+      <c r="CL9">
+        <v>49</v>
+      </c>
     </row>
-    <row r="10" spans="1:89">
+    <row r="10" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -41801,8 +42164,11 @@
       <c r="CK10">
         <v>85</v>
       </c>
+      <c r="CL10">
+        <v>85</v>
+      </c>
     </row>
-    <row r="11" spans="1:89">
+    <row r="11" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -42070,8 +42436,11 @@
       <c r="CK11">
         <v>116</v>
       </c>
+      <c r="CL11">
+        <v>117</v>
+      </c>
     </row>
-    <row r="12" spans="1:89" ht="28.8">
+    <row r="12" spans="1:90" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -42339,8 +42708,11 @@
       <c r="CK12">
         <v>20</v>
       </c>
+      <c r="CL12">
+        <v>21</v>
+      </c>
     </row>
-    <row r="13" spans="1:89">
+    <row r="13" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -42606,6 +42978,9 @@
         <v>0</v>
       </c>
       <c r="CK13">
+        <v>1</v>
+      </c>
+      <c r="CL13">
         <v>1</v>
       </c>
     </row>
@@ -42616,67 +42991,67 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:BH23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BI23"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="BH5" sqref="BH5"/>
+    <sheetView topLeftCell="AO1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="BI5" sqref="BI5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="42" max="45" width="8.88671875" customWidth="1"/>
+    <col min="42" max="45" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60">
-      <c r="C1" s="53" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="C1" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
     </row>
-    <row r="2" spans="1:60">
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
     </row>
-    <row r="3" spans="1:60">
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
     </row>
-    <row r="4" spans="1:60">
+    <row r="4" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -42691,7 +43066,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:60">
+    <row r="5" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -42863,11 +43238,14 @@
       <c r="BG5" s="9">
         <v>44027</v>
       </c>
-      <c r="BH5" t="s">
+      <c r="BH5" s="9">
+        <v>44028</v>
+      </c>
+      <c r="BI5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>120</v>
       </c>
@@ -43042,8 +43420,11 @@
       <c r="BG6">
         <v>158</v>
       </c>
+      <c r="BH6">
+        <v>158</v>
+      </c>
     </row>
-    <row r="7" spans="1:60">
+    <row r="7" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -43218,8 +43599,11 @@
       <c r="BG7">
         <v>36</v>
       </c>
+      <c r="BH7">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" spans="1:60">
+    <row r="8" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
@@ -43227,7 +43611,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:60">
+    <row r="9" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -43402,8 +43786,11 @@
       <c r="BG9">
         <v>1</v>
       </c>
+      <c r="BH9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:60">
+    <row r="10" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>121</v>
       </c>
@@ -43578,8 +43965,11 @@
       <c r="BG10">
         <v>23</v>
       </c>
+      <c r="BH10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:60">
+    <row r="11" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>122</v>
       </c>
@@ -43754,8 +44144,11 @@
       <c r="BG11">
         <v>9</v>
       </c>
+      <c r="BH11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:60">
+    <row r="12" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -43930,13 +44323,16 @@
       <c r="BG12">
         <v>3</v>
       </c>
+      <c r="BH12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:60">
+    <row r="13" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:60">
+    <row r="14" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -44111,8 +44507,11 @@
       <c r="BG14">
         <v>1</v>
       </c>
+      <c r="BH14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:60">
+    <row r="15" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -44287,8 +44686,11 @@
       <c r="BG15">
         <v>0</v>
       </c>
+      <c r="BH15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:60">
+    <row r="16" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -44463,8 +44865,11 @@
       <c r="BG16">
         <v>3</v>
       </c>
+      <c r="BH16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:59">
+    <row r="17" spans="1:60" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -44639,8 +45044,11 @@
       <c r="BG17">
         <v>12</v>
       </c>
+      <c r="BH17">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:59">
+    <row r="18" spans="1:60" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -44815,8 +45223,11 @@
       <c r="BG18">
         <v>3</v>
       </c>
+      <c r="BH18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:59">
+    <row r="19" spans="1:60" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -44991,8 +45402,11 @@
       <c r="BG19">
         <v>2</v>
       </c>
+      <c r="BH19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:59">
+    <row r="20" spans="1:60" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -45167,8 +45581,11 @@
       <c r="BG20">
         <v>2</v>
       </c>
+      <c r="BH20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:59">
+    <row r="21" spans="1:60" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -45343,8 +45760,11 @@
       <c r="BG21">
         <v>6</v>
       </c>
+      <c r="BH21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:59" ht="28.8">
+    <row r="22" spans="1:60" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -45519,8 +45939,11 @@
       <c r="BG22">
         <v>4</v>
       </c>
+      <c r="BH22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:59" ht="28.8">
+    <row r="23" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
         <v>123</v>
       </c>
@@ -45693,6 +46116,9 @@
         <v>3</v>
       </c>
       <c r="BG23">
+        <v>3</v>
+      </c>
+      <c r="BH23">
         <v>3</v>
       </c>
     </row>
@@ -45705,37 +46131,37 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A1" s="54" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+    <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
     </row>
-    <row r="2" spans="1:7" ht="36.6" customHeight="1">
-      <c r="A2" s="56" t="s">
+    <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -45744,7 +46170,7 @@
       <c r="C2" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="55" t="s">
         <v>114</v>
       </c>
       <c r="E2" s="29" t="s">
@@ -45757,11 +46183,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1">
-      <c r="A3" s="56"/>
+    <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="54"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="57"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="25" t="s">
         <v>92</v>
       </c>
@@ -45772,11 +46198,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A4" s="56"/>
+    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="54"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="57"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="25" t="s">
         <v>86</v>
       </c>
@@ -45785,45 +46211,45 @@
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A5" s="56"/>
+    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="54"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
-      <c r="D5" s="57"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="25" t="s">
         <v>87</v>
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A6" s="56"/>
+    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="54"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="57"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1">
-      <c r="A7" s="56"/>
+    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="54"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
-      <c r="D7" s="57"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="25" t="s">
         <v>93</v>
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" ht="14.4" customHeight="1">
+    <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>94</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C8" s="28">
         <v>2</v>
@@ -45832,7 +46258,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F8" s="28">
         <v>0</v>
@@ -45841,9 +46267,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.4" customHeight="1">
+    <row r="9" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>95</v>
@@ -45855,7 +46281,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F9" s="28">
         <v>0</v>
@@ -45864,12 +46290,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.4" customHeight="1">
+    <row r="10" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>96</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="C10" s="28">
         <v>5</v>
@@ -45878,7 +46304,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F10" s="28">
         <v>1</v>
@@ -45887,21 +46313,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.4" customHeight="1">
+    <row r="11" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>97</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C11" s="28">
         <v>24</v>
       </c>
       <c r="D11" s="28">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F11" s="28">
         <v>0</v>
@@ -45910,12 +46336,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.4" customHeight="1">
+    <row r="12" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>98</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="C12" s="28">
         <v>2</v>
@@ -45924,7 +46350,7 @@
         <v>6</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="F12" s="28">
         <v>0</v>
@@ -45933,7 +46359,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.4" customHeight="1">
+    <row r="13" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>126</v>
       </c>
@@ -45956,12 +46382,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.4" customHeight="1">
+    <row r="14" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>99</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="C14" s="28">
         <v>2</v>
@@ -45979,18 +46405,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.4" customHeight="1">
+    <row r="15" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>100</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C15" s="28">
         <v>13</v>
       </c>
       <c r="D15" s="28">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E15" s="28" t="s">
         <v>135</v>
@@ -46002,21 +46428,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>116</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="C16" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="28">
         <v>18</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F16" s="28">
         <v>0</v>
@@ -46025,12 +46451,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.4" customHeight="1">
+    <row r="17" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>101</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="C17" s="28">
         <v>9</v>
@@ -46045,15 +46471,15 @@
         <v>1</v>
       </c>
       <c r="G17" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.4" customHeight="1">
+    <row r="18" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>102</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C18" s="28">
         <v>9</v>
@@ -46062,7 +46488,7 @@
         <v>32</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F18" s="28">
         <v>0</v>
@@ -46071,21 +46497,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.4" customHeight="1">
+    <row r="19" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>103</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C19" s="28">
         <v>14</v>
       </c>
       <c r="D19" s="28">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F19" s="28">
         <v>0</v>
@@ -46094,12 +46520,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.4" customHeight="1">
+    <row r="20" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>104</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C20" s="28">
         <v>14</v>
@@ -46117,12 +46543,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.4" customHeight="1">
+    <row r="21" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>105</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C21" s="28">
         <v>1</v>
@@ -46131,7 +46557,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F21" s="28">
         <v>0</v>
@@ -46140,21 +46566,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.4" customHeight="1">
+    <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>107</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="C22" s="28">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D22" s="28">
         <v>74</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="F22" s="28">
         <v>2</v>
@@ -46163,12 +46589,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.6" customHeight="1">
+    <row r="23" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="C23" s="28">
         <v>7</v>
@@ -46177,7 +46603,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F23" s="28">
         <v>1</v>
@@ -46186,12 +46612,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18" customHeight="1">
+    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>109</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C24" s="28">
         <v>7</v>
@@ -46200,7 +46626,7 @@
         <v>10</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F24" s="28">
         <v>0</v>
@@ -46209,21 +46635,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="33.6" customHeight="1">
+    <row r="25" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
         <v>117</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="C25" s="28">
         <v>20</v>
       </c>
       <c r="D25" s="28">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F25" s="28">
         <v>1</v>
@@ -46232,53 +46658,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.399999999999999" customHeight="1">
-      <c r="A26" s="46" t="s">
+    <row r="26" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="45" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C26" s="28">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D26" s="28">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F26" s="28">
         <v>7</v>
       </c>
       <c r="G26" s="28">
-        <v>252</v>
-      </c>
-      <c r="H26" s="47"/>
+        <v>253</v>
+      </c>
+      <c r="H26" s="46"/>
     </row>
-    <row r="27" spans="1:8" ht="17.399999999999999" customHeight="1">
+    <row r="27" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="B27" s="43" t="s">
-        <v>177</v>
-      </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="49"/>
+      <c r="B27" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="47"/>
     </row>
-    <row r="28" spans="1:8" ht="17.399999999999999" customHeight="1">
+    <row r="28" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="27"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
     </row>
-    <row r="29" spans="1:8" ht="17.399999999999999" customHeight="1"/>
+    <row r="29" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
@@ -46292,9 +46718,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46501,27 +46930,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -46546,9 +46963,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Results from July 18, 2020 08:46:40 AM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/work/WashingtonDC/data.xlsx
+++ b/workflow/python/work/WashingtonDC/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7110" tabRatio="807"/>
+    <workbookView xWindow="510" yWindow="555" windowWidth="20730" windowHeight="7110" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="181">
   <si>
     <t>Testing</t>
   </si>
@@ -518,32 +518,6 @@
     <t>40; (36)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">As of July 16, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>158 cases</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for COVID-19 testing,  and 36 (22.7%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
-    </r>
-  </si>
-  <si>
     <t>As of July 16, 2020</t>
   </si>
   <si>
@@ -599,6 +573,32 @@
   </si>
   <si>
     <t>1002; (380)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As of July 17, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>159 cases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for COVID-19 testing,  and 36 (22.6%) have been confirmed positive. The decedents submitted for testing did not have a confirmed COVID-19 test result and were not admitted to a hospital at the time.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -941,7 +941,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1276,7 +1276,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1284,11 +1284,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ED119"/>
+  <dimension ref="A1:EE119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="DZ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EF4" sqref="EF4"/>
+      <selection pane="topRight" activeCell="EG5" sqref="EG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,10 +1304,10 @@
     <col min="98" max="102" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="104" max="118" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="128" max="134" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="128" max="135" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1704,8 +1704,11 @@
       <c r="ED1" s="48">
         <v>44028</v>
       </c>
+      <c r="EE1" s="48">
+        <v>44029</v>
+      </c>
     </row>
-    <row r="2" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1729,7 +1732,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2111,8 +2114,11 @@
       <c r="ED3">
         <v>141607</v>
       </c>
+      <c r="EE3">
+        <v>144955</v>
+      </c>
     </row>
-    <row r="4" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2289,8 +2295,11 @@
       <c r="ED4">
         <v>103849</v>
       </c>
+      <c r="EE4">
+        <v>105271</v>
+      </c>
     </row>
-    <row r="5" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2693,8 +2702,11 @@
       <c r="ED5">
         <v>11115</v>
       </c>
+      <c r="EE5">
+        <v>11194</v>
+      </c>
     </row>
-    <row r="6" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3079,8 +3091,11 @@
       <c r="ED6">
         <v>577</v>
       </c>
+      <c r="EE6">
+        <v>578</v>
+      </c>
     </row>
-    <row r="7" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3435,11 +3450,14 @@
       <c r="ED7">
         <v>1863</v>
       </c>
+      <c r="EE7">
+        <v>1877</v>
+      </c>
     </row>
-    <row r="8" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3686,8 +3704,11 @@
       <c r="ED9">
         <v>345</v>
       </c>
+      <c r="EE9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -4036,8 +4057,11 @@
       <c r="ED10">
         <v>96</v>
       </c>
+      <c r="EE10">
+        <v>84</v>
+      </c>
     </row>
-    <row r="11" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4386,8 +4410,11 @@
       <c r="ED11">
         <v>440</v>
       </c>
+      <c r="EE11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4736,8 +4763,11 @@
       <c r="ED12">
         <v>199</v>
       </c>
+      <c r="EE12">
+        <v>200</v>
+      </c>
     </row>
-    <row r="13" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -5086,8 +5116,11 @@
       <c r="ED13">
         <v>241</v>
       </c>
+      <c r="EE13">
+        <v>240</v>
+      </c>
     </row>
-    <row r="14" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -5298,8 +5331,11 @@
       <c r="ED14">
         <v>87</v>
       </c>
+      <c r="EE14">
+        <v>88</v>
+      </c>
     </row>
-    <row r="15" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -5480,8 +5516,11 @@
       <c r="ED15">
         <v>17</v>
       </c>
+      <c r="EE15">
+        <v>17</v>
+      </c>
     </row>
-    <row r="16" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -5692,8 +5731,11 @@
       <c r="ED16">
         <v>1999</v>
       </c>
+      <c r="EE16">
+        <v>1972</v>
+      </c>
     </row>
-    <row r="17" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -5904,13 +5946,16 @@
       <c r="ED17" s="23">
         <v>0.8</v>
       </c>
+      <c r="EE17" s="23">
+        <v>0.79</v>
+      </c>
     </row>
-    <row r="19" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -5918,7 +5963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:134" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -6267,8 +6312,11 @@
       <c r="ED21">
         <v>120</v>
       </c>
+      <c r="EE21">
+        <v>120</v>
+      </c>
     </row>
-    <row r="22" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -6563,8 +6611,11 @@
       <c r="ED22">
         <v>5</v>
       </c>
+      <c r="EE22">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -6859,8 +6910,11 @@
       <c r="ED23">
         <v>115</v>
       </c>
+      <c r="EE23">
+        <v>115</v>
+      </c>
     </row>
-    <row r="24" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -7200,8 +7254,11 @@
       <c r="ED24">
         <v>6</v>
       </c>
+      <c r="EE24">
+        <v>70</v>
+      </c>
     </row>
-    <row r="25" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -7541,8 +7598,11 @@
       <c r="ED25">
         <v>69</v>
       </c>
+      <c r="EE25">
+        <v>75</v>
+      </c>
     </row>
-    <row r="26" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -7882,13 +7942,16 @@
       <c r="ED26">
         <v>1712</v>
       </c>
+      <c r="EE26">
+        <v>1716</v>
+      </c>
     </row>
-    <row r="28" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -8237,8 +8300,11 @@
       <c r="ED29">
         <v>176</v>
       </c>
+      <c r="EE29">
+        <v>179</v>
+      </c>
     </row>
-    <row r="30" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -8533,8 +8599,11 @@
       <c r="ED30">
         <v>39</v>
       </c>
+      <c r="EE30">
+        <v>42</v>
+      </c>
     </row>
-    <row r="31" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -8829,8 +8898,11 @@
       <c r="ED31">
         <v>137</v>
       </c>
+      <c r="EE31">
+        <v>137</v>
+      </c>
     </row>
-    <row r="32" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -9170,8 +9242,11 @@
       <c r="ED32">
         <v>125</v>
       </c>
+      <c r="EE32">
+        <v>130</v>
+      </c>
     </row>
-    <row r="33" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -9511,8 +9586,11 @@
       <c r="ED33">
         <v>164</v>
       </c>
+      <c r="EE33">
+        <v>175</v>
+      </c>
     </row>
-    <row r="34" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -9852,8 +9930,11 @@
       <c r="ED34">
         <v>1401</v>
       </c>
+      <c r="EE34">
+        <v>1413</v>
+      </c>
     </row>
-    <row r="35" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -9974,13 +10055,16 @@
       <c r="ED35">
         <v>1</v>
       </c>
+      <c r="EE35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -10317,8 +10401,11 @@
       <c r="ED38">
         <v>88</v>
       </c>
+      <c r="EE38">
+        <v>88</v>
+      </c>
     </row>
-    <row r="39" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -10607,8 +10694,11 @@
       <c r="ED39">
         <v>2</v>
       </c>
+      <c r="EE39">
+        <v>2</v>
+      </c>
     </row>
-    <row r="40" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -10897,8 +10987,11 @@
       <c r="ED40">
         <v>85</v>
       </c>
+      <c r="EE40">
+        <v>85</v>
+      </c>
     </row>
-    <row r="41" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -11232,8 +11325,11 @@
       <c r="ED41">
         <v>0</v>
       </c>
+      <c r="EE41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -11564,8 +11660,11 @@
       <c r="ED42">
         <v>2</v>
       </c>
+      <c r="EE42">
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -11902,8 +12001,11 @@
       <c r="ED43">
         <v>296</v>
       </c>
+      <c r="EE43">
+        <v>296</v>
+      </c>
     </row>
-    <row r="44" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -12174,16 +12276,19 @@
       <c r="ED44">
         <v>1</v>
       </c>
+      <c r="EE44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -12526,8 +12631,11 @@
       <c r="ED47">
         <v>207</v>
       </c>
+      <c r="EE47">
+        <v>207</v>
+      </c>
     </row>
-    <row r="48" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -12822,8 +12930,11 @@
       <c r="ED48">
         <v>0</v>
       </c>
+      <c r="EE48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -13118,8 +13229,11 @@
       <c r="ED49">
         <v>200</v>
       </c>
+      <c r="EE49">
+        <v>200</v>
+      </c>
     </row>
-    <row r="50" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -13459,8 +13573,11 @@
       <c r="ED50">
         <v>66</v>
       </c>
+      <c r="EE50">
+        <v>65</v>
+      </c>
     </row>
-    <row r="51" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -13755,8 +13872,11 @@
       <c r="ED51">
         <v>66</v>
       </c>
+      <c r="EE51">
+        <v>65</v>
+      </c>
     </row>
-    <row r="52" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -14048,8 +14168,11 @@
       <c r="ED52">
         <v>1209</v>
       </c>
+      <c r="EE52">
+        <v>1216</v>
+      </c>
     </row>
-    <row r="53" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -14335,16 +14458,19 @@
       <c r="ED53">
         <v>1</v>
       </c>
+      <c r="EE53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -14672,8 +14798,11 @@
       <c r="ED56">
         <v>35</v>
       </c>
+      <c r="EE56">
+        <v>35</v>
+      </c>
     </row>
-    <row r="57" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -14965,8 +15094,11 @@
       <c r="ED57">
         <v>2</v>
       </c>
+      <c r="EE57">
+        <v>2</v>
+      </c>
     </row>
-    <row r="58" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -15258,8 +15390,11 @@
       <c r="ED58">
         <v>32</v>
       </c>
+      <c r="EE58">
+        <v>32</v>
+      </c>
     </row>
-    <row r="59" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -15587,8 +15722,11 @@
       <c r="ED59">
         <v>2</v>
       </c>
+      <c r="EE59">
+        <v>2</v>
+      </c>
     </row>
-    <row r="60" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -15916,8 +16054,11 @@
       <c r="ED60">
         <v>5</v>
       </c>
+      <c r="EE60">
+        <v>4</v>
+      </c>
     </row>
-    <row r="61" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -16245,8 +16386,11 @@
       <c r="ED61">
         <v>176</v>
       </c>
+      <c r="EE61">
+        <v>172</v>
+      </c>
     </row>
-    <row r="62" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -16532,8 +16676,11 @@
       <c r="ED62">
         <v>1</v>
       </c>
+      <c r="EE62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -16861,8 +17008,11 @@
       <c r="ED64">
         <v>13</v>
       </c>
+      <c r="EE64">
+        <v>13</v>
+      </c>
     </row>
-    <row r="65" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -17154,8 +17304,11 @@
       <c r="ED65">
         <v>0</v>
       </c>
+      <c r="EE65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -17447,8 +17600,11 @@
       <c r="ED66">
         <v>13</v>
       </c>
+      <c r="EE66">
+        <v>13</v>
+      </c>
     </row>
-    <row r="67" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -17776,8 +17932,11 @@
       <c r="ED67">
         <v>67</v>
       </c>
+      <c r="EE67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -18106,8 +18265,11 @@
       <c r="ED68">
         <v>67</v>
       </c>
+      <c r="EE68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -18435,8 +18597,11 @@
       <c r="ED69">
         <v>0</v>
       </c>
+      <c r="EE69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -18728,11 +18893,14 @@
       <c r="ED70">
         <v>0</v>
       </c>
+      <c r="EE70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>119</v>
       </c>
@@ -18910,8 +19078,11 @@
       <c r="ED72">
         <v>11</v>
       </c>
+      <c r="EE72">
+        <v>11</v>
+      </c>
     </row>
-    <row r="73" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>119</v>
       </c>
@@ -19089,8 +19260,11 @@
       <c r="ED73">
         <v>2</v>
       </c>
+      <c r="EE73">
+        <v>2</v>
+      </c>
     </row>
-    <row r="74" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
@@ -19268,8 +19442,11 @@
       <c r="ED74">
         <v>9</v>
       </c>
+      <c r="EE74">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>119</v>
       </c>
@@ -19447,8 +19624,11 @@
       <c r="ED75">
         <v>2</v>
       </c>
+      <c r="EE75">
+        <v>2</v>
+      </c>
     </row>
-    <row r="76" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -19626,8 +19806,11 @@
       <c r="ED76">
         <v>4</v>
       </c>
+      <c r="EE76">
+        <v>4</v>
+      </c>
     </row>
-    <row r="77" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>119</v>
       </c>
@@ -19805,13 +19988,16 @@
       <c r="ED77">
         <v>48</v>
       </c>
+      <c r="EE77">
+        <v>48</v>
+      </c>
     </row>
-    <row r="79" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -20142,8 +20328,11 @@
       <c r="ED80">
         <v>328</v>
       </c>
+      <c r="EE80">
+        <v>328</v>
+      </c>
     </row>
-    <row r="81" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -20475,7 +20664,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -20807,7 +20996,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -21096,8 +21285,11 @@
       <c r="ED83">
         <v>21</v>
       </c>
+      <c r="EE83">
+        <v>21</v>
+      </c>
     </row>
-    <row r="85" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -21428,8 +21620,11 @@
       <c r="ED85">
         <v>125</v>
       </c>
+      <c r="EE85">
+        <v>125</v>
+      </c>
     </row>
-    <row r="86" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -21760,8 +21955,11 @@
       <c r="ED86">
         <v>6</v>
       </c>
+      <c r="EE86">
+        <v>6</v>
+      </c>
     </row>
-    <row r="87" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -22092,8 +22290,11 @@
       <c r="ED87">
         <v>16</v>
       </c>
+      <c r="EE87">
+        <v>16</v>
+      </c>
     </row>
-    <row r="88" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -22424,8 +22625,11 @@
       <c r="ED88">
         <v>262</v>
       </c>
+      <c r="EE88">
+        <v>262</v>
+      </c>
     </row>
-    <row r="89" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -22630,8 +22834,11 @@
       <c r="ED89">
         <v>1</v>
       </c>
+      <c r="EE89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -22962,8 +23169,11 @@
       <c r="ED91">
         <v>82</v>
       </c>
+      <c r="EE91">
+        <v>82</v>
+      </c>
     </row>
-    <row r="92" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -23294,8 +23504,11 @@
       <c r="ED92">
         <v>0</v>
       </c>
+      <c r="EE92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -23614,8 +23827,11 @@
       <c r="ED93">
         <v>193</v>
       </c>
+      <c r="EE93">
+        <v>193</v>
+      </c>
     </row>
-    <row r="94" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -23946,8 +24162,11 @@
       <c r="ED94">
         <v>62</v>
       </c>
+      <c r="EE94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -24236,11 +24455,14 @@
       <c r="ED95">
         <v>14</v>
       </c>
+      <c r="EE95">
+        <v>14</v>
+      </c>
     </row>
-    <row r="96" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>130</v>
       </c>
@@ -24388,8 +24610,11 @@
       <c r="ED97">
         <v>14</v>
       </c>
+      <c r="EE97">
+        <v>14</v>
+      </c>
     </row>
-    <row r="98" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>130</v>
       </c>
@@ -24537,8 +24762,11 @@
       <c r="ED98">
         <v>11</v>
       </c>
+      <c r="EE98">
+        <v>11</v>
+      </c>
     </row>
-    <row r="99" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>130</v>
       </c>
@@ -24686,8 +24914,11 @@
       <c r="ED99">
         <v>55</v>
       </c>
+      <c r="EE99">
+        <v>55</v>
+      </c>
     </row>
-    <row r="100" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
@@ -24835,8 +25066,11 @@
       <c r="ED100">
         <v>1</v>
       </c>
+      <c r="EE100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -25086,8 +25320,11 @@
       <c r="ED102">
         <v>212</v>
       </c>
+      <c r="EE102">
+        <v>213</v>
+      </c>
     </row>
-    <row r="103" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -25337,8 +25574,11 @@
       <c r="ED103">
         <v>140</v>
       </c>
+      <c r="EE103">
+        <v>140</v>
+      </c>
     </row>
-    <row r="104" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -25586,6 +25826,9 @@
         <v>28</v>
       </c>
       <c r="ED104">
+        <v>28</v>
+      </c>
+      <c r="EE104">
         <v>28</v>
       </c>
     </row>
@@ -25602,11 +25845,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:DE11"/>
+  <dimension ref="A2:DF11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DE2" sqref="DE2:DE11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="CO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DG2" sqref="DG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25616,7 +25859,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:109" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:110" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -25944,8 +26187,11 @@
       <c r="DE2" s="9">
         <v>44028</v>
       </c>
+      <c r="DF2" s="9">
+        <v>44029</v>
+      </c>
     </row>
-    <row r="3" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -26273,8 +26519,11 @@
       <c r="DE3">
         <v>1578</v>
       </c>
+      <c r="DF3">
+        <v>1585</v>
+      </c>
     </row>
-    <row r="4" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -26602,8 +26851,11 @@
       <c r="DE4">
         <v>677</v>
       </c>
+      <c r="DF4">
+        <v>683</v>
+      </c>
     </row>
-    <row r="5" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -26931,8 +27183,11 @@
       <c r="DE5">
         <v>521</v>
       </c>
+      <c r="DF5">
+        <v>525</v>
+      </c>
     </row>
-    <row r="6" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -27260,8 +27515,11 @@
       <c r="DE6">
         <v>2262</v>
       </c>
+      <c r="DF6">
+        <v>2266</v>
+      </c>
     </row>
-    <row r="7" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -27589,8 +27847,11 @@
       <c r="DE7">
         <v>1654</v>
       </c>
+      <c r="DF7">
+        <v>1667</v>
+      </c>
     </row>
-    <row r="8" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -27918,8 +28179,11 @@
       <c r="DE8">
         <v>1021</v>
       </c>
+      <c r="DF8">
+        <v>1038</v>
+      </c>
     </row>
-    <row r="9" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -28247,8 +28511,11 @@
       <c r="DE9">
         <v>1596</v>
       </c>
+      <c r="DF9">
+        <v>1613</v>
+      </c>
     </row>
-    <row r="10" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -28576,8 +28843,11 @@
       <c r="DE10">
         <v>1627</v>
       </c>
+      <c r="DF10">
+        <v>1638</v>
+      </c>
     </row>
-    <row r="11" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -28903,6 +29173,9 @@
         <v>179</v>
       </c>
       <c r="DE11">
+        <v>179</v>
+      </c>
+      <c r="DF11">
         <v>179</v>
       </c>
     </row>
@@ -28914,11 +29187,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:CZ17"/>
+  <dimension ref="A2:DA17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CZ14" sqref="CZ14:CZ17"/>
+      <pane xSplit="1" topLeftCell="CH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DB2" sqref="DB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28928,7 +29201,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:104" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:105" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -29239,8 +29512,11 @@
       <c r="CZ2" s="9">
         <v>44028</v>
       </c>
+      <c r="DA2" s="9">
+        <v>44029</v>
+      </c>
     </row>
-    <row r="3" spans="1:104" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:105" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>36</v>
       </c>
@@ -29249,7 +29525,7 @@
       <c r="D3" s="9"/>
       <c r="CP3" s="4"/>
     </row>
-    <row r="4" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -29562,8 +29838,11 @@
       <c r="CZ4">
         <v>11115</v>
       </c>
+      <c r="DA4">
+        <v>11194</v>
+      </c>
     </row>
-    <row r="5" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -29876,8 +30155,11 @@
       <c r="CZ5">
         <v>144</v>
       </c>
+      <c r="DA5">
+        <v>168</v>
+      </c>
     </row>
-    <row r="6" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -30190,8 +30472,11 @@
       <c r="CZ6">
         <v>2290</v>
       </c>
+      <c r="DA6">
+        <v>2873</v>
+      </c>
     </row>
-    <row r="7" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -30504,8 +30789,11 @@
       <c r="CZ7">
         <v>5496</v>
       </c>
+      <c r="DA7">
+        <v>5530</v>
+      </c>
     </row>
-    <row r="8" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -30818,8 +31106,11 @@
       <c r="CZ8">
         <v>171</v>
       </c>
+      <c r="DA8">
+        <v>172</v>
+      </c>
     </row>
-    <row r="9" spans="1:104" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:105" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -31132,8 +31423,11 @@
       <c r="CZ9">
         <v>27</v>
       </c>
+      <c r="DA9">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:104" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:105" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -31442,8 +31736,11 @@
       <c r="CZ10">
         <v>30</v>
       </c>
+      <c r="DA10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="11" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -31756,8 +32053,11 @@
       <c r="CZ11">
         <v>2867</v>
       </c>
+      <c r="DA11">
+        <v>2873</v>
+      </c>
     </row>
-    <row r="12" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -32070,8 +32370,11 @@
       <c r="CZ12">
         <v>90</v>
       </c>
+      <c r="DA12">
+        <v>90</v>
+      </c>
     </row>
-    <row r="13" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -32082,7 +32385,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -32395,8 +32698,11 @@
       <c r="CZ14">
         <v>1355</v>
       </c>
+      <c r="DA14">
+        <v>1374</v>
+      </c>
     </row>
-    <row r="15" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -32709,8 +33015,11 @@
       <c r="CZ15">
         <v>3082</v>
       </c>
+      <c r="DA15">
+        <v>3090</v>
+      </c>
     </row>
-    <row r="16" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -33023,8 +33332,11 @@
       <c r="CZ16">
         <v>6569</v>
       </c>
+      <c r="DA16">
+        <v>6712</v>
+      </c>
     </row>
-    <row r="17" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -33336,6 +33648,9 @@
       </c>
       <c r="CZ17">
         <v>19</v>
+      </c>
+      <c r="DA17">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -33346,11 +33661,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CZ9"/>
+  <dimension ref="A1:DA9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CZ4" sqref="CZ4:CZ8"/>
+      <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DA3" sqref="DA3:DA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33359,7 +33674,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:105" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -33669,14 +33984,17 @@
       <c r="CZ1" s="9">
         <v>44028</v>
       </c>
+      <c r="DA1" s="9">
+        <v>44029</v>
+      </c>
     </row>
-    <row r="2" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -33990,8 +34308,11 @@
       <c r="CZ3">
         <v>577</v>
       </c>
+      <c r="DA3">
+        <v>578</v>
+      </c>
     </row>
-    <row r="4" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -34304,8 +34625,11 @@
       <c r="CZ4">
         <v>8</v>
       </c>
+      <c r="DA4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:104" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:105" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -34618,8 +34942,11 @@
       <c r="CZ5">
         <v>426</v>
       </c>
+      <c r="DA5">
+        <v>426</v>
+      </c>
     </row>
-    <row r="6" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -34932,8 +35259,11 @@
       <c r="CZ6">
         <v>75</v>
       </c>
+      <c r="DA6">
+        <v>76</v>
+      </c>
     </row>
-    <row r="7" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -35246,8 +35576,11 @@
       <c r="CZ7">
         <v>62</v>
       </c>
+      <c r="DA7">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -35560,8 +35893,11 @@
       <c r="CZ8">
         <v>6</v>
       </c>
+      <c r="DA8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:104" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -35603,11 +35939,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CR5"/>
+  <dimension ref="A1:CS5"/>
   <sheetViews>
     <sheetView zoomScale="95" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CR3" sqref="CR3:CR5"/>
+      <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CT1" sqref="CT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35615,7 +35951,7 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:97" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -35901,13 +36237,16 @@
       <c r="CR1" s="9">
         <v>44028</v>
       </c>
+      <c r="CS1" s="9">
+        <v>44029</v>
+      </c>
     </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
@@ -36196,8 +36535,11 @@
       <c r="CR3">
         <v>577</v>
       </c>
+      <c r="CS3">
+        <v>578</v>
+      </c>
     </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>153</v>
       </c>
@@ -36486,8 +36828,11 @@
       <c r="CR4">
         <v>245</v>
       </c>
+      <c r="CS4">
+        <v>245</v>
+      </c>
     </row>
-    <row r="5" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>152</v>
       </c>
@@ -36775,6 +37120,9 @@
       </c>
       <c r="CR5">
         <v>332</v>
+      </c>
+      <c r="CS5">
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -36785,11 +37133,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CR11"/>
+  <dimension ref="A1:CS11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CR3" sqref="CR3:CR11"/>
+      <pane xSplit="1" topLeftCell="CB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CT1" sqref="CT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36797,7 +37145,7 @@
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:97" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -37083,13 +37431,16 @@
       <c r="CR1" s="9">
         <v>44028</v>
       </c>
+      <c r="CS1" s="9">
+        <v>44029</v>
+      </c>
     </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -37378,8 +37729,11 @@
       <c r="CR3">
         <v>577</v>
       </c>
+      <c r="CS3">
+        <v>578</v>
+      </c>
     </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>143</v>
       </c>
@@ -37668,8 +38022,11 @@
       <c r="CR4">
         <v>0</v>
       </c>
+      <c r="CS4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>144</v>
       </c>
@@ -37958,8 +38315,11 @@
       <c r="CR5">
         <v>3</v>
       </c>
+      <c r="CS5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>145</v>
       </c>
@@ -38248,8 +38608,11 @@
       <c r="CR6">
         <v>8</v>
       </c>
+      <c r="CS6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>146</v>
       </c>
@@ -38538,8 +38901,11 @@
       <c r="CR7">
         <v>19</v>
       </c>
+      <c r="CS7">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>147</v>
       </c>
@@ -38828,8 +39194,11 @@
       <c r="CR8">
         <v>66</v>
       </c>
+      <c r="CS8">
+        <v>66</v>
+      </c>
     </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>148</v>
       </c>
@@ -39118,8 +39487,11 @@
       <c r="CR9">
         <v>136</v>
       </c>
+      <c r="CS9">
+        <v>136</v>
+      </c>
     </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>149</v>
       </c>
@@ -39408,8 +39780,11 @@
       <c r="CR10">
         <v>147</v>
       </c>
+      <c r="CS10">
+        <v>147</v>
+      </c>
     </row>
-    <row r="11" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>150</v>
       </c>
@@ -39696,6 +40071,9 @@
         <v>196</v>
       </c>
       <c r="CR11">
+        <v>198</v>
+      </c>
+      <c r="CS11">
         <v>198</v>
       </c>
     </row>
@@ -39707,11 +40085,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:CL13"/>
+  <dimension ref="A2:CM13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CM12" sqref="CM12"/>
+      <pane xSplit="1" topLeftCell="BW1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CK14" sqref="CK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39720,7 +40098,7 @@
     <col min="57" max="57" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:90" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:91" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -39991,8 +40369,11 @@
       <c r="CL2" s="9">
         <v>44028</v>
       </c>
+      <c r="CM2" s="9">
+        <v>44029</v>
+      </c>
     </row>
-    <row r="3" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -40263,8 +40644,11 @@
       <c r="CL3">
         <v>577</v>
       </c>
+      <c r="CM3">
+        <v>578</v>
+      </c>
     </row>
-    <row r="4" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -40535,8 +40919,11 @@
       <c r="CL4">
         <v>62</v>
       </c>
+      <c r="CM4">
+        <v>63</v>
+      </c>
     </row>
-    <row r="5" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -40807,8 +41194,11 @@
       <c r="CL5">
         <v>33</v>
       </c>
+      <c r="CM5">
+        <v>33</v>
+      </c>
     </row>
-    <row r="6" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -41079,8 +41469,11 @@
       <c r="CL6">
         <v>33</v>
       </c>
+      <c r="CM6">
+        <v>33</v>
+      </c>
     </row>
-    <row r="7" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -41351,8 +41744,11 @@
       <c r="CL7">
         <v>84</v>
       </c>
+      <c r="CM7">
+        <v>84</v>
+      </c>
     </row>
-    <row r="8" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -41623,8 +42019,11 @@
       <c r="CL8">
         <v>92</v>
       </c>
+      <c r="CM8">
+        <v>92</v>
+      </c>
     </row>
-    <row r="9" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -41895,8 +42294,11 @@
       <c r="CL9">
         <v>49</v>
       </c>
+      <c r="CM9">
+        <v>49</v>
+      </c>
     </row>
-    <row r="10" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -42167,8 +42569,11 @@
       <c r="CL10">
         <v>85</v>
       </c>
+      <c r="CM10">
+        <v>85</v>
+      </c>
     </row>
-    <row r="11" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -42439,8 +42844,11 @@
       <c r="CL11">
         <v>117</v>
       </c>
+      <c r="CM11">
+        <v>117</v>
+      </c>
     </row>
-    <row r="12" spans="1:90" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:91" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -42711,8 +43119,11 @@
       <c r="CL12">
         <v>21</v>
       </c>
+      <c r="CM12">
+        <v>21</v>
+      </c>
     </row>
-    <row r="13" spans="1:90" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -42981,6 +43392,9 @@
         <v>1</v>
       </c>
       <c r="CL13">
+        <v>1</v>
+      </c>
+      <c r="CM13">
         <v>1</v>
       </c>
     </row>
@@ -42994,8 +43408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI23"/>
   <sheetViews>
-    <sheetView topLeftCell="AO1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="BI5" sqref="BI5"/>
+    <sheetView topLeftCell="AN1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="BJ5" sqref="BJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43006,7 +43420,7 @@
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.25">
       <c r="C1" s="51" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
@@ -43241,8 +43655,8 @@
       <c r="BH5" s="9">
         <v>44028</v>
       </c>
-      <c r="BI5" t="s">
-        <v>129</v>
+      <c r="BI5" s="9">
+        <v>44029</v>
       </c>
     </row>
     <row r="6" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
@@ -43423,6 +43837,9 @@
       <c r="BH6">
         <v>158</v>
       </c>
+      <c r="BI6">
+        <v>159</v>
+      </c>
     </row>
     <row r="7" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -43602,6 +44019,9 @@
       <c r="BH7">
         <v>36</v>
       </c>
+      <c r="BI7">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
@@ -43789,6 +44209,9 @@
       <c r="BH9">
         <v>1</v>
       </c>
+      <c r="BI9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
@@ -43968,6 +44391,9 @@
       <c r="BH10">
         <v>23</v>
       </c>
+      <c r="BI10">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
@@ -44147,6 +44573,9 @@
       <c r="BH11">
         <v>9</v>
       </c>
+      <c r="BI11">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
@@ -44326,6 +44755,9 @@
       <c r="BH12">
         <v>3</v>
       </c>
+      <c r="BI12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
@@ -44510,6 +44942,9 @@
       <c r="BH14">
         <v>1</v>
       </c>
+      <c r="BI14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
@@ -44689,6 +45124,9 @@
       <c r="BH15">
         <v>0</v>
       </c>
+      <c r="BI15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
@@ -44868,8 +45306,11 @@
       <c r="BH16">
         <v>3</v>
       </c>
+      <c r="BI16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:60" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -45047,8 +45488,11 @@
       <c r="BH17">
         <v>12</v>
       </c>
+      <c r="BI17">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:60" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -45226,8 +45670,11 @@
       <c r="BH18">
         <v>3</v>
       </c>
+      <c r="BI18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:60" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -45405,8 +45852,11 @@
       <c r="BH19">
         <v>2</v>
       </c>
+      <c r="BI19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:60" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -45584,8 +46034,11 @@
       <c r="BH20">
         <v>2</v>
       </c>
+      <c r="BI20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:60" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -45763,8 +46216,11 @@
       <c r="BH21">
         <v>6</v>
       </c>
+      <c r="BI21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:60" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:61" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -45942,8 +46398,11 @@
       <c r="BH22">
         <v>4</v>
       </c>
+      <c r="BI22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:61" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>123</v>
       </c>
@@ -46119,6 +46578,9 @@
         <v>3</v>
       </c>
       <c r="BH23">
+        <v>3</v>
+      </c>
+      <c r="BI23">
         <v>3</v>
       </c>
     </row>
@@ -46134,7 +46596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -46151,7 +46613,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -46249,7 +46711,7 @@
         <v>94</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C8" s="28">
         <v>2</v>
@@ -46295,7 +46757,7 @@
         <v>96</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C10" s="28">
         <v>5</v>
@@ -46318,7 +46780,7 @@
         <v>97</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C11" s="28">
         <v>24</v>
@@ -46341,7 +46803,7 @@
         <v>98</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="28">
         <v>2</v>
@@ -46387,7 +46849,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" s="28">
         <v>2</v>
@@ -46410,7 +46872,7 @@
         <v>100</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C15" s="28">
         <v>13</v>
@@ -46433,7 +46895,7 @@
         <v>116</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C16" s="28">
         <v>4</v>
@@ -46456,7 +46918,7 @@
         <v>101</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C17" s="28">
         <v>9</v>
@@ -46479,7 +46941,7 @@
         <v>102</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C18" s="28">
         <v>9</v>
@@ -46502,7 +46964,7 @@
         <v>103</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C19" s="28">
         <v>14</v>
@@ -46525,7 +46987,7 @@
         <v>104</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C20" s="28">
         <v>14</v>
@@ -46571,7 +47033,7 @@
         <v>107</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" s="28">
         <v>28</v>
@@ -46594,7 +47056,7 @@
         <v>108</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="28">
         <v>7</v>
@@ -46617,7 +47079,7 @@
         <v>109</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C24" s="28">
         <v>7</v>
@@ -46640,7 +47102,7 @@
         <v>117</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C25" s="28">
         <v>20</v>
@@ -46663,7 +47125,7 @@
         <v>49</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C26" s="28">
         <v>161</v>
@@ -46672,7 +47134,7 @@
         <v>469</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F26" s="28">
         <v>7</v>
@@ -46687,7 +47149,7 @@
         <v>110</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
@@ -46965,15 +47427,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
Results from July 19, 2020 03:42:03 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/work/WashingtonDC/data.xlsx
+++ b/workflow/python/work/WashingtonDC/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="555" windowWidth="20730" windowHeight="7110" tabRatio="807"/>
+    <workbookView xWindow="0" yWindow="555" windowWidth="20730" windowHeight="7110" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="181">
   <si>
     <t>Testing</t>
   </si>
@@ -576,7 +576,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of July 17, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of July 18, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -1284,11 +1284,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EE119"/>
+  <dimension ref="A1:EF119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="DZ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EG5" sqref="EG5"/>
+      <pane xSplit="2" topLeftCell="EA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="EH3" sqref="EH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,10 +1304,10 @@
     <col min="98" max="102" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="104" max="118" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="128" max="135" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="128" max="136" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1707,8 +1707,11 @@
       <c r="EE1" s="48">
         <v>44029</v>
       </c>
+      <c r="EF1" s="48">
+        <v>44030</v>
+      </c>
     </row>
-    <row r="2" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1732,7 +1735,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2117,8 +2120,11 @@
       <c r="EE3">
         <v>144955</v>
       </c>
+      <c r="EF3">
+        <v>147765</v>
+      </c>
     </row>
-    <row r="4" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2298,8 +2304,11 @@
       <c r="EE4">
         <v>105271</v>
       </c>
+      <c r="EF4">
+        <v>106925</v>
+      </c>
     </row>
-    <row r="5" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2705,8 +2714,11 @@
       <c r="EE5">
         <v>11194</v>
       </c>
+      <c r="EF5">
+        <v>11261</v>
+      </c>
     </row>
-    <row r="6" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3094,8 +3106,11 @@
       <c r="EE6">
         <v>578</v>
       </c>
+      <c r="EF6">
+        <v>578</v>
+      </c>
     </row>
-    <row r="7" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3453,11 +3468,14 @@
       <c r="EE7">
         <v>1877</v>
       </c>
+      <c r="EF7">
+        <v>1886</v>
+      </c>
     </row>
-    <row r="8" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3707,8 +3725,11 @@
       <c r="EE9">
         <v>345</v>
       </c>
+      <c r="EF9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -4060,8 +4081,11 @@
       <c r="EE10">
         <v>84</v>
       </c>
+      <c r="EF10">
+        <v>84</v>
+      </c>
     </row>
-    <row r="11" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4413,8 +4437,11 @@
       <c r="EE11">
         <v>440</v>
       </c>
+      <c r="EF11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4766,8 +4793,11 @@
       <c r="EE12">
         <v>200</v>
       </c>
+      <c r="EF12">
+        <v>192</v>
+      </c>
     </row>
-    <row r="13" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -5119,8 +5149,11 @@
       <c r="EE13">
         <v>240</v>
       </c>
+      <c r="EF13">
+        <v>248</v>
+      </c>
     </row>
-    <row r="14" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -5334,8 +5367,11 @@
       <c r="EE14">
         <v>88</v>
       </c>
+      <c r="EF14">
+        <v>91</v>
+      </c>
     </row>
-    <row r="15" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -5519,8 +5555,11 @@
       <c r="EE15">
         <v>17</v>
       </c>
+      <c r="EF15">
+        <v>17</v>
+      </c>
     </row>
-    <row r="16" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -5734,8 +5773,11 @@
       <c r="EE16">
         <v>1972</v>
       </c>
+      <c r="EF16">
+        <v>1902</v>
+      </c>
     </row>
-    <row r="17" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -5949,13 +5991,16 @@
       <c r="EE17" s="23">
         <v>0.79</v>
       </c>
+      <c r="EF17" s="23">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="19" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -5963,7 +6008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -6315,8 +6360,11 @@
       <c r="EE21">
         <v>120</v>
       </c>
+      <c r="EF21">
+        <v>120</v>
+      </c>
     </row>
-    <row r="22" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -6614,8 +6662,11 @@
       <c r="EE22">
         <v>5</v>
       </c>
+      <c r="EF22">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -6913,8 +6964,11 @@
       <c r="EE23">
         <v>115</v>
       </c>
+      <c r="EF23">
+        <v>115</v>
+      </c>
     </row>
-    <row r="24" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -7257,8 +7311,11 @@
       <c r="EE24">
         <v>70</v>
       </c>
+      <c r="EF24">
+        <v>68</v>
+      </c>
     </row>
-    <row r="25" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -7601,8 +7658,11 @@
       <c r="EE25">
         <v>75</v>
       </c>
+      <c r="EF25">
+        <v>73</v>
+      </c>
     </row>
-    <row r="26" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -7945,13 +8005,16 @@
       <c r="EE26">
         <v>1716</v>
       </c>
+      <c r="EF26">
+        <v>1721</v>
+      </c>
     </row>
-    <row r="28" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:136" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -8303,8 +8366,11 @@
       <c r="EE29">
         <v>179</v>
       </c>
+      <c r="EF29">
+        <v>179</v>
+      </c>
     </row>
-    <row r="30" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -8602,8 +8668,11 @@
       <c r="EE30">
         <v>42</v>
       </c>
+      <c r="EF30">
+        <v>42</v>
+      </c>
     </row>
-    <row r="31" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -8901,8 +8970,11 @@
       <c r="EE31">
         <v>137</v>
       </c>
+      <c r="EF31">
+        <v>137</v>
+      </c>
     </row>
-    <row r="32" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -9245,8 +9317,11 @@
       <c r="EE32">
         <v>130</v>
       </c>
+      <c r="EF32">
+        <v>127</v>
+      </c>
     </row>
-    <row r="33" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -9589,8 +9664,11 @@
       <c r="EE33">
         <v>175</v>
       </c>
+      <c r="EF33">
+        <v>169</v>
+      </c>
     </row>
-    <row r="34" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -9933,8 +10011,11 @@
       <c r="EE34">
         <v>1413</v>
       </c>
+      <c r="EF34">
+        <v>1416</v>
+      </c>
     </row>
-    <row r="35" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -10058,13 +10139,16 @@
       <c r="EE35">
         <v>1</v>
       </c>
+      <c r="EF35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:136" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -10404,8 +10488,11 @@
       <c r="EE38">
         <v>88</v>
       </c>
+      <c r="EF38">
+        <v>88</v>
+      </c>
     </row>
-    <row r="39" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -10697,8 +10784,11 @@
       <c r="EE39">
         <v>2</v>
       </c>
+      <c r="EF39">
+        <v>2</v>
+      </c>
     </row>
-    <row r="40" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -10990,8 +11080,11 @@
       <c r="EE40">
         <v>85</v>
       </c>
+      <c r="EF40">
+        <v>85</v>
+      </c>
     </row>
-    <row r="41" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -11328,8 +11421,11 @@
       <c r="EE41">
         <v>0</v>
       </c>
+      <c r="EF41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -11663,8 +11759,11 @@
       <c r="EE42">
         <v>2</v>
       </c>
+      <c r="EF42">
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -12004,8 +12103,11 @@
       <c r="EE43">
         <v>296</v>
       </c>
+      <c r="EF43">
+        <v>296</v>
+      </c>
     </row>
-    <row r="44" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -12279,16 +12381,19 @@
       <c r="EE44">
         <v>1</v>
       </c>
+      <c r="EF44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:136" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -12634,8 +12739,11 @@
       <c r="EE47">
         <v>207</v>
       </c>
+      <c r="EF47">
+        <v>207</v>
+      </c>
     </row>
-    <row r="48" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -12933,8 +13041,11 @@
       <c r="EE48">
         <v>0</v>
       </c>
+      <c r="EF48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -13232,8 +13343,11 @@
       <c r="EE49">
         <v>200</v>
       </c>
+      <c r="EF49">
+        <v>200</v>
+      </c>
     </row>
-    <row r="50" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -13576,8 +13690,11 @@
       <c r="EE50">
         <v>65</v>
       </c>
+      <c r="EF50">
+        <v>71</v>
+      </c>
     </row>
-    <row r="51" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -13875,8 +13992,11 @@
       <c r="EE51">
         <v>65</v>
       </c>
+      <c r="EF51">
+        <v>65</v>
+      </c>
     </row>
-    <row r="52" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -14171,8 +14291,11 @@
       <c r="EE52">
         <v>1216</v>
       </c>
+      <c r="EF52">
+        <v>1212</v>
+      </c>
     </row>
-    <row r="53" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -14461,16 +14584,19 @@
       <c r="EE53">
         <v>1</v>
       </c>
+      <c r="EF53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:136" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -14801,8 +14927,11 @@
       <c r="EE56">
         <v>35</v>
       </c>
+      <c r="EF56">
+        <v>35</v>
+      </c>
     </row>
-    <row r="57" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -15097,8 +15226,11 @@
       <c r="EE57">
         <v>2</v>
       </c>
+      <c r="EF57">
+        <v>2</v>
+      </c>
     </row>
-    <row r="58" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -15393,8 +15525,11 @@
       <c r="EE58">
         <v>32</v>
       </c>
+      <c r="EF58">
+        <v>32</v>
+      </c>
     </row>
-    <row r="59" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -15725,8 +15860,11 @@
       <c r="EE59">
         <v>2</v>
       </c>
+      <c r="EF59">
+        <v>2</v>
+      </c>
     </row>
-    <row r="60" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -16057,8 +16195,11 @@
       <c r="EE60">
         <v>4</v>
       </c>
+      <c r="EF60">
+        <v>4</v>
+      </c>
     </row>
-    <row r="61" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -16389,8 +16530,11 @@
       <c r="EE61">
         <v>172</v>
       </c>
+      <c r="EF61">
+        <v>176</v>
+      </c>
     </row>
-    <row r="62" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -16679,8 +16823,11 @@
       <c r="EE62">
         <v>1</v>
       </c>
+      <c r="EF62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -17011,8 +17158,11 @@
       <c r="EE64">
         <v>13</v>
       </c>
+      <c r="EF64">
+        <v>13</v>
+      </c>
     </row>
-    <row r="65" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -17307,8 +17457,11 @@
       <c r="EE65">
         <v>0</v>
       </c>
+      <c r="EF65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -17603,8 +17756,11 @@
       <c r="EE66">
         <v>13</v>
       </c>
+      <c r="EF66">
+        <v>13</v>
+      </c>
     </row>
-    <row r="67" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -17935,8 +18091,11 @@
       <c r="EE67">
         <v>0</v>
       </c>
+      <c r="EF67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -18268,8 +18427,11 @@
       <c r="EE68">
         <v>0</v>
       </c>
+      <c r="EF68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -18600,8 +18762,11 @@
       <c r="EE69">
         <v>0</v>
       </c>
+      <c r="EF69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -18896,11 +19061,14 @@
       <c r="EE70">
         <v>0</v>
       </c>
+      <c r="EF70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>119</v>
       </c>
@@ -19081,8 +19249,11 @@
       <c r="EE72">
         <v>11</v>
       </c>
+      <c r="EF72">
+        <v>11</v>
+      </c>
     </row>
-    <row r="73" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>119</v>
       </c>
@@ -19263,8 +19434,11 @@
       <c r="EE73">
         <v>2</v>
       </c>
+      <c r="EF73">
+        <v>2</v>
+      </c>
     </row>
-    <row r="74" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
@@ -19445,8 +19619,11 @@
       <c r="EE74">
         <v>9</v>
       </c>
+      <c r="EF74">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>119</v>
       </c>
@@ -19627,8 +19804,11 @@
       <c r="EE75">
         <v>2</v>
       </c>
+      <c r="EF75">
+        <v>2</v>
+      </c>
     </row>
-    <row r="76" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -19809,8 +19989,11 @@
       <c r="EE76">
         <v>4</v>
       </c>
+      <c r="EF76">
+        <v>4</v>
+      </c>
     </row>
-    <row r="77" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>119</v>
       </c>
@@ -19991,13 +20174,16 @@
       <c r="EE77">
         <v>48</v>
       </c>
+      <c r="EF77">
+        <v>48</v>
+      </c>
     </row>
-    <row r="79" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:136" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -20331,8 +20517,11 @@
       <c r="EE80">
         <v>328</v>
       </c>
+      <c r="EF80">
+        <v>329</v>
+      </c>
     </row>
-    <row r="81" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -20664,7 +20853,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -20996,7 +21185,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -21288,8 +21477,11 @@
       <c r="EE83">
         <v>21</v>
       </c>
+      <c r="EF83">
+        <v>21</v>
+      </c>
     </row>
-    <row r="85" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -21623,8 +21815,11 @@
       <c r="EE85">
         <v>125</v>
       </c>
+      <c r="EF85">
+        <v>125</v>
+      </c>
     </row>
-    <row r="86" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -21958,8 +22153,11 @@
       <c r="EE86">
         <v>6</v>
       </c>
+      <c r="EF86">
+        <v>6</v>
+      </c>
     </row>
-    <row r="87" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -22293,8 +22491,11 @@
       <c r="EE87">
         <v>16</v>
       </c>
+      <c r="EF87">
+        <v>16</v>
+      </c>
     </row>
-    <row r="88" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -22628,8 +22829,11 @@
       <c r="EE88">
         <v>262</v>
       </c>
+      <c r="EF88">
+        <v>262</v>
+      </c>
     </row>
-    <row r="89" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -22837,8 +23041,11 @@
       <c r="EE89">
         <v>1</v>
       </c>
+      <c r="EF89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -23172,8 +23379,11 @@
       <c r="EE91">
         <v>82</v>
       </c>
+      <c r="EF91">
+        <v>82</v>
+      </c>
     </row>
-    <row r="92" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -23507,8 +23717,11 @@
       <c r="EE92">
         <v>0</v>
       </c>
+      <c r="EF92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -23830,8 +24043,11 @@
       <c r="EE93">
         <v>193</v>
       </c>
+      <c r="EF93">
+        <v>191</v>
+      </c>
     </row>
-    <row r="94" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -24165,8 +24381,11 @@
       <c r="EE94">
         <v>62</v>
       </c>
+      <c r="EF94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -24458,11 +24677,14 @@
       <c r="EE95">
         <v>14</v>
       </c>
+      <c r="EF95">
+        <v>14</v>
+      </c>
     </row>
-    <row r="96" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>130</v>
       </c>
@@ -24613,8 +24835,11 @@
       <c r="EE97">
         <v>14</v>
       </c>
+      <c r="EF97">
+        <v>14</v>
+      </c>
     </row>
-    <row r="98" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>130</v>
       </c>
@@ -24765,8 +24990,11 @@
       <c r="EE98">
         <v>11</v>
       </c>
+      <c r="EF98">
+        <v>11</v>
+      </c>
     </row>
-    <row r="99" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>130</v>
       </c>
@@ -24917,8 +25145,11 @@
       <c r="EE99">
         <v>55</v>
       </c>
+      <c r="EF99">
+        <v>55</v>
+      </c>
     </row>
-    <row r="100" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
@@ -25069,8 +25300,11 @@
       <c r="EE100">
         <v>1</v>
       </c>
+      <c r="EF100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -25323,8 +25557,11 @@
       <c r="EE102">
         <v>213</v>
       </c>
+      <c r="EF102">
+        <v>213</v>
+      </c>
     </row>
-    <row r="103" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -25577,8 +25814,11 @@
       <c r="EE103">
         <v>140</v>
       </c>
+      <c r="EF103">
+        <v>140</v>
+      </c>
     </row>
-    <row r="104" spans="1:135" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -25829,6 +26069,9 @@
         <v>28</v>
       </c>
       <c r="EE104">
+        <v>28</v>
+      </c>
+      <c r="EF104">
         <v>28</v>
       </c>
     </row>
@@ -25845,11 +26088,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:DF11"/>
+  <dimension ref="A2:DG11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DG2" sqref="DG2"/>
+      <selection pane="topRight" activeCell="DH2" sqref="DH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25859,7 +26102,7 @@
     <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:110" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:111" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -26190,8 +26433,11 @@
       <c r="DF2" s="9">
         <v>44029</v>
       </c>
+      <c r="DG2" s="9">
+        <v>44030</v>
+      </c>
     </row>
-    <row r="3" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -26522,8 +26768,11 @@
       <c r="DF3">
         <v>1585</v>
       </c>
+      <c r="DG3">
+        <v>1592</v>
+      </c>
     </row>
-    <row r="4" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -26854,8 +27103,11 @@
       <c r="DF4">
         <v>683</v>
       </c>
+      <c r="DG4">
+        <v>692</v>
+      </c>
     </row>
-    <row r="5" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -27186,8 +27438,11 @@
       <c r="DF5">
         <v>525</v>
       </c>
+      <c r="DG5">
+        <v>532</v>
+      </c>
     </row>
-    <row r="6" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -27518,8 +27773,11 @@
       <c r="DF6">
         <v>2266</v>
       </c>
+      <c r="DG6">
+        <v>2273</v>
+      </c>
     </row>
-    <row r="7" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -27850,8 +28108,11 @@
       <c r="DF7">
         <v>1667</v>
       </c>
+      <c r="DG7">
+        <v>1676</v>
+      </c>
     </row>
-    <row r="8" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -28182,8 +28443,11 @@
       <c r="DF8">
         <v>1038</v>
       </c>
+      <c r="DG8">
+        <v>1053</v>
+      </c>
     </row>
-    <row r="9" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -28514,8 +28778,11 @@
       <c r="DF9">
         <v>1613</v>
       </c>
+      <c r="DG9">
+        <v>1623</v>
+      </c>
     </row>
-    <row r="10" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -28846,8 +29113,11 @@
       <c r="DF10">
         <v>1638</v>
       </c>
+      <c r="DG10">
+        <v>1641</v>
+      </c>
     </row>
-    <row r="11" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -29176,6 +29446,9 @@
         <v>179</v>
       </c>
       <c r="DF11">
+        <v>179</v>
+      </c>
+      <c r="DG11">
         <v>179</v>
       </c>
     </row>
@@ -29187,11 +29460,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:DA17"/>
+  <dimension ref="A2:DB17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DB2" sqref="DB2"/>
+      <selection pane="topRight" activeCell="DC2" sqref="DC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29201,7 +29474,7 @@
     <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:105" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:106" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -29515,8 +29788,11 @@
       <c r="DA2" s="9">
         <v>44029</v>
       </c>
+      <c r="DB2" s="9">
+        <v>44030</v>
+      </c>
     </row>
-    <row r="3" spans="1:105" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:106" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>36</v>
       </c>
@@ -29525,7 +29801,7 @@
       <c r="D3" s="9"/>
       <c r="CP3" s="4"/>
     </row>
-    <row r="4" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -29841,8 +30117,11 @@
       <c r="DA4">
         <v>11194</v>
       </c>
+      <c r="DB4">
+        <v>11261</v>
+      </c>
     </row>
-    <row r="5" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -30158,8 +30437,11 @@
       <c r="DA5">
         <v>168</v>
       </c>
+      <c r="DB5">
+        <v>200</v>
+      </c>
     </row>
-    <row r="6" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -30475,8 +30757,11 @@
       <c r="DA6">
         <v>2873</v>
       </c>
+      <c r="DB6">
+        <v>2308</v>
+      </c>
     </row>
-    <row r="7" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -30792,8 +31077,11 @@
       <c r="DA7">
         <v>5530</v>
       </c>
+      <c r="DB7">
+        <v>5550</v>
+      </c>
     </row>
-    <row r="8" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -31109,8 +31397,11 @@
       <c r="DA8">
         <v>172</v>
       </c>
+      <c r="DB8">
+        <v>175</v>
+      </c>
     </row>
-    <row r="9" spans="1:105" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:106" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -31426,8 +31717,11 @@
       <c r="DA9">
         <v>27</v>
       </c>
+      <c r="DB9">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:105" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:106" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -31739,8 +32033,11 @@
       <c r="DA10">
         <v>30</v>
       </c>
+      <c r="DB10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="11" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -32056,8 +32353,11 @@
       <c r="DA11">
         <v>2873</v>
       </c>
+      <c r="DB11">
+        <v>2882</v>
+      </c>
     </row>
-    <row r="12" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -32373,8 +32673,11 @@
       <c r="DA12">
         <v>90</v>
       </c>
+      <c r="DB12">
+        <v>89</v>
+      </c>
     </row>
-    <row r="13" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -32385,7 +32688,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -32701,8 +33004,11 @@
       <c r="DA14">
         <v>1374</v>
       </c>
+      <c r="DB14">
+        <v>1408</v>
+      </c>
     </row>
-    <row r="15" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -33018,8 +33324,11 @@
       <c r="DA15">
         <v>3090</v>
       </c>
+      <c r="DB15">
+        <v>3096</v>
+      </c>
     </row>
-    <row r="16" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -33335,8 +33644,11 @@
       <c r="DA16">
         <v>6712</v>
       </c>
+      <c r="DB16">
+        <v>6740</v>
+      </c>
     </row>
-    <row r="17" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -33651,6 +33963,9 @@
       </c>
       <c r="DA17">
         <v>18</v>
+      </c>
+      <c r="DB17">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -33661,11 +33976,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DA9"/>
+  <dimension ref="A1:DB9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DA3" sqref="DA3:DA8"/>
+      <selection pane="topRight" activeCell="DC1" sqref="DC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33674,7 +33989,7 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:105" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:106" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -33987,14 +34302,17 @@
       <c r="DA1" s="9">
         <v>44029</v>
       </c>
+      <c r="DB1" s="9">
+        <v>44030</v>
+      </c>
     </row>
-    <row r="2" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -34311,8 +34629,11 @@
       <c r="DA3">
         <v>578</v>
       </c>
+      <c r="DB3">
+        <v>578</v>
+      </c>
     </row>
-    <row r="4" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -34628,8 +34949,11 @@
       <c r="DA4">
         <v>8</v>
       </c>
+      <c r="DB4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:105" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:106" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -34945,8 +35269,11 @@
       <c r="DA5">
         <v>426</v>
       </c>
+      <c r="DB5">
+        <v>426</v>
+      </c>
     </row>
-    <row r="6" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -35262,8 +35589,11 @@
       <c r="DA6">
         <v>76</v>
       </c>
+      <c r="DB6">
+        <v>76</v>
+      </c>
     </row>
-    <row r="7" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -35579,8 +35909,11 @@
       <c r="DA7">
         <v>62</v>
       </c>
+      <c r="DB7">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -35896,8 +36229,11 @@
       <c r="DA8">
         <v>6</v>
       </c>
+      <c r="DB8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:105" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -35939,11 +36275,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CS5"/>
+  <dimension ref="A1:CT5"/>
   <sheetViews>
     <sheetView zoomScale="95" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CT1" sqref="CT1"/>
+      <selection pane="topRight" activeCell="CU1" sqref="CU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35951,7 +36287,7 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -36240,13 +36576,16 @@
       <c r="CS1" s="9">
         <v>44029</v>
       </c>
+      <c r="CT1" s="9">
+        <v>44030</v>
+      </c>
     </row>
-    <row r="2" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
@@ -36538,8 +36877,11 @@
       <c r="CS3">
         <v>578</v>
       </c>
+      <c r="CT3">
+        <v>578</v>
+      </c>
     </row>
-    <row r="4" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>153</v>
       </c>
@@ -36831,8 +37173,11 @@
       <c r="CS4">
         <v>245</v>
       </c>
+      <c r="CT4">
+        <v>245</v>
+      </c>
     </row>
-    <row r="5" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>152</v>
       </c>
@@ -37122,6 +37467,9 @@
         <v>332</v>
       </c>
       <c r="CS5">
+        <v>333</v>
+      </c>
+      <c r="CT5">
         <v>333</v>
       </c>
     </row>
@@ -37133,11 +37481,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CS11"/>
+  <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CT1" sqref="CT1"/>
+      <selection pane="topRight" activeCell="CU1" sqref="CU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37145,7 +37493,7 @@
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -37434,13 +37782,16 @@
       <c r="CS1" s="9">
         <v>44029</v>
       </c>
+      <c r="CT1" s="9">
+        <v>44030</v>
+      </c>
     </row>
-    <row r="2" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -37732,8 +38083,11 @@
       <c r="CS3">
         <v>578</v>
       </c>
+      <c r="CT3">
+        <v>578</v>
+      </c>
     </row>
-    <row r="4" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>143</v>
       </c>
@@ -38025,8 +38379,11 @@
       <c r="CS4">
         <v>0</v>
       </c>
+      <c r="CT4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>144</v>
       </c>
@@ -38318,8 +38675,11 @@
       <c r="CS5">
         <v>3</v>
       </c>
+      <c r="CT5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>145</v>
       </c>
@@ -38611,8 +38971,11 @@
       <c r="CS6">
         <v>8</v>
       </c>
+      <c r="CT6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>146</v>
       </c>
@@ -38904,8 +39267,11 @@
       <c r="CS7">
         <v>20</v>
       </c>
+      <c r="CT7">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>147</v>
       </c>
@@ -39197,8 +39563,11 @@
       <c r="CS8">
         <v>66</v>
       </c>
+      <c r="CT8">
+        <v>66</v>
+      </c>
     </row>
-    <row r="9" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>148</v>
       </c>
@@ -39490,8 +39859,11 @@
       <c r="CS9">
         <v>136</v>
       </c>
+      <c r="CT9">
+        <v>136</v>
+      </c>
     </row>
-    <row r="10" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>149</v>
       </c>
@@ -39783,8 +40155,11 @@
       <c r="CS10">
         <v>147</v>
       </c>
+      <c r="CT10">
+        <v>147</v>
+      </c>
     </row>
-    <row r="11" spans="1:97" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>150</v>
       </c>
@@ -40074,6 +40449,9 @@
         <v>198</v>
       </c>
       <c r="CS11">
+        <v>198</v>
+      </c>
+      <c r="CT11">
         <v>198</v>
       </c>
     </row>
@@ -40085,11 +40463,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:CM13"/>
+  <dimension ref="A2:CN13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CK14" sqref="CK14"/>
+      <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CN16" sqref="CN16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40098,7 +40476,7 @@
     <col min="57" max="57" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:91" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:92" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -40372,8 +40750,11 @@
       <c r="CM2" s="9">
         <v>44029</v>
       </c>
+      <c r="CN2" s="9">
+        <v>44030</v>
+      </c>
     </row>
-    <row r="3" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -40647,8 +41028,11 @@
       <c r="CM3">
         <v>578</v>
       </c>
+      <c r="CN3">
+        <v>578</v>
+      </c>
     </row>
-    <row r="4" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -40922,8 +41306,11 @@
       <c r="CM4">
         <v>63</v>
       </c>
+      <c r="CN4">
+        <v>63</v>
+      </c>
     </row>
-    <row r="5" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -41197,8 +41584,11 @@
       <c r="CM5">
         <v>33</v>
       </c>
+      <c r="CN5">
+        <v>33</v>
+      </c>
     </row>
-    <row r="6" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -41472,8 +41862,11 @@
       <c r="CM6">
         <v>33</v>
       </c>
+      <c r="CN6">
+        <v>33</v>
+      </c>
     </row>
-    <row r="7" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -41747,8 +42140,11 @@
       <c r="CM7">
         <v>84</v>
       </c>
+      <c r="CN7">
+        <v>84</v>
+      </c>
     </row>
-    <row r="8" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -42022,8 +42418,11 @@
       <c r="CM8">
         <v>92</v>
       </c>
+      <c r="CN8">
+        <v>92</v>
+      </c>
     </row>
-    <row r="9" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -42297,8 +42696,11 @@
       <c r="CM9">
         <v>49</v>
       </c>
+      <c r="CN9">
+        <v>49</v>
+      </c>
     </row>
-    <row r="10" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -42572,8 +42974,11 @@
       <c r="CM10">
         <v>85</v>
       </c>
+      <c r="CN10">
+        <v>85</v>
+      </c>
     </row>
-    <row r="11" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -42847,8 +43252,11 @@
       <c r="CM11">
         <v>117</v>
       </c>
+      <c r="CN11">
+        <v>117</v>
+      </c>
     </row>
-    <row r="12" spans="1:91" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:92" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -43122,8 +43530,11 @@
       <c r="CM12">
         <v>21</v>
       </c>
+      <c r="CN12">
+        <v>21</v>
+      </c>
     </row>
-    <row r="13" spans="1:91" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -43395,6 +43806,9 @@
         <v>1</v>
       </c>
       <c r="CM13">
+        <v>1</v>
+      </c>
+      <c r="CN13">
         <v>1</v>
       </c>
     </row>
@@ -43406,10 +43820,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BI23"/>
+  <dimension ref="A1:BK23"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="BJ5" sqref="BJ5"/>
+    <sheetView topLeftCell="AU1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="BK5" sqref="BK5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43418,7 +43832,7 @@
     <col min="42" max="45" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="C1" s="51" t="s">
         <v>180</v>
       </c>
@@ -43435,7 +43849,7 @@
       <c r="N1" s="51"/>
       <c r="O1" s="51"/>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
@@ -43450,7 +43864,7 @@
       <c r="N2" s="51"/>
       <c r="O2" s="51"/>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="E3" s="51"/>
@@ -43465,7 +43879,7 @@
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
     </row>
-    <row r="4" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -43480,7 +43894,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -43658,8 +44072,14 @@
       <c r="BI5" s="9">
         <v>44029</v>
       </c>
+      <c r="BJ5" s="9">
+        <v>44030</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="6" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>120</v>
       </c>
@@ -43840,8 +44260,11 @@
       <c r="BI6">
         <v>159</v>
       </c>
+      <c r="BJ6">
+        <v>159</v>
+      </c>
     </row>
-    <row r="7" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -44022,8 +44445,11 @@
       <c r="BI7">
         <v>36</v>
       </c>
+      <c r="BJ7">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
@@ -44031,7 +44457,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -44212,8 +44638,11 @@
       <c r="BI9">
         <v>1</v>
       </c>
+      <c r="BJ9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>121</v>
       </c>
@@ -44394,8 +44823,11 @@
       <c r="BI10">
         <v>23</v>
       </c>
+      <c r="BJ10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>122</v>
       </c>
@@ -44576,8 +45008,11 @@
       <c r="BI11">
         <v>9</v>
       </c>
+      <c r="BJ11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -44758,13 +45193,16 @@
       <c r="BI12">
         <v>3</v>
       </c>
+      <c r="BJ12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -44945,8 +45383,11 @@
       <c r="BI14">
         <v>1</v>
       </c>
+      <c r="BJ14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -45127,8 +45568,11 @@
       <c r="BI15">
         <v>0</v>
       </c>
+      <c r="BJ15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -45309,8 +45753,11 @@
       <c r="BI16">
         <v>3</v>
       </c>
+      <c r="BJ16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -45491,8 +45938,11 @@
       <c r="BI17">
         <v>12</v>
       </c>
+      <c r="BJ17">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -45673,8 +46123,11 @@
       <c r="BI18">
         <v>3</v>
       </c>
+      <c r="BJ18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -45855,8 +46308,11 @@
       <c r="BI19">
         <v>2</v>
       </c>
+      <c r="BJ19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -46037,8 +46493,11 @@
       <c r="BI20">
         <v>2</v>
       </c>
+      <c r="BJ20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:61" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -46219,8 +46678,11 @@
       <c r="BI21">
         <v>6</v>
       </c>
+      <c r="BJ21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:61" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:62" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -46401,8 +46863,11 @@
       <c r="BI22">
         <v>4</v>
       </c>
+      <c r="BJ22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:61" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:62" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>123</v>
       </c>
@@ -46581,6 +47046,9 @@
         <v>3</v>
       </c>
       <c r="BI23">
+        <v>3</v>
+      </c>
+      <c r="BJ23">
         <v>3</v>
       </c>
     </row>
@@ -47180,6 +47648,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -47188,7 +47662,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -47391,13 +47865,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -47405,7 +47890,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -47422,21 +47907,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Results from July 20, 2020 05:28:54 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/work/WashingtonDC/data.xlsx
+++ b/workflow/python/work/WashingtonDC/data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{D8A8C525-9AD6-4328-8A76-D2E05990132D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F2B61730-33A5-4499-809C-5C479CBF2B0B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="555" windowWidth="20730" windowHeight="7110" tabRatio="807"/>
+    <workbookView xWindow="0" yWindow="552" windowWidth="23040" windowHeight="7116" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
     <sheet name="Community Cases Tested By OCME" sheetId="7" r:id="rId8"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -576,7 +582,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of July 18, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of July 19, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -604,7 +610,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -941,7 +947,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA38EB-A376-4FCE-9F96-95B919EB7113}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1276,38 +1282,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EF119"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:EG119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="EA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EH3" sqref="EH3"/>
+      <selection pane="topRight" activeCell="EH1" sqref="EH1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="40" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="80" max="88" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="98" max="102" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="104" max="118" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="128" max="136" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="40" max="57" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="88" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="98" max="102" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="104" max="118" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="128" max="137" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:137" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1710,8 +1716,11 @@
       <c r="EF1" s="48">
         <v>44030</v>
       </c>
+      <c r="EG1" s="48">
+        <v>44031</v>
+      </c>
     </row>
-    <row r="2" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:137" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1735,7 +1744,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2123,8 +2132,11 @@
       <c r="EF3">
         <v>147765</v>
       </c>
+      <c r="EG3">
+        <v>151740</v>
+      </c>
     </row>
-    <row r="4" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2307,8 +2319,11 @@
       <c r="EF4">
         <v>106925</v>
       </c>
+      <c r="EG4">
+        <v>109067</v>
+      </c>
     </row>
-    <row r="5" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2717,8 +2732,11 @@
       <c r="EF5">
         <v>11261</v>
       </c>
+      <c r="EG5">
+        <v>11339</v>
+      </c>
     </row>
-    <row r="6" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3109,8 +3127,11 @@
       <c r="EF6">
         <v>578</v>
       </c>
+      <c r="EG6">
+        <v>579</v>
+      </c>
     </row>
-    <row r="7" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3471,11 +3492,14 @@
       <c r="EF7">
         <v>1886</v>
       </c>
+      <c r="EG7">
+        <v>1909</v>
+      </c>
     </row>
-    <row r="8" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3728,8 +3752,11 @@
       <c r="EF9">
         <v>345</v>
       </c>
+      <c r="EG9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -4084,8 +4111,11 @@
       <c r="EF10">
         <v>84</v>
       </c>
+      <c r="EG10">
+        <v>74</v>
+      </c>
     </row>
-    <row r="11" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4440,8 +4470,11 @@
       <c r="EF11">
         <v>440</v>
       </c>
+      <c r="EG11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4796,8 +4829,11 @@
       <c r="EF12">
         <v>192</v>
       </c>
+      <c r="EG12">
+        <v>187</v>
+      </c>
     </row>
-    <row r="13" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -5152,8 +5188,11 @@
       <c r="EF13">
         <v>248</v>
       </c>
+      <c r="EG13">
+        <v>253</v>
+      </c>
     </row>
-    <row r="14" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -5370,8 +5409,11 @@
       <c r="EF14">
         <v>91</v>
       </c>
+      <c r="EG14">
+        <v>83</v>
+      </c>
     </row>
-    <row r="15" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -5558,8 +5600,11 @@
       <c r="EF15">
         <v>17</v>
       </c>
+      <c r="EG15">
+        <v>19</v>
+      </c>
     </row>
-    <row r="16" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -5776,8 +5821,11 @@
       <c r="EF16">
         <v>1902</v>
       </c>
+      <c r="EG16">
+        <v>1863</v>
+      </c>
     </row>
-    <row r="17" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -5994,13 +6042,16 @@
       <c r="EF17" s="23">
         <v>0.76</v>
       </c>
+      <c r="EG17" s="23">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="19" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:137" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -6008,7 +6059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -6363,8 +6414,11 @@
       <c r="EF21">
         <v>120</v>
       </c>
+      <c r="EG21">
+        <v>120</v>
+      </c>
     </row>
-    <row r="22" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -6665,8 +6719,11 @@
       <c r="EF22">
         <v>5</v>
       </c>
+      <c r="EG22">
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -6967,8 +7024,11 @@
       <c r="EF23">
         <v>115</v>
       </c>
+      <c r="EG23">
+        <v>115</v>
+      </c>
     </row>
-    <row r="24" spans="1:136" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -7314,8 +7374,11 @@
       <c r="EF24">
         <v>68</v>
       </c>
+      <c r="EG24">
+        <v>68</v>
+      </c>
     </row>
-    <row r="25" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -7661,8 +7724,11 @@
       <c r="EF25">
         <v>73</v>
       </c>
+      <c r="EG25">
+        <v>73</v>
+      </c>
     </row>
-    <row r="26" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -8008,13 +8074,16 @@
       <c r="EF26">
         <v>1721</v>
       </c>
+      <c r="EG26">
+        <v>1721</v>
+      </c>
     </row>
-    <row r="28" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:137" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -8369,8 +8438,11 @@
       <c r="EF29">
         <v>179</v>
       </c>
+      <c r="EG29">
+        <v>179</v>
+      </c>
     </row>
-    <row r="30" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -8671,8 +8743,11 @@
       <c r="EF30">
         <v>42</v>
       </c>
+      <c r="EG30">
+        <v>42</v>
+      </c>
     </row>
-    <row r="31" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -8973,8 +9048,11 @@
       <c r="EF31">
         <v>137</v>
       </c>
+      <c r="EG31">
+        <v>137</v>
+      </c>
     </row>
-    <row r="32" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -9320,8 +9398,11 @@
       <c r="EF32">
         <v>127</v>
       </c>
+      <c r="EG32">
+        <v>127</v>
+      </c>
     </row>
-    <row r="33" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -9667,8 +9748,11 @@
       <c r="EF33">
         <v>169</v>
       </c>
+      <c r="EG33">
+        <v>169</v>
+      </c>
     </row>
-    <row r="34" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -10014,8 +10098,11 @@
       <c r="EF34">
         <v>1416</v>
       </c>
+      <c r="EG34">
+        <v>1416</v>
+      </c>
     </row>
-    <row r="35" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -10142,13 +10229,16 @@
       <c r="EF35">
         <v>1</v>
       </c>
+      <c r="EG35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:137" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -10491,8 +10581,11 @@
       <c r="EF38">
         <v>88</v>
       </c>
+      <c r="EG38">
+        <v>88</v>
+      </c>
     </row>
-    <row r="39" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -10787,8 +10880,11 @@
       <c r="EF39">
         <v>2</v>
       </c>
+      <c r="EG39">
+        <v>2</v>
+      </c>
     </row>
-    <row r="40" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -11083,8 +11179,11 @@
       <c r="EF40">
         <v>85</v>
       </c>
+      <c r="EG40">
+        <v>85</v>
+      </c>
     </row>
-    <row r="41" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -11424,8 +11523,11 @@
       <c r="EF41">
         <v>0</v>
       </c>
+      <c r="EG41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -11762,8 +11864,11 @@
       <c r="EF42">
         <v>2</v>
       </c>
+      <c r="EG42">
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -12106,8 +12211,11 @@
       <c r="EF43">
         <v>296</v>
       </c>
+      <c r="EG43">
+        <v>296</v>
+      </c>
     </row>
-    <row r="44" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -12384,16 +12492,19 @@
       <c r="EF44">
         <v>1</v>
       </c>
+      <c r="EG44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:137" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -12742,8 +12853,11 @@
       <c r="EF47">
         <v>207</v>
       </c>
+      <c r="EG47">
+        <v>207</v>
+      </c>
     </row>
-    <row r="48" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -13044,8 +13158,11 @@
       <c r="EF48">
         <v>0</v>
       </c>
+      <c r="EG48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -13346,8 +13463,11 @@
       <c r="EF49">
         <v>200</v>
       </c>
+      <c r="EG49">
+        <v>200</v>
+      </c>
     </row>
-    <row r="50" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -13693,8 +13813,11 @@
       <c r="EF50">
         <v>71</v>
       </c>
+      <c r="EG50">
+        <v>75</v>
+      </c>
     </row>
-    <row r="51" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -13995,8 +14118,11 @@
       <c r="EF51">
         <v>65</v>
       </c>
+      <c r="EG51">
+        <v>75</v>
+      </c>
     </row>
-    <row r="52" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -14294,8 +14420,11 @@
       <c r="EF52">
         <v>1212</v>
       </c>
+      <c r="EG52">
+        <v>1214</v>
+      </c>
     </row>
-    <row r="53" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -14587,16 +14716,19 @@
       <c r="EF53">
         <v>1</v>
       </c>
+      <c r="EG53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:137" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -14930,8 +15062,11 @@
       <c r="EF56">
         <v>35</v>
       </c>
+      <c r="EG56">
+        <v>35</v>
+      </c>
     </row>
-    <row r="57" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -15229,8 +15364,11 @@
       <c r="EF57">
         <v>2</v>
       </c>
+      <c r="EG57">
+        <v>2</v>
+      </c>
     </row>
-    <row r="58" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -15528,8 +15666,11 @@
       <c r="EF58">
         <v>32</v>
       </c>
+      <c r="EG58">
+        <v>32</v>
+      </c>
     </row>
-    <row r="59" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -15863,8 +16004,11 @@
       <c r="EF59">
         <v>2</v>
       </c>
+      <c r="EG59">
+        <v>2</v>
+      </c>
     </row>
-    <row r="60" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -16198,8 +16342,11 @@
       <c r="EF60">
         <v>4</v>
       </c>
+      <c r="EG60">
+        <v>4</v>
+      </c>
     </row>
-    <row r="61" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -16533,8 +16680,11 @@
       <c r="EF61">
         <v>176</v>
       </c>
+      <c r="EG61">
+        <v>176</v>
+      </c>
     </row>
-    <row r="62" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -16826,8 +16976,11 @@
       <c r="EF62">
         <v>1</v>
       </c>
+      <c r="EG62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -17161,8 +17314,11 @@
       <c r="EF64">
         <v>13</v>
       </c>
+      <c r="EG64">
+        <v>13</v>
+      </c>
     </row>
-    <row r="65" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -17460,8 +17616,11 @@
       <c r="EF65">
         <v>0</v>
       </c>
+      <c r="EG65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -17759,8 +17918,11 @@
       <c r="EF66">
         <v>13</v>
       </c>
+      <c r="EG66">
+        <v>13</v>
+      </c>
     </row>
-    <row r="67" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -18094,8 +18256,11 @@
       <c r="EF67">
         <v>0</v>
       </c>
+      <c r="EG67">
+        <v>66</v>
+      </c>
     </row>
-    <row r="68" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -18430,8 +18595,11 @@
       <c r="EF68">
         <v>0</v>
       </c>
+      <c r="EG68">
+        <v>66</v>
+      </c>
     </row>
-    <row r="69" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -18765,8 +18933,11 @@
       <c r="EF69">
         <v>0</v>
       </c>
+      <c r="EG69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -19064,11 +19235,14 @@
       <c r="EF70">
         <v>0</v>
       </c>
+      <c r="EG70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>119</v>
       </c>
@@ -19252,8 +19426,11 @@
       <c r="EF72">
         <v>11</v>
       </c>
+      <c r="EG72">
+        <v>11</v>
+      </c>
     </row>
-    <row r="73" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>119</v>
       </c>
@@ -19437,8 +19614,11 @@
       <c r="EF73">
         <v>2</v>
       </c>
+      <c r="EG73">
+        <v>2</v>
+      </c>
     </row>
-    <row r="74" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
@@ -19622,8 +19802,11 @@
       <c r="EF74">
         <v>9</v>
       </c>
+      <c r="EG74">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>119</v>
       </c>
@@ -19807,8 +19990,11 @@
       <c r="EF75">
         <v>2</v>
       </c>
+      <c r="EG75">
+        <v>2</v>
+      </c>
     </row>
-    <row r="76" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -19992,8 +20178,11 @@
       <c r="EF76">
         <v>4</v>
       </c>
+      <c r="EG76">
+        <v>4</v>
+      </c>
     </row>
-    <row r="77" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>119</v>
       </c>
@@ -20177,13 +20366,16 @@
       <c r="EF77">
         <v>48</v>
       </c>
+      <c r="EG77">
+        <v>48</v>
+      </c>
     </row>
-    <row r="79" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:137" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -20520,8 +20712,11 @@
       <c r="EF80">
         <v>329</v>
       </c>
+      <c r="EG80">
+        <v>329</v>
+      </c>
     </row>
-    <row r="81" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -20852,8 +21047,17 @@
       <c r="ED81">
         <v>67</v>
       </c>
+      <c r="EE81">
+        <v>66</v>
+      </c>
+      <c r="EF81">
+        <v>68</v>
+      </c>
+      <c r="EG81">
+        <v>77</v>
+      </c>
     </row>
-    <row r="82" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -21184,8 +21388,17 @@
       <c r="ED82">
         <v>63</v>
       </c>
+      <c r="EE82">
+        <v>63</v>
+      </c>
+      <c r="EF82">
+        <v>66</v>
+      </c>
+      <c r="EG82">
+        <v>68</v>
+      </c>
     </row>
-    <row r="83" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -21480,8 +21693,11 @@
       <c r="EF83">
         <v>21</v>
       </c>
+      <c r="EG83">
+        <v>21</v>
+      </c>
     </row>
-    <row r="85" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -21818,8 +22034,11 @@
       <c r="EF85">
         <v>125</v>
       </c>
+      <c r="EG85">
+        <v>125</v>
+      </c>
     </row>
-    <row r="86" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -22156,8 +22375,11 @@
       <c r="EF86">
         <v>6</v>
       </c>
+      <c r="EG86">
+        <v>6</v>
+      </c>
     </row>
-    <row r="87" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -22494,8 +22716,11 @@
       <c r="EF87">
         <v>16</v>
       </c>
+      <c r="EG87">
+        <v>16</v>
+      </c>
     </row>
-    <row r="88" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -22832,8 +23057,11 @@
       <c r="EF88">
         <v>262</v>
       </c>
+      <c r="EG88">
+        <v>262</v>
+      </c>
     </row>
-    <row r="89" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -23044,8 +23272,11 @@
       <c r="EF89">
         <v>1</v>
       </c>
+      <c r="EG89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -23382,8 +23613,11 @@
       <c r="EF91">
         <v>82</v>
       </c>
+      <c r="EG91">
+        <v>82</v>
+      </c>
     </row>
-    <row r="92" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -23720,8 +23954,11 @@
       <c r="EF92">
         <v>0</v>
       </c>
+      <c r="EG92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -24046,8 +24283,11 @@
       <c r="EF93">
         <v>191</v>
       </c>
+      <c r="EG93">
+        <v>191</v>
+      </c>
     </row>
-    <row r="94" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -24384,8 +24624,11 @@
       <c r="EF94">
         <v>62</v>
       </c>
+      <c r="EG94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -24680,11 +24923,14 @@
       <c r="EF95">
         <v>14</v>
       </c>
+      <c r="EG95">
+        <v>14</v>
+      </c>
     </row>
-    <row r="96" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>130</v>
       </c>
@@ -24838,8 +25084,11 @@
       <c r="EF97">
         <v>14</v>
       </c>
+      <c r="EG97">
+        <v>14</v>
+      </c>
     </row>
-    <row r="98" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>130</v>
       </c>
@@ -24993,8 +25242,11 @@
       <c r="EF98">
         <v>11</v>
       </c>
+      <c r="EG98">
+        <v>11</v>
+      </c>
     </row>
-    <row r="99" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>130</v>
       </c>
@@ -25148,8 +25400,11 @@
       <c r="EF99">
         <v>55</v>
       </c>
+      <c r="EG99">
+        <v>55</v>
+      </c>
     </row>
-    <row r="100" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
@@ -25303,8 +25558,11 @@
       <c r="EF100">
         <v>1</v>
       </c>
+      <c r="EG100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -25560,8 +25818,11 @@
       <c r="EF102">
         <v>213</v>
       </c>
+      <c r="EG102">
+        <v>215</v>
+      </c>
     </row>
-    <row r="103" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -25817,8 +26078,11 @@
       <c r="EF103">
         <v>140</v>
       </c>
+      <c r="EG103">
+        <v>140</v>
+      </c>
     </row>
-    <row r="104" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:137" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -26074,8 +26338,11 @@
       <c r="EF104">
         <v>28</v>
       </c>
+      <c r="EG104">
+        <v>28</v>
+      </c>
     </row>
-    <row r="119" spans="52:52" x14ac:dyDescent="0.25">
+    <row r="119" spans="52:52" x14ac:dyDescent="0.3">
       <c r="AZ119">
         <v>9</v>
       </c>
@@ -26087,22 +26354,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:DG11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:DH11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DH2" sqref="DH2"/>
+      <selection pane="topRight" activeCell="DI2" sqref="DI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:111" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:112" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -26436,8 +26703,11 @@
       <c r="DG2" s="9">
         <v>44030</v>
       </c>
+      <c r="DH2" s="9">
+        <v>44031</v>
+      </c>
     </row>
-    <row r="3" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:112" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -26771,8 +27041,11 @@
       <c r="DG3">
         <v>1592</v>
       </c>
+      <c r="DH3">
+        <v>1602</v>
+      </c>
     </row>
-    <row r="4" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:112" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -27106,8 +27379,11 @@
       <c r="DG4">
         <v>692</v>
       </c>
+      <c r="DH4">
+        <v>700</v>
+      </c>
     </row>
-    <row r="5" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:112" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -27441,8 +27717,11 @@
       <c r="DG5">
         <v>532</v>
       </c>
+      <c r="DH5">
+        <v>534</v>
+      </c>
     </row>
-    <row r="6" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:112" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -27776,8 +28055,11 @@
       <c r="DG6">
         <v>2273</v>
       </c>
+      <c r="DH6">
+        <v>2283</v>
+      </c>
     </row>
-    <row r="7" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:112" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -28111,8 +28393,11 @@
       <c r="DG7">
         <v>1676</v>
       </c>
+      <c r="DH7">
+        <v>1693</v>
+      </c>
     </row>
-    <row r="8" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:112" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -28446,8 +28731,11 @@
       <c r="DG8">
         <v>1053</v>
       </c>
+      <c r="DH8">
+        <v>1065</v>
+      </c>
     </row>
-    <row r="9" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:112" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -28781,8 +29069,11 @@
       <c r="DG9">
         <v>1623</v>
       </c>
+      <c r="DH9">
+        <v>1629</v>
+      </c>
     </row>
-    <row r="10" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:112" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -29116,8 +29407,11 @@
       <c r="DG10">
         <v>1641</v>
       </c>
+      <c r="DH10">
+        <v>1649</v>
+      </c>
     </row>
-    <row r="11" spans="1:111" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:112" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -29450,6 +29744,9 @@
       </c>
       <c r="DG11">
         <v>179</v>
+      </c>
+      <c r="DH11">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -29459,22 +29756,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:DB17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:DC17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DC2" sqref="DC2"/>
+      <selection pane="topRight" activeCell="DD2" sqref="DD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="10" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" customWidth="1"/>
+    <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:106" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:107" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -29791,8 +30088,11 @@
       <c r="DB2" s="9">
         <v>44030</v>
       </c>
+      <c r="DC2" s="9">
+        <v>44031</v>
+      </c>
     </row>
-    <row r="3" spans="1:106" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:107" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>36</v>
       </c>
@@ -29801,7 +30101,7 @@
       <c r="D3" s="9"/>
       <c r="CP3" s="4"/>
     </row>
-    <row r="4" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -30120,8 +30420,11 @@
       <c r="DB4">
         <v>11261</v>
       </c>
+      <c r="DC4">
+        <v>11339</v>
+      </c>
     </row>
-    <row r="5" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -30440,8 +30743,11 @@
       <c r="DB5">
         <v>200</v>
       </c>
+      <c r="DC5">
+        <v>214</v>
+      </c>
     </row>
-    <row r="6" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -30760,8 +31066,11 @@
       <c r="DB6">
         <v>2308</v>
       </c>
+      <c r="DC6">
+        <v>2320</v>
+      </c>
     </row>
-    <row r="7" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -31080,8 +31389,11 @@
       <c r="DB7">
         <v>5550</v>
       </c>
+      <c r="DC7">
+        <v>5576</v>
+      </c>
     </row>
-    <row r="8" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -31400,8 +31712,11 @@
       <c r="DB8">
         <v>175</v>
       </c>
+      <c r="DC8">
+        <v>177</v>
+      </c>
     </row>
-    <row r="9" spans="1:106" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:107" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -31720,8 +32035,11 @@
       <c r="DB9">
         <v>27</v>
       </c>
+      <c r="DC9">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:106" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:107" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -32036,8 +32354,11 @@
       <c r="DB10">
         <v>30</v>
       </c>
+      <c r="DC10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="11" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -32356,8 +32677,11 @@
       <c r="DB11">
         <v>2882</v>
       </c>
+      <c r="DC11">
+        <v>2906</v>
+      </c>
     </row>
-    <row r="12" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -32676,8 +33000,11 @@
       <c r="DB12">
         <v>89</v>
       </c>
+      <c r="DC12">
+        <v>89</v>
+      </c>
     </row>
-    <row r="13" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -32688,7 +33015,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -33007,8 +33334,11 @@
       <c r="DB14">
         <v>1408</v>
       </c>
+      <c r="DC14">
+        <v>1447</v>
+      </c>
     </row>
-    <row r="15" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -33327,8 +33657,11 @@
       <c r="DB15">
         <v>3096</v>
       </c>
+      <c r="DC15">
+        <v>3101</v>
+      </c>
     </row>
-    <row r="16" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -33647,8 +33980,11 @@
       <c r="DB16">
         <v>6740</v>
       </c>
+      <c r="DC16">
+        <v>6774</v>
+      </c>
     </row>
-    <row r="17" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -33965,6 +34301,9 @@
         <v>18</v>
       </c>
       <c r="DB17">
+        <v>17</v>
+      </c>
+      <c r="DC17">
         <v>17</v>
       </c>
     </row>
@@ -33975,21 +34314,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DB9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:DC9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DC1" sqref="DC1"/>
+      <selection pane="topRight" activeCell="DD1" sqref="DD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:106" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:107" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -34305,14 +34644,17 @@
       <c r="DB1" s="9">
         <v>44030</v>
       </c>
+      <c r="DC1" s="9">
+        <v>44031</v>
+      </c>
     </row>
-    <row r="2" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -34632,8 +34974,11 @@
       <c r="DB3">
         <v>578</v>
       </c>
+      <c r="DC3">
+        <v>579</v>
+      </c>
     </row>
-    <row r="4" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -34952,8 +35297,11 @@
       <c r="DB4">
         <v>8</v>
       </c>
+      <c r="DC4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:106" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:107" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -35272,8 +35620,11 @@
       <c r="DB5">
         <v>426</v>
       </c>
+      <c r="DC5">
+        <v>427</v>
+      </c>
     </row>
-    <row r="6" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -35592,8 +35943,11 @@
       <c r="DB6">
         <v>76</v>
       </c>
+      <c r="DC6">
+        <v>76</v>
+      </c>
     </row>
-    <row r="7" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -35912,8 +36266,11 @@
       <c r="DB7">
         <v>62</v>
       </c>
+      <c r="DC7">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -36232,8 +36589,11 @@
       <c r="DB8">
         <v>6</v>
       </c>
+      <c r="DC8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:106" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:107" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -36274,20 +36634,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CT5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:CU5"/>
   <sheetViews>
     <sheetView zoomScale="95" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CU1" sqref="CU1"/>
+      <selection pane="topRight" activeCell="CV1" sqref="CV1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -36579,13 +36939,16 @@
       <c r="CT1" s="9">
         <v>44030</v>
       </c>
+      <c r="CU1" s="9">
+        <v>44031</v>
+      </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
@@ -36880,8 +37243,11 @@
       <c r="CT3">
         <v>578</v>
       </c>
+      <c r="CU3">
+        <v>579</v>
+      </c>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>153</v>
       </c>
@@ -37176,8 +37542,11 @@
       <c r="CT4">
         <v>245</v>
       </c>
+      <c r="CU4">
+        <v>246</v>
+      </c>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>152</v>
       </c>
@@ -37470,6 +37839,9 @@
         <v>333</v>
       </c>
       <c r="CT5">
+        <v>333</v>
+      </c>
+      <c r="CU5">
         <v>333</v>
       </c>
     </row>
@@ -37480,20 +37852,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CT11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:CU11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CU1" sqref="CU1"/>
+      <selection pane="topRight" activeCell="CV1" sqref="CV1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -37785,13 +38157,16 @@
       <c r="CT1" s="9">
         <v>44030</v>
       </c>
+      <c r="CU1" s="9">
+        <v>44031</v>
+      </c>
     </row>
-    <row r="2" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -38086,8 +38461,11 @@
       <c r="CT3">
         <v>578</v>
       </c>
+      <c r="CU3">
+        <v>579</v>
+      </c>
     </row>
-    <row r="4" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>143</v>
       </c>
@@ -38382,8 +38760,11 @@
       <c r="CT4">
         <v>0</v>
       </c>
+      <c r="CU4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>144</v>
       </c>
@@ -38678,8 +39059,11 @@
       <c r="CT5">
         <v>3</v>
       </c>
+      <c r="CU5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>145</v>
       </c>
@@ -38974,8 +39358,11 @@
       <c r="CT6">
         <v>8</v>
       </c>
+      <c r="CU6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>146</v>
       </c>
@@ -39270,8 +39657,11 @@
       <c r="CT7">
         <v>20</v>
       </c>
+      <c r="CU7">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>147</v>
       </c>
@@ -39566,8 +39956,11 @@
       <c r="CT8">
         <v>66</v>
       </c>
+      <c r="CU8">
+        <v>66</v>
+      </c>
     </row>
-    <row r="9" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>148</v>
       </c>
@@ -39862,8 +40255,11 @@
       <c r="CT9">
         <v>136</v>
       </c>
+      <c r="CU9">
+        <v>136</v>
+      </c>
     </row>
-    <row r="10" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>149</v>
       </c>
@@ -40158,8 +40554,11 @@
       <c r="CT10">
         <v>147</v>
       </c>
+      <c r="CU10">
+        <v>147</v>
+      </c>
     </row>
-    <row r="11" spans="1:98" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>150</v>
       </c>
@@ -40453,6 +40852,9 @@
       </c>
       <c r="CT11">
         <v>198</v>
+      </c>
+      <c r="CU11">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -40462,21 +40864,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:CN13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A2:CO13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CN16" sqref="CN16"/>
+      <selection pane="topRight" activeCell="CP2" sqref="CP2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="57" max="57" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="57" max="57" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:92" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:93" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -40753,8 +41155,11 @@
       <c r="CN2" s="9">
         <v>44030</v>
       </c>
+      <c r="CO2" s="9">
+        <v>44031</v>
+      </c>
     </row>
-    <row r="3" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -41031,8 +41436,11 @@
       <c r="CN3">
         <v>578</v>
       </c>
+      <c r="CO3">
+        <v>579</v>
+      </c>
     </row>
-    <row r="4" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -41309,8 +41717,11 @@
       <c r="CN4">
         <v>63</v>
       </c>
+      <c r="CO4">
+        <v>63</v>
+      </c>
     </row>
-    <row r="5" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -41587,8 +41998,11 @@
       <c r="CN5">
         <v>33</v>
       </c>
+      <c r="CO5">
+        <v>33</v>
+      </c>
     </row>
-    <row r="6" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -41865,8 +42279,11 @@
       <c r="CN6">
         <v>33</v>
       </c>
+      <c r="CO6">
+        <v>33</v>
+      </c>
     </row>
-    <row r="7" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -42143,8 +42560,11 @@
       <c r="CN7">
         <v>84</v>
       </c>
+      <c r="CO7">
+        <v>84</v>
+      </c>
     </row>
-    <row r="8" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -42421,8 +42841,11 @@
       <c r="CN8">
         <v>92</v>
       </c>
+      <c r="CO8">
+        <v>92</v>
+      </c>
     </row>
-    <row r="9" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -42699,8 +43122,11 @@
       <c r="CN9">
         <v>49</v>
       </c>
+      <c r="CO9">
+        <v>50</v>
+      </c>
     </row>
-    <row r="10" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -42977,8 +43403,11 @@
       <c r="CN10">
         <v>85</v>
       </c>
+      <c r="CO10">
+        <v>85</v>
+      </c>
     </row>
-    <row r="11" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -43255,8 +43684,11 @@
       <c r="CN11">
         <v>117</v>
       </c>
+      <c r="CO11">
+        <v>117</v>
+      </c>
     </row>
-    <row r="12" spans="1:92" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:93" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -43533,8 +43965,11 @@
       <c r="CN12">
         <v>21</v>
       </c>
+      <c r="CO12">
+        <v>21</v>
+      </c>
     </row>
-    <row r="13" spans="1:92" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -43809,6 +44244,9 @@
         <v>1</v>
       </c>
       <c r="CN13">
+        <v>1</v>
+      </c>
+      <c r="CO13">
         <v>1</v>
       </c>
     </row>
@@ -43819,20 +44257,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:BL23"/>
   <sheetViews>
-    <sheetView topLeftCell="AU1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="BK5" sqref="BK5"/>
+    <sheetView topLeftCell="AT1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="BL5" sqref="BL5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="42" max="45" width="8.85546875" customWidth="1"/>
+    <col min="42" max="45" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.3">
       <c r="C1" s="51" t="s">
         <v>180</v>
       </c>
@@ -43849,7 +44287,7 @@
       <c r="N1" s="51"/>
       <c r="O1" s="51"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
@@ -43864,7 +44302,7 @@
       <c r="N2" s="51"/>
       <c r="O2" s="51"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="E3" s="51"/>
@@ -43879,7 +44317,7 @@
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
     </row>
-    <row r="4" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -43894,7 +44332,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -44075,11 +44513,14 @@
       <c r="BJ5" s="9">
         <v>44030</v>
       </c>
-      <c r="BK5" t="s">
+      <c r="BK5" s="9">
+        <v>44031</v>
+      </c>
+      <c r="BL5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>120</v>
       </c>
@@ -44263,8 +44704,11 @@
       <c r="BJ6">
         <v>159</v>
       </c>
+      <c r="BK6">
+        <v>159</v>
+      </c>
     </row>
-    <row r="7" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -44448,8 +44892,11 @@
       <c r="BJ7">
         <v>36</v>
       </c>
+      <c r="BK7">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
@@ -44457,7 +44904,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -44641,8 +45088,11 @@
       <c r="BJ9">
         <v>1</v>
       </c>
+      <c r="BK9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>121</v>
       </c>
@@ -44826,8 +45276,11 @@
       <c r="BJ10">
         <v>23</v>
       </c>
+      <c r="BK10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>122</v>
       </c>
@@ -45011,8 +45464,11 @@
       <c r="BJ11">
         <v>9</v>
       </c>
+      <c r="BK11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -45196,13 +45652,16 @@
       <c r="BJ12">
         <v>3</v>
       </c>
+      <c r="BK12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -45386,8 +45845,11 @@
       <c r="BJ14">
         <v>1</v>
       </c>
+      <c r="BK14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -45571,8 +46033,11 @@
       <c r="BJ15">
         <v>0</v>
       </c>
+      <c r="BK15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -45756,8 +46221,11 @@
       <c r="BJ16">
         <v>3</v>
       </c>
+      <c r="BK16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -45941,8 +46409,11 @@
       <c r="BJ17">
         <v>12</v>
       </c>
+      <c r="BK17">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -46126,8 +46597,11 @@
       <c r="BJ18">
         <v>3</v>
       </c>
+      <c r="BK18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -46311,8 +46785,11 @@
       <c r="BJ19">
         <v>2</v>
       </c>
+      <c r="BK19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -46496,8 +46973,11 @@
       <c r="BJ20">
         <v>2</v>
       </c>
+      <c r="BK20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -46681,8 +47161,11 @@
       <c r="BJ21">
         <v>6</v>
       </c>
+      <c r="BK21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:62" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -46866,8 +47349,11 @@
       <c r="BJ22">
         <v>4</v>
       </c>
+      <c r="BK22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:62" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>123</v>
       </c>
@@ -47049,6 +47535,9 @@
         <v>3</v>
       </c>
       <c r="BJ23">
+        <v>3</v>
+      </c>
+      <c r="BK23">
         <v>3</v>
       </c>
     </row>
@@ -47061,21 +47550,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -47090,7 +47579,7 @@
       <c r="F1" s="53"/>
       <c r="G1" s="53"/>
     </row>
-    <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="54" t="s">
         <v>85</v>
       </c>
@@ -47128,7 +47617,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="54"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -47141,7 +47630,7 @@
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="54"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
@@ -47152,7 +47641,7 @@
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="54"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
@@ -47163,7 +47652,7 @@
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="54"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
@@ -47174,7 +47663,7 @@
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>94</v>
       </c>
@@ -47197,7 +47686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>141</v>
       </c>
@@ -47220,7 +47709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>96</v>
       </c>
@@ -47243,7 +47732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>97</v>
       </c>
@@ -47266,7 +47755,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>98</v>
       </c>
@@ -47289,7 +47778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>126</v>
       </c>
@@ -47312,7 +47801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>99</v>
       </c>
@@ -47335,7 +47824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>100</v>
       </c>
@@ -47381,7 +47870,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>101</v>
       </c>
@@ -47404,7 +47893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>102</v>
       </c>
@@ -47427,7 +47916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>103</v>
       </c>
@@ -47450,7 +47939,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>104</v>
       </c>
@@ -47473,7 +47962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>105</v>
       </c>
@@ -47496,7 +47985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>107</v>
       </c>
@@ -47588,7 +48077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="45" t="s">
         <v>49</v>
       </c>
@@ -47612,7 +48101,7 @@
       </c>
       <c r="H26" s="46"/>
     </row>
-    <row r="27" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>110</v>
       </c>
@@ -47626,7 +48115,7 @@
       <c r="G27" s="49"/>
       <c r="H27" s="47"/>
     </row>
-    <row r="28" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="27"/>
       <c r="C28" s="43"/>
       <c r="D28" s="43"/>
@@ -47634,7 +48123,7 @@
       <c r="F28" s="43"/>
       <c r="G28" s="43"/>
     </row>
-    <row r="29" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
@@ -47648,18 +48137,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47866,26 +48355,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Results from July 22, 2020 07:53:15 AM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/work/WashingtonDC/data.xlsx
+++ b/workflow/python/work/WashingtonDC/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{D8A8C525-9AD6-4328-8A76-D2E05990132D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{51EE4AEC-4CE1-4046-ABCE-56D8803949D6}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="8_{D8A8C525-9AD6-4328-8A76-D2E05990132D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E447C524-B713-4EF7-A1E4-0C5E15152980}"/>
   <bookViews>
-    <workbookView xWindow="-996" yWindow="3960" windowWidth="23040" windowHeight="7116" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-216" yWindow="264" windowWidth="23040" windowHeight="7116" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Community Cases Tested By OCME" sheetId="7" r:id="rId8"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="181">
   <si>
     <t>Testing</t>
   </si>
@@ -582,7 +582,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of July 20, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of July 21, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -1290,11 +1290,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EH119"/>
+  <dimension ref="A1:EI119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="EA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EH104" sqref="EH104"/>
+      <selection pane="topRight" activeCell="EJ1" sqref="EJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1310,10 +1310,10 @@
     <col min="98" max="102" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="104" max="118" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="128" max="138" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="128" max="139" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:139" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1722,8 +1722,11 @@
       <c r="EH1" s="48">
         <v>44032</v>
       </c>
+      <c r="EI1" s="48">
+        <v>44033</v>
+      </c>
     </row>
-    <row r="2" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1747,7 +1750,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2141,8 +2144,11 @@
       <c r="EH3">
         <v>155711</v>
       </c>
+      <c r="EI3">
+        <v>159572</v>
+      </c>
     </row>
-    <row r="4" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2331,8 +2337,11 @@
       <c r="EH4">
         <v>111244</v>
       </c>
+      <c r="EI4">
+        <v>113858</v>
+      </c>
     </row>
-    <row r="5" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2747,8 +2756,11 @@
       <c r="EH5">
         <v>11427</v>
       </c>
+      <c r="EI5">
+        <v>11529</v>
+      </c>
     </row>
-    <row r="6" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3145,8 +3157,11 @@
       <c r="EH6">
         <v>580</v>
       </c>
+      <c r="EI6">
+        <v>580</v>
+      </c>
     </row>
-    <row r="7" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3513,11 +3528,14 @@
       <c r="EH7">
         <v>1932</v>
       </c>
+      <c r="EI7">
+        <v>1974</v>
+      </c>
     </row>
-    <row r="8" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3776,8 +3794,11 @@
       <c r="EH9">
         <v>345</v>
       </c>
+      <c r="EI9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -4138,8 +4159,11 @@
       <c r="EH10">
         <v>73</v>
       </c>
+      <c r="EI10">
+        <v>80</v>
+      </c>
     </row>
-    <row r="11" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4500,8 +4524,11 @@
       <c r="EH11">
         <v>440</v>
       </c>
+      <c r="EI11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4862,8 +4889,11 @@
       <c r="EH12">
         <v>188</v>
       </c>
+      <c r="EI12">
+        <v>184</v>
+      </c>
     </row>
-    <row r="13" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -5224,8 +5254,11 @@
       <c r="EH13">
         <v>252</v>
       </c>
+      <c r="EI13">
+        <v>256</v>
+      </c>
     </row>
-    <row r="14" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -5448,8 +5481,11 @@
       <c r="EH14">
         <v>83</v>
       </c>
+      <c r="EI14">
+        <v>81</v>
+      </c>
     </row>
-    <row r="15" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -5642,8 +5678,11 @@
       <c r="EH15">
         <v>19</v>
       </c>
+      <c r="EI15">
+        <v>18</v>
+      </c>
     </row>
-    <row r="16" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -5866,8 +5905,11 @@
       <c r="EH16">
         <v>1912</v>
       </c>
+      <c r="EI16">
+        <v>2005</v>
+      </c>
     </row>
-    <row r="17" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -6090,13 +6132,16 @@
       <c r="EH17" s="23">
         <v>0.77</v>
       </c>
+      <c r="EI17" s="23">
+        <v>0.81</v>
+      </c>
     </row>
-    <row r="19" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -6104,7 +6149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -6465,8 +6510,11 @@
       <c r="EH21">
         <v>121</v>
       </c>
+      <c r="EI21">
+        <v>122</v>
+      </c>
     </row>
-    <row r="22" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -6773,8 +6821,11 @@
       <c r="EH22">
         <v>6</v>
       </c>
+      <c r="EI22">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -7081,8 +7132,11 @@
       <c r="EH23">
         <v>116</v>
       </c>
+      <c r="EI23">
+        <v>116</v>
+      </c>
     </row>
-    <row r="24" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -7434,8 +7488,11 @@
       <c r="EH24">
         <v>74</v>
       </c>
+      <c r="EI24">
+        <v>59</v>
+      </c>
     </row>
-    <row r="25" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -7787,8 +7844,11 @@
       <c r="EH25">
         <v>80</v>
       </c>
+      <c r="EI25">
+        <v>65</v>
+      </c>
     </row>
-    <row r="26" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -8140,13 +8200,16 @@
       <c r="EH26">
         <v>1721</v>
       </c>
+      <c r="EI26">
+        <v>1758</v>
+      </c>
     </row>
-    <row r="28" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -8507,8 +8570,11 @@
       <c r="EH29">
         <v>180</v>
       </c>
+      <c r="EI29">
+        <v>180</v>
+      </c>
     </row>
-    <row r="30" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -8815,8 +8881,11 @@
       <c r="EH30">
         <v>42</v>
       </c>
+      <c r="EI30">
+        <v>40</v>
+      </c>
     </row>
-    <row r="31" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -9123,8 +9192,11 @@
       <c r="EH31">
         <v>138</v>
       </c>
+      <c r="EI31">
+        <v>139</v>
+      </c>
     </row>
-    <row r="32" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -9476,8 +9548,11 @@
       <c r="EH32">
         <v>117</v>
       </c>
+      <c r="EI32">
+        <v>107</v>
+      </c>
     </row>
-    <row r="33" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -9829,8 +9904,11 @@
       <c r="EH33">
         <v>169</v>
       </c>
+      <c r="EI33">
+        <v>147</v>
+      </c>
     </row>
-    <row r="34" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -10182,8 +10260,11 @@
       <c r="EH34">
         <v>1435</v>
       </c>
+      <c r="EI34">
+        <v>1449</v>
+      </c>
     </row>
-    <row r="35" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -10316,13 +10397,16 @@
       <c r="EH35">
         <v>1</v>
       </c>
+      <c r="EI35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -10671,8 +10755,11 @@
       <c r="EH38">
         <v>89</v>
       </c>
+      <c r="EI38">
+        <v>90</v>
+      </c>
     </row>
-    <row r="39" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -10973,8 +11060,11 @@
       <c r="EH39">
         <v>3</v>
       </c>
+      <c r="EI39">
+        <v>4</v>
+      </c>
     </row>
-    <row r="40" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -11275,8 +11365,11 @@
       <c r="EH40">
         <v>85</v>
       </c>
+      <c r="EI40">
+        <v>85</v>
+      </c>
     </row>
-    <row r="41" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -11622,8 +11715,11 @@
       <c r="EH41">
         <v>0</v>
       </c>
+      <c r="EI41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -11966,8 +12062,11 @@
       <c r="EH42">
         <v>3</v>
       </c>
+      <c r="EI42">
+        <v>4</v>
+      </c>
     </row>
-    <row r="43" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -12316,8 +12415,11 @@
       <c r="EH43">
         <v>296</v>
       </c>
+      <c r="EI43">
+        <v>296</v>
+      </c>
     </row>
-    <row r="44" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -12600,16 +12702,19 @@
       <c r="EH44">
         <v>1</v>
       </c>
+      <c r="EI44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -12964,8 +13069,11 @@
       <c r="EH47">
         <v>208</v>
       </c>
+      <c r="EI47">
+        <v>208</v>
+      </c>
     </row>
-    <row r="48" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -13272,8 +13380,11 @@
       <c r="EH48">
         <v>1</v>
       </c>
+      <c r="EI48">
+        <v>1</v>
+      </c>
     </row>
-    <row r="49" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -13580,8 +13691,11 @@
       <c r="EH49">
         <v>200</v>
       </c>
+      <c r="EI49">
+        <v>200</v>
+      </c>
     </row>
-    <row r="50" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -13933,8 +14047,11 @@
       <c r="EH50">
         <v>75</v>
       </c>
+      <c r="EI50">
+        <v>59</v>
+      </c>
     </row>
-    <row r="51" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -14241,8 +14358,11 @@
       <c r="EH51">
         <v>76</v>
       </c>
+      <c r="EI51">
+        <v>59</v>
+      </c>
     </row>
-    <row r="52" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -14546,8 +14666,11 @@
       <c r="EH52">
         <v>1213</v>
       </c>
+      <c r="EI52">
+        <v>1226</v>
+      </c>
     </row>
-    <row r="53" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -14845,16 +14968,19 @@
       <c r="EH53">
         <v>1</v>
       </c>
+      <c r="EI53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -15194,8 +15320,11 @@
       <c r="EH56">
         <v>35</v>
       </c>
+      <c r="EI56">
+        <v>35</v>
+      </c>
     </row>
-    <row r="57" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -15499,8 +15628,11 @@
       <c r="EH57">
         <v>2</v>
       </c>
+      <c r="EI57">
+        <v>3</v>
+      </c>
     </row>
-    <row r="58" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -15804,8 +15936,11 @@
       <c r="EH58">
         <v>32</v>
       </c>
+      <c r="EI58">
+        <v>32</v>
+      </c>
     </row>
-    <row r="59" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -16145,8 +16280,11 @@
       <c r="EH59">
         <v>2</v>
       </c>
+      <c r="EI59">
+        <v>1</v>
+      </c>
     </row>
-    <row r="60" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -16486,8 +16624,11 @@
       <c r="EH60">
         <v>4</v>
       </c>
+      <c r="EI60">
+        <v>4</v>
+      </c>
     </row>
-    <row r="61" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -16827,8 +16968,11 @@
       <c r="EH61">
         <v>176</v>
       </c>
+      <c r="EI61">
+        <v>177</v>
+      </c>
     </row>
-    <row r="62" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -17126,8 +17270,11 @@
       <c r="EH62">
         <v>1</v>
       </c>
+      <c r="EI62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -17467,8 +17614,11 @@
       <c r="EH64">
         <v>13</v>
       </c>
+      <c r="EI64">
+        <v>13</v>
+      </c>
     </row>
-    <row r="65" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -17772,8 +17922,11 @@
       <c r="EH65">
         <v>0</v>
       </c>
+      <c r="EI65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -18077,8 +18230,11 @@
       <c r="EH66">
         <v>13</v>
       </c>
+      <c r="EI66">
+        <v>13</v>
+      </c>
     </row>
-    <row r="67" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -18418,8 +18574,11 @@
       <c r="EH67">
         <v>65</v>
       </c>
+      <c r="EI67">
+        <v>6</v>
+      </c>
     </row>
-    <row r="68" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -18760,8 +18919,11 @@
       <c r="EH68">
         <v>65</v>
       </c>
+      <c r="EI68">
+        <v>66</v>
+      </c>
     </row>
-    <row r="69" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -19101,8 +19263,11 @@
       <c r="EH69">
         <v>0</v>
       </c>
+      <c r="EI69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -19406,11 +19571,14 @@
       <c r="EH70">
         <v>0</v>
       </c>
+      <c r="EI70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>119</v>
       </c>
@@ -19600,8 +19768,11 @@
       <c r="EH72">
         <v>11</v>
       </c>
+      <c r="EI72">
+        <v>11</v>
+      </c>
     </row>
-    <row r="73" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>119</v>
       </c>
@@ -19791,8 +19962,11 @@
       <c r="EH73">
         <v>2</v>
       </c>
+      <c r="EI73">
+        <v>2</v>
+      </c>
     </row>
-    <row r="74" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
@@ -19982,8 +20156,11 @@
       <c r="EH74">
         <v>9</v>
       </c>
+      <c r="EI74">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>119</v>
       </c>
@@ -20173,8 +20350,11 @@
       <c r="EH75">
         <v>3</v>
       </c>
+      <c r="EI75">
+        <v>3</v>
+      </c>
     </row>
-    <row r="76" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -20364,8 +20544,11 @@
       <c r="EH76">
         <v>5</v>
       </c>
+      <c r="EI76">
+        <v>5</v>
+      </c>
     </row>
-    <row r="77" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>119</v>
       </c>
@@ -20555,13 +20738,16 @@
       <c r="EH77">
         <v>48</v>
       </c>
+      <c r="EI77">
+        <v>48</v>
+      </c>
     </row>
-    <row r="79" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -20904,8 +21090,11 @@
       <c r="EH80">
         <v>330</v>
       </c>
+      <c r="EI80">
+        <v>330</v>
+      </c>
     </row>
-    <row r="81" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -21248,8 +21437,11 @@
       <c r="EH81">
         <v>84</v>
       </c>
+      <c r="EI81">
+        <v>78</v>
+      </c>
     </row>
-    <row r="82" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -21592,8 +21784,11 @@
       <c r="EH82">
         <v>80</v>
       </c>
+      <c r="EI82">
+        <v>75</v>
+      </c>
     </row>
-    <row r="83" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -21894,8 +22089,11 @@
       <c r="EH83">
         <v>21</v>
       </c>
+      <c r="EI83">
+        <v>21</v>
+      </c>
     </row>
-    <row r="85" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -22238,8 +22436,11 @@
       <c r="EH85">
         <v>130</v>
       </c>
+      <c r="EI85">
+        <v>130</v>
+      </c>
     </row>
-    <row r="86" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -22582,8 +22783,11 @@
       <c r="EH86">
         <v>4</v>
       </c>
+      <c r="EI86">
+        <v>5</v>
+      </c>
     </row>
-    <row r="87" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -22926,8 +23130,11 @@
       <c r="EH87">
         <v>15</v>
       </c>
+      <c r="EI87">
+        <v>13</v>
+      </c>
     </row>
-    <row r="88" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -23270,8 +23477,11 @@
       <c r="EH88">
         <v>266</v>
       </c>
+      <c r="EI88">
+        <v>269</v>
+      </c>
     </row>
-    <row r="89" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -23488,8 +23698,11 @@
       <c r="EH89">
         <v>1</v>
       </c>
+      <c r="EI89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -23832,8 +24045,11 @@
       <c r="EH91">
         <v>82</v>
       </c>
+      <c r="EI91">
+        <v>82</v>
+      </c>
     </row>
-    <row r="92" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -24176,8 +24392,11 @@
       <c r="EH92">
         <v>0</v>
       </c>
+      <c r="EI92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -24508,8 +24727,11 @@
       <c r="EH93">
         <v>191</v>
       </c>
+      <c r="EI93">
+        <v>191</v>
+      </c>
     </row>
-    <row r="94" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -24852,8 +25074,11 @@
       <c r="EH94">
         <v>62</v>
       </c>
+      <c r="EI94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -25154,11 +25379,14 @@
       <c r="EH95">
         <v>14</v>
       </c>
+      <c r="EI95">
+        <v>14</v>
+      </c>
     </row>
-    <row r="96" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>130</v>
       </c>
@@ -25318,8 +25546,11 @@
       <c r="EH97">
         <v>14</v>
       </c>
+      <c r="EI97">
+        <v>14</v>
+      </c>
     </row>
-    <row r="98" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>130</v>
       </c>
@@ -25479,8 +25710,11 @@
       <c r="EH98">
         <v>11</v>
       </c>
+      <c r="EI98">
+        <v>11</v>
+      </c>
     </row>
-    <row r="99" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>130</v>
       </c>
@@ -25640,8 +25874,11 @@
       <c r="EH99">
         <v>55</v>
       </c>
+      <c r="EI99">
+        <v>55</v>
+      </c>
     </row>
-    <row r="100" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
@@ -25801,8 +26038,11 @@
       <c r="EH100">
         <v>1</v>
       </c>
+      <c r="EI100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -26064,8 +26304,11 @@
       <c r="EH102">
         <v>217</v>
       </c>
+      <c r="EI102">
+        <v>220</v>
+      </c>
     </row>
-    <row r="103" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -26327,8 +26570,11 @@
       <c r="EH103">
         <v>140</v>
       </c>
+      <c r="EI103">
+        <v>140</v>
+      </c>
     </row>
-    <row r="104" spans="1:138" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:139" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -26588,6 +26834,9 @@
         <v>28</v>
       </c>
       <c r="EH104">
+        <v>29</v>
+      </c>
+      <c r="EI104">
         <v>29</v>
       </c>
     </row>
@@ -26604,11 +26853,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:DI11"/>
+  <dimension ref="A2:DJ11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DJ2" sqref="DJ2"/>
+      <pane xSplit="1" topLeftCell="CQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DK2" sqref="DK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26618,7 +26867,7 @@
     <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:113" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:114" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -26958,8 +27207,11 @@
       <c r="DI2" s="9">
         <v>44032</v>
       </c>
+      <c r="DJ2" s="9">
+        <v>44033</v>
+      </c>
     </row>
-    <row r="3" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -27299,8 +27551,11 @@
       <c r="DI3">
         <v>1606</v>
       </c>
+      <c r="DJ3">
+        <v>1614</v>
+      </c>
     </row>
-    <row r="4" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -27640,8 +27895,11 @@
       <c r="DI4">
         <v>691</v>
       </c>
+      <c r="DJ4">
+        <v>698</v>
+      </c>
     </row>
-    <row r="5" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -27981,8 +28239,11 @@
       <c r="DI5">
         <v>540</v>
       </c>
+      <c r="DJ5">
+        <v>543</v>
+      </c>
     </row>
-    <row r="6" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -28322,8 +28583,11 @@
       <c r="DI6">
         <v>2301</v>
       </c>
+      <c r="DJ6">
+        <v>2316</v>
+      </c>
     </row>
-    <row r="7" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -28663,8 +28927,11 @@
       <c r="DI7">
         <v>1708</v>
       </c>
+      <c r="DJ7">
+        <v>1723</v>
+      </c>
     </row>
-    <row r="8" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -29004,8 +29271,11 @@
       <c r="DI8">
         <v>1070</v>
       </c>
+      <c r="DJ8">
+        <v>1077</v>
+      </c>
     </row>
-    <row r="9" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -29345,8 +29615,11 @@
       <c r="DI9">
         <v>1646</v>
       </c>
+      <c r="DJ9">
+        <v>1665</v>
+      </c>
     </row>
-    <row r="10" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -29686,8 +29959,11 @@
       <c r="DI10">
         <v>1661</v>
       </c>
+      <c r="DJ10">
+        <v>1686</v>
+      </c>
     </row>
-    <row r="11" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -30026,6 +30302,9 @@
       </c>
       <c r="DI11">
         <v>204</v>
+      </c>
+      <c r="DJ11">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -30036,11 +30315,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:DD17"/>
+  <dimension ref="A2:DE17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DE2" sqref="DE2"/>
+      <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DF2" sqref="DF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30050,7 +30329,7 @@
     <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:108" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:109" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -30373,8 +30652,11 @@
       <c r="DD2" s="9">
         <v>44032</v>
       </c>
+      <c r="DE2" s="9">
+        <v>44033</v>
+      </c>
     </row>
-    <row r="3" spans="1:108" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:109" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>36</v>
       </c>
@@ -30383,7 +30665,7 @@
       <c r="D3" s="9"/>
       <c r="CP3" s="4"/>
     </row>
-    <row r="4" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -30706,10 +30988,13 @@
         <v>11339</v>
       </c>
       <c r="DD4">
-        <v>1142</v>
+        <v>11427</v>
+      </c>
+      <c r="DE4">
+        <v>11529</v>
       </c>
     </row>
-    <row r="5" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -31034,8 +31319,11 @@
       <c r="DD5">
         <v>281</v>
       </c>
+      <c r="DE5">
+        <v>250</v>
+      </c>
     </row>
-    <row r="6" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -31360,8 +31648,11 @@
       <c r="DD6">
         <v>2325</v>
       </c>
+      <c r="DE6">
+        <v>2343</v>
+      </c>
     </row>
-    <row r="7" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -31686,8 +31977,11 @@
       <c r="DD7">
         <v>5591</v>
       </c>
+      <c r="DE7">
+        <v>5637</v>
+      </c>
     </row>
-    <row r="8" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -32012,8 +32306,11 @@
       <c r="DD8">
         <v>177</v>
       </c>
+      <c r="DE8">
+        <v>178</v>
+      </c>
     </row>
-    <row r="9" spans="1:108" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:109" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -32338,8 +32635,11 @@
       <c r="DD9">
         <v>27</v>
       </c>
+      <c r="DE9">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:108" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:109" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -32660,8 +32960,11 @@
       <c r="DD10">
         <v>30</v>
       </c>
+      <c r="DE10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="11" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -32986,8 +33289,11 @@
       <c r="DD11">
         <v>2907</v>
       </c>
+      <c r="DE11">
+        <v>2976</v>
+      </c>
     </row>
-    <row r="12" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -33312,8 +33618,11 @@
       <c r="DD12">
         <v>89</v>
       </c>
+      <c r="DE12">
+        <v>88</v>
+      </c>
     </row>
-    <row r="13" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -33324,7 +33633,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -33649,8 +33958,11 @@
       <c r="DD14">
         <v>1515</v>
       </c>
+      <c r="DE14">
+        <v>1540</v>
+      </c>
     </row>
-    <row r="15" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -33975,8 +34287,11 @@
       <c r="DD15">
         <v>3104</v>
       </c>
+      <c r="DE15">
+        <v>3116</v>
+      </c>
     </row>
-    <row r="16" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -34301,8 +34616,11 @@
       <c r="DD16">
         <v>6791</v>
       </c>
+      <c r="DE16">
+        <v>6857</v>
+      </c>
     </row>
-    <row r="17" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -34626,6 +34944,9 @@
       </c>
       <c r="DD17">
         <v>17</v>
+      </c>
+      <c r="DE17">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -34636,11 +34957,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:DD9"/>
+  <dimension ref="A1:DE9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DE1" sqref="DE1"/>
+      <selection pane="topRight" activeCell="DF1" sqref="DF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34649,7 +34970,7 @@
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:109" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -34971,14 +35292,17 @@
       <c r="DD1" s="9">
         <v>44032</v>
       </c>
+      <c r="DE1" s="9">
+        <v>44033</v>
+      </c>
     </row>
-    <row r="2" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -35304,8 +35628,11 @@
       <c r="DD3">
         <v>580</v>
       </c>
+      <c r="DE3">
+        <v>580</v>
+      </c>
     </row>
-    <row r="4" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -35630,8 +35957,11 @@
       <c r="DD4">
         <v>8</v>
       </c>
+      <c r="DE4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:108" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:109" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -35956,8 +36286,11 @@
       <c r="DD5">
         <v>428</v>
       </c>
+      <c r="DE5">
+        <v>428</v>
+      </c>
     </row>
-    <row r="6" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -36282,8 +36615,11 @@
       <c r="DD6">
         <v>76</v>
       </c>
+      <c r="DE6">
+        <v>76</v>
+      </c>
     </row>
-    <row r="7" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -36608,8 +36944,11 @@
       <c r="DD7">
         <v>62</v>
       </c>
+      <c r="DE7">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -36934,8 +37273,11 @@
       <c r="DD8">
         <v>3</v>
       </c>
+      <c r="DE8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:108" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:109" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -36980,11 +37322,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:CV5"/>
+  <dimension ref="A1:CW5"/>
   <sheetViews>
     <sheetView zoomScale="95" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CW1" sqref="CW1"/>
+      <selection pane="topRight" activeCell="CX1" sqref="CX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36992,7 +37334,7 @@
     <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -37290,13 +37632,16 @@
       <c r="CV1" s="9">
         <v>44032</v>
       </c>
+      <c r="CW1" s="9">
+        <v>44033</v>
+      </c>
     </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
@@ -37597,8 +37942,11 @@
       <c r="CV3">
         <v>580</v>
       </c>
+      <c r="CW3">
+        <v>580</v>
+      </c>
     </row>
-    <row r="4" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>153</v>
       </c>
@@ -37899,8 +38247,11 @@
       <c r="CV4">
         <v>246</v>
       </c>
+      <c r="CW4">
+        <v>246</v>
+      </c>
     </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>152</v>
       </c>
@@ -38199,6 +38550,9 @@
         <v>333</v>
       </c>
       <c r="CV5">
+        <v>334</v>
+      </c>
+      <c r="CW5">
         <v>334</v>
       </c>
     </row>
@@ -38210,11 +38564,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:CV11"/>
+  <dimension ref="A1:CX11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CW1" sqref="CW1"/>
+      <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CX1" sqref="CX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38222,7 +38576,7 @@
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:102" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -38520,13 +38874,19 @@
       <c r="CV1" s="9">
         <v>44032</v>
       </c>
+      <c r="CW1" s="9">
+        <v>44033</v>
+      </c>
+      <c r="CX1" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -38827,8 +39187,11 @@
       <c r="CV3">
         <v>580</v>
       </c>
+      <c r="CW3">
+        <v>580</v>
+      </c>
     </row>
-    <row r="4" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>143</v>
       </c>
@@ -39129,8 +39492,11 @@
       <c r="CV4">
         <v>0</v>
       </c>
+      <c r="CW4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>144</v>
       </c>
@@ -39431,8 +39797,11 @@
       <c r="CV5">
         <v>3</v>
       </c>
+      <c r="CW5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>145</v>
       </c>
@@ -39733,8 +40102,11 @@
       <c r="CV6">
         <v>8</v>
       </c>
+      <c r="CW6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>146</v>
       </c>
@@ -40035,8 +40407,11 @@
       <c r="CV7">
         <v>20</v>
       </c>
+      <c r="CW7">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>147</v>
       </c>
@@ -40337,8 +40712,11 @@
       <c r="CV8">
         <v>67</v>
       </c>
+      <c r="CW8">
+        <v>67</v>
+      </c>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>148</v>
       </c>
@@ -40639,8 +41017,11 @@
       <c r="CV9">
         <v>136</v>
       </c>
+      <c r="CW9">
+        <v>136</v>
+      </c>
     </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>149</v>
       </c>
@@ -40941,8 +41322,11 @@
       <c r="CV10">
         <v>147</v>
       </c>
+      <c r="CW10">
+        <v>147</v>
+      </c>
     </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>150</v>
       </c>
@@ -41241,6 +41625,9 @@
         <v>199</v>
       </c>
       <c r="CV11">
+        <v>199</v>
+      </c>
+      <c r="CW11">
         <v>199</v>
       </c>
     </row>
@@ -41252,11 +41639,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A2:CP13"/>
+  <dimension ref="A2:CR13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CQ2" sqref="CQ2"/>
+      <selection pane="topRight" activeCell="CR2" sqref="CR2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41265,7 +41652,7 @@
     <col min="57" max="57" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:94" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:96" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -41548,8 +41935,14 @@
       <c r="CP2" s="9">
         <v>44032</v>
       </c>
+      <c r="CQ2" s="9">
+        <v>44033</v>
+      </c>
+      <c r="CR2" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="3" spans="1:94" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -41832,8 +42225,11 @@
       <c r="CP3">
         <v>580</v>
       </c>
+      <c r="CQ3">
+        <v>580</v>
+      </c>
     </row>
-    <row r="4" spans="1:94" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -42116,8 +42512,11 @@
       <c r="CP4">
         <v>64</v>
       </c>
+      <c r="CQ4">
+        <v>64</v>
+      </c>
     </row>
-    <row r="5" spans="1:94" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -42400,8 +42799,11 @@
       <c r="CP5">
         <v>33</v>
       </c>
+      <c r="CQ5">
+        <v>33</v>
+      </c>
     </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -42684,8 +43086,11 @@
       <c r="CP6">
         <v>33</v>
       </c>
+      <c r="CQ6">
+        <v>33</v>
+      </c>
     </row>
-    <row r="7" spans="1:94" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -42968,8 +43373,11 @@
       <c r="CP7">
         <v>84</v>
       </c>
+      <c r="CQ7">
+        <v>84</v>
+      </c>
     </row>
-    <row r="8" spans="1:94" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -43252,8 +43660,11 @@
       <c r="CP8">
         <v>92</v>
       </c>
+      <c r="CQ8">
+        <v>92</v>
+      </c>
     </row>
-    <row r="9" spans="1:94" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -43536,8 +43947,11 @@
       <c r="CP9">
         <v>50</v>
       </c>
+      <c r="CQ9">
+        <v>50</v>
+      </c>
     </row>
-    <row r="10" spans="1:94" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -43820,8 +44234,11 @@
       <c r="CP10">
         <v>85</v>
       </c>
+      <c r="CQ10">
+        <v>85</v>
+      </c>
     </row>
-    <row r="11" spans="1:94" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -44104,8 +44521,11 @@
       <c r="CP11">
         <v>117</v>
       </c>
+      <c r="CQ11">
+        <v>117</v>
+      </c>
     </row>
-    <row r="12" spans="1:94" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:96" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -44388,8 +44808,11 @@
       <c r="CP12">
         <v>21</v>
       </c>
+      <c r="CQ12">
+        <v>21</v>
+      </c>
     </row>
-    <row r="13" spans="1:94" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -44670,6 +45093,9 @@
         <v>1</v>
       </c>
       <c r="CP13">
+        <v>1</v>
+      </c>
+      <c r="CQ13">
         <v>1</v>
       </c>
     </row>
@@ -44681,10 +45107,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:BL23"/>
+  <dimension ref="A1:BN23"/>
   <sheetViews>
-    <sheetView zoomScale="96" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:O3"/>
+    <sheetView topLeftCell="AU1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="BN5" sqref="BN5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44693,7 +45119,7 @@
     <col min="42" max="45" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
       <c r="C1" s="51" t="s">
         <v>180</v>
       </c>
@@ -44710,7 +45136,7 @@
       <c r="N1" s="51"/>
       <c r="O1" s="51"/>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
@@ -44725,7 +45151,7 @@
       <c r="N2" s="51"/>
       <c r="O2" s="51"/>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="E3" s="51"/>
@@ -44740,7 +45166,7 @@
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -44755,7 +45181,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -44942,8 +45368,14 @@
       <c r="BL5" s="9">
         <v>44032</v>
       </c>
+      <c r="BM5" s="9">
+        <v>44033</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>120</v>
       </c>
@@ -45133,8 +45565,11 @@
       <c r="BL6">
         <v>159</v>
       </c>
+      <c r="BM6">
+        <v>159</v>
+      </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -45324,8 +45759,11 @@
       <c r="BL7">
         <v>36</v>
       </c>
+      <c r="BM7">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
@@ -45333,7 +45771,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -45523,8 +45961,11 @@
       <c r="BL9">
         <v>1</v>
       </c>
+      <c r="BM9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>121</v>
       </c>
@@ -45714,8 +46155,11 @@
       <c r="BL10">
         <v>23</v>
       </c>
+      <c r="BM10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>122</v>
       </c>
@@ -45905,8 +46349,11 @@
       <c r="BL11">
         <v>9</v>
       </c>
+      <c r="BM11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -46096,13 +46543,16 @@
       <c r="BL12">
         <v>3</v>
       </c>
+      <c r="BM12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -46292,8 +46742,11 @@
       <c r="BL14">
         <v>1</v>
       </c>
+      <c r="BM14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -46483,8 +46936,11 @@
       <c r="BL15">
         <v>0</v>
       </c>
+      <c r="BM15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -46674,8 +47130,11 @@
       <c r="BL16">
         <v>3</v>
       </c>
+      <c r="BM16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -46865,8 +47324,11 @@
       <c r="BL17">
         <v>12</v>
       </c>
+      <c r="BM17">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -47056,8 +47518,11 @@
       <c r="BL18">
         <v>3</v>
       </c>
+      <c r="BM18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -47247,8 +47712,11 @@
       <c r="BL19">
         <v>2</v>
       </c>
+      <c r="BM19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -47438,8 +47906,11 @@
       <c r="BL20">
         <v>2</v>
       </c>
+      <c r="BM20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -47629,8 +48100,11 @@
       <c r="BL21">
         <v>6</v>
       </c>
+      <c r="BM21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:64" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:65" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -47820,8 +48294,11 @@
       <c r="BL22">
         <v>4</v>
       </c>
+      <c r="BM22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:64" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:65" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>123</v>
       </c>
@@ -48009,6 +48486,9 @@
         <v>3</v>
       </c>
       <c r="BL23">
+        <v>3</v>
+      </c>
+      <c r="BM23">
         <v>3</v>
       </c>
     </row>
@@ -48608,6 +49088,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -48810,22 +49305,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -48842,29 +49347,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Results from July 23, 2020 02:34:11 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/work/WashingtonDC/data.xlsx
+++ b/workflow/python/work/WashingtonDC/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="8_{D8A8C525-9AD6-4328-8A76-D2E05990132D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E447C524-B713-4EF7-A1E4-0C5E15152980}"/>
+  <xr:revisionPtr revIDLastSave="424" documentId="8_{D8A8C525-9AD6-4328-8A76-D2E05990132D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{62A1C24C-0E4A-4805-8179-40F00075A7FF}"/>
   <bookViews>
-    <workbookView xWindow="-216" yWindow="264" windowWidth="23040" windowHeight="7116" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-576" yWindow="504" windowWidth="23040" windowHeight="7116" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Community Cases Tested By OCME" sheetId="7" r:id="rId8"/>
     <sheet name="Long-Term Care Facilities" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="181">
   <si>
     <t>Testing</t>
   </si>
@@ -582,7 +582,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of July 21, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of July 22, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -1290,11 +1290,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EI119"/>
+  <dimension ref="A1:EJ119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="EA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EJ1" sqref="EJ1"/>
+      <selection pane="topRight" activeCell="EK1" sqref="EK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1310,10 +1310,10 @@
     <col min="98" max="102" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="104" max="118" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="128" max="139" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="128" max="140" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:140" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1725,8 +1725,11 @@
       <c r="EI1" s="48">
         <v>44033</v>
       </c>
+      <c r="EJ1" s="48">
+        <v>44034</v>
+      </c>
     </row>
-    <row r="2" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:140" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1750,7 +1753,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2147,8 +2150,11 @@
       <c r="EI3">
         <v>159572</v>
       </c>
+      <c r="EJ3">
+        <v>162021</v>
+      </c>
     </row>
-    <row r="4" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2340,8 +2346,11 @@
       <c r="EI4">
         <v>113858</v>
       </c>
+      <c r="EJ4">
+        <v>115353</v>
+      </c>
     </row>
-    <row r="5" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2759,8 +2768,11 @@
       <c r="EI5">
         <v>11529</v>
       </c>
+      <c r="EJ5">
+        <v>11571</v>
+      </c>
     </row>
-    <row r="6" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3160,8 +3172,11 @@
       <c r="EI6">
         <v>580</v>
       </c>
+      <c r="EJ6">
+        <v>581</v>
+      </c>
     </row>
-    <row r="7" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3531,11 +3546,14 @@
       <c r="EI7">
         <v>1974</v>
       </c>
+      <c r="EJ7">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="8" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3797,8 +3815,11 @@
       <c r="EI9">
         <v>345</v>
       </c>
+      <c r="EJ9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -4162,8 +4183,11 @@
       <c r="EI10">
         <v>80</v>
       </c>
+      <c r="EJ10">
+        <v>76</v>
+      </c>
     </row>
-    <row r="11" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4527,8 +4551,11 @@
       <c r="EI11">
         <v>440</v>
       </c>
+      <c r="EJ11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4892,8 +4919,11 @@
       <c r="EI12">
         <v>184</v>
       </c>
+      <c r="EJ12">
+        <v>179</v>
+      </c>
     </row>
-    <row r="13" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -5257,8 +5287,11 @@
       <c r="EI13">
         <v>256</v>
       </c>
+      <c r="EJ13">
+        <v>261</v>
+      </c>
     </row>
-    <row r="14" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -5484,8 +5517,11 @@
       <c r="EI14">
         <v>81</v>
       </c>
+      <c r="EJ14">
+        <v>91</v>
+      </c>
     </row>
-    <row r="15" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -5681,8 +5717,11 @@
       <c r="EI15">
         <v>18</v>
       </c>
+      <c r="EJ15">
+        <v>22</v>
+      </c>
     </row>
-    <row r="16" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -5908,8 +5947,11 @@
       <c r="EI16">
         <v>2005</v>
       </c>
+      <c r="EJ16">
+        <v>2024</v>
+      </c>
     </row>
-    <row r="17" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -6135,13 +6177,16 @@
       <c r="EI17" s="23">
         <v>0.81</v>
       </c>
+      <c r="EJ17" s="23">
+        <v>0.81</v>
+      </c>
     </row>
-    <row r="19" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:140" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -6149,7 +6194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -6513,8 +6558,11 @@
       <c r="EI21">
         <v>122</v>
       </c>
+      <c r="EJ21">
+        <v>123</v>
+      </c>
     </row>
-    <row r="22" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -6824,8 +6872,11 @@
       <c r="EI22">
         <v>6</v>
       </c>
+      <c r="EJ22">
+        <v>8</v>
+      </c>
     </row>
-    <row r="23" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -7135,8 +7186,11 @@
       <c r="EI23">
         <v>116</v>
       </c>
+      <c r="EJ23">
+        <v>115</v>
+      </c>
     </row>
-    <row r="24" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -7491,8 +7545,11 @@
       <c r="EI24">
         <v>59</v>
       </c>
+      <c r="EJ24">
+        <v>57</v>
+      </c>
     </row>
-    <row r="25" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -7847,8 +7904,11 @@
       <c r="EI25">
         <v>65</v>
       </c>
+      <c r="EJ25">
+        <v>65</v>
+      </c>
     </row>
-    <row r="26" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -8203,13 +8263,16 @@
       <c r="EI26">
         <v>1758</v>
       </c>
+      <c r="EJ26">
+        <v>1763</v>
+      </c>
     </row>
-    <row r="28" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:140" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -8573,8 +8636,11 @@
       <c r="EI29">
         <v>180</v>
       </c>
+      <c r="EJ29">
+        <v>184</v>
+      </c>
     </row>
-    <row r="30" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -8884,8 +8950,11 @@
       <c r="EI30">
         <v>40</v>
       </c>
+      <c r="EJ30">
+        <v>43</v>
+      </c>
     </row>
-    <row r="31" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -9195,8 +9264,11 @@
       <c r="EI31">
         <v>139</v>
       </c>
+      <c r="EJ31">
+        <v>140</v>
+      </c>
     </row>
-    <row r="32" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -9551,8 +9623,11 @@
       <c r="EI32">
         <v>107</v>
       </c>
+      <c r="EJ32">
+        <v>109</v>
+      </c>
     </row>
-    <row r="33" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -9907,8 +9982,11 @@
       <c r="EI33">
         <v>147</v>
       </c>
+      <c r="EJ33">
+        <v>152</v>
+      </c>
     </row>
-    <row r="34" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -10263,8 +10341,11 @@
       <c r="EI34">
         <v>1449</v>
       </c>
+      <c r="EJ34">
+        <v>1455</v>
+      </c>
     </row>
-    <row r="35" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -10400,13 +10481,16 @@
       <c r="EI35">
         <v>1</v>
       </c>
+      <c r="EJ35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:140" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -10758,8 +10842,11 @@
       <c r="EI38">
         <v>90</v>
       </c>
+      <c r="EJ38">
+        <v>90</v>
+      </c>
     </row>
-    <row r="39" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -11063,8 +11150,11 @@
       <c r="EI39">
         <v>4</v>
       </c>
+      <c r="EJ39">
+        <v>4</v>
+      </c>
     </row>
-    <row r="40" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -11368,8 +11458,11 @@
       <c r="EI40">
         <v>85</v>
       </c>
+      <c r="EJ40">
+        <v>85</v>
+      </c>
     </row>
-    <row r="41" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -11718,8 +11811,11 @@
       <c r="EI41">
         <v>0</v>
       </c>
+      <c r="EJ41">
+        <v>5</v>
+      </c>
     </row>
-    <row r="42" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -12065,8 +12161,11 @@
       <c r="EI42">
         <v>4</v>
       </c>
+      <c r="EJ42">
+        <v>9</v>
+      </c>
     </row>
-    <row r="43" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -12418,8 +12517,11 @@
       <c r="EI43">
         <v>296</v>
       </c>
+      <c r="EJ43">
+        <v>296</v>
+      </c>
     </row>
-    <row r="44" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -12705,16 +12807,19 @@
       <c r="EI44">
         <v>1</v>
       </c>
+      <c r="EJ44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:140" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -13072,8 +13177,11 @@
       <c r="EI47">
         <v>208</v>
       </c>
+      <c r="EJ47">
+        <v>208</v>
+      </c>
     </row>
-    <row r="48" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -13383,8 +13491,11 @@
       <c r="EI48">
         <v>1</v>
       </c>
+      <c r="EJ48">
+        <v>1</v>
+      </c>
     </row>
-    <row r="49" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -13694,8 +13805,11 @@
       <c r="EI49">
         <v>200</v>
       </c>
+      <c r="EJ49">
+        <v>200</v>
+      </c>
     </row>
-    <row r="50" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -14050,8 +14164,11 @@
       <c r="EI50">
         <v>59</v>
       </c>
+      <c r="EJ50">
+        <v>60</v>
+      </c>
     </row>
-    <row r="51" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -14361,8 +14478,11 @@
       <c r="EI51">
         <v>59</v>
       </c>
+      <c r="EJ51">
+        <v>61</v>
+      </c>
     </row>
-    <row r="52" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -14669,8 +14789,11 @@
       <c r="EI52">
         <v>1226</v>
       </c>
+      <c r="EJ52">
+        <v>1231</v>
+      </c>
     </row>
-    <row r="53" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -14971,16 +15094,19 @@
       <c r="EI53">
         <v>1</v>
       </c>
+      <c r="EJ53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:140" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -15323,8 +15449,11 @@
       <c r="EI56">
         <v>35</v>
       </c>
+      <c r="EJ56">
+        <v>35</v>
+      </c>
     </row>
-    <row r="57" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -15631,8 +15760,11 @@
       <c r="EI57">
         <v>3</v>
       </c>
+      <c r="EJ57">
+        <v>2</v>
+      </c>
     </row>
-    <row r="58" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -15939,8 +16071,11 @@
       <c r="EI58">
         <v>32</v>
       </c>
+      <c r="EJ58">
+        <v>32</v>
+      </c>
     </row>
-    <row r="59" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -16283,8 +16418,11 @@
       <c r="EI59">
         <v>1</v>
       </c>
+      <c r="EJ59">
+        <v>2</v>
+      </c>
     </row>
-    <row r="60" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -16627,8 +16765,11 @@
       <c r="EI60">
         <v>4</v>
       </c>
+      <c r="EJ60">
+        <v>4</v>
+      </c>
     </row>
-    <row r="61" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -16971,8 +17112,11 @@
       <c r="EI61">
         <v>177</v>
       </c>
+      <c r="EJ61">
+        <v>177</v>
+      </c>
     </row>
-    <row r="62" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -17273,8 +17417,11 @@
       <c r="EI62">
         <v>1</v>
       </c>
+      <c r="EJ62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -17617,8 +17764,11 @@
       <c r="EI64">
         <v>13</v>
       </c>
+      <c r="EJ64">
+        <v>13</v>
+      </c>
     </row>
-    <row r="65" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -17925,8 +18075,11 @@
       <c r="EI65">
         <v>0</v>
       </c>
+      <c r="EJ65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -18233,8 +18386,11 @@
       <c r="EI66">
         <v>13</v>
       </c>
+      <c r="EJ66">
+        <v>13</v>
+      </c>
     </row>
-    <row r="67" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -18577,8 +18733,11 @@
       <c r="EI67">
         <v>6</v>
       </c>
+      <c r="EJ67">
+        <v>66</v>
+      </c>
     </row>
-    <row r="68" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -18922,8 +19081,11 @@
       <c r="EI68">
         <v>66</v>
       </c>
+      <c r="EJ68">
+        <v>66</v>
+      </c>
     </row>
-    <row r="69" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -19266,8 +19428,11 @@
       <c r="EI69">
         <v>0</v>
       </c>
+      <c r="EJ69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -19574,11 +19739,14 @@
       <c r="EI70">
         <v>0</v>
       </c>
+      <c r="EJ70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>119</v>
       </c>
@@ -19771,8 +19939,11 @@
       <c r="EI72">
         <v>11</v>
       </c>
+      <c r="EJ72">
+        <v>111</v>
+      </c>
     </row>
-    <row r="73" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>119</v>
       </c>
@@ -19965,8 +20136,11 @@
       <c r="EI73">
         <v>2</v>
       </c>
+      <c r="EJ73">
+        <v>2</v>
+      </c>
     </row>
-    <row r="74" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
@@ -20159,8 +20333,11 @@
       <c r="EI74">
         <v>9</v>
       </c>
+      <c r="EJ74">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>119</v>
       </c>
@@ -20353,8 +20530,11 @@
       <c r="EI75">
         <v>3</v>
       </c>
+      <c r="EJ75">
+        <v>3</v>
+      </c>
     </row>
-    <row r="76" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -20547,8 +20727,11 @@
       <c r="EI76">
         <v>5</v>
       </c>
+      <c r="EJ76">
+        <v>5</v>
+      </c>
     </row>
-    <row r="77" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>119</v>
       </c>
@@ -20741,13 +20924,16 @@
       <c r="EI77">
         <v>48</v>
       </c>
+      <c r="EJ77">
+        <v>48</v>
+      </c>
     </row>
-    <row r="79" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:140" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -21093,8 +21279,11 @@
       <c r="EI80">
         <v>330</v>
       </c>
+      <c r="EJ80">
+        <v>330</v>
+      </c>
     </row>
-    <row r="81" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -21440,8 +21629,11 @@
       <c r="EI81">
         <v>78</v>
       </c>
+      <c r="EJ81">
+        <v>79</v>
+      </c>
     </row>
-    <row r="82" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -21787,8 +21979,11 @@
       <c r="EI82">
         <v>75</v>
       </c>
+      <c r="EJ82">
+        <v>75</v>
+      </c>
     </row>
-    <row r="83" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -22092,8 +22287,11 @@
       <c r="EI83">
         <v>21</v>
       </c>
+      <c r="EJ83">
+        <v>21</v>
+      </c>
     </row>
-    <row r="85" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -22439,8 +22637,11 @@
       <c r="EI85">
         <v>130</v>
       </c>
+      <c r="EJ85">
+        <v>130</v>
+      </c>
     </row>
-    <row r="86" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -22786,8 +22987,11 @@
       <c r="EI86">
         <v>5</v>
       </c>
+      <c r="EJ86">
+        <v>5</v>
+      </c>
     </row>
-    <row r="87" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -23133,8 +23337,11 @@
       <c r="EI87">
         <v>13</v>
       </c>
+      <c r="EJ87">
+        <v>13</v>
+      </c>
     </row>
-    <row r="88" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -23480,8 +23687,11 @@
       <c r="EI88">
         <v>269</v>
       </c>
+      <c r="EJ88">
+        <v>270</v>
+      </c>
     </row>
-    <row r="89" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -23701,8 +23911,11 @@
       <c r="EI89">
         <v>1</v>
       </c>
+      <c r="EJ89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -24048,8 +24261,11 @@
       <c r="EI91">
         <v>82</v>
       </c>
+      <c r="EJ91">
+        <v>82</v>
+      </c>
     </row>
-    <row r="92" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -24395,8 +24611,11 @@
       <c r="EI92">
         <v>0</v>
       </c>
+      <c r="EJ92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -24730,8 +24949,11 @@
       <c r="EI93">
         <v>191</v>
       </c>
+      <c r="EJ93">
+        <v>191</v>
+      </c>
     </row>
-    <row r="94" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -25077,8 +25299,11 @@
       <c r="EI94">
         <v>62</v>
       </c>
+      <c r="EJ94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -25382,11 +25607,14 @@
       <c r="EI95">
         <v>14</v>
       </c>
+      <c r="EJ95">
+        <v>14</v>
+      </c>
     </row>
-    <row r="96" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>130</v>
       </c>
@@ -25549,8 +25777,11 @@
       <c r="EI97">
         <v>14</v>
       </c>
+      <c r="EJ97">
+        <v>14</v>
+      </c>
     </row>
-    <row r="98" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>130</v>
       </c>
@@ -25713,8 +25944,11 @@
       <c r="EI98">
         <v>11</v>
       </c>
+      <c r="EJ98">
+        <v>11</v>
+      </c>
     </row>
-    <row r="99" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>130</v>
       </c>
@@ -25877,8 +26111,11 @@
       <c r="EI99">
         <v>55</v>
       </c>
+      <c r="EJ99">
+        <v>55</v>
+      </c>
     </row>
-    <row r="100" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
@@ -26041,8 +26278,11 @@
       <c r="EI100">
         <v>1</v>
       </c>
+      <c r="EJ100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -26307,8 +26547,11 @@
       <c r="EI102">
         <v>220</v>
       </c>
+      <c r="EJ102">
+        <v>223</v>
+      </c>
     </row>
-    <row r="103" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -26573,8 +26816,11 @@
       <c r="EI103">
         <v>140</v>
       </c>
+      <c r="EJ103">
+        <v>140</v>
+      </c>
     </row>
-    <row r="104" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:140" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -26837,6 +27083,9 @@
         <v>29</v>
       </c>
       <c r="EI104">
+        <v>29</v>
+      </c>
+      <c r="EJ104">
         <v>29</v>
       </c>
     </row>
@@ -26853,11 +27102,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:DJ11"/>
+  <dimension ref="A2:DK11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DK2" sqref="DK2"/>
+      <pane xSplit="1" topLeftCell="CS1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DL2" sqref="DL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26867,7 +27116,7 @@
     <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:114" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:115" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -27210,8 +27459,11 @@
       <c r="DJ2" s="9">
         <v>44033</v>
       </c>
+      <c r="DK2" s="9">
+        <v>44034</v>
+      </c>
     </row>
-    <row r="3" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -27554,8 +27806,11 @@
       <c r="DJ3">
         <v>1614</v>
       </c>
+      <c r="DK3">
+        <v>1624</v>
+      </c>
     </row>
-    <row r="4" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -27898,8 +28153,11 @@
       <c r="DJ4">
         <v>698</v>
       </c>
+      <c r="DK4">
+        <v>704</v>
+      </c>
     </row>
-    <row r="5" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -28242,8 +28500,11 @@
       <c r="DJ5">
         <v>543</v>
       </c>
+      <c r="DK5">
+        <v>540</v>
+      </c>
     </row>
-    <row r="6" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -28586,8 +28847,11 @@
       <c r="DJ6">
         <v>2316</v>
       </c>
+      <c r="DK6">
+        <v>2320</v>
+      </c>
     </row>
-    <row r="7" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -28930,8 +29194,11 @@
       <c r="DJ7">
         <v>1723</v>
       </c>
+      <c r="DK7">
+        <v>1732</v>
+      </c>
     </row>
-    <row r="8" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -29274,8 +29541,11 @@
       <c r="DJ8">
         <v>1077</v>
       </c>
+      <c r="DK8">
+        <v>1080</v>
+      </c>
     </row>
-    <row r="9" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -29618,8 +29888,11 @@
       <c r="DJ9">
         <v>1665</v>
       </c>
+      <c r="DK9">
+        <v>1669</v>
+      </c>
     </row>
-    <row r="10" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -29962,8 +30235,11 @@
       <c r="DJ10">
         <v>1686</v>
       </c>
+      <c r="DK10">
+        <v>1688</v>
+      </c>
     </row>
-    <row r="11" spans="1:114" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -30305,6 +30581,9 @@
       </c>
       <c r="DJ11">
         <v>207</v>
+      </c>
+      <c r="DK11">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -30315,11 +30594,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:DE17"/>
+  <dimension ref="A2:DF17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DF2" sqref="DF2"/>
+      <selection pane="topRight" activeCell="DG2" sqref="DG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30329,7 +30608,7 @@
     <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:109" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:110" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -30655,8 +30934,11 @@
       <c r="DE2" s="9">
         <v>44033</v>
       </c>
+      <c r="DF2" s="9">
+        <v>44034</v>
+      </c>
     </row>
-    <row r="3" spans="1:109" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:110" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>36</v>
       </c>
@@ -30665,7 +30947,7 @@
       <c r="D3" s="9"/>
       <c r="CP3" s="4"/>
     </row>
-    <row r="4" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -30993,8 +31275,11 @@
       <c r="DE4">
         <v>11529</v>
       </c>
+      <c r="DF4">
+        <v>11571</v>
+      </c>
     </row>
-    <row r="5" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -31322,8 +31607,11 @@
       <c r="DE5">
         <v>250</v>
       </c>
+      <c r="DF5">
+        <v>210</v>
+      </c>
     </row>
-    <row r="6" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -31651,8 +31939,11 @@
       <c r="DE6">
         <v>2343</v>
       </c>
+      <c r="DF6">
+        <v>2348</v>
+      </c>
     </row>
-    <row r="7" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -31980,8 +32271,11 @@
       <c r="DE7">
         <v>5637</v>
       </c>
+      <c r="DF7">
+        <v>5681</v>
+      </c>
     </row>
-    <row r="8" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -32309,8 +32603,11 @@
       <c r="DE8">
         <v>178</v>
       </c>
+      <c r="DF8">
+        <v>178</v>
+      </c>
     </row>
-    <row r="9" spans="1:109" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:110" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -32638,8 +32935,11 @@
       <c r="DE9">
         <v>27</v>
       </c>
+      <c r="DF9">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:109" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:110" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -32963,8 +33263,11 @@
       <c r="DE10">
         <v>30</v>
       </c>
+      <c r="DF10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="11" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -33292,8 +33595,11 @@
       <c r="DE11">
         <v>2976</v>
       </c>
+      <c r="DF11">
+        <v>3010</v>
+      </c>
     </row>
-    <row r="12" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -33621,8 +33927,11 @@
       <c r="DE12">
         <v>88</v>
       </c>
+      <c r="DF12">
+        <v>87</v>
+      </c>
     </row>
-    <row r="13" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -33633,7 +33942,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -33961,8 +34270,11 @@
       <c r="DE14">
         <v>1540</v>
       </c>
+      <c r="DF14">
+        <v>1533</v>
+      </c>
     </row>
-    <row r="15" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -34290,8 +34602,11 @@
       <c r="DE15">
         <v>3116</v>
       </c>
+      <c r="DF15">
+        <v>3121</v>
+      </c>
     </row>
-    <row r="16" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -34619,8 +34934,11 @@
       <c r="DE16">
         <v>6857</v>
       </c>
+      <c r="DF16">
+        <v>6901</v>
+      </c>
     </row>
-    <row r="17" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -34946,6 +35264,9 @@
         <v>17</v>
       </c>
       <c r="DE17">
+        <v>16</v>
+      </c>
+      <c r="DF17">
         <v>16</v>
       </c>
     </row>
@@ -34957,11 +35278,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:DE9"/>
+  <dimension ref="A1:DF9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DF1" sqref="DF1"/>
+      <selection pane="topRight" activeCell="DG1" sqref="DG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34970,7 +35291,7 @@
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:110" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -35295,14 +35616,17 @@
       <c r="DE1" s="9">
         <v>44033</v>
       </c>
+      <c r="DF1" s="9">
+        <v>44034</v>
+      </c>
     </row>
-    <row r="2" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -35631,8 +35955,11 @@
       <c r="DE3">
         <v>580</v>
       </c>
+      <c r="DF3">
+        <v>581</v>
+      </c>
     </row>
-    <row r="4" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -35960,8 +36287,11 @@
       <c r="DE4">
         <v>8</v>
       </c>
+      <c r="DF4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:109" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:110" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -36289,8 +36619,11 @@
       <c r="DE5">
         <v>428</v>
       </c>
+      <c r="DF5">
+        <v>429</v>
+      </c>
     </row>
-    <row r="6" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -36618,8 +36951,11 @@
       <c r="DE6">
         <v>76</v>
       </c>
+      <c r="DF6">
+        <v>76</v>
+      </c>
     </row>
-    <row r="7" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -36947,8 +37283,11 @@
       <c r="DE7">
         <v>62</v>
       </c>
+      <c r="DF7">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -37276,8 +37615,11 @@
       <c r="DE8">
         <v>6</v>
       </c>
+      <c r="DF8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -37322,11 +37664,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:CW5"/>
+  <dimension ref="A1:CX5"/>
   <sheetViews>
     <sheetView zoomScale="95" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CX1" sqref="CX1"/>
+      <pane xSplit="1" topLeftCell="CF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CY1" sqref="CY1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37334,7 +37676,7 @@
     <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:102" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -37635,13 +37977,16 @@
       <c r="CW1" s="9">
         <v>44033</v>
       </c>
+      <c r="CX1" s="9">
+        <v>44034</v>
+      </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
@@ -37945,8 +38290,11 @@
       <c r="CW3">
         <v>580</v>
       </c>
+      <c r="CX3">
+        <v>581</v>
+      </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>153</v>
       </c>
@@ -38250,8 +38598,11 @@
       <c r="CW4">
         <v>246</v>
       </c>
+      <c r="CX4">
+        <v>247</v>
+      </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>152</v>
       </c>
@@ -38553,6 +38904,9 @@
         <v>334</v>
       </c>
       <c r="CW5">
+        <v>334</v>
+      </c>
+      <c r="CX5">
         <v>334</v>
       </c>
     </row>
@@ -38568,7 +38922,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CX1" sqref="CX1"/>
+      <selection pane="topRight" activeCell="CY1" sqref="CY1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38877,8 +39231,8 @@
       <c r="CW1" s="9">
         <v>44033</v>
       </c>
-      <c r="CX1" s="2" t="s">
-        <v>129</v>
+      <c r="CX1" s="9">
+        <v>44034</v>
       </c>
     </row>
     <row r="2" spans="1:102" x14ac:dyDescent="0.3">
@@ -39190,6 +39544,9 @@
       <c r="CW3">
         <v>580</v>
       </c>
+      <c r="CX3">
+        <v>581</v>
+      </c>
     </row>
     <row r="4" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -39495,6 +39852,9 @@
       <c r="CW4">
         <v>0</v>
       </c>
+      <c r="CX4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -39800,6 +40160,9 @@
       <c r="CW5">
         <v>3</v>
       </c>
+      <c r="CX5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -40105,6 +40468,9 @@
       <c r="CW6">
         <v>8</v>
       </c>
+      <c r="CX6">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
@@ -40410,6 +40776,9 @@
       <c r="CW7">
         <v>20</v>
       </c>
+      <c r="CX7">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -40715,6 +41084,9 @@
       <c r="CW8">
         <v>67</v>
       </c>
+      <c r="CX8">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
@@ -41020,6 +41392,9 @@
       <c r="CW9">
         <v>136</v>
       </c>
+      <c r="CX9">
+        <v>136</v>
+      </c>
     </row>
     <row r="10" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
@@ -41325,6 +41700,9 @@
       <c r="CW10">
         <v>147</v>
       </c>
+      <c r="CX10">
+        <v>147</v>
+      </c>
     </row>
     <row r="11" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
@@ -41628,6 +42006,9 @@
         <v>199</v>
       </c>
       <c r="CW11">
+        <v>199</v>
+      </c>
+      <c r="CX11">
         <v>199</v>
       </c>
     </row>
@@ -41643,7 +42024,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CR2" sqref="CR2"/>
+      <selection pane="topRight" activeCell="CS2" sqref="CS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41938,8 +42319,8 @@
       <c r="CQ2" s="9">
         <v>44033</v>
       </c>
-      <c r="CR2" s="2" t="s">
-        <v>129</v>
+      <c r="CR2" s="9">
+        <v>44034</v>
       </c>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.3">
@@ -42228,6 +42609,9 @@
       <c r="CQ3">
         <v>580</v>
       </c>
+      <c r="CR3">
+        <v>581</v>
+      </c>
     </row>
     <row r="4" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
@@ -42513,6 +42897,9 @@
         <v>64</v>
       </c>
       <c r="CQ4">
+        <v>64</v>
+      </c>
+      <c r="CR4">
         <v>64</v>
       </c>
     </row>
@@ -42802,6 +43189,9 @@
       <c r="CQ5">
         <v>33</v>
       </c>
+      <c r="CR5">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
@@ -43089,6 +43479,9 @@
       <c r="CQ6">
         <v>33</v>
       </c>
+      <c r="CR6">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -43376,6 +43769,9 @@
       <c r="CQ7">
         <v>84</v>
       </c>
+      <c r="CR7">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -43663,6 +44059,9 @@
       <c r="CQ8">
         <v>92</v>
       </c>
+      <c r="CR8">
+        <v>92</v>
+      </c>
     </row>
     <row r="9" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
@@ -43950,6 +44349,9 @@
       <c r="CQ9">
         <v>50</v>
       </c>
+      <c r="CR9">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
@@ -44237,6 +44639,9 @@
       <c r="CQ10">
         <v>85</v>
       </c>
+      <c r="CR10">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
@@ -44524,6 +44929,9 @@
       <c r="CQ11">
         <v>117</v>
       </c>
+      <c r="CR11">
+        <v>117</v>
+      </c>
     </row>
     <row r="12" spans="1:96" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
@@ -44811,6 +45219,9 @@
       <c r="CQ12">
         <v>21</v>
       </c>
+      <c r="CR12">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
@@ -45096,6 +45507,9 @@
         <v>1</v>
       </c>
       <c r="CQ13">
+        <v>1</v>
+      </c>
+      <c r="CR13">
         <v>1</v>
       </c>
     </row>
@@ -45109,8 +45523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BN23"/>
   <sheetViews>
-    <sheetView topLeftCell="AU1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="BN5" sqref="BN5"/>
+    <sheetView topLeftCell="BK1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="BO5" sqref="BO5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45371,8 +45785,8 @@
       <c r="BM5" s="9">
         <v>44033</v>
       </c>
-      <c r="BN5" t="s">
-        <v>129</v>
+      <c r="BN5" s="9">
+        <v>44034</v>
       </c>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.3">
@@ -45568,6 +45982,9 @@
       <c r="BM6">
         <v>159</v>
       </c>
+      <c r="BN6">
+        <v>159</v>
+      </c>
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -45762,6 +46179,9 @@
       <c r="BM7">
         <v>36</v>
       </c>
+      <c r="BN7">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
@@ -45964,6 +46384,9 @@
       <c r="BM9">
         <v>1</v>
       </c>
+      <c r="BN9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
@@ -46158,6 +46581,9 @@
       <c r="BM10">
         <v>23</v>
       </c>
+      <c r="BN10">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
@@ -46352,6 +46778,9 @@
       <c r="BM11">
         <v>9</v>
       </c>
+      <c r="BN11">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
@@ -46546,6 +46975,9 @@
       <c r="BM12">
         <v>3</v>
       </c>
+      <c r="BN12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
@@ -46745,6 +47177,9 @@
       <c r="BM14">
         <v>1</v>
       </c>
+      <c r="BN14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
@@ -46939,6 +47374,9 @@
       <c r="BM15">
         <v>0</v>
       </c>
+      <c r="BN15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
@@ -47133,8 +47571,11 @@
       <c r="BM16">
         <v>3</v>
       </c>
+      <c r="BN16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -47327,8 +47768,11 @@
       <c r="BM17">
         <v>12</v>
       </c>
+      <c r="BN17">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -47521,8 +47965,11 @@
       <c r="BM18">
         <v>3</v>
       </c>
+      <c r="BN18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -47715,8 +48162,11 @@
       <c r="BM19">
         <v>2</v>
       </c>
+      <c r="BN19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -47909,8 +48359,11 @@
       <c r="BM20">
         <v>2</v>
       </c>
+      <c r="BN20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -48103,8 +48556,11 @@
       <c r="BM21">
         <v>6</v>
       </c>
+      <c r="BN21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:65" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:66" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -48297,8 +48753,11 @@
       <c r="BM22">
         <v>4</v>
       </c>
+      <c r="BN22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:65" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:66" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>123</v>
       </c>
@@ -48489,6 +48948,9 @@
         <v>3</v>
       </c>
       <c r="BM23">
+        <v>3</v>
+      </c>
+      <c r="BN23">
         <v>3</v>
       </c>
     </row>
@@ -49088,21 +49550,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C154F8D92A1190498EC67EE37256270A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a145d1f7d2fc6bfdea86e9d796031e6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e61eea9-d51d-4f9c-960b-1b037651d93e" xmlns:ns4="248ed0f8-11d3-4141-bb91-6b69a0801941" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87b2ee5a90a671ef9b646f531a040769" ns3:_="" ns4:_="">
     <xsd:import namespace="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
@@ -49305,32 +49752,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE449021-9205-42BF-A2AE-CC419CEBA6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -49347,4 +49784,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Results from July 27, 2020 07:42:32 AM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/work/WashingtonDC/data.xlsx
+++ b/workflow/python/work/WashingtonDC/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dcgovict-my.sharepoint.com/personal/ramona_yun1_dc_gov/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="424" documentId="8_{D8A8C525-9AD6-4328-8A76-D2E05990132D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{62A1C24C-0E4A-4805-8179-40F00075A7FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C609F5D3-EE66-4DAC-85C2-5C973AD2CD6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-576" yWindow="504" windowWidth="23040" windowHeight="7116" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="624" yWindow="2640" windowWidth="23040" windowHeight="7116" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="181">
   <si>
     <t>Testing</t>
   </si>
@@ -455,9 +455,6 @@
     <t>12; (9)</t>
   </si>
   <si>
-    <t>19; (2)</t>
-  </si>
-  <si>
     <t>5; (1)</t>
   </si>
   <si>
@@ -506,25 +503,10 @@
     <t>16; (11)</t>
   </si>
   <si>
-    <t>13; (10)</t>
-  </si>
-  <si>
-    <t>4; (3)</t>
-  </si>
-  <si>
     <t>57; (4)</t>
   </si>
   <si>
-    <t>24; (18)</t>
-  </si>
-  <si>
     <t>21; (17)</t>
-  </si>
-  <si>
-    <t>40; (36)</t>
-  </si>
-  <si>
-    <t>As of July 16, 2020</t>
   </si>
   <si>
     <t>10; (2)</t>
@@ -533,16 +515,10 @@
     <t>24; (1)</t>
   </si>
   <si>
-    <t>113; (61)</t>
-  </si>
-  <si>
     <t>8; (5)</t>
   </si>
   <si>
     <t>3; (1)</t>
-  </si>
-  <si>
-    <t>67; (44)</t>
   </si>
   <si>
     <t>22; (9)</t>
@@ -566,23 +542,47 @@
     <t>23; (9)</t>
   </si>
   <si>
-    <t>17; (1)</t>
+    <t>As of July 23, 2020</t>
   </si>
   <si>
-    <t>80; (2)</t>
+    <t>5; (3)</t>
   </si>
   <si>
-    <t>697; (214)</t>
+    <t>20; (3)</t>
   </si>
   <si>
-    <t>305; (166)</t>
+    <t>114; (62)</t>
   </si>
   <si>
-    <t>1002; (380)</t>
+    <t>68; (44)</t>
+  </si>
+  <si>
+    <t>25; (18)</t>
+  </si>
+  <si>
+    <t>41; (37)</t>
+  </si>
+  <si>
+    <t>18; (1)</t>
+  </si>
+  <si>
+    <t>81; (2)</t>
+  </si>
+  <si>
+    <t>20; (10)</t>
+  </si>
+  <si>
+    <t>701; (215)</t>
+  </si>
+  <si>
+    <t>316; (168)</t>
+  </si>
+  <si>
+    <t>1017; (383)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">As of July 22, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
+      <t xml:space="preserve">As of July 25, 2020, the Office of the Chief Medical Examiner (OCME) has submitted </t>
     </r>
     <r>
       <rPr>
@@ -771,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -895,6 +895,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1290,11 +1291,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EJ119"/>
+  <dimension ref="A1:EN119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="EA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EK1" sqref="EK1"/>
+      <pane xSplit="2" topLeftCell="EJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="EN1" sqref="EN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1310,10 +1311,10 @@
     <col min="98" max="102" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="104" max="118" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="128" max="140" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="128" max="143" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:144" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -1728,8 +1729,20 @@
       <c r="EJ1" s="48">
         <v>44034</v>
       </c>
+      <c r="EK1" s="48">
+        <v>44035</v>
+      </c>
+      <c r="EL1" s="48">
+        <v>44036</v>
+      </c>
+      <c r="EM1" s="48">
+        <v>44037</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="2" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:144" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1753,7 +1766,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2153,8 +2166,17 @@
       <c r="EJ3">
         <v>162021</v>
       </c>
+      <c r="EK3" s="51">
+        <v>165260</v>
+      </c>
+      <c r="EL3">
+        <v>169009</v>
+      </c>
+      <c r="EM3">
+        <v>171598</v>
+      </c>
     </row>
-    <row r="4" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2349,8 +2371,17 @@
       <c r="EJ4">
         <v>115353</v>
       </c>
+      <c r="EK4" s="51">
+        <v>115353</v>
+      </c>
+      <c r="EL4">
+        <v>119013</v>
+      </c>
+      <c r="EM4">
+        <v>120259</v>
+      </c>
     </row>
-    <row r="5" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2771,8 +2802,17 @@
       <c r="EJ5">
         <v>11571</v>
       </c>
+      <c r="EK5" s="51">
+        <v>11649</v>
+      </c>
+      <c r="EL5">
+        <v>11717</v>
+      </c>
+      <c r="EM5">
+        <v>11780</v>
+      </c>
     </row>
-    <row r="6" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3175,8 +3215,17 @@
       <c r="EJ6">
         <v>581</v>
       </c>
+      <c r="EK6">
+        <v>581</v>
+      </c>
+      <c r="EL6">
+        <v>581</v>
+      </c>
+      <c r="EM6">
+        <v>581</v>
+      </c>
     </row>
-    <row r="7" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3549,11 +3598,20 @@
       <c r="EJ7">
         <v>2020</v>
       </c>
+      <c r="EK7">
+        <v>9582</v>
+      </c>
+      <c r="EL7">
+        <v>9603</v>
+      </c>
+      <c r="EM7">
+        <v>9607</v>
+      </c>
     </row>
-    <row r="8" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3818,8 +3876,17 @@
       <c r="EJ9">
         <v>345</v>
       </c>
+      <c r="EK9">
+        <v>345</v>
+      </c>
+      <c r="EL9">
+        <v>345</v>
+      </c>
+      <c r="EM9">
+        <v>345</v>
+      </c>
     </row>
-    <row r="10" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -4186,8 +4253,17 @@
       <c r="EJ10">
         <v>76</v>
       </c>
+      <c r="EK10">
+        <v>79</v>
+      </c>
+      <c r="EL10">
+        <v>79</v>
+      </c>
+      <c r="EM10">
+        <v>86</v>
+      </c>
     </row>
-    <row r="11" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4554,8 +4630,17 @@
       <c r="EJ11">
         <v>440</v>
       </c>
+      <c r="EK11">
+        <v>440</v>
+      </c>
+      <c r="EL11">
+        <v>440</v>
+      </c>
+      <c r="EM11">
+        <v>440</v>
+      </c>
     </row>
-    <row r="12" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4922,8 +5007,17 @@
       <c r="EJ12">
         <v>179</v>
       </c>
+      <c r="EK12">
+        <v>178</v>
+      </c>
+      <c r="EL12">
+        <v>180</v>
+      </c>
+      <c r="EM12">
+        <v>171</v>
+      </c>
     </row>
-    <row r="13" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -5290,8 +5384,17 @@
       <c r="EJ13">
         <v>261</v>
       </c>
+      <c r="EK13">
+        <v>262</v>
+      </c>
+      <c r="EL13">
+        <v>260</v>
+      </c>
+      <c r="EM13">
+        <v>269</v>
+      </c>
     </row>
-    <row r="14" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -5520,8 +5623,17 @@
       <c r="EJ14">
         <v>91</v>
       </c>
+      <c r="EK14">
+        <v>97</v>
+      </c>
+      <c r="EL14">
+        <v>95</v>
+      </c>
+      <c r="EM14">
+        <v>85</v>
+      </c>
     </row>
-    <row r="15" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -5720,8 +5832,17 @@
       <c r="EJ15">
         <v>22</v>
       </c>
+      <c r="EK15">
+        <v>21</v>
+      </c>
+      <c r="EL15">
+        <v>28</v>
+      </c>
+      <c r="EM15">
+        <v>22</v>
+      </c>
     </row>
-    <row r="16" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -5950,8 +6071,17 @@
       <c r="EJ16">
         <v>2024</v>
       </c>
+      <c r="EK16">
+        <v>2009</v>
+      </c>
+      <c r="EL16">
+        <v>1988</v>
+      </c>
+      <c r="EM16">
+        <v>1881</v>
+      </c>
     </row>
-    <row r="17" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -6180,13 +6310,22 @@
       <c r="EJ17" s="23">
         <v>0.81</v>
       </c>
+      <c r="EK17" s="23">
+        <v>0.81</v>
+      </c>
+      <c r="EL17" s="23">
+        <v>0.79</v>
+      </c>
+      <c r="EM17" s="23">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="19" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:144" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -6194,7 +6333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -6561,8 +6700,20 @@
       <c r="EJ21">
         <v>123</v>
       </c>
+      <c r="EK21">
+        <v>124</v>
+      </c>
+      <c r="EL21">
+        <v>124</v>
+      </c>
+      <c r="EM21">
+        <v>124</v>
+      </c>
+      <c r="EN21" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="22" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -6875,8 +7026,17 @@
       <c r="EJ22">
         <v>8</v>
       </c>
+      <c r="EK22">
+        <v>7</v>
+      </c>
+      <c r="EL22">
+        <v>8</v>
+      </c>
+      <c r="EM22">
+        <v>8</v>
+      </c>
     </row>
-    <row r="23" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -7189,8 +7349,17 @@
       <c r="EJ23">
         <v>115</v>
       </c>
+      <c r="EK23">
+        <v>117</v>
+      </c>
+      <c r="EL23">
+        <v>116</v>
+      </c>
+      <c r="EM23">
+        <v>116</v>
+      </c>
     </row>
-    <row r="24" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -7548,8 +7717,17 @@
       <c r="EJ24">
         <v>57</v>
       </c>
+      <c r="EK24">
+        <v>67</v>
+      </c>
+      <c r="EL24">
+        <v>75</v>
+      </c>
+      <c r="EM24">
+        <v>75</v>
+      </c>
     </row>
-    <row r="25" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -7907,8 +8085,17 @@
       <c r="EJ25">
         <v>65</v>
       </c>
+      <c r="EK25">
+        <v>74</v>
+      </c>
+      <c r="EL25">
+        <v>83</v>
+      </c>
+      <c r="EM25">
+        <v>83</v>
+      </c>
     </row>
-    <row r="26" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -8266,13 +8453,22 @@
       <c r="EJ26">
         <v>1763</v>
       </c>
+      <c r="EK26">
+        <v>1765</v>
+      </c>
+      <c r="EL26">
+        <v>1765</v>
+      </c>
+      <c r="EM26">
+        <v>1765</v>
+      </c>
     </row>
-    <row r="28" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:144" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -8639,8 +8835,17 @@
       <c r="EJ29">
         <v>184</v>
       </c>
+      <c r="EK29">
+        <v>186</v>
+      </c>
+      <c r="EL29">
+        <v>187</v>
+      </c>
+      <c r="EM29">
+        <v>190</v>
+      </c>
     </row>
-    <row r="30" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -8953,8 +9158,17 @@
       <c r="EJ30">
         <v>43</v>
       </c>
+      <c r="EK30">
+        <v>42</v>
+      </c>
+      <c r="EL30">
+        <v>40</v>
+      </c>
+      <c r="EM30">
+        <v>43</v>
+      </c>
     </row>
-    <row r="31" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -9267,8 +9481,17 @@
       <c r="EJ31">
         <v>140</v>
       </c>
+      <c r="EK31">
+        <v>143</v>
+      </c>
+      <c r="EL31">
+        <v>146</v>
+      </c>
+      <c r="EM31">
+        <v>146</v>
+      </c>
     </row>
-    <row r="32" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:144" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -9626,8 +9849,17 @@
       <c r="EJ32">
         <v>109</v>
       </c>
+      <c r="EK32">
+        <v>111</v>
+      </c>
+      <c r="EL32">
+        <v>105</v>
+      </c>
+      <c r="EM32">
+        <v>98</v>
+      </c>
     </row>
-    <row r="33" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -9985,8 +10217,17 @@
       <c r="EJ33">
         <v>152</v>
       </c>
+      <c r="EK33">
+        <v>153</v>
+      </c>
+      <c r="EL33">
+        <v>145</v>
+      </c>
+      <c r="EM33">
+        <v>141</v>
+      </c>
     </row>
-    <row r="34" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -10344,8 +10585,17 @@
       <c r="EJ34">
         <v>1455</v>
       </c>
+      <c r="EK34">
+        <v>1464</v>
+      </c>
+      <c r="EL34">
+        <v>1479</v>
+      </c>
+      <c r="EM34">
+        <v>1485</v>
+      </c>
     </row>
-    <row r="35" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -10484,13 +10734,22 @@
       <c r="EJ35">
         <v>1</v>
       </c>
+      <c r="EK35">
+        <v>1</v>
+      </c>
+      <c r="EL35">
+        <v>1</v>
+      </c>
+      <c r="EM35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:143" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -10845,8 +11104,17 @@
       <c r="EJ38">
         <v>90</v>
       </c>
+      <c r="EK38">
+        <v>90</v>
+      </c>
+      <c r="EL38">
+        <v>90</v>
+      </c>
+      <c r="EM38">
+        <v>90</v>
+      </c>
     </row>
-    <row r="39" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -11153,8 +11421,17 @@
       <c r="EJ39">
         <v>4</v>
       </c>
+      <c r="EK39">
+        <v>4</v>
+      </c>
+      <c r="EL39">
+        <v>4</v>
+      </c>
+      <c r="EM39">
+        <v>4</v>
+      </c>
     </row>
-    <row r="40" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -11461,8 +11738,17 @@
       <c r="EJ40">
         <v>85</v>
       </c>
+      <c r="EK40">
+        <v>85</v>
+      </c>
+      <c r="EL40">
+        <v>85</v>
+      </c>
+      <c r="EM40">
+        <v>85</v>
+      </c>
     </row>
-    <row r="41" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -11814,8 +12100,17 @@
       <c r="EJ41">
         <v>5</v>
       </c>
+      <c r="EK41">
+        <v>5</v>
+      </c>
+      <c r="EL41">
+        <v>5</v>
+      </c>
+      <c r="EM41">
+        <v>5</v>
+      </c>
     </row>
-    <row r="42" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -12164,8 +12459,17 @@
       <c r="EJ42">
         <v>9</v>
       </c>
+      <c r="EK42">
+        <v>9</v>
+      </c>
+      <c r="EL42">
+        <v>9</v>
+      </c>
+      <c r="EM42">
+        <v>9</v>
+      </c>
     </row>
-    <row r="43" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -12520,8 +12824,17 @@
       <c r="EJ43">
         <v>296</v>
       </c>
+      <c r="EK43">
+        <v>296</v>
+      </c>
+      <c r="EL43">
+        <v>296</v>
+      </c>
+      <c r="EM43">
+        <v>296</v>
+      </c>
     </row>
-    <row r="44" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -12810,16 +13123,25 @@
       <c r="EJ44">
         <v>1</v>
       </c>
+      <c r="EK44">
+        <v>1</v>
+      </c>
+      <c r="EL44">
+        <v>1</v>
+      </c>
+      <c r="EM44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:143" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -13180,8 +13502,17 @@
       <c r="EJ47">
         <v>208</v>
       </c>
+      <c r="EK47">
+        <v>208</v>
+      </c>
+      <c r="EL47">
+        <v>208</v>
+      </c>
+      <c r="EM47">
+        <v>208</v>
+      </c>
     </row>
-    <row r="48" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -13494,8 +13825,17 @@
       <c r="EJ48">
         <v>1</v>
       </c>
+      <c r="EK48">
+        <v>1</v>
+      </c>
+      <c r="EL48">
+        <v>1</v>
+      </c>
+      <c r="EM48">
+        <v>1</v>
+      </c>
     </row>
-    <row r="49" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -13808,8 +14148,17 @@
       <c r="EJ49">
         <v>200</v>
       </c>
+      <c r="EK49">
+        <v>200</v>
+      </c>
+      <c r="EL49">
+        <v>200</v>
+      </c>
+      <c r="EM49">
+        <v>200</v>
+      </c>
     </row>
-    <row r="50" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -14167,8 +14516,17 @@
       <c r="EJ50">
         <v>60</v>
       </c>
+      <c r="EK50">
+        <v>62</v>
+      </c>
+      <c r="EL50">
+        <v>60</v>
+      </c>
+      <c r="EM50">
+        <v>70</v>
+      </c>
     </row>
-    <row r="51" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -14481,8 +14839,17 @@
       <c r="EJ51">
         <v>61</v>
       </c>
+      <c r="EK51">
+        <v>63</v>
+      </c>
+      <c r="EL51">
+        <v>61</v>
+      </c>
+      <c r="EM51">
+        <v>71</v>
+      </c>
     </row>
-    <row r="52" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -14792,8 +15159,17 @@
       <c r="EJ52">
         <v>1231</v>
       </c>
+      <c r="EK52">
+        <v>1225</v>
+      </c>
+      <c r="EL52">
+        <v>1227</v>
+      </c>
+      <c r="EM52">
+        <v>1224</v>
+      </c>
     </row>
-    <row r="53" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
@@ -15097,16 +15473,25 @@
       <c r="EJ53">
         <v>1</v>
       </c>
+      <c r="EK53">
+        <v>1</v>
+      </c>
+      <c r="EL53">
+        <v>1</v>
+      </c>
+      <c r="EM53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:143" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -15452,8 +15837,17 @@
       <c r="EJ56">
         <v>35</v>
       </c>
+      <c r="EK56">
+        <v>35</v>
+      </c>
+      <c r="EL56">
+        <v>36</v>
+      </c>
+      <c r="EM56">
+        <v>35</v>
+      </c>
     </row>
-    <row r="57" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -15763,8 +16157,17 @@
       <c r="EJ57">
         <v>2</v>
       </c>
+      <c r="EK57">
+        <v>1</v>
+      </c>
+      <c r="EL57">
+        <v>1</v>
+      </c>
+      <c r="EM57">
+        <v>1</v>
+      </c>
     </row>
-    <row r="58" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -16074,8 +16477,17 @@
       <c r="EJ58">
         <v>32</v>
       </c>
+      <c r="EK58">
+        <v>33</v>
+      </c>
+      <c r="EL58">
+        <v>34</v>
+      </c>
+      <c r="EM58">
+        <v>33</v>
+      </c>
     </row>
-    <row r="59" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -16421,8 +16833,17 @@
       <c r="EJ59">
         <v>2</v>
       </c>
+      <c r="EK59">
+        <v>0</v>
+      </c>
+      <c r="EL59">
+        <v>1</v>
+      </c>
+      <c r="EM59">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -16768,8 +17189,17 @@
       <c r="EJ60">
         <v>4</v>
       </c>
+      <c r="EK60">
+        <v>1</v>
+      </c>
+      <c r="EL60">
+        <v>2</v>
+      </c>
+      <c r="EM60">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -17115,8 +17545,17 @@
       <c r="EJ61">
         <v>177</v>
       </c>
+      <c r="EK61">
+        <v>179</v>
+      </c>
+      <c r="EL61">
+        <v>181</v>
+      </c>
+      <c r="EM61">
+        <v>180</v>
+      </c>
     </row>
-    <row r="62" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
@@ -17420,8 +17859,17 @@
       <c r="EJ62">
         <v>1</v>
       </c>
+      <c r="EK62">
+        <v>1</v>
+      </c>
+      <c r="EL62">
+        <v>1</v>
+      </c>
+      <c r="EM62">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>20</v>
       </c>
@@ -17767,8 +18215,17 @@
       <c r="EJ64">
         <v>13</v>
       </c>
+      <c r="EK64">
+        <v>14</v>
+      </c>
+      <c r="EL64">
+        <v>14</v>
+      </c>
+      <c r="EM64">
+        <v>14</v>
+      </c>
     </row>
-    <row r="65" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
@@ -18078,8 +18535,17 @@
       <c r="EJ65">
         <v>0</v>
       </c>
+      <c r="EK65">
+        <v>1</v>
+      </c>
+      <c r="EL65">
+        <v>1</v>
+      </c>
+      <c r="EM65">
+        <v>1</v>
+      </c>
     </row>
-    <row r="66" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
@@ -18389,8 +18855,17 @@
       <c r="EJ66">
         <v>13</v>
       </c>
+      <c r="EK66">
+        <v>13</v>
+      </c>
+      <c r="EL66">
+        <v>13</v>
+      </c>
+      <c r="EM66">
+        <v>13</v>
+      </c>
     </row>
-    <row r="67" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -18736,8 +19211,17 @@
       <c r="EJ67">
         <v>66</v>
       </c>
+      <c r="EK67">
+        <v>66</v>
+      </c>
+      <c r="EL67">
+        <v>65</v>
+      </c>
+      <c r="EM67">
+        <v>65</v>
+      </c>
     </row>
-    <row r="68" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -19084,8 +19568,17 @@
       <c r="EJ68">
         <v>66</v>
       </c>
+      <c r="EK68">
+        <v>67</v>
+      </c>
+      <c r="EL68">
+        <v>66</v>
+      </c>
+      <c r="EM68">
+        <v>66</v>
+      </c>
     </row>
-    <row r="69" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -19431,8 +19924,17 @@
       <c r="EJ69">
         <v>0</v>
       </c>
+      <c r="EK69">
+        <v>0</v>
+      </c>
+      <c r="EL69">
+        <v>0</v>
+      </c>
+      <c r="EM69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -19742,11 +20244,20 @@
       <c r="EJ70">
         <v>0</v>
       </c>
+      <c r="EK70">
+        <v>0</v>
+      </c>
+      <c r="EL70">
+        <v>0</v>
+      </c>
+      <c r="EM70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>119</v>
       </c>
@@ -19940,10 +20451,19 @@
         <v>11</v>
       </c>
       <c r="EJ72">
-        <v>111</v>
+        <v>11</v>
+      </c>
+      <c r="EK72">
+        <v>12</v>
+      </c>
+      <c r="EL72">
+        <v>12</v>
+      </c>
+      <c r="EM72">
+        <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>119</v>
       </c>
@@ -20139,8 +20659,17 @@
       <c r="EJ73">
         <v>2</v>
       </c>
+      <c r="EK73">
+        <v>3</v>
+      </c>
+      <c r="EL73">
+        <v>3</v>
+      </c>
+      <c r="EM73">
+        <v>3</v>
+      </c>
     </row>
-    <row r="74" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>119</v>
       </c>
@@ -20336,8 +20865,17 @@
       <c r="EJ74">
         <v>9</v>
       </c>
+      <c r="EK74">
+        <v>9</v>
+      </c>
+      <c r="EL74">
+        <v>9</v>
+      </c>
+      <c r="EM74">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>119</v>
       </c>
@@ -20533,8 +21071,17 @@
       <c r="EJ75">
         <v>3</v>
       </c>
+      <c r="EK75">
+        <v>2</v>
+      </c>
+      <c r="EL75">
+        <v>6</v>
+      </c>
+      <c r="EM75">
+        <v>7</v>
+      </c>
     </row>
-    <row r="76" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>119</v>
       </c>
@@ -20730,8 +21277,17 @@
       <c r="EJ76">
         <v>5</v>
       </c>
+      <c r="EK76">
+        <v>5</v>
+      </c>
+      <c r="EL76">
+        <v>9</v>
+      </c>
+      <c r="EM76">
+        <v>10</v>
+      </c>
     </row>
-    <row r="77" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>119</v>
       </c>
@@ -20927,13 +21483,22 @@
       <c r="EJ77">
         <v>48</v>
       </c>
+      <c r="EK77">
+        <v>47</v>
+      </c>
+      <c r="EL77">
+        <v>51</v>
+      </c>
+      <c r="EM77">
+        <v>51</v>
+      </c>
     </row>
-    <row r="79" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:143" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -21282,8 +21847,17 @@
       <c r="EJ80">
         <v>330</v>
       </c>
+      <c r="EK80">
+        <v>331</v>
+      </c>
+      <c r="EL80">
+        <v>331</v>
+      </c>
+      <c r="EM80">
+        <v>331</v>
+      </c>
     </row>
-    <row r="81" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -21632,8 +22206,11 @@
       <c r="EJ81">
         <v>79</v>
       </c>
+      <c r="EK81">
+        <v>79</v>
+      </c>
     </row>
-    <row r="82" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -21982,8 +22559,11 @@
       <c r="EJ82">
         <v>75</v>
       </c>
+      <c r="EK82">
+        <v>74</v>
+      </c>
     </row>
-    <row r="83" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -22290,8 +22870,17 @@
       <c r="EJ83">
         <v>21</v>
       </c>
+      <c r="EK83">
+        <v>21</v>
+      </c>
+      <c r="EL83">
+        <v>21</v>
+      </c>
+      <c r="EM83">
+        <v>21</v>
+      </c>
     </row>
-    <row r="85" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -22640,8 +23229,17 @@
       <c r="EJ85">
         <v>130</v>
       </c>
+      <c r="EK85">
+        <v>130</v>
+      </c>
+      <c r="EL85">
+        <v>130</v>
+      </c>
+      <c r="EM85">
+        <v>130</v>
+      </c>
     </row>
-    <row r="86" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -22990,8 +23588,17 @@
       <c r="EJ86">
         <v>5</v>
       </c>
+      <c r="EK86">
+        <v>5</v>
+      </c>
+      <c r="EL86">
+        <v>5</v>
+      </c>
+      <c r="EM86">
+        <v>5</v>
+      </c>
     </row>
-    <row r="87" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>28</v>
       </c>
@@ -23340,8 +23947,17 @@
       <c r="EJ87">
         <v>13</v>
       </c>
+      <c r="EK87">
+        <v>13</v>
+      </c>
+      <c r="EL87">
+        <v>13</v>
+      </c>
+      <c r="EM87">
+        <v>13</v>
+      </c>
     </row>
-    <row r="88" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>28</v>
       </c>
@@ -23690,8 +24306,17 @@
       <c r="EJ88">
         <v>270</v>
       </c>
+      <c r="EK88">
+        <v>270</v>
+      </c>
+      <c r="EL88">
+        <v>270</v>
+      </c>
+      <c r="EM88">
+        <v>270</v>
+      </c>
     </row>
-    <row r="89" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -23914,8 +24539,17 @@
       <c r="EJ89">
         <v>1</v>
       </c>
+      <c r="EK89">
+        <v>1</v>
+      </c>
+      <c r="EL89">
+        <v>1</v>
+      </c>
+      <c r="EM89">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>29</v>
       </c>
@@ -24264,8 +24898,17 @@
       <c r="EJ91">
         <v>82</v>
       </c>
+      <c r="EK91">
+        <v>82</v>
+      </c>
+      <c r="EL91">
+        <v>82</v>
+      </c>
+      <c r="EM91">
+        <v>82</v>
+      </c>
     </row>
-    <row r="92" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
@@ -24614,8 +25257,17 @@
       <c r="EJ92">
         <v>0</v>
       </c>
+      <c r="EK92">
+        <v>0</v>
+      </c>
+      <c r="EL92">
+        <v>0</v>
+      </c>
+      <c r="EM92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>29</v>
       </c>
@@ -24952,8 +25604,17 @@
       <c r="EJ93">
         <v>191</v>
       </c>
+      <c r="EK93">
+        <v>191</v>
+      </c>
+      <c r="EL93">
+        <v>191</v>
+      </c>
+      <c r="EM93">
+        <v>191</v>
+      </c>
     </row>
-    <row r="94" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>29</v>
       </c>
@@ -25302,8 +25963,17 @@
       <c r="EJ94">
         <v>62</v>
       </c>
+      <c r="EK94">
+        <v>62</v>
+      </c>
+      <c r="EL94">
+        <v>62</v>
+      </c>
+      <c r="EM94">
+        <v>62</v>
+      </c>
     </row>
-    <row r="95" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>29</v>
       </c>
@@ -25610,11 +26280,20 @@
       <c r="EJ95">
         <v>14</v>
       </c>
+      <c r="EK95">
+        <v>14</v>
+      </c>
+      <c r="EL95">
+        <v>14</v>
+      </c>
+      <c r="EM95">
+        <v>14</v>
+      </c>
     </row>
-    <row r="96" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>130</v>
       </c>
@@ -25780,8 +26459,17 @@
       <c r="EJ97">
         <v>14</v>
       </c>
+      <c r="EK97">
+        <v>14</v>
+      </c>
+      <c r="EL97">
+        <v>14</v>
+      </c>
+      <c r="EM97">
+        <v>14</v>
+      </c>
     </row>
-    <row r="98" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>130</v>
       </c>
@@ -25947,8 +26635,17 @@
       <c r="EJ98">
         <v>11</v>
       </c>
+      <c r="EK98">
+        <v>11</v>
+      </c>
+      <c r="EL98">
+        <v>11</v>
+      </c>
+      <c r="EM98">
+        <v>11</v>
+      </c>
     </row>
-    <row r="99" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>130</v>
       </c>
@@ -26114,8 +26811,17 @@
       <c r="EJ99">
         <v>55</v>
       </c>
+      <c r="EK99">
+        <v>55</v>
+      </c>
+      <c r="EL99">
+        <v>55</v>
+      </c>
+      <c r="EM99">
+        <v>55</v>
+      </c>
     </row>
-    <row r="100" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
@@ -26281,8 +26987,17 @@
       <c r="EJ100">
         <v>1</v>
       </c>
+      <c r="EK100">
+        <v>1</v>
+      </c>
+      <c r="EL100">
+        <v>1</v>
+      </c>
+      <c r="EM100">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>79</v>
       </c>
@@ -26550,8 +27265,17 @@
       <c r="EJ102">
         <v>223</v>
       </c>
+      <c r="EK102">
+        <v>223</v>
+      </c>
+      <c r="EL102">
+        <v>223</v>
+      </c>
+      <c r="EM102">
+        <v>223</v>
+      </c>
     </row>
-    <row r="103" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>79</v>
       </c>
@@ -26819,8 +27543,17 @@
       <c r="EJ103">
         <v>140</v>
       </c>
+      <c r="EK103">
+        <v>140</v>
+      </c>
+      <c r="EL103">
+        <v>140</v>
+      </c>
+      <c r="EM103">
+        <v>140</v>
+      </c>
     </row>
-    <row r="104" spans="1:140" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:143" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
@@ -27086,6 +27819,15 @@
         <v>29</v>
       </c>
       <c r="EJ104">
+        <v>29</v>
+      </c>
+      <c r="EK104">
+        <v>29</v>
+      </c>
+      <c r="EL104">
+        <v>29</v>
+      </c>
+      <c r="EM104">
         <v>29</v>
       </c>
     </row>
@@ -27102,11 +27844,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:DK11"/>
+  <dimension ref="A2:DN11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CS1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DL2" sqref="DL2"/>
+      <pane xSplit="1" topLeftCell="DI1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DO2" sqref="DO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27116,7 +27858,7 @@
     <col min="15" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:115" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:118" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -27462,8 +28204,17 @@
       <c r="DK2" s="9">
         <v>44034</v>
       </c>
+      <c r="DL2" s="9">
+        <v>44035</v>
+      </c>
+      <c r="DM2" s="9">
+        <v>44036</v>
+      </c>
+      <c r="DN2" s="9">
+        <v>44037</v>
+      </c>
     </row>
-    <row r="3" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -27809,8 +28560,17 @@
       <c r="DK3">
         <v>1624</v>
       </c>
+      <c r="DL3">
+        <v>1635</v>
+      </c>
+      <c r="DM3">
+        <v>1642</v>
+      </c>
+      <c r="DN3">
+        <v>1652</v>
+      </c>
     </row>
-    <row r="4" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -28156,8 +28916,17 @@
       <c r="DK4">
         <v>704</v>
       </c>
+      <c r="DL4">
+        <v>714</v>
+      </c>
+      <c r="DM4">
+        <v>718</v>
+      </c>
+      <c r="DN4">
+        <v>727</v>
+      </c>
     </row>
-    <row r="5" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -28503,8 +29272,17 @@
       <c r="DK5">
         <v>540</v>
       </c>
+      <c r="DL5">
+        <v>542</v>
+      </c>
+      <c r="DM5">
+        <v>545</v>
+      </c>
+      <c r="DN5">
+        <v>549</v>
+      </c>
     </row>
-    <row r="6" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -28850,8 +29628,17 @@
       <c r="DK6">
         <v>2320</v>
       </c>
+      <c r="DL6">
+        <v>2329</v>
+      </c>
+      <c r="DM6">
+        <v>2342</v>
+      </c>
+      <c r="DN6">
+        <v>2352</v>
+      </c>
     </row>
-    <row r="7" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -29117,7 +29904,7 @@
         <v>1532</v>
       </c>
       <c r="CK7">
-        <v>540</v>
+        <v>1540</v>
       </c>
       <c r="CL7">
         <v>1546</v>
@@ -29197,8 +29984,17 @@
       <c r="DK7">
         <v>1732</v>
       </c>
+      <c r="DL7">
+        <v>1744</v>
+      </c>
+      <c r="DM7">
+        <v>1754</v>
+      </c>
+      <c r="DN7">
+        <v>1759</v>
+      </c>
     </row>
-    <row r="8" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -29544,8 +30340,17 @@
       <c r="DK8">
         <v>1080</v>
       </c>
+      <c r="DL8">
+        <v>1087</v>
+      </c>
+      <c r="DM8">
+        <v>1094</v>
+      </c>
+      <c r="DN8">
+        <v>1098</v>
+      </c>
     </row>
-    <row r="9" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -29891,8 +30696,17 @@
       <c r="DK9">
         <v>1669</v>
       </c>
+      <c r="DL9">
+        <v>1682</v>
+      </c>
+      <c r="DM9">
+        <v>1692</v>
+      </c>
+      <c r="DN9">
+        <v>1699</v>
+      </c>
     </row>
-    <row r="10" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -30238,8 +31052,17 @@
       <c r="DK10">
         <v>1688</v>
       </c>
+      <c r="DL10">
+        <v>1702</v>
+      </c>
+      <c r="DM10">
+        <v>1715</v>
+      </c>
+      <c r="DN10">
+        <v>1725</v>
+      </c>
     </row>
-    <row r="11" spans="1:115" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -30584,6 +31407,15 @@
       </c>
       <c r="DK11">
         <v>214</v>
+      </c>
+      <c r="DL11">
+        <v>214</v>
+      </c>
+      <c r="DM11">
+        <v>215</v>
+      </c>
+      <c r="DN11">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -30594,11 +31426,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:DF17"/>
+  <dimension ref="A2:DI17"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DG2" sqref="DG2"/>
+    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="DE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DJ2" sqref="DJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30608,7 +31440,7 @@
     <col min="10" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:110" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:113" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="12">
         <v>43926</v>
@@ -30937,8 +31769,17 @@
       <c r="DF2" s="9">
         <v>44034</v>
       </c>
+      <c r="DG2" s="9">
+        <v>44035</v>
+      </c>
+      <c r="DH2" s="9">
+        <v>44036</v>
+      </c>
+      <c r="DI2" s="9">
+        <v>44037</v>
+      </c>
     </row>
-    <row r="3" spans="1:110" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:113" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>36</v>
       </c>
@@ -30947,7 +31788,7 @@
       <c r="D3" s="9"/>
       <c r="CP3" s="4"/>
     </row>
-    <row r="4" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>49</v>
       </c>
@@ -31278,8 +32119,17 @@
       <c r="DF4">
         <v>11571</v>
       </c>
+      <c r="DG4">
+        <v>11649</v>
+      </c>
+      <c r="DH4">
+        <v>11717</v>
+      </c>
+      <c r="DI4" s="38">
+        <v>11780</v>
+      </c>
     </row>
-    <row r="5" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
@@ -31610,8 +32460,17 @@
       <c r="DF5">
         <v>210</v>
       </c>
+      <c r="DG5">
+        <v>176</v>
+      </c>
+      <c r="DH5">
+        <v>195</v>
+      </c>
+      <c r="DI5">
+        <v>204</v>
+      </c>
     </row>
-    <row r="6" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
@@ -31942,8 +32801,17 @@
       <c r="DF6">
         <v>2348</v>
       </c>
+      <c r="DG6">
+        <v>2367</v>
+      </c>
+      <c r="DH6">
+        <v>2378</v>
+      </c>
+      <c r="DI6" s="38">
+        <v>2389</v>
+      </c>
     </row>
-    <row r="7" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -32274,8 +33142,17 @@
       <c r="DF7">
         <v>5681</v>
       </c>
+      <c r="DG7">
+        <v>5750</v>
+      </c>
+      <c r="DH7">
+        <v>5781</v>
+      </c>
+      <c r="DI7" s="38">
+        <v>5802</v>
+      </c>
     </row>
-    <row r="8" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -32606,8 +33483,17 @@
       <c r="DF8">
         <v>178</v>
       </c>
+      <c r="DG8">
+        <v>182</v>
+      </c>
+      <c r="DH8">
+        <v>182</v>
+      </c>
+      <c r="DI8">
+        <v>183</v>
+      </c>
     </row>
-    <row r="9" spans="1:110" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:113" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -32938,8 +33824,17 @@
       <c r="DF9">
         <v>27</v>
       </c>
+      <c r="DG9">
+        <v>27</v>
+      </c>
+      <c r="DH9">
+        <v>28</v>
+      </c>
+      <c r="DI9">
+        <v>28</v>
+      </c>
     </row>
-    <row r="10" spans="1:110" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:113" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -33266,8 +34161,17 @@
       <c r="DF10">
         <v>30</v>
       </c>
+      <c r="DG10">
+        <v>30</v>
+      </c>
+      <c r="DH10">
+        <v>30</v>
+      </c>
+      <c r="DI10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="11" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>41</v>
       </c>
@@ -33598,8 +34502,17 @@
       <c r="DF11">
         <v>3010</v>
       </c>
+      <c r="DG11">
+        <v>3030</v>
+      </c>
+      <c r="DH11">
+        <v>3036</v>
+      </c>
+      <c r="DI11" s="38">
+        <v>3055</v>
+      </c>
     </row>
-    <row r="12" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
@@ -33930,8 +34843,17 @@
       <c r="DF12">
         <v>87</v>
       </c>
+      <c r="DG12">
+        <v>87</v>
+      </c>
+      <c r="DH12">
+        <v>87</v>
+      </c>
+      <c r="DI12">
+        <v>88</v>
+      </c>
     </row>
-    <row r="13" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -33941,8 +34863,9 @@
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
+      <c r="DI13" s="38"/>
     </row>
-    <row r="14" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
@@ -34273,8 +35196,17 @@
       <c r="DF14">
         <v>1533</v>
       </c>
+      <c r="DG14">
+        <v>1512</v>
+      </c>
+      <c r="DH14">
+        <v>1526</v>
+      </c>
+      <c r="DI14">
+        <v>1543</v>
+      </c>
     </row>
-    <row r="15" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>44</v>
       </c>
@@ -34605,8 +35537,17 @@
       <c r="DF15">
         <v>3121</v>
       </c>
+      <c r="DG15">
+        <v>3136</v>
+      </c>
+      <c r="DH15">
+        <v>3146</v>
+      </c>
+      <c r="DI15" s="38">
+        <v>3154</v>
+      </c>
     </row>
-    <row r="16" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -34937,8 +35878,17 @@
       <c r="DF16">
         <v>6901</v>
       </c>
+      <c r="DG16">
+        <v>6985</v>
+      </c>
+      <c r="DH16">
+        <v>7029</v>
+      </c>
+      <c r="DI16" s="38">
+        <v>7067</v>
+      </c>
     </row>
-    <row r="17" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
@@ -35267,6 +36217,15 @@
         <v>16</v>
       </c>
       <c r="DF17">
+        <v>16</v>
+      </c>
+      <c r="DG17">
+        <v>16</v>
+      </c>
+      <c r="DH17">
+        <v>16</v>
+      </c>
+      <c r="DI17" s="38">
         <v>16</v>
       </c>
     </row>
@@ -35278,11 +36237,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:DF9"/>
+  <dimension ref="A1:DJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DG1" sqref="DG1"/>
+      <pane xSplit="1" topLeftCell="DD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DJ1" sqref="DJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35291,7 +36250,7 @@
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:110" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:114" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43926</v>
       </c>
@@ -35619,14 +36578,26 @@
       <c r="DF1" s="9">
         <v>44034</v>
       </c>
+      <c r="DG1" s="9">
+        <v>44035</v>
+      </c>
+      <c r="DH1" s="9">
+        <v>44036</v>
+      </c>
+      <c r="DI1" s="9">
+        <v>44037</v>
+      </c>
+      <c r="DJ1" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="2" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -35958,8 +36929,17 @@
       <c r="DF3">
         <v>581</v>
       </c>
+      <c r="DG3">
+        <v>581</v>
+      </c>
+      <c r="DH3">
+        <v>581</v>
+      </c>
+      <c r="DI3">
+        <v>581</v>
+      </c>
     </row>
-    <row r="4" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
@@ -36290,8 +37270,17 @@
       <c r="DF4">
         <v>8</v>
       </c>
+      <c r="DG4">
+        <v>8</v>
+      </c>
+      <c r="DH4">
+        <v>8</v>
+      </c>
+      <c r="DI4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:110" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:114" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
@@ -36622,8 +37611,17 @@
       <c r="DF5">
         <v>429</v>
       </c>
+      <c r="DG5">
+        <v>429</v>
+      </c>
+      <c r="DH5">
+        <v>429</v>
+      </c>
+      <c r="DI5">
+        <v>429</v>
+      </c>
     </row>
-    <row r="6" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -36954,8 +37952,17 @@
       <c r="DF6">
         <v>76</v>
       </c>
+      <c r="DG6">
+        <v>76</v>
+      </c>
+      <c r="DH6">
+        <v>76</v>
+      </c>
+      <c r="DI6">
+        <v>76</v>
+      </c>
     </row>
-    <row r="7" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -37286,8 +38293,17 @@
       <c r="DF7">
         <v>62</v>
       </c>
+      <c r="DG7">
+        <v>62</v>
+      </c>
+      <c r="DH7">
+        <v>62</v>
+      </c>
+      <c r="DI7">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>34</v>
       </c>
@@ -37618,8 +38634,17 @@
       <c r="DF8">
         <v>6</v>
       </c>
+      <c r="DG8">
+        <v>6</v>
+      </c>
+      <c r="DH8">
+        <v>6</v>
+      </c>
+      <c r="DI8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:114" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
@@ -37664,11 +38689,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:CX5"/>
+  <dimension ref="A1:DB5"/>
   <sheetViews>
     <sheetView zoomScale="95" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CY1" sqref="CY1"/>
+      <pane xSplit="1" topLeftCell="CH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DB1" sqref="DB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37676,7 +38701,7 @@
     <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:106" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -37980,13 +39005,25 @@
       <c r="CX1" s="9">
         <v>44034</v>
       </c>
+      <c r="CY1" s="9">
+        <v>44035</v>
+      </c>
+      <c r="CZ1" s="9">
+        <v>44036</v>
+      </c>
+      <c r="DA1" s="9">
+        <v>44037</v>
+      </c>
+      <c r="DB1" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="2" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
@@ -38293,10 +39330,19 @@
       <c r="CX3">
         <v>581</v>
       </c>
+      <c r="CY3">
+        <v>581</v>
+      </c>
+      <c r="CZ3">
+        <v>581</v>
+      </c>
+      <c r="DA3">
+        <v>581</v>
+      </c>
     </row>
-    <row r="4" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4">
         <v>26</v>
@@ -38601,10 +39647,19 @@
       <c r="CX4">
         <v>247</v>
       </c>
+      <c r="CY4">
+        <v>247</v>
+      </c>
+      <c r="CZ4">
+        <v>247</v>
+      </c>
+      <c r="DA4">
+        <v>247</v>
+      </c>
     </row>
-    <row r="5" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -38907,6 +39962,15 @@
         <v>334</v>
       </c>
       <c r="CX5">
+        <v>334</v>
+      </c>
+      <c r="CY5">
+        <v>334</v>
+      </c>
+      <c r="CZ5">
+        <v>334</v>
+      </c>
+      <c r="DA5">
         <v>334</v>
       </c>
     </row>
@@ -38918,11 +39982,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:CX11"/>
+  <dimension ref="A1:DB11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CY1" sqref="CY1"/>
+      <pane xSplit="1" topLeftCell="CK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DB1" sqref="DB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38930,7 +39994,7 @@
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:106" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9">
         <v>43934</v>
       </c>
@@ -39234,13 +40298,25 @@
       <c r="CX1" s="9">
         <v>44034</v>
       </c>
+      <c r="CY1" s="9">
+        <v>44035</v>
+      </c>
+      <c r="CZ1" s="9">
+        <v>44036</v>
+      </c>
+      <c r="DA1" s="9">
+        <v>44037</v>
+      </c>
+      <c r="DB1" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="2" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -39547,318 +40623,336 @@
       <c r="CX3">
         <v>581</v>
       </c>
+      <c r="CY3">
+        <v>581</v>
+      </c>
+      <c r="CZ3">
+        <v>581</v>
+      </c>
+      <c r="DA3">
+        <v>581</v>
+      </c>
     </row>
-    <row r="4" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <v>0</v>
+      </c>
+      <c r="BA4">
+        <v>0</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BD4">
+        <v>0</v>
+      </c>
+      <c r="BE4">
+        <v>0</v>
+      </c>
+      <c r="BF4">
+        <v>0</v>
+      </c>
+      <c r="BG4">
+        <v>0</v>
+      </c>
+      <c r="BH4">
+        <v>0</v>
+      </c>
+      <c r="BI4">
+        <v>0</v>
+      </c>
+      <c r="BJ4">
+        <v>0</v>
+      </c>
+      <c r="BK4">
+        <v>0</v>
+      </c>
+      <c r="BL4">
+        <v>0</v>
+      </c>
+      <c r="BM4">
+        <v>0</v>
+      </c>
+      <c r="BN4">
+        <v>0</v>
+      </c>
+      <c r="BO4">
+        <v>0</v>
+      </c>
+      <c r="BP4">
+        <v>0</v>
+      </c>
+      <c r="BQ4">
+        <v>0</v>
+      </c>
+      <c r="BR4">
+        <v>0</v>
+      </c>
+      <c r="BS4">
+        <v>0</v>
+      </c>
+      <c r="BT4">
+        <v>0</v>
+      </c>
+      <c r="BU4">
+        <v>0</v>
+      </c>
+      <c r="BV4">
+        <v>0</v>
+      </c>
+      <c r="BW4">
+        <v>0</v>
+      </c>
+      <c r="BX4">
+        <v>0</v>
+      </c>
+      <c r="BY4">
+        <v>0</v>
+      </c>
+      <c r="BZ4">
+        <v>0</v>
+      </c>
+      <c r="CA4">
+        <v>0</v>
+      </c>
+      <c r="CB4">
+        <v>0</v>
+      </c>
+      <c r="CC4">
+        <v>0</v>
+      </c>
+      <c r="CD4">
+        <v>0</v>
+      </c>
+      <c r="CE4">
+        <v>0</v>
+      </c>
+      <c r="CF4">
+        <v>0</v>
+      </c>
+      <c r="CG4">
+        <v>0</v>
+      </c>
+      <c r="CH4">
+        <v>0</v>
+      </c>
+      <c r="CI4">
+        <v>0</v>
+      </c>
+      <c r="CJ4">
+        <v>0</v>
+      </c>
+      <c r="CK4">
+        <v>0</v>
+      </c>
+      <c r="CL4">
+        <v>0</v>
+      </c>
+      <c r="CM4">
+        <v>0</v>
+      </c>
+      <c r="CN4">
+        <v>0</v>
+      </c>
+      <c r="CO4">
+        <v>0</v>
+      </c>
+      <c r="CP4">
+        <v>0</v>
+      </c>
+      <c r="CQ4">
+        <v>0</v>
+      </c>
+      <c r="CR4">
+        <v>0</v>
+      </c>
+      <c r="CS4">
+        <v>0</v>
+      </c>
+      <c r="CT4">
+        <v>0</v>
+      </c>
+      <c r="CU4">
+        <v>0</v>
+      </c>
+      <c r="CV4">
+        <v>0</v>
+      </c>
+      <c r="CW4">
+        <v>0</v>
+      </c>
+      <c r="CX4">
+        <v>0</v>
+      </c>
+      <c r="CY4">
+        <v>0</v>
+      </c>
+      <c r="CZ4">
+        <v>0</v>
+      </c>
+      <c r="DA4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:106" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <v>1</v>
-      </c>
-      <c r="V4">
-        <v>1</v>
-      </c>
-      <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
-      </c>
-      <c r="AJ4">
-        <v>0</v>
-      </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
-      <c r="AM4">
-        <v>0</v>
-      </c>
-      <c r="AN4">
-        <v>0</v>
-      </c>
-      <c r="AO4">
-        <v>0</v>
-      </c>
-      <c r="AP4">
-        <v>0</v>
-      </c>
-      <c r="AQ4">
-        <v>0</v>
-      </c>
-      <c r="AR4">
-        <v>0</v>
-      </c>
-      <c r="AS4">
-        <v>0</v>
-      </c>
-      <c r="AT4">
-        <v>0</v>
-      </c>
-      <c r="AU4">
-        <v>0</v>
-      </c>
-      <c r="AV4">
-        <v>0</v>
-      </c>
-      <c r="AW4">
-        <v>0</v>
-      </c>
-      <c r="AX4">
-        <v>0</v>
-      </c>
-      <c r="AY4">
-        <v>0</v>
-      </c>
-      <c r="AZ4">
-        <v>0</v>
-      </c>
-      <c r="BA4">
-        <v>0</v>
-      </c>
-      <c r="BB4">
-        <v>0</v>
-      </c>
-      <c r="BC4">
-        <v>0</v>
-      </c>
-      <c r="BD4">
-        <v>0</v>
-      </c>
-      <c r="BE4">
-        <v>0</v>
-      </c>
-      <c r="BF4">
-        <v>0</v>
-      </c>
-      <c r="BG4">
-        <v>0</v>
-      </c>
-      <c r="BH4">
-        <v>0</v>
-      </c>
-      <c r="BI4">
-        <v>0</v>
-      </c>
-      <c r="BJ4">
-        <v>0</v>
-      </c>
-      <c r="BK4">
-        <v>0</v>
-      </c>
-      <c r="BL4">
-        <v>0</v>
-      </c>
-      <c r="BM4">
-        <v>0</v>
-      </c>
-      <c r="BN4">
-        <v>0</v>
-      </c>
-      <c r="BO4">
-        <v>0</v>
-      </c>
-      <c r="BP4">
-        <v>0</v>
-      </c>
-      <c r="BQ4">
-        <v>0</v>
-      </c>
-      <c r="BR4">
-        <v>0</v>
-      </c>
-      <c r="BS4">
-        <v>0</v>
-      </c>
-      <c r="BT4">
-        <v>0</v>
-      </c>
-      <c r="BU4">
-        <v>0</v>
-      </c>
-      <c r="BV4">
-        <v>0</v>
-      </c>
-      <c r="BW4">
-        <v>0</v>
-      </c>
-      <c r="BX4">
-        <v>0</v>
-      </c>
-      <c r="BY4">
-        <v>0</v>
-      </c>
-      <c r="BZ4">
-        <v>0</v>
-      </c>
-      <c r="CA4">
-        <v>0</v>
-      </c>
-      <c r="CB4">
-        <v>0</v>
-      </c>
-      <c r="CC4">
-        <v>0</v>
-      </c>
-      <c r="CD4">
-        <v>0</v>
-      </c>
-      <c r="CE4">
-        <v>0</v>
-      </c>
-      <c r="CF4">
-        <v>0</v>
-      </c>
-      <c r="CG4">
-        <v>0</v>
-      </c>
-      <c r="CH4">
-        <v>0</v>
-      </c>
-      <c r="CI4">
-        <v>0</v>
-      </c>
-      <c r="CJ4">
-        <v>0</v>
-      </c>
-      <c r="CK4">
-        <v>0</v>
-      </c>
-      <c r="CL4">
-        <v>0</v>
-      </c>
-      <c r="CM4">
-        <v>0</v>
-      </c>
-      <c r="CN4">
-        <v>0</v>
-      </c>
-      <c r="CO4">
-        <v>0</v>
-      </c>
-      <c r="CP4">
-        <v>0</v>
-      </c>
-      <c r="CQ4">
-        <v>0</v>
-      </c>
-      <c r="CR4">
-        <v>0</v>
-      </c>
-      <c r="CS4">
-        <v>0</v>
-      </c>
-      <c r="CT4">
-        <v>0</v>
-      </c>
-      <c r="CU4">
-        <v>0</v>
-      </c>
-      <c r="CV4">
-        <v>0</v>
-      </c>
-      <c r="CW4">
-        <v>0</v>
-      </c>
-      <c r="CX4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -40163,10 +41257,19 @@
       <c r="CX5">
         <v>4</v>
       </c>
+      <c r="CY5">
+        <v>4</v>
+      </c>
+      <c r="CZ5">
+        <v>4</v>
+      </c>
+      <c r="DA5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -40471,10 +41574,19 @@
       <c r="CX6">
         <v>8</v>
       </c>
+      <c r="CY6">
+        <v>8</v>
+      </c>
+      <c r="CZ6">
+        <v>8</v>
+      </c>
+      <c r="DA6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -40779,10 +41891,19 @@
       <c r="CX7">
         <v>20</v>
       </c>
+      <c r="CY7">
+        <v>20</v>
+      </c>
+      <c r="CZ7">
+        <v>20</v>
+      </c>
+      <c r="DA7">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -41087,10 +42208,19 @@
       <c r="CX8">
         <v>67</v>
       </c>
+      <c r="CY8">
+        <v>67</v>
+      </c>
+      <c r="CZ8">
+        <v>67</v>
+      </c>
+      <c r="DA8">
+        <v>67</v>
+      </c>
     </row>
-    <row r="9" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9">
         <v>19</v>
@@ -41395,10 +42525,19 @@
       <c r="CX9">
         <v>136</v>
       </c>
+      <c r="CY9">
+        <v>136</v>
+      </c>
+      <c r="CZ9">
+        <v>136</v>
+      </c>
+      <c r="DA9">
+        <v>136</v>
+      </c>
     </row>
-    <row r="10" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B10">
         <v>15</v>
@@ -41703,10 +42842,19 @@
       <c r="CX10">
         <v>147</v>
       </c>
+      <c r="CY10">
+        <v>147</v>
+      </c>
+      <c r="CZ10">
+        <v>147</v>
+      </c>
+      <c r="DA10">
+        <v>147</v>
+      </c>
     </row>
-    <row r="11" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11">
         <v>15</v>
@@ -42009,6 +43157,15 @@
         <v>199</v>
       </c>
       <c r="CX11">
+        <v>199</v>
+      </c>
+      <c r="CY11">
+        <v>199</v>
+      </c>
+      <c r="CZ11">
+        <v>199</v>
+      </c>
+      <c r="DA11">
         <v>199</v>
       </c>
     </row>
@@ -42020,11 +43177,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A2:CR13"/>
+  <dimension ref="A2:CV13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CS2" sqref="CS2"/>
+      <selection pane="topRight" activeCell="CV2" sqref="CV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42033,7 +43190,7 @@
     <col min="57" max="57" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:96" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:100" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -42322,8 +43479,20 @@
       <c r="CR2" s="9">
         <v>44034</v>
       </c>
+      <c r="CS2" s="9">
+        <v>44035</v>
+      </c>
+      <c r="CT2" s="9">
+        <v>44036</v>
+      </c>
+      <c r="CU2" s="9">
+        <v>44037</v>
+      </c>
+      <c r="CV2" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -42612,8 +43781,17 @@
       <c r="CR3">
         <v>581</v>
       </c>
+      <c r="CS3">
+        <v>581</v>
+      </c>
+      <c r="CT3">
+        <v>581</v>
+      </c>
+      <c r="CU3">
+        <v>581</v>
+      </c>
     </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -42902,8 +44080,17 @@
       <c r="CR4">
         <v>64</v>
       </c>
+      <c r="CS4">
+        <v>64</v>
+      </c>
+      <c r="CT4">
+        <v>64</v>
+      </c>
+      <c r="CU4">
+        <v>64</v>
+      </c>
     </row>
-    <row r="5" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -43192,8 +44379,17 @@
       <c r="CR5">
         <v>33</v>
       </c>
+      <c r="CS5">
+        <v>33</v>
+      </c>
+      <c r="CT5">
+        <v>33</v>
+      </c>
+      <c r="CU5">
+        <v>33</v>
+      </c>
     </row>
-    <row r="6" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -43482,8 +44678,17 @@
       <c r="CR6">
         <v>33</v>
       </c>
+      <c r="CS6">
+        <v>33</v>
+      </c>
+      <c r="CT6">
+        <v>33</v>
+      </c>
+      <c r="CU6">
+        <v>33</v>
+      </c>
     </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -43772,8 +44977,17 @@
       <c r="CR7">
         <v>85</v>
       </c>
+      <c r="CS7">
+        <v>85</v>
+      </c>
+      <c r="CT7">
+        <v>85</v>
+      </c>
+      <c r="CU7">
+        <v>85</v>
+      </c>
     </row>
-    <row r="8" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -44062,8 +45276,17 @@
       <c r="CR8">
         <v>92</v>
       </c>
+      <c r="CS8">
+        <v>92</v>
+      </c>
+      <c r="CT8">
+        <v>92</v>
+      </c>
+      <c r="CU8">
+        <v>92</v>
+      </c>
     </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -44352,8 +45575,17 @@
       <c r="CR9">
         <v>50</v>
       </c>
+      <c r="CS9">
+        <v>50</v>
+      </c>
+      <c r="CT9">
+        <v>50</v>
+      </c>
+      <c r="CU9">
+        <v>50</v>
+      </c>
     </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -44642,8 +45874,17 @@
       <c r="CR10">
         <v>85</v>
       </c>
+      <c r="CS10">
+        <v>85</v>
+      </c>
+      <c r="CT10">
+        <v>85</v>
+      </c>
+      <c r="CU10">
+        <v>85</v>
+      </c>
     </row>
-    <row r="11" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -44932,8 +46173,17 @@
       <c r="CR11">
         <v>117</v>
       </c>
+      <c r="CS11">
+        <v>117</v>
+      </c>
+      <c r="CT11">
+        <v>117</v>
+      </c>
+      <c r="CU11">
+        <v>117</v>
+      </c>
     </row>
-    <row r="12" spans="1:96" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:100" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>71</v>
       </c>
@@ -45222,8 +46472,14 @@
       <c r="CR12">
         <v>21</v>
       </c>
+      <c r="CS12">
+        <v>21</v>
+      </c>
+      <c r="CT12">
+        <v>21</v>
+      </c>
     </row>
-    <row r="13" spans="1:96" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -45510,6 +46766,12 @@
         <v>1</v>
       </c>
       <c r="CR13">
+        <v>1</v>
+      </c>
+      <c r="CS13">
+        <v>1</v>
+      </c>
+      <c r="CT13">
         <v>1</v>
       </c>
     </row>
@@ -45521,10 +46783,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:BN23"/>
+  <dimension ref="A1:BR23"/>
   <sheetViews>
-    <sheetView topLeftCell="BK1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="BO5" sqref="BO5"/>
+    <sheetView topLeftCell="BB1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="BR5" sqref="BR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45533,54 +46795,54 @@
     <col min="42" max="45" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
-      <c r="C1" s="51" t="s">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="C1" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
+    <row r="2" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
+    <row r="3" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.3">
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
@@ -45595,7 +46857,7 @@
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.3">
       <c r="C5" s="9">
         <v>43971</v>
       </c>
@@ -45788,8 +47050,20 @@
       <c r="BN5" s="9">
         <v>44034</v>
       </c>
+      <c r="BO5" s="9">
+        <v>44035</v>
+      </c>
+      <c r="BP5" s="9">
+        <v>44036</v>
+      </c>
+      <c r="BQ5" s="9">
+        <v>44037</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>120</v>
       </c>
@@ -45985,8 +47259,17 @@
       <c r="BN6">
         <v>159</v>
       </c>
+      <c r="BO6">
+        <v>159</v>
+      </c>
+      <c r="BP6">
+        <v>159</v>
+      </c>
+      <c r="BQ6">
+        <v>159</v>
+      </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -46182,8 +47465,17 @@
       <c r="BN7">
         <v>36</v>
       </c>
+      <c r="BO7">
+        <v>36</v>
+      </c>
+      <c r="BP7">
+        <v>36</v>
+      </c>
+      <c r="BQ7">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>36</v>
       </c>
@@ -46191,7 +47483,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -46387,8 +47679,17 @@
       <c r="BN9">
         <v>1</v>
       </c>
+      <c r="BO9">
+        <v>1</v>
+      </c>
+      <c r="BP9">
+        <v>1</v>
+      </c>
+      <c r="BQ9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>121</v>
       </c>
@@ -46584,8 +47885,17 @@
       <c r="BN10">
         <v>23</v>
       </c>
+      <c r="BO10">
+        <v>23</v>
+      </c>
+      <c r="BP10">
+        <v>23</v>
+      </c>
+      <c r="BQ10">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>122</v>
       </c>
@@ -46781,8 +48091,17 @@
       <c r="BN11">
         <v>9</v>
       </c>
+      <c r="BO11">
+        <v>9</v>
+      </c>
+      <c r="BP11">
+        <v>9</v>
+      </c>
+      <c r="BQ11">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>37</v>
       </c>
@@ -46978,13 +48297,22 @@
       <c r="BN12">
         <v>3</v>
       </c>
+      <c r="BO12">
+        <v>3</v>
+      </c>
+      <c r="BP12">
+        <v>3</v>
+      </c>
+      <c r="BQ12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A14" s="31">
         <v>1</v>
       </c>
@@ -47180,8 +48508,17 @@
       <c r="BN14">
         <v>1</v>
       </c>
+      <c r="BO14">
+        <v>1</v>
+      </c>
+      <c r="BP14">
+        <v>1</v>
+      </c>
+      <c r="BQ14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
         <v>2</v>
       </c>
@@ -47377,8 +48714,17 @@
       <c r="BN15">
         <v>0</v>
       </c>
+      <c r="BO15">
+        <v>0</v>
+      </c>
+      <c r="BP15">
+        <v>0</v>
+      </c>
+      <c r="BQ15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
         <v>3</v>
       </c>
@@ -47574,8 +48920,17 @@
       <c r="BN16">
         <v>3</v>
       </c>
+      <c r="BO16">
+        <v>3</v>
+      </c>
+      <c r="BP16">
+        <v>3</v>
+      </c>
+      <c r="BQ16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A17" s="31">
         <v>4</v>
       </c>
@@ -47771,8 +49126,17 @@
       <c r="BN17">
         <v>12</v>
       </c>
+      <c r="BO17">
+        <v>12</v>
+      </c>
+      <c r="BP17">
+        <v>12</v>
+      </c>
+      <c r="BQ17">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
         <v>5</v>
       </c>
@@ -47968,8 +49332,17 @@
       <c r="BN18">
         <v>3</v>
       </c>
+      <c r="BO18">
+        <v>3</v>
+      </c>
+      <c r="BP18">
+        <v>3</v>
+      </c>
+      <c r="BQ18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A19" s="31">
         <v>6</v>
       </c>
@@ -48165,8 +49538,17 @@
       <c r="BN19">
         <v>2</v>
       </c>
+      <c r="BO19">
+        <v>2</v>
+      </c>
+      <c r="BP19">
+        <v>2</v>
+      </c>
+      <c r="BQ19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <v>7</v>
       </c>
@@ -48362,8 +49744,17 @@
       <c r="BN20">
         <v>2</v>
       </c>
+      <c r="BO20">
+        <v>2</v>
+      </c>
+      <c r="BP20">
+        <v>2</v>
+      </c>
+      <c r="BQ20">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A21" s="31">
         <v>8</v>
       </c>
@@ -48559,8 +49950,17 @@
       <c r="BN21">
         <v>6</v>
       </c>
+      <c r="BO21">
+        <v>6</v>
+      </c>
+      <c r="BP21">
+        <v>6</v>
+      </c>
+      <c r="BQ21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="1:66" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:69" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
@@ -48756,8 +50156,17 @@
       <c r="BN22">
         <v>4</v>
       </c>
+      <c r="BO22">
+        <v>4</v>
+      </c>
+      <c r="BP22">
+        <v>4</v>
+      </c>
+      <c r="BQ22">
+        <v>4</v>
+      </c>
     </row>
-    <row r="23" spans="1:66" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:69" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>123</v>
       </c>
@@ -48951,6 +50360,15 @@
         <v>3</v>
       </c>
       <c r="BN23">
+        <v>3</v>
+      </c>
+      <c r="BO23">
+        <v>3</v>
+      </c>
+      <c r="BP23">
+        <v>3</v>
+      </c>
+      <c r="BQ23">
         <v>3</v>
       </c>
     </row>
@@ -48982,18 +50400,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
+      <c r="A1" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="55" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -49002,7 +50420,7 @@
       <c r="C2" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="56" t="s">
         <v>114</v>
       </c>
       <c r="E2" s="29" t="s">
@@ -49016,10 +50434,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="55"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="25" t="s">
         <v>92</v>
       </c>
@@ -49031,10 +50449,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="55"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="25" t="s">
         <v>86</v>
       </c>
@@ -49044,10 +50462,10 @@
       <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
-      <c r="D5" s="55"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="25" t="s">
         <v>87</v>
       </c>
@@ -49055,10 +50473,10 @@
       <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
+      <c r="A6" s="55"/>
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="55"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="25" t="s">
         <v>88</v>
       </c>
@@ -49066,10 +50484,10 @@
       <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:7" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26"/>
-      <c r="D7" s="55"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="25" t="s">
         <v>93</v>
       </c>
@@ -49081,7 +50499,7 @@
         <v>94</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C8" s="28">
         <v>2</v>
@@ -49090,7 +50508,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F8" s="28">
         <v>0</v>
@@ -49101,7 +50519,7 @@
     </row>
     <row r="9" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>95</v>
@@ -49113,7 +50531,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="F9" s="28">
         <v>0</v>
@@ -49127,7 +50545,7 @@
         <v>96</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C10" s="28">
         <v>5</v>
@@ -49136,7 +50554,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="F10" s="28">
         <v>1</v>
@@ -49150,7 +50568,7 @@
         <v>97</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C11" s="28">
         <v>24</v>
@@ -49159,7 +50577,7 @@
         <v>86</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F11" s="28">
         <v>0</v>
@@ -49173,16 +50591,16 @@
         <v>98</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C12" s="28">
         <v>2</v>
       </c>
       <c r="D12" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F12" s="28">
         <v>0</v>
@@ -49219,7 +50637,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C14" s="28">
         <v>2</v>
@@ -49242,10 +50660,10 @@
         <v>100</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C15" s="28">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D15" s="28">
         <v>55</v>
@@ -49265,7 +50683,7 @@
         <v>116</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C16" s="28">
         <v>4</v>
@@ -49274,13 +50692,13 @@
         <v>18</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F16" s="28">
         <v>0</v>
       </c>
       <c r="G16" s="28">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -49288,7 +50706,7 @@
         <v>101</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C17" s="28">
         <v>9</v>
@@ -49311,13 +50729,13 @@
         <v>102</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C18" s="28">
         <v>9</v>
       </c>
       <c r="D18" s="28">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E18" s="28" t="s">
         <v>136</v>
@@ -49334,7 +50752,7 @@
         <v>103</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C19" s="28">
         <v>14</v>
@@ -49343,7 +50761,7 @@
         <v>47</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="F19" s="28">
         <v>0</v>
@@ -49357,7 +50775,7 @@
         <v>104</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C20" s="28">
         <v>14</v>
@@ -49380,7 +50798,7 @@
         <v>105</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C21" s="28">
         <v>1</v>
@@ -49389,7 +50807,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F21" s="28">
         <v>0</v>
@@ -49403,16 +50821,16 @@
         <v>107</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C22" s="28">
         <v>28</v>
       </c>
       <c r="D22" s="28">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="F22" s="28">
         <v>2</v>
@@ -49426,7 +50844,7 @@
         <v>108</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C23" s="28">
         <v>7</v>
@@ -49449,7 +50867,7 @@
         <v>109</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C24" s="28">
         <v>7</v>
@@ -49458,7 +50876,7 @@
         <v>10</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F24" s="28">
         <v>0</v>
@@ -49472,7 +50890,7 @@
         <v>117</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C25" s="28">
         <v>20</v>
@@ -49481,7 +50899,7 @@
         <v>58</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="F25" s="28">
         <v>1</v>
@@ -49498,10 +50916,10 @@
         <v>177</v>
       </c>
       <c r="C26" s="28">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D26" s="28">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E26" s="28" t="s">
         <v>178</v>
@@ -49510,7 +50928,7 @@
         <v>7</v>
       </c>
       <c r="G26" s="28">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H26" s="46"/>
     </row>
@@ -49753,18 +51171,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49787,26 +51205,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD396E8E-4714-4CC9-8EAA-3025B907ED6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DEDEF4E-2681-4E64-A6E5-9E41742A3664}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="8e61eea9-d51d-4f9c-960b-1b037651d93e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="248ed0f8-11d3-4141-bb91-6b69a0801941"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>